<commit_message>
Update lands data - 2025-09-26 20:29
</commit_message>
<xml_diff>
--- a/lands-scraped.xlsx
+++ b/lands-scraped.xlsx
@@ -27236,7 +27236,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -27273,996 +27273,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>8757</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>8758</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>2118</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>8759</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>8760</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>8761</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>8762</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>8763</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>8764</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>8765</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>8766</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>8767</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>526</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>8768</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>8769</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>8770</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8771</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>526</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>8772</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>8773</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>8774</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8775</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>526</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>3145</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>8776</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>8777</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>8778</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>526</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>8779</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>8780</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>8781</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>8782</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>982</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>8783</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>8784</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>8785</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>8786</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>8787</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>982</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>8788</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>8789</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>8790</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>8791</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>982</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>753</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>8792</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>8793</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>8794</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>982</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>2920</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>8795</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>8796</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>8797</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>8798</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>1533</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>8799</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>8800</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>8801</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>8802</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>8803</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>1533</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>8804</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>8805</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>8806</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>8807</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>8808</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>1533</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>8809</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>8810</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>8806</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>8811</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>8812</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>1533</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>8813</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>8814</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>8815</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>8816</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>1533</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>8817</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>8818</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>8814</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>8819</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>8820</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>2434</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>2840</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>8821</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>8822</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>8823</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>8824</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>3144</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>3228</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>8825</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>8826</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>8827</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>3144</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>8828</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>8829</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>961</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>3381</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>3534</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>8830</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>8831</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>961</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>3381</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>3534</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>8832</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>8833</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>961</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>3381</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>3534</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>8832</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>8834</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>8835</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>3381</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>8836</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>8837</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>8838</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>8839</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>3615</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>8840</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>8841</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>8842</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>8843</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>3615</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>8844</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>8845</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>8846</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>8847</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>8848</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>4336</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>8849</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>8850</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>8851</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>8852</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>8853</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>4336</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>8854</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>8855</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>8856</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>8857</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>8858</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>4947</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>2952</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>8859</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>8860</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>8861</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>8862</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>5158</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>5293</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>8863</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>8864</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>8865</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>5158</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>3428</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>8866</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>8867</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>8868</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>8869</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>5158</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>597</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>8870</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>8871</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>8872</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>5158</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>2058</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>8873</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>8874</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>8875</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>8876</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>5978</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>641</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>8877</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>8878</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>8879</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>8880</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>5978</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>641</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>8870</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>8881</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>8054</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>5978</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>480</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>8882</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>8883</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>8884</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>8885</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>6104</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>1483</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>8886</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>8887</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>8888</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>8889</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>6104</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>1796</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>8890</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>8891</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>8892</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>8054</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>6104</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>8893</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>8894</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>8895</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>8896</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>8897</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>6104</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>699</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>8898</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>8899</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>8900</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>8901</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>6744</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>8902</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>8903</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>8904</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>8905</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>6744</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>6938</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>6939</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>8906</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>8907</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>8908</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>7265</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>8909</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>8910</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>8911</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>8912</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>7265</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>8913</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>8914</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>8915</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>8916</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>7847</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>2827</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>8917</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>8918</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>8919</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>8920</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>7949</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>5445</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>8921</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>8922</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>8923</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>8924</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>7949</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>8101</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>8925</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>8926</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>8927</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>1924</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>7949</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>8928</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>8929</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>8930</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>5268</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>8246</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>8931</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>8932</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
-    <hyperlink ref="A10" r:id="rId9"/>
-    <hyperlink ref="A11" r:id="rId10"/>
-    <hyperlink ref="A12" r:id="rId11"/>
-    <hyperlink ref="A13" r:id="rId12"/>
-    <hyperlink ref="A14" r:id="rId13"/>
-    <hyperlink ref="A15" r:id="rId14"/>
-    <hyperlink ref="A16" r:id="rId15"/>
-    <hyperlink ref="A17" r:id="rId16"/>
-    <hyperlink ref="A18" r:id="rId17"/>
-    <hyperlink ref="A19" r:id="rId18"/>
-    <hyperlink ref="A20" r:id="rId19"/>
-    <hyperlink ref="A21" r:id="rId20"/>
-    <hyperlink ref="A22" r:id="rId21"/>
-    <hyperlink ref="A23" r:id="rId22"/>
-    <hyperlink ref="A24" r:id="rId23"/>
-    <hyperlink ref="A25" r:id="rId24"/>
-    <hyperlink ref="A26" r:id="rId25"/>
-    <hyperlink ref="A27" r:id="rId26"/>
-    <hyperlink ref="A28" r:id="rId27"/>
-    <hyperlink ref="A29" r:id="rId28"/>
-    <hyperlink ref="A30" r:id="rId29"/>
-    <hyperlink ref="A31" r:id="rId30"/>
-    <hyperlink ref="A32" r:id="rId31"/>
-    <hyperlink ref="A33" r:id="rId32"/>
-    <hyperlink ref="A34" r:id="rId33"/>
-    <hyperlink ref="A35" r:id="rId34"/>
-    <hyperlink ref="A36" r:id="rId35"/>
-    <hyperlink ref="A37" r:id="rId36"/>
-    <hyperlink ref="A38" r:id="rId37"/>
-    <hyperlink ref="A39" r:id="rId38"/>
-    <hyperlink ref="A40" r:id="rId39"/>
-    <hyperlink ref="A41" r:id="rId40"/>
-    <hyperlink ref="A42" r:id="rId41"/>
-    <hyperlink ref="A43" r:id="rId42"/>
-    <hyperlink ref="A44" r:id="rId43"/>
-    <hyperlink ref="A45" r:id="rId44"/>
-    <hyperlink ref="A46" r:id="rId45"/>
-    <hyperlink ref="A47" r:id="rId46"/>
-    <hyperlink ref="A48" r:id="rId47"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
@@ -28270,7 +27281,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2164"/>
+  <dimension ref="A1:F2211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -71566,6 +70577,946 @@
       </c>
       <c r="F2164" s="3" t="s">
         <v>8756</v>
+      </c>
+    </row>
+    <row r="2165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2165" s="4" t="s">
+        <v>8757</v>
+      </c>
+      <c r="B2165" s="3" t="s">
+        <v>8758</v>
+      </c>
+      <c r="C2165" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D2165" s="3" t="s">
+        <v>2118</v>
+      </c>
+      <c r="E2165" s="3" t="s">
+        <v>8759</v>
+      </c>
+      <c r="F2165" s="3" t="s">
+        <v>8760</v>
+      </c>
+    </row>
+    <row r="2166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2166" s="4" t="s">
+        <v>8761</v>
+      </c>
+      <c r="B2166" s="3" t="s">
+        <v>8762</v>
+      </c>
+      <c r="C2166" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="D2166" s="3" t="s">
+        <v>8763</v>
+      </c>
+      <c r="E2166" s="3" t="s">
+        <v>8764</v>
+      </c>
+      <c r="F2166" s="3" t="s">
+        <v>8765</v>
+      </c>
+    </row>
+    <row r="2167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2167" s="4" t="s">
+        <v>8766</v>
+      </c>
+      <c r="B2167" s="3" t="s">
+        <v>8767</v>
+      </c>
+      <c r="C2167" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="D2167" s="3" t="s">
+        <v>8768</v>
+      </c>
+      <c r="E2167" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2167" s="3" t="s">
+        <v>8769</v>
+      </c>
+    </row>
+    <row r="2168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2168" s="4" t="s">
+        <v>8770</v>
+      </c>
+      <c r="B2168" s="3" t="s">
+        <v>8771</v>
+      </c>
+      <c r="C2168" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="D2168" s="3" t="s">
+        <v>8772</v>
+      </c>
+      <c r="E2168" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2168" s="3" t="s">
+        <v>8773</v>
+      </c>
+    </row>
+    <row r="2169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2169" s="4" t="s">
+        <v>8774</v>
+      </c>
+      <c r="B2169" s="3" t="s">
+        <v>8775</v>
+      </c>
+      <c r="C2169" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="D2169" s="3" t="s">
+        <v>3145</v>
+      </c>
+      <c r="E2169" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2169" s="3" t="s">
+        <v>8776</v>
+      </c>
+    </row>
+    <row r="2170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2170" s="4" t="s">
+        <v>8777</v>
+      </c>
+      <c r="B2170" s="3" t="s">
+        <v>8778</v>
+      </c>
+      <c r="C2170" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="D2170" s="3" t="s">
+        <v>8779</v>
+      </c>
+      <c r="E2170" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2170" s="3" t="s">
+        <v>8780</v>
+      </c>
+    </row>
+    <row r="2171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2171" s="4" t="s">
+        <v>8781</v>
+      </c>
+      <c r="B2171" s="3" t="s">
+        <v>8782</v>
+      </c>
+      <c r="C2171" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="D2171" s="3" t="s">
+        <v>8783</v>
+      </c>
+      <c r="E2171" s="3" t="s">
+        <v>8784</v>
+      </c>
+      <c r="F2171" s="3" t="s">
+        <v>8785</v>
+      </c>
+    </row>
+    <row r="2172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2172" s="4" t="s">
+        <v>8786</v>
+      </c>
+      <c r="B2172" s="3" t="s">
+        <v>8787</v>
+      </c>
+      <c r="C2172" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="D2172" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2172" s="3" t="s">
+        <v>8788</v>
+      </c>
+      <c r="F2172" s="3" t="s">
+        <v>8789</v>
+      </c>
+    </row>
+    <row r="2173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2173" s="4" t="s">
+        <v>8790</v>
+      </c>
+      <c r="B2173" s="3" t="s">
+        <v>8791</v>
+      </c>
+      <c r="C2173" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="D2173" s="3" t="s">
+        <v>753</v>
+      </c>
+      <c r="E2173" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2173" s="3" t="s">
+        <v>8792</v>
+      </c>
+    </row>
+    <row r="2174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2174" s="4" t="s">
+        <v>8793</v>
+      </c>
+      <c r="B2174" s="3" t="s">
+        <v>8794</v>
+      </c>
+      <c r="C2174" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="D2174" s="3" t="s">
+        <v>2920</v>
+      </c>
+      <c r="E2174" s="3" t="s">
+        <v>8795</v>
+      </c>
+      <c r="F2174" s="3" t="s">
+        <v>8796</v>
+      </c>
+    </row>
+    <row r="2175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2175" s="4" t="s">
+        <v>8797</v>
+      </c>
+      <c r="B2175" s="3" t="s">
+        <v>8798</v>
+      </c>
+      <c r="C2175" s="3" t="s">
+        <v>1533</v>
+      </c>
+      <c r="D2175" s="3" t="s">
+        <v>8799</v>
+      </c>
+      <c r="E2175" s="3" t="s">
+        <v>8800</v>
+      </c>
+      <c r="F2175" s="3" t="s">
+        <v>8801</v>
+      </c>
+    </row>
+    <row r="2176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2176" s="4" t="s">
+        <v>8802</v>
+      </c>
+      <c r="B2176" s="3" t="s">
+        <v>8803</v>
+      </c>
+      <c r="C2176" s="3" t="s">
+        <v>1533</v>
+      </c>
+      <c r="D2176" s="3" t="s">
+        <v>8804</v>
+      </c>
+      <c r="E2176" s="3" t="s">
+        <v>8805</v>
+      </c>
+      <c r="F2176" s="3" t="s">
+        <v>8806</v>
+      </c>
+    </row>
+    <row r="2177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2177" s="4" t="s">
+        <v>8807</v>
+      </c>
+      <c r="B2177" s="3" t="s">
+        <v>8808</v>
+      </c>
+      <c r="C2177" s="3" t="s">
+        <v>1533</v>
+      </c>
+      <c r="D2177" s="3" t="s">
+        <v>8809</v>
+      </c>
+      <c r="E2177" s="3" t="s">
+        <v>8810</v>
+      </c>
+      <c r="F2177" s="3" t="s">
+        <v>8806</v>
+      </c>
+    </row>
+    <row r="2178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2178" s="4" t="s">
+        <v>8811</v>
+      </c>
+      <c r="B2178" s="3" t="s">
+        <v>8812</v>
+      </c>
+      <c r="C2178" s="3" t="s">
+        <v>1533</v>
+      </c>
+      <c r="D2178" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2178" s="3" t="s">
+        <v>8813</v>
+      </c>
+      <c r="F2178" s="3" t="s">
+        <v>8814</v>
+      </c>
+    </row>
+    <row r="2179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2179" s="4" t="s">
+        <v>8815</v>
+      </c>
+      <c r="B2179" s="3" t="s">
+        <v>8816</v>
+      </c>
+      <c r="C2179" s="3" t="s">
+        <v>1533</v>
+      </c>
+      <c r="D2179" s="3" t="s">
+        <v>8817</v>
+      </c>
+      <c r="E2179" s="3" t="s">
+        <v>8818</v>
+      </c>
+      <c r="F2179" s="3" t="s">
+        <v>8814</v>
+      </c>
+    </row>
+    <row r="2180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2180" s="4" t="s">
+        <v>8819</v>
+      </c>
+      <c r="B2180" s="3" t="s">
+        <v>8820</v>
+      </c>
+      <c r="C2180" s="3" t="s">
+        <v>2434</v>
+      </c>
+      <c r="D2180" s="3" t="s">
+        <v>2840</v>
+      </c>
+      <c r="E2180" s="3" t="s">
+        <v>8821</v>
+      </c>
+      <c r="F2180" s="3" t="s">
+        <v>8822</v>
+      </c>
+    </row>
+    <row r="2181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2181" s="4" t="s">
+        <v>8823</v>
+      </c>
+      <c r="B2181" s="3" t="s">
+        <v>8824</v>
+      </c>
+      <c r="C2181" s="3" t="s">
+        <v>3144</v>
+      </c>
+      <c r="D2181" s="3" t="s">
+        <v>3228</v>
+      </c>
+      <c r="E2181" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2181" s="3" t="s">
+        <v>8825</v>
+      </c>
+    </row>
+    <row r="2182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2182" s="4" t="s">
+        <v>8826</v>
+      </c>
+      <c r="B2182" s="3" t="s">
+        <v>8827</v>
+      </c>
+      <c r="C2182" s="3" t="s">
+        <v>3144</v>
+      </c>
+      <c r="D2182" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2182" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2182" s="3" t="s">
+        <v>8828</v>
+      </c>
+    </row>
+    <row r="2183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2183" s="4" t="s">
+        <v>8829</v>
+      </c>
+      <c r="B2183" s="3" t="s">
+        <v>961</v>
+      </c>
+      <c r="C2183" s="3" t="s">
+        <v>3381</v>
+      </c>
+      <c r="D2183" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E2183" s="3" t="s">
+        <v>3534</v>
+      </c>
+      <c r="F2183" s="3" t="s">
+        <v>8830</v>
+      </c>
+    </row>
+    <row r="2184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2184" s="4" t="s">
+        <v>8831</v>
+      </c>
+      <c r="B2184" s="3" t="s">
+        <v>961</v>
+      </c>
+      <c r="C2184" s="3" t="s">
+        <v>3381</v>
+      </c>
+      <c r="D2184" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E2184" s="3" t="s">
+        <v>3534</v>
+      </c>
+      <c r="F2184" s="3" t="s">
+        <v>8832</v>
+      </c>
+    </row>
+    <row r="2185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2185" s="4" t="s">
+        <v>8833</v>
+      </c>
+      <c r="B2185" s="3" t="s">
+        <v>961</v>
+      </c>
+      <c r="C2185" s="3" t="s">
+        <v>3381</v>
+      </c>
+      <c r="D2185" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E2185" s="3" t="s">
+        <v>3534</v>
+      </c>
+      <c r="F2185" s="3" t="s">
+        <v>8832</v>
+      </c>
+    </row>
+    <row r="2186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2186" s="4" t="s">
+        <v>8834</v>
+      </c>
+      <c r="B2186" s="3" t="s">
+        <v>8835</v>
+      </c>
+      <c r="C2186" s="3" t="s">
+        <v>3381</v>
+      </c>
+      <c r="D2186" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E2186" s="3" t="s">
+        <v>8836</v>
+      </c>
+      <c r="F2186" s="3" t="s">
+        <v>8837</v>
+      </c>
+    </row>
+    <row r="2187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2187" s="4" t="s">
+        <v>8838</v>
+      </c>
+      <c r="B2187" s="3" t="s">
+        <v>8839</v>
+      </c>
+      <c r="C2187" s="3" t="s">
+        <v>3615</v>
+      </c>
+      <c r="D2187" s="3" t="s">
+        <v>8840</v>
+      </c>
+      <c r="E2187" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2187" s="3" t="s">
+        <v>8841</v>
+      </c>
+    </row>
+    <row r="2188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2188" s="4" t="s">
+        <v>8842</v>
+      </c>
+      <c r="B2188" s="3" t="s">
+        <v>8843</v>
+      </c>
+      <c r="C2188" s="3" t="s">
+        <v>3615</v>
+      </c>
+      <c r="D2188" s="3" t="s">
+        <v>8844</v>
+      </c>
+      <c r="E2188" s="3" t="s">
+        <v>8845</v>
+      </c>
+      <c r="F2188" s="3" t="s">
+        <v>8846</v>
+      </c>
+    </row>
+    <row r="2189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2189" s="4" t="s">
+        <v>8847</v>
+      </c>
+      <c r="B2189" s="3" t="s">
+        <v>8848</v>
+      </c>
+      <c r="C2189" s="3" t="s">
+        <v>4336</v>
+      </c>
+      <c r="D2189" s="3" t="s">
+        <v>8849</v>
+      </c>
+      <c r="E2189" s="3" t="s">
+        <v>8850</v>
+      </c>
+      <c r="F2189" s="3" t="s">
+        <v>8851</v>
+      </c>
+    </row>
+    <row r="2190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2190" s="4" t="s">
+        <v>8852</v>
+      </c>
+      <c r="B2190" s="3" t="s">
+        <v>8853</v>
+      </c>
+      <c r="C2190" s="3" t="s">
+        <v>4336</v>
+      </c>
+      <c r="D2190" s="3" t="s">
+        <v>8854</v>
+      </c>
+      <c r="E2190" s="3" t="s">
+        <v>8855</v>
+      </c>
+      <c r="F2190" s="3" t="s">
+        <v>8856</v>
+      </c>
+    </row>
+    <row r="2191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2191" s="4" t="s">
+        <v>8857</v>
+      </c>
+      <c r="B2191" s="3" t="s">
+        <v>8858</v>
+      </c>
+      <c r="C2191" s="3" t="s">
+        <v>4947</v>
+      </c>
+      <c r="D2191" s="3" t="s">
+        <v>2952</v>
+      </c>
+      <c r="E2191" s="3" t="s">
+        <v>8859</v>
+      </c>
+      <c r="F2191" s="3" t="s">
+        <v>8860</v>
+      </c>
+    </row>
+    <row r="2192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2192" s="4" t="s">
+        <v>8861</v>
+      </c>
+      <c r="B2192" s="3" t="s">
+        <v>8862</v>
+      </c>
+      <c r="C2192" s="3" t="s">
+        <v>5158</v>
+      </c>
+      <c r="D2192" s="3" t="s">
+        <v>5293</v>
+      </c>
+      <c r="E2192" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2192" s="3" t="s">
+        <v>8863</v>
+      </c>
+    </row>
+    <row r="2193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2193" s="4" t="s">
+        <v>8864</v>
+      </c>
+      <c r="B2193" s="3" t="s">
+        <v>8865</v>
+      </c>
+      <c r="C2193" s="3" t="s">
+        <v>5158</v>
+      </c>
+      <c r="D2193" s="3" t="s">
+        <v>3428</v>
+      </c>
+      <c r="E2193" s="3" t="s">
+        <v>8866</v>
+      </c>
+      <c r="F2193" s="3" t="s">
+        <v>8867</v>
+      </c>
+    </row>
+    <row r="2194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2194" s="4" t="s">
+        <v>8868</v>
+      </c>
+      <c r="B2194" s="3" t="s">
+        <v>8869</v>
+      </c>
+      <c r="C2194" s="3" t="s">
+        <v>5158</v>
+      </c>
+      <c r="D2194" s="3" t="s">
+        <v>597</v>
+      </c>
+      <c r="E2194" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2194" s="3" t="s">
+        <v>8870</v>
+      </c>
+    </row>
+    <row r="2195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2195" s="4" t="s">
+        <v>8871</v>
+      </c>
+      <c r="B2195" s="3" t="s">
+        <v>8872</v>
+      </c>
+      <c r="C2195" s="3" t="s">
+        <v>5158</v>
+      </c>
+      <c r="D2195" s="3" t="s">
+        <v>2058</v>
+      </c>
+      <c r="E2195" s="3" t="s">
+        <v>8873</v>
+      </c>
+      <c r="F2195" s="3" t="s">
+        <v>8874</v>
+      </c>
+    </row>
+    <row r="2196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2196" s="4" t="s">
+        <v>8875</v>
+      </c>
+      <c r="B2196" s="3" t="s">
+        <v>8876</v>
+      </c>
+      <c r="C2196" s="3" t="s">
+        <v>5978</v>
+      </c>
+      <c r="D2196" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="E2196" s="3" t="s">
+        <v>8877</v>
+      </c>
+      <c r="F2196" s="3" t="s">
+        <v>8878</v>
+      </c>
+    </row>
+    <row r="2197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2197" s="4" t="s">
+        <v>8879</v>
+      </c>
+      <c r="B2197" s="3" t="s">
+        <v>8880</v>
+      </c>
+      <c r="C2197" s="3" t="s">
+        <v>5978</v>
+      </c>
+      <c r="D2197" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="E2197" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2197" s="3" t="s">
+        <v>8870</v>
+      </c>
+    </row>
+    <row r="2198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2198" s="4" t="s">
+        <v>8881</v>
+      </c>
+      <c r="B2198" s="3" t="s">
+        <v>8054</v>
+      </c>
+      <c r="C2198" s="3" t="s">
+        <v>5978</v>
+      </c>
+      <c r="D2198" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="E2198" s="3" t="s">
+        <v>8882</v>
+      </c>
+      <c r="F2198" s="3" t="s">
+        <v>8883</v>
+      </c>
+    </row>
+    <row r="2199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2199" s="4" t="s">
+        <v>8884</v>
+      </c>
+      <c r="B2199" s="3" t="s">
+        <v>8885</v>
+      </c>
+      <c r="C2199" s="3" t="s">
+        <v>6104</v>
+      </c>
+      <c r="D2199" s="3" t="s">
+        <v>1483</v>
+      </c>
+      <c r="E2199" s="3" t="s">
+        <v>8886</v>
+      </c>
+      <c r="F2199" s="3" t="s">
+        <v>8887</v>
+      </c>
+    </row>
+    <row r="2200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2200" s="4" t="s">
+        <v>8888</v>
+      </c>
+      <c r="B2200" s="3" t="s">
+        <v>8889</v>
+      </c>
+      <c r="C2200" s="3" t="s">
+        <v>6104</v>
+      </c>
+      <c r="D2200" s="3" t="s">
+        <v>1796</v>
+      </c>
+      <c r="E2200" s="3" t="s">
+        <v>8890</v>
+      </c>
+      <c r="F2200" s="3" t="s">
+        <v>8891</v>
+      </c>
+    </row>
+    <row r="2201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2201" s="4" t="s">
+        <v>8892</v>
+      </c>
+      <c r="B2201" s="3" t="s">
+        <v>8054</v>
+      </c>
+      <c r="C2201" s="3" t="s">
+        <v>6104</v>
+      </c>
+      <c r="D2201" s="3" t="s">
+        <v>8893</v>
+      </c>
+      <c r="E2201" s="3" t="s">
+        <v>8894</v>
+      </c>
+      <c r="F2201" s="3" t="s">
+        <v>8895</v>
+      </c>
+    </row>
+    <row r="2202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2202" s="4" t="s">
+        <v>8896</v>
+      </c>
+      <c r="B2202" s="3" t="s">
+        <v>8897</v>
+      </c>
+      <c r="C2202" s="3" t="s">
+        <v>6104</v>
+      </c>
+      <c r="D2202" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="E2202" s="3" t="s">
+        <v>8898</v>
+      </c>
+      <c r="F2202" s="3" t="s">
+        <v>8899</v>
+      </c>
+    </row>
+    <row r="2203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2203" s="4" t="s">
+        <v>8900</v>
+      </c>
+      <c r="B2203" s="3" t="s">
+        <v>8901</v>
+      </c>
+      <c r="C2203" s="3" t="s">
+        <v>6744</v>
+      </c>
+      <c r="D2203" s="3" t="s">
+        <v>8902</v>
+      </c>
+      <c r="E2203" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2203" s="3" t="s">
+        <v>8903</v>
+      </c>
+    </row>
+    <row r="2204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2204" s="4" t="s">
+        <v>8904</v>
+      </c>
+      <c r="B2204" s="3" t="s">
+        <v>8905</v>
+      </c>
+      <c r="C2204" s="3" t="s">
+        <v>6744</v>
+      </c>
+      <c r="D2204" s="3" t="s">
+        <v>6938</v>
+      </c>
+      <c r="E2204" s="3" t="s">
+        <v>6939</v>
+      </c>
+      <c r="F2204" s="3" t="s">
+        <v>8906</v>
+      </c>
+    </row>
+    <row r="2205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2205" s="4" t="s">
+        <v>8907</v>
+      </c>
+      <c r="B2205" s="3" t="s">
+        <v>8908</v>
+      </c>
+      <c r="C2205" s="3" t="s">
+        <v>7265</v>
+      </c>
+      <c r="D2205" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2205" s="3" t="s">
+        <v>8909</v>
+      </c>
+      <c r="F2205" s="3" t="s">
+        <v>8910</v>
+      </c>
+    </row>
+    <row r="2206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2206" s="4" t="s">
+        <v>8911</v>
+      </c>
+      <c r="B2206" s="3" t="s">
+        <v>8912</v>
+      </c>
+      <c r="C2206" s="3" t="s">
+        <v>7265</v>
+      </c>
+      <c r="D2206" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="E2206" s="3" t="s">
+        <v>8913</v>
+      </c>
+      <c r="F2206" s="3" t="s">
+        <v>8914</v>
+      </c>
+    </row>
+    <row r="2207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2207" s="4" t="s">
+        <v>8915</v>
+      </c>
+      <c r="B2207" s="3" t="s">
+        <v>8916</v>
+      </c>
+      <c r="C2207" s="3" t="s">
+        <v>7847</v>
+      </c>
+      <c r="D2207" s="3" t="s">
+        <v>2827</v>
+      </c>
+      <c r="E2207" s="3" t="s">
+        <v>8917</v>
+      </c>
+      <c r="F2207" s="3" t="s">
+        <v>8918</v>
+      </c>
+    </row>
+    <row r="2208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2208" s="4" t="s">
+        <v>8919</v>
+      </c>
+      <c r="B2208" s="3" t="s">
+        <v>8920</v>
+      </c>
+      <c r="C2208" s="3" t="s">
+        <v>7949</v>
+      </c>
+      <c r="D2208" s="3" t="s">
+        <v>5445</v>
+      </c>
+      <c r="E2208" s="3" t="s">
+        <v>8921</v>
+      </c>
+      <c r="F2208" s="3" t="s">
+        <v>8922</v>
+      </c>
+    </row>
+    <row r="2209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2209" s="4" t="s">
+        <v>8923</v>
+      </c>
+      <c r="B2209" s="3" t="s">
+        <v>8924</v>
+      </c>
+      <c r="C2209" s="3" t="s">
+        <v>7949</v>
+      </c>
+      <c r="D2209" s="3" t="s">
+        <v>8101</v>
+      </c>
+      <c r="E2209" s="3" t="s">
+        <v>8925</v>
+      </c>
+      <c r="F2209" s="3" t="s">
+        <v>8926</v>
+      </c>
+    </row>
+    <row r="2210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2210" s="4" t="s">
+        <v>8927</v>
+      </c>
+      <c r="B2210" s="3" t="s">
+        <v>1924</v>
+      </c>
+      <c r="C2210" s="3" t="s">
+        <v>7949</v>
+      </c>
+      <c r="D2210" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2210" s="3" t="s">
+        <v>8928</v>
+      </c>
+      <c r="F2210" s="3" t="s">
+        <v>8929</v>
+      </c>
+    </row>
+    <row r="2211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2211" s="4" t="s">
+        <v>8930</v>
+      </c>
+      <c r="B2211" s="3" t="s">
+        <v>5268</v>
+      </c>
+      <c r="C2211" s="3" t="s">
+        <v>8246</v>
+      </c>
+      <c r="D2211" s="3" t="s">
+        <v>8931</v>
+      </c>
+      <c r="E2211" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2211" s="3" t="s">
+        <v>8932</v>
       </c>
     </row>
   </sheetData>
@@ -73733,6 +73684,53 @@
     <hyperlink ref="A2162" r:id="rId2161"/>
     <hyperlink ref="A2163" r:id="rId2162"/>
     <hyperlink ref="A2164" r:id="rId2163"/>
+    <hyperlink ref="A2165" r:id="rId2164"/>
+    <hyperlink ref="A2166" r:id="rId2165"/>
+    <hyperlink ref="A2167" r:id="rId2166"/>
+    <hyperlink ref="A2168" r:id="rId2167"/>
+    <hyperlink ref="A2169" r:id="rId2168"/>
+    <hyperlink ref="A2170" r:id="rId2169"/>
+    <hyperlink ref="A2171" r:id="rId2170"/>
+    <hyperlink ref="A2172" r:id="rId2171"/>
+    <hyperlink ref="A2173" r:id="rId2172"/>
+    <hyperlink ref="A2174" r:id="rId2173"/>
+    <hyperlink ref="A2175" r:id="rId2174"/>
+    <hyperlink ref="A2176" r:id="rId2175"/>
+    <hyperlink ref="A2177" r:id="rId2176"/>
+    <hyperlink ref="A2178" r:id="rId2177"/>
+    <hyperlink ref="A2179" r:id="rId2178"/>
+    <hyperlink ref="A2180" r:id="rId2179"/>
+    <hyperlink ref="A2181" r:id="rId2180"/>
+    <hyperlink ref="A2182" r:id="rId2181"/>
+    <hyperlink ref="A2183" r:id="rId2182"/>
+    <hyperlink ref="A2184" r:id="rId2183"/>
+    <hyperlink ref="A2185" r:id="rId2184"/>
+    <hyperlink ref="A2186" r:id="rId2185"/>
+    <hyperlink ref="A2187" r:id="rId2186"/>
+    <hyperlink ref="A2188" r:id="rId2187"/>
+    <hyperlink ref="A2189" r:id="rId2188"/>
+    <hyperlink ref="A2190" r:id="rId2189"/>
+    <hyperlink ref="A2191" r:id="rId2190"/>
+    <hyperlink ref="A2192" r:id="rId2191"/>
+    <hyperlink ref="A2193" r:id="rId2192"/>
+    <hyperlink ref="A2194" r:id="rId2193"/>
+    <hyperlink ref="A2195" r:id="rId2194"/>
+    <hyperlink ref="A2196" r:id="rId2195"/>
+    <hyperlink ref="A2197" r:id="rId2196"/>
+    <hyperlink ref="A2198" r:id="rId2197"/>
+    <hyperlink ref="A2199" r:id="rId2198"/>
+    <hyperlink ref="A2200" r:id="rId2199"/>
+    <hyperlink ref="A2201" r:id="rId2200"/>
+    <hyperlink ref="A2202" r:id="rId2201"/>
+    <hyperlink ref="A2203" r:id="rId2202"/>
+    <hyperlink ref="A2204" r:id="rId2203"/>
+    <hyperlink ref="A2205" r:id="rId2204"/>
+    <hyperlink ref="A2206" r:id="rId2205"/>
+    <hyperlink ref="A2207" r:id="rId2206"/>
+    <hyperlink ref="A2208" r:id="rId2207"/>
+    <hyperlink ref="A2209" r:id="rId2208"/>
+    <hyperlink ref="A2210" r:id="rId2209"/>
+    <hyperlink ref="A2211" r:id="rId2210"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Update lands data - 2025-09-27 05:45
</commit_message>
<xml_diff>
--- a/lands-scraped.xlsx
+++ b/lands-scraped.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13272" uniqueCount="8933">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13278" uniqueCount="8938">
   <si>
     <t>link</t>
   </si>
@@ -26814,6 +26814,21 @@
   </si>
   <si>
     <t>26.09.2025 22:51</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/iecavas-nov/ajggp.html</t>
+  </si>
+  <si>
+    <t>11 000 € (18.09 €/m²)</t>
+  </si>
+  <si>
+    <t>608 m²</t>
+  </si>
+  <si>
+    <t>40640102010</t>
+  </si>
+  <si>
+    <t>27.09.2025 07:20</t>
   </si>
 </sst>
 </file>
@@ -27236,7 +27251,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -27273,7 +27288,30 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>8933</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8934</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8935</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>8936</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>8937</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update lands data - 2025-09-27 05:55
</commit_message>
<xml_diff>
--- a/lands-scraped.xlsx
+++ b/lands-scraped.xlsx
@@ -27251,7 +27251,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -27288,30 +27288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>8933</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>8934</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>526</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>8935</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>8936</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>8937</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
@@ -27319,7 +27296,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2211"/>
+  <dimension ref="A1:F2212"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -71555,6 +71532,26 @@
       </c>
       <c r="F2211" s="3" t="s">
         <v>8932</v>
+      </c>
+    </row>
+    <row r="2212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2212" s="4" t="s">
+        <v>8933</v>
+      </c>
+      <c r="B2212" s="3" t="s">
+        <v>8934</v>
+      </c>
+      <c r="C2212" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="D2212" s="3" t="s">
+        <v>8935</v>
+      </c>
+      <c r="E2212" s="3" t="s">
+        <v>8936</v>
+      </c>
+      <c r="F2212" s="3" t="s">
+        <v>8937</v>
       </c>
     </row>
   </sheetData>
@@ -73769,6 +73766,7 @@
     <hyperlink ref="A2209" r:id="rId2208"/>
     <hyperlink ref="A2210" r:id="rId2209"/>
     <hyperlink ref="A2211" r:id="rId2210"/>
+    <hyperlink ref="A2212" r:id="rId2211"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Update lands data - 2025-09-29 12:21
</commit_message>
<xml_diff>
--- a/lands-scraped.xlsx
+++ b/lands-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11077" uniqueCount="6918">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11337" uniqueCount="7074">
   <si>
     <t>link</t>
   </si>
@@ -20772,6 +20772,474 @@
   </si>
   <si>
     <t>3998 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/aizkraukle-and-reg/aizkraukles/fjfbf.html</t>
+  </si>
+  <si>
+    <t>25 000 € (19.86 €/m²)</t>
+  </si>
+  <si>
+    <t>1259 m²</t>
+  </si>
+  <si>
+    <t>32010010217</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/vecsaules-pag/bdfcbg.html</t>
+  </si>
+  <si>
+    <t>14 000 € (11.67 €/m²)</t>
+  </si>
+  <si>
+    <t>40920010431</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/davinu-pag/jonnx.html</t>
+  </si>
+  <si>
+    <t>50 000 € (0.56 €/m²)</t>
+  </si>
+  <si>
+    <t>40560070001</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/rundales-pag/cnbki.html</t>
+  </si>
+  <si>
+    <t>1 800 € (4.44 €/m²)</t>
+  </si>
+  <si>
+    <t>405 m²</t>
+  </si>
+  <si>
+    <t>40760030260</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/rundales-pag/aaakc.html</t>
+  </si>
+  <si>
+    <t>19 990 € (8 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/cesis/hccpe.html</t>
+  </si>
+  <si>
+    <t>16 500 € (7.95 €/m²)</t>
+  </si>
+  <si>
+    <t>2076 m²</t>
+  </si>
+  <si>
+    <t>42720070780</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/cesis/ahpel.html</t>
+  </si>
+  <si>
+    <t>19 500 € (7.92 €/m²)</t>
+  </si>
+  <si>
+    <t>2462 m²</t>
+  </si>
+  <si>
+    <t>42720070790</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/priekulu-pag/becipb.html</t>
+  </si>
+  <si>
+    <t>125 000 € (2.50 €/m²)</t>
+  </si>
+  <si>
+    <t>4272 007 0332</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/priekulu-pag/dclxm.html</t>
+  </si>
+  <si>
+    <t>65 000 € (0.65 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/cesis/amggl.html</t>
+  </si>
+  <si>
+    <t>299 900 € (14.67 €/m²)</t>
+  </si>
+  <si>
+    <t>20443 m²</t>
+  </si>
+  <si>
+    <t>42010090534</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/raiskuma-pag/bedhcm.html</t>
+  </si>
+  <si>
+    <t>33 000 € (3.30 €/m²)</t>
+  </si>
+  <si>
+    <t>42740110493</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/tabores-pag/bxfobk.html</t>
+  </si>
+  <si>
+    <t>2 600 € (0.51 €/m²)</t>
+  </si>
+  <si>
+    <t>5138 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/daugavpils/bklod.html</t>
+  </si>
+  <si>
+    <t>80 000 € (1.15 €/m²)</t>
+  </si>
+  <si>
+    <t>6.98 ha.</t>
+  </si>
+  <si>
+    <t>44860010515</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/dobele-and-reg/auce/cxion.html</t>
+  </si>
+  <si>
+    <t>20 000 € (1.51 €/m²)</t>
+  </si>
+  <si>
+    <t>13221 m²</t>
+  </si>
+  <si>
+    <t>46050212128</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jaunsvirlaukas-pag/ibllx.html</t>
+  </si>
+  <si>
+    <t>54560020388</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jelgava/dihxf.html</t>
+  </si>
+  <si>
+    <t>40 293 € (37 €/m²)</t>
+  </si>
+  <si>
+    <t>1089 m²</t>
+  </si>
+  <si>
+    <t>9000070334</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jelgava/hkmpe.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/svetes-pag/ajmmd.html</t>
+  </si>
+  <si>
+    <t>23 500 € (1.18 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jaunsvirlaukas-pag/eecbh.html</t>
+  </si>
+  <si>
+    <t>52 000 € (1.30 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/gludas-pag/dxodl.html</t>
+  </si>
+  <si>
+    <t>129 000 € (1.42 €/m²)</t>
+  </si>
+  <si>
+    <t>9.06 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kraslava-and-reg/asunes-pag/jmlcd.html</t>
+  </si>
+  <si>
+    <t>8 000 € (0.27 €/m²)</t>
+  </si>
+  <si>
+    <t>60460040372</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kraslava-and-reg/ezernieku-pag/lxoje.html</t>
+  </si>
+  <si>
+    <t>3 000 € (0.30 €/m²)</t>
+  </si>
+  <si>
+    <t>6056-004-0276</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kraslava-and-reg/kalniesu-pag/eindn.html</t>
+  </si>
+  <si>
+    <t>15 900 € (0.88 €/m²)</t>
+  </si>
+  <si>
+    <t>60680040321</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/limbadzi-and-reg/salacgriva/fjhng.html</t>
+  </si>
+  <si>
+    <t>37 000 € (13.30 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ludza-and-reg/rundenu-pag/ikede.html</t>
+  </si>
+  <si>
+    <t>60 000 € (0.57 €/m²)</t>
+  </si>
+  <si>
+    <t>10.48 ha.</t>
+  </si>
+  <si>
+    <t>68920010017</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ludza-and-reg/karsava/bxcnih.html</t>
+  </si>
+  <si>
+    <t>2 500 € (1.67 €/m²)</t>
+  </si>
+  <si>
+    <t>0.15 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ludza-and-reg/karsava/pgkhh.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/lielvarde/anhco.html</t>
+  </si>
+  <si>
+    <t>10 500 € (1.05 €/m²)</t>
+  </si>
+  <si>
+    <t>74330020500</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ikskile/bbinp.html</t>
+  </si>
+  <si>
+    <t>49 000 € (37.49 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/lielvardes-l-t/angjl.html</t>
+  </si>
+  <si>
+    <t>18 900 € (0.79 €/m²)</t>
+  </si>
+  <si>
+    <t>74330050045</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/taurupes-pag/nndhx.html</t>
+  </si>
+  <si>
+    <t>80 000 € (0.50 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/taurupes-pag/fgfmb.html</t>
+  </si>
+  <si>
+    <t>12 000 € (1.37 €/m²)</t>
+  </si>
+  <si>
+    <t>8730 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/cornajas-pag/elmxm.html</t>
+  </si>
+  <si>
+    <t>78460070284</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/cornajas-pag/mepkx.html</t>
+  </si>
+  <si>
+    <t>78460070194</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/dricanu-pag/cgbdek.html</t>
+  </si>
+  <si>
+    <t>21 300 € (0.30 €/m²)</t>
+  </si>
+  <si>
+    <t>78500030078</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/rezekne/bdlxij.html</t>
+  </si>
+  <si>
+    <t>18 500 € (4.63 €/m²)</t>
+  </si>
+  <si>
+    <t>78560030032</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/rezekne/bbiogi.html</t>
+  </si>
+  <si>
+    <t>26 600 € (10.02 €/m²)</t>
+  </si>
+  <si>
+    <t>2656 m²</t>
+  </si>
+  <si>
+    <t>21000150512</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/saldus-and-reg/novadnieku-pag/afkgx.html</t>
+  </si>
+  <si>
+    <t>84720030116</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/kolkas-pag/ipopb.html</t>
+  </si>
+  <si>
+    <t>260 000 € (5 €/m²)</t>
+  </si>
+  <si>
+    <t>88620060006, 007, 0138</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/dundagas-pag/ixiil.html</t>
+  </si>
+  <si>
+    <t>23 800 € (1.19 €/m²)</t>
+  </si>
+  <si>
+    <t>88500260079</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/stende/cgfofj.html</t>
+  </si>
+  <si>
+    <t>19 500 € (4.88 €/m²)</t>
+  </si>
+  <si>
+    <t>88150010065</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/semes-pag/hipfi.html</t>
+  </si>
+  <si>
+    <t>90780080052</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/tukums/aahbf.html</t>
+  </si>
+  <si>
+    <t>74 760 € (40 €/m²)</t>
+  </si>
+  <si>
+    <t>1869 m²</t>
+  </si>
+  <si>
+    <t>90010040004</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/lapmezciema-nov/aaphm.html</t>
+  </si>
+  <si>
+    <t>37 000 € (13.21 €/m²)</t>
+  </si>
+  <si>
+    <t>0.28 ha.</t>
+  </si>
+  <si>
+    <t>90660041157</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/ventspils/ofmgm.html</t>
+  </si>
+  <si>
+    <t>18 190 € (5 €/m²)</t>
+  </si>
+  <si>
+    <t>3638 m²</t>
+  </si>
+  <si>
+    <t>27000270134</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/ventspils/bgnjj.html</t>
+  </si>
+  <si>
+    <t>75 310 € (10 €/m²)</t>
+  </si>
+  <si>
+    <t>7531 m²</t>
+  </si>
+  <si>
+    <t>27000270113</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/ventspils/bjhfg.html</t>
+  </si>
+  <si>
+    <t>78 050 € (10 €/m²)</t>
+  </si>
+  <si>
+    <t>7805 m²</t>
+  </si>
+  <si>
+    <t>27000270132</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/ventspils/ejgph.html</t>
+  </si>
+  <si>
+    <t>17 165 € (5 €/m²)</t>
+  </si>
+  <si>
+    <t>3433 m²</t>
+  </si>
+  <si>
+    <t>27000270133</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/ugales-pag/enmng.html</t>
+  </si>
+  <si>
+    <t>98700030034</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/ugales-pag/fjfcf.html</t>
+  </si>
+  <si>
+    <t>7 000 € (0.70 €/m²)</t>
+  </si>
+  <si>
+    <t>98700040120</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/varves-pag/aaaed.html</t>
+  </si>
+  <si>
+    <t>15 000 € (5.19 €/m²)</t>
+  </si>
+  <si>
+    <t>2892 m²</t>
+  </si>
+  <si>
+    <t>98840010133</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/other/fbfnj.html</t>
+  </si>
+  <si>
+    <t>29 000 € (674.42 €/m²)</t>
+  </si>
+  <si>
+    <t>43 m²</t>
   </si>
 </sst>
 </file>
@@ -21207,7 +21675,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -21246,1162 +21714,1042 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>6752</v>
+        <v>6918</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>4342</v>
+        <v>6919</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>561</v>
+        <v>6920</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>6753</v>
+        <v>6921</v>
       </c>
       <c r="F2" s="3">
-        <v>45927.27986111111</v>
+        <v>45929.60486111111</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>6754</v>
+        <v>6922</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>6755</v>
+        <v>6923</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>243</v>
+        <v>419</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>1680</v>
+        <v>111</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>6756</v>
+        <v>6924</v>
       </c>
       <c r="F3" s="3">
-        <v>45926.381944444445</v>
+        <v>45929.54236111111</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>6757</v>
+        <v>6925</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>6758</v>
+        <v>6926</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>324</v>
+        <v>419</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>6759</v>
+        <v>1430</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>6760</v>
+        <v>6927</v>
       </c>
       <c r="F4" s="3">
-        <v>45926.83263888889</v>
+        <v>45928.52222222222</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>6761</v>
+        <v>6928</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>6762</v>
+        <v>6929</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>419</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>6763</v>
+        <v>6930</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>6764</v>
+        <v>6931</v>
       </c>
       <c r="F5" s="3">
-        <v>45927.180555555555</v>
+        <v>45927.55208333333</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>6765</v>
+        <v>6932</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>6766</v>
+        <v>6933</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>419</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>6767</v>
+        <v>1632</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="3">
-        <v>45926.402083333334</v>
+        <v>45927.54375</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>6768</v>
+        <v>6934</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>6769</v>
+        <v>6935</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>419</v>
+        <v>772</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>6770</v>
+        <v>6936</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>10</v>
+        <v>6937</v>
       </c>
       <c r="F7" s="3">
-        <v>45926.28125</v>
+        <v>45929.57430555555</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>6771</v>
+        <v>6938</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>6772</v>
+        <v>6939</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>419</v>
+        <v>772</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>2489</v>
+        <v>6940</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>10</v>
+        <v>6941</v>
       </c>
       <c r="F8" s="3">
-        <v>45926.28055555555</v>
+        <v>45929.57430555555</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>6773</v>
+        <v>6942</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>6774</v>
+        <v>6943</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>419</v>
+        <v>772</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>6775</v>
+        <v>77</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>10</v>
+        <v>6944</v>
       </c>
       <c r="F9" s="3">
-        <v>45926.240277777775</v>
+        <v>45929.51944444445</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>6776</v>
+        <v>6945</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>6777</v>
+        <v>6946</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>772</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>6778</v>
+        <v>325</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>6779</v>
+        <v>992</v>
       </c>
       <c r="F10" s="3">
-        <v>45926.7625</v>
+        <v>45928.78194444445</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>6780</v>
+        <v>6947</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>6781</v>
+        <v>6948</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>772</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>32</v>
+        <v>6949</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>6782</v>
+        <v>6950</v>
       </c>
       <c r="F11" s="3">
-        <v>45926.52569444444</v>
+        <v>45928.555555555555</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>6783</v>
+        <v>6951</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>6784</v>
+        <v>6952</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>772</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>596</v>
+        <v>561</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>10</v>
+        <v>6953</v>
       </c>
       <c r="F12" s="3">
-        <v>45926.27777777778</v>
+        <v>45928.415972222225</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>6785</v>
+        <v>6954</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>6786</v>
+        <v>6955</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>772</v>
+        <v>1218</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>2318</v>
+        <v>6956</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>6787</v>
+        <v>10</v>
       </c>
       <c r="F13" s="3">
-        <v>45926.228472222225</v>
+        <v>45929.54791666666</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>6788</v>
+        <v>6957</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>6789</v>
+        <v>6958</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>772</v>
+        <v>1218</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>383</v>
+        <v>6959</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>6790</v>
+        <v>6960</v>
       </c>
       <c r="F14" s="3">
-        <v>45925.597916666666</v>
+        <v>45929.45138888889</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>6791</v>
+        <v>6961</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>6792</v>
+        <v>6962</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>1218</v>
+        <v>1569</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>6793</v>
+        <v>6963</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>6794</v>
+        <v>6964</v>
       </c>
       <c r="F15" s="3">
-        <v>45926.59027777778</v>
+        <v>45929.632638888885</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>6795</v>
+        <v>6965</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>6796</v>
+        <v>4426</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>1218</v>
+        <v>1929</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>6797</v>
+        <v>2896</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>6798</v>
+        <v>6966</v>
       </c>
       <c r="F16" s="3">
-        <v>45926.43611111111</v>
+        <v>45929.52013888889</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>6799</v>
+        <v>6967</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>6800</v>
+        <v>6968</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>1218</v>
+        <v>1929</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>6801</v>
+        <v>6969</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>6802</v>
+        <v>6970</v>
       </c>
       <c r="F17" s="3">
-        <v>45926.43611111111</v>
+        <v>45929.49791666667</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>6803</v>
+        <v>6971</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>6804</v>
+        <v>2283</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>1218</v>
+        <v>1929</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>63</v>
+        <v>2284</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>6805</v>
+        <v>2285</v>
       </c>
       <c r="F18" s="3">
-        <v>45926.38958333334</v>
+        <v>45929.441666666666</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>6806</v>
+        <v>6972</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>6807</v>
+        <v>6973</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>1218</v>
+        <v>1929</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>6808</v>
+        <v>171</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>6809</v>
+        <v>2261</v>
       </c>
       <c r="F19" s="3">
-        <v>45926.38958333334</v>
+        <v>45929.3875</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>6810</v>
+        <v>6974</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>6811</v>
+        <v>6975</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>1218</v>
+        <v>1929</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>77</v>
+        <v>353</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>6812</v>
+        <v>10</v>
       </c>
       <c r="F20" s="3">
-        <v>45925.74444444444</v>
+        <v>45928.94305555556</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>6813</v>
+        <v>6976</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>6814</v>
+        <v>6977</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>1929</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>2258</v>
+        <v>6978</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>6815</v>
+        <v>10</v>
       </c>
       <c r="F21" s="3">
-        <v>45926.40972222222</v>
+        <v>45928.464583333334</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>6816</v>
+        <v>6979</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>6817</v>
+        <v>6980</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>1929</v>
+        <v>2488</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>6818</v>
+        <v>201</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>6819</v>
+        <v>6981</v>
       </c>
       <c r="F22" s="3">
-        <v>45925.743055555555</v>
+        <v>45929.33333333333</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>6820</v>
+        <v>6982</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>6821</v>
+        <v>6983</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>2488</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>2552</v>
+        <v>32</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>10</v>
+        <v>6984</v>
       </c>
       <c r="F23" s="3">
-        <v>45926.73611111111</v>
+        <v>45928.802777777775</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>6822</v>
+        <v>6985</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>6823</v>
+        <v>6986</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>2488</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>149</v>
+        <v>390</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>10</v>
+        <v>6987</v>
       </c>
       <c r="F24" s="3">
-        <v>45926.288194444445</v>
+        <v>45927.89722222222</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>6824</v>
+        <v>6988</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>6825</v>
+        <v>6989</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>2488</v>
+        <v>3398</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>383</v>
+        <v>3454</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F25" s="3">
-        <v>45925.72986111111</v>
+        <v>45929.450694444444</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>6826</v>
+        <v>6990</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>756</v>
+        <v>6991</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>2671</v>
+        <v>3762</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>171</v>
+        <v>6992</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>2785</v>
+        <v>6993</v>
       </c>
       <c r="F26" s="3">
-        <v>45926.36388888889</v>
+        <v>45928.68611111111</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>6827</v>
+        <v>6994</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>756</v>
+        <v>6995</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>2671</v>
+        <v>3762</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>171</v>
+        <v>6996</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>2785</v>
+        <v>10</v>
       </c>
       <c r="F27" s="3">
-        <v>45926.36111111111</v>
+        <v>45928.54375</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>6828</v>
+        <v>6997</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>756</v>
+        <v>3761</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>2671</v>
+        <v>3762</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>171</v>
+        <v>866</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>2785</v>
+        <v>10</v>
       </c>
       <c r="F28" s="3">
-        <v>45926.36111111111</v>
+        <v>45928.54375</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>6829</v>
+        <v>6998</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>6830</v>
+        <v>6999</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>2671</v>
+        <v>4034</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>171</v>
+        <v>32</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>6831</v>
+        <v>7000</v>
       </c>
       <c r="F29" s="3">
-        <v>45926.35902777778</v>
+        <v>45928.92569444445</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>6832</v>
+        <v>7001</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>6833</v>
+        <v>7002</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>2846</v>
+        <v>4034</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>6834</v>
+        <v>6426</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F30" s="3">
-        <v>45926.643055555556</v>
+        <v>45928</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>6835</v>
+        <v>7003</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>6836</v>
+        <v>7004</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>2846</v>
+        <v>4034</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>6837</v>
+        <v>2244</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>6838</v>
+        <v>7005</v>
       </c>
       <c r="F31" s="3">
-        <v>45926.43541666667</v>
+        <v>45927.89791666667</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>6839</v>
+        <v>7006</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>6840</v>
+        <v>7007</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>3398</v>
+        <v>4034</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>6841</v>
+        <v>575</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>6842</v>
+        <v>10</v>
       </c>
       <c r="F32" s="3">
-        <v>45926.34097222222</v>
+        <v>45927.80972222222</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>6843</v>
+        <v>7008</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>6844</v>
+        <v>7009</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>3398</v>
+        <v>4034</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>6845</v>
+        <v>7010</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>6846</v>
+        <v>10</v>
       </c>
       <c r="F33" s="3">
-        <v>45926.32777777778</v>
+        <v>45927.64166666666</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>6847</v>
+        <v>7011</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>6848</v>
+        <v>403</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>3868</v>
+        <v>4770</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>2343</v>
+        <v>77</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>6849</v>
+        <v>7012</v>
       </c>
       <c r="F34" s="3">
-        <v>45926.72013888889</v>
+        <v>45928.80972222222</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>6850</v>
+        <v>7013</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>6851</v>
+        <v>1989</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>4034</v>
+        <v>4770</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>4142</v>
+        <v>171</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>10</v>
+        <v>7014</v>
       </c>
       <c r="F35" s="3">
-        <v>45926.50277777778</v>
+        <v>45928.808333333334</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>6852</v>
+        <v>7015</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>6853</v>
+        <v>7016</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>4034</v>
+        <v>4770</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>2707</v>
+        <v>407</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>6854</v>
+        <v>7017</v>
       </c>
       <c r="F36" s="3">
-        <v>45926.40486111111</v>
+        <v>45928.67638888889</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>6855</v>
+        <v>7018</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>6856</v>
+        <v>7019</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>4034</v>
+        <v>4770</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>474</v>
+        <v>2343</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>10</v>
+        <v>7020</v>
       </c>
       <c r="F37" s="3">
-        <v>45926.33333333333</v>
+        <v>45928.54375</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>6857</v>
+        <v>7021</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>6858</v>
+        <v>7022</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>4034</v>
+        <v>4770</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>1632</v>
+        <v>7023</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>6859</v>
+        <v>7024</v>
       </c>
       <c r="F38" s="3">
-        <v>45926.3</v>
+        <v>45927.59722222222</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>6860</v>
+        <v>7025</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>6861</v>
+        <v>4774</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>4034</v>
+        <v>5147</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>1632</v>
+        <v>561</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>10</v>
+        <v>7026</v>
       </c>
       <c r="F39" s="3">
-        <v>45926.20625</v>
+        <v>45929.60486111111</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>6862</v>
+        <v>7027</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>6863</v>
+        <v>7028</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>4034</v>
+        <v>5266</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>6864</v>
+        <v>4778</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>6865</v>
+        <v>7029</v>
       </c>
       <c r="F40" s="3">
-        <v>45925.790972222225</v>
+        <v>45929.47430555556</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>6866</v>
+        <v>7030</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>6867</v>
+        <v>7031</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>4671</v>
+        <v>5266</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>508</v>
+        <v>171</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>6868</v>
+        <v>7032</v>
       </c>
       <c r="F41" s="3">
-        <v>45926.59236111111</v>
+        <v>45929.34583333333</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>6869</v>
+        <v>7033</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>6870</v>
+        <v>7034</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>4671</v>
+        <v>5266</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>508</v>
+        <v>2343</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>10</v>
+        <v>7035</v>
       </c>
       <c r="F42" s="3">
-        <v>45926.33333333333</v>
+        <v>45928.84722222222</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>6871</v>
+        <v>7036</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>6290</v>
+        <v>3789</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>4671</v>
+        <v>5674</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>383</v>
+        <v>3790</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>6872</v>
+        <v>7037</v>
       </c>
       <c r="F43" s="3">
-        <v>45926.330555555556</v>
+        <v>45929.61319444445</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>6873</v>
+        <v>7038</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>6874</v>
+        <v>7039</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>4770</v>
+        <v>5674</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>1156</v>
+        <v>7040</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>6875</v>
+        <v>7041</v>
       </c>
       <c r="F44" s="3">
-        <v>45926.72222222222</v>
+        <v>45929.60763888889</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>6876</v>
+        <v>7042</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>6877</v>
+        <v>7043</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>4770</v>
+        <v>5674</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>1430</v>
+        <v>7044</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>6878</v>
+        <v>7045</v>
       </c>
       <c r="F45" s="3">
-        <v>45926.38055555556</v>
+        <v>45928.88402777778</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>6879</v>
+        <v>7046</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>6290</v>
+        <v>7047</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>4770</v>
+        <v>6439</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>6880</v>
+        <v>7048</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>6881</v>
+        <v>7049</v>
       </c>
       <c r="F46" s="3">
-        <v>45926.37430555555</v>
+        <v>45929.60555555555</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>6882</v>
+        <v>7050</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>6883</v>
+        <v>7051</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>4770</v>
+        <v>6439</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>554</v>
+        <v>7052</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>6884</v>
+        <v>7053</v>
       </c>
       <c r="F47" s="3">
-        <v>45926.32916666666</v>
+        <v>45929.60555555555</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>6885</v>
+        <v>7054</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>6886</v>
+        <v>7055</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>4770</v>
+        <v>6439</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>201</v>
+        <v>7056</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>6887</v>
+        <v>7057</v>
       </c>
       <c r="F48" s="3">
-        <v>45926.20416666666</v>
+        <v>45929.60555555555</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>6888</v>
+        <v>7058</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>6889</v>
+        <v>7059</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>5266</v>
+        <v>6439</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>6890</v>
+        <v>7060</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>10</v>
+        <v>7061</v>
       </c>
       <c r="F49" s="3">
-        <v>45926.42708333333</v>
+        <v>45929.57291666667</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>6891</v>
+        <v>7062</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>6892</v>
+        <v>323</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>5266</v>
+        <v>6439</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>5417</v>
+        <v>325</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>5418</v>
+        <v>7063</v>
       </c>
       <c r="F50" s="3">
-        <v>45926.34027777778</v>
+        <v>45929.40069444444</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>6893</v>
+        <v>7064</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>6894</v>
+        <v>7065</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>5674</v>
+        <v>6439</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>108</v>
+        <v>32</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>6895</v>
+        <v>7066</v>
       </c>
       <c r="F51" s="3">
-        <v>45926.524305555555</v>
+        <v>45928.99166666667</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>6896</v>
+        <v>7067</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>6897</v>
+        <v>7068</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>5674</v>
+        <v>6439</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>353</v>
+        <v>7069</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>6898</v>
+        <v>7070</v>
       </c>
       <c r="F52" s="3">
-        <v>45926.231944444444</v>
+        <v>45928.47430555556</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>6899</v>
+        <v>7071</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>6900</v>
+        <v>7072</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>6133</v>
+        <v>1194</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>2248</v>
+        <v>7073</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>6901</v>
+        <v>10</v>
       </c>
       <c r="F53" s="3">
-        <v>45926.23888888889</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="8" t="s">
-        <v>6902</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>6903</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>6207</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>4262</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>6904</v>
-      </c>
-      <c r="F54" s="3">
-        <v>45926.65902777778</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
-        <v>6905</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>6906</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>6207</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>6327</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>6907</v>
-      </c>
-      <c r="F55" s="3">
-        <v>45926.569444444445</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
-        <v>6908</v>
-      </c>
-      <c r="B56" s="9" t="s">
-        <v>1527</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>6207</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>6909</v>
-      </c>
-      <c r="F56" s="3">
-        <v>45926.32430555555</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="8" t="s">
-        <v>6910</v>
-      </c>
-      <c r="B57" s="9" t="s">
-        <v>6911</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>6207</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>6912</v>
-      </c>
-      <c r="E57" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F57" s="3">
-        <v>45925.68541666667</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="8" t="s">
-        <v>6913</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>6914</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>6207</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>6915</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F58" s="3">
-        <v>45925.59861111111</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
-        <v>6916</v>
-      </c>
-      <c r="B59" s="9" t="s">
-        <v>4123</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>6917</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F59" s="3">
-        <v>45926.82708333334</v>
+        <v>45928.39444444445</v>
       </c>
     </row>
   </sheetData>
@@ -22458,12 +22806,6 @@
     <hyperlink ref="A51" r:id="rId50"/>
     <hyperlink ref="A52" r:id="rId51"/>
     <hyperlink ref="A53" r:id="rId52"/>
-    <hyperlink ref="A54" r:id="rId53"/>
-    <hyperlink ref="A55" r:id="rId54"/>
-    <hyperlink ref="A56" r:id="rId55"/>
-    <hyperlink ref="A57" r:id="rId56"/>
-    <hyperlink ref="A58" r:id="rId57"/>
-    <hyperlink ref="A59" r:id="rId58"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -22472,7 +22814,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2156"/>
+  <dimension ref="A1:F2214"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -65608,6 +65950,1166 @@
       </c>
       <c r="F2156" s="3">
         <v>45927.34444444445</v>
+      </c>
+    </row>
+    <row r="2157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2157" s="4" t="s">
+        <v>6752</v>
+      </c>
+      <c r="B2157" s="3" t="s">
+        <v>4342</v>
+      </c>
+      <c r="C2157" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2157" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="E2157" s="3" t="s">
+        <v>6753</v>
+      </c>
+      <c r="F2157" s="3">
+        <v>45927.27986111111</v>
+      </c>
+    </row>
+    <row r="2158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2158" s="4" t="s">
+        <v>6754</v>
+      </c>
+      <c r="B2158" s="3" t="s">
+        <v>6755</v>
+      </c>
+      <c r="C2158" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D2158" s="3" t="s">
+        <v>1680</v>
+      </c>
+      <c r="E2158" s="3" t="s">
+        <v>6756</v>
+      </c>
+      <c r="F2158" s="3">
+        <v>45926.381944444445</v>
+      </c>
+    </row>
+    <row r="2159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2159" s="4" t="s">
+        <v>6757</v>
+      </c>
+      <c r="B2159" s="3" t="s">
+        <v>6758</v>
+      </c>
+      <c r="C2159" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="D2159" s="3" t="s">
+        <v>6759</v>
+      </c>
+      <c r="E2159" s="3" t="s">
+        <v>6760</v>
+      </c>
+      <c r="F2159" s="3">
+        <v>45926.83263888889</v>
+      </c>
+    </row>
+    <row r="2160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2160" s="4" t="s">
+        <v>6761</v>
+      </c>
+      <c r="B2160" s="3" t="s">
+        <v>6762</v>
+      </c>
+      <c r="C2160" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2160" s="3" t="s">
+        <v>6763</v>
+      </c>
+      <c r="E2160" s="3" t="s">
+        <v>6764</v>
+      </c>
+      <c r="F2160" s="3">
+        <v>45927.180555555555</v>
+      </c>
+    </row>
+    <row r="2161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2161" s="4" t="s">
+        <v>6765</v>
+      </c>
+      <c r="B2161" s="3" t="s">
+        <v>6766</v>
+      </c>
+      <c r="C2161" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2161" s="3" t="s">
+        <v>6767</v>
+      </c>
+      <c r="E2161" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2161" s="3">
+        <v>45926.402083333334</v>
+      </c>
+    </row>
+    <row r="2162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2162" s="4" t="s">
+        <v>6768</v>
+      </c>
+      <c r="B2162" s="3" t="s">
+        <v>6769</v>
+      </c>
+      <c r="C2162" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2162" s="3" t="s">
+        <v>6770</v>
+      </c>
+      <c r="E2162" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2162" s="3">
+        <v>45926.28125</v>
+      </c>
+    </row>
+    <row r="2163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2163" s="4" t="s">
+        <v>6771</v>
+      </c>
+      <c r="B2163" s="3" t="s">
+        <v>6772</v>
+      </c>
+      <c r="C2163" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2163" s="3" t="s">
+        <v>2489</v>
+      </c>
+      <c r="E2163" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2163" s="3">
+        <v>45926.28055555555</v>
+      </c>
+    </row>
+    <row r="2164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2164" s="4" t="s">
+        <v>6773</v>
+      </c>
+      <c r="B2164" s="3" t="s">
+        <v>6774</v>
+      </c>
+      <c r="C2164" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2164" s="3" t="s">
+        <v>6775</v>
+      </c>
+      <c r="E2164" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2164" s="3">
+        <v>45926.240277777775</v>
+      </c>
+    </row>
+    <row r="2165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2165" s="4" t="s">
+        <v>6776</v>
+      </c>
+      <c r="B2165" s="3" t="s">
+        <v>6777</v>
+      </c>
+      <c r="C2165" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2165" s="3" t="s">
+        <v>6778</v>
+      </c>
+      <c r="E2165" s="3" t="s">
+        <v>6779</v>
+      </c>
+      <c r="F2165" s="3">
+        <v>45926.7625</v>
+      </c>
+    </row>
+    <row r="2166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2166" s="4" t="s">
+        <v>6780</v>
+      </c>
+      <c r="B2166" s="3" t="s">
+        <v>6781</v>
+      </c>
+      <c r="C2166" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2166" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2166" s="3" t="s">
+        <v>6782</v>
+      </c>
+      <c r="F2166" s="3">
+        <v>45926.52569444444</v>
+      </c>
+    </row>
+    <row r="2167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2167" s="4" t="s">
+        <v>6783</v>
+      </c>
+      <c r="B2167" s="3" t="s">
+        <v>6784</v>
+      </c>
+      <c r="C2167" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2167" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="E2167" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2167" s="3">
+        <v>45926.27777777778</v>
+      </c>
+    </row>
+    <row r="2168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2168" s="4" t="s">
+        <v>6785</v>
+      </c>
+      <c r="B2168" s="3" t="s">
+        <v>6786</v>
+      </c>
+      <c r="C2168" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2168" s="3" t="s">
+        <v>2318</v>
+      </c>
+      <c r="E2168" s="3" t="s">
+        <v>6787</v>
+      </c>
+      <c r="F2168" s="3">
+        <v>45926.228472222225</v>
+      </c>
+    </row>
+    <row r="2169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2169" s="4" t="s">
+        <v>6788</v>
+      </c>
+      <c r="B2169" s="3" t="s">
+        <v>6789</v>
+      </c>
+      <c r="C2169" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2169" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E2169" s="3" t="s">
+        <v>6790</v>
+      </c>
+      <c r="F2169" s="3">
+        <v>45925.597916666666</v>
+      </c>
+    </row>
+    <row r="2170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2170" s="4" t="s">
+        <v>6791</v>
+      </c>
+      <c r="B2170" s="3" t="s">
+        <v>6792</v>
+      </c>
+      <c r="C2170" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2170" s="3" t="s">
+        <v>6793</v>
+      </c>
+      <c r="E2170" s="3" t="s">
+        <v>6794</v>
+      </c>
+      <c r="F2170" s="3">
+        <v>45926.59027777778</v>
+      </c>
+    </row>
+    <row r="2171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2171" s="4" t="s">
+        <v>6795</v>
+      </c>
+      <c r="B2171" s="3" t="s">
+        <v>6796</v>
+      </c>
+      <c r="C2171" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2171" s="3" t="s">
+        <v>6797</v>
+      </c>
+      <c r="E2171" s="3" t="s">
+        <v>6798</v>
+      </c>
+      <c r="F2171" s="3">
+        <v>45926.43611111111</v>
+      </c>
+    </row>
+    <row r="2172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2172" s="4" t="s">
+        <v>6799</v>
+      </c>
+      <c r="B2172" s="3" t="s">
+        <v>6800</v>
+      </c>
+      <c r="C2172" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2172" s="3" t="s">
+        <v>6801</v>
+      </c>
+      <c r="E2172" s="3" t="s">
+        <v>6802</v>
+      </c>
+      <c r="F2172" s="3">
+        <v>45926.43611111111</v>
+      </c>
+    </row>
+    <row r="2173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2173" s="4" t="s">
+        <v>6803</v>
+      </c>
+      <c r="B2173" s="3" t="s">
+        <v>6804</v>
+      </c>
+      <c r="C2173" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2173" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2173" s="3" t="s">
+        <v>6805</v>
+      </c>
+      <c r="F2173" s="3">
+        <v>45926.38958333334</v>
+      </c>
+    </row>
+    <row r="2174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2174" s="4" t="s">
+        <v>6806</v>
+      </c>
+      <c r="B2174" s="3" t="s">
+        <v>6807</v>
+      </c>
+      <c r="C2174" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2174" s="3" t="s">
+        <v>6808</v>
+      </c>
+      <c r="E2174" s="3" t="s">
+        <v>6809</v>
+      </c>
+      <c r="F2174" s="3">
+        <v>45926.38958333334</v>
+      </c>
+    </row>
+    <row r="2175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2175" s="4" t="s">
+        <v>6810</v>
+      </c>
+      <c r="B2175" s="3" t="s">
+        <v>6811</v>
+      </c>
+      <c r="C2175" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2175" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2175" s="3" t="s">
+        <v>6812</v>
+      </c>
+      <c r="F2175" s="3">
+        <v>45925.74444444444</v>
+      </c>
+    </row>
+    <row r="2176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2176" s="4" t="s">
+        <v>6813</v>
+      </c>
+      <c r="B2176" s="3" t="s">
+        <v>6814</v>
+      </c>
+      <c r="C2176" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2176" s="3" t="s">
+        <v>2258</v>
+      </c>
+      <c r="E2176" s="3" t="s">
+        <v>6815</v>
+      </c>
+      <c r="F2176" s="3">
+        <v>45926.40972222222</v>
+      </c>
+    </row>
+    <row r="2177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2177" s="4" t="s">
+        <v>6816</v>
+      </c>
+      <c r="B2177" s="3" t="s">
+        <v>6817</v>
+      </c>
+      <c r="C2177" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2177" s="3" t="s">
+        <v>6818</v>
+      </c>
+      <c r="E2177" s="3" t="s">
+        <v>6819</v>
+      </c>
+      <c r="F2177" s="3">
+        <v>45925.743055555555</v>
+      </c>
+    </row>
+    <row r="2178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2178" s="4" t="s">
+        <v>6820</v>
+      </c>
+      <c r="B2178" s="3" t="s">
+        <v>6821</v>
+      </c>
+      <c r="C2178" s="3" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D2178" s="3" t="s">
+        <v>2552</v>
+      </c>
+      <c r="E2178" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2178" s="3">
+        <v>45926.73611111111</v>
+      </c>
+    </row>
+    <row r="2179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2179" s="4" t="s">
+        <v>6822</v>
+      </c>
+      <c r="B2179" s="3" t="s">
+        <v>6823</v>
+      </c>
+      <c r="C2179" s="3" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D2179" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E2179" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2179" s="3">
+        <v>45926.288194444445</v>
+      </c>
+    </row>
+    <row r="2180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2180" s="4" t="s">
+        <v>6824</v>
+      </c>
+      <c r="B2180" s="3" t="s">
+        <v>6825</v>
+      </c>
+      <c r="C2180" s="3" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D2180" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E2180" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2180" s="3">
+        <v>45925.72986111111</v>
+      </c>
+    </row>
+    <row r="2181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2181" s="4" t="s">
+        <v>6826</v>
+      </c>
+      <c r="B2181" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="C2181" s="3" t="s">
+        <v>2671</v>
+      </c>
+      <c r="D2181" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2181" s="3" t="s">
+        <v>2785</v>
+      </c>
+      <c r="F2181" s="3">
+        <v>45926.36388888889</v>
+      </c>
+    </row>
+    <row r="2182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2182" s="4" t="s">
+        <v>6827</v>
+      </c>
+      <c r="B2182" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="C2182" s="3" t="s">
+        <v>2671</v>
+      </c>
+      <c r="D2182" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2182" s="3" t="s">
+        <v>2785</v>
+      </c>
+      <c r="F2182" s="3">
+        <v>45926.36111111111</v>
+      </c>
+    </row>
+    <row r="2183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2183" s="4" t="s">
+        <v>6828</v>
+      </c>
+      <c r="B2183" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="C2183" s="3" t="s">
+        <v>2671</v>
+      </c>
+      <c r="D2183" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2183" s="3" t="s">
+        <v>2785</v>
+      </c>
+      <c r="F2183" s="3">
+        <v>45926.36111111111</v>
+      </c>
+    </row>
+    <row r="2184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2184" s="4" t="s">
+        <v>6829</v>
+      </c>
+      <c r="B2184" s="3" t="s">
+        <v>6830</v>
+      </c>
+      <c r="C2184" s="3" t="s">
+        <v>2671</v>
+      </c>
+      <c r="D2184" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2184" s="3" t="s">
+        <v>6831</v>
+      </c>
+      <c r="F2184" s="3">
+        <v>45926.35902777778</v>
+      </c>
+    </row>
+    <row r="2185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2185" s="4" t="s">
+        <v>6832</v>
+      </c>
+      <c r="B2185" s="3" t="s">
+        <v>6833</v>
+      </c>
+      <c r="C2185" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2185" s="3" t="s">
+        <v>6834</v>
+      </c>
+      <c r="E2185" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2185" s="3">
+        <v>45926.643055555556</v>
+      </c>
+    </row>
+    <row r="2186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2186" s="4" t="s">
+        <v>6835</v>
+      </c>
+      <c r="B2186" s="3" t="s">
+        <v>6836</v>
+      </c>
+      <c r="C2186" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2186" s="3" t="s">
+        <v>6837</v>
+      </c>
+      <c r="E2186" s="3" t="s">
+        <v>6838</v>
+      </c>
+      <c r="F2186" s="3">
+        <v>45926.43541666667</v>
+      </c>
+    </row>
+    <row r="2187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2187" s="4" t="s">
+        <v>6839</v>
+      </c>
+      <c r="B2187" s="3" t="s">
+        <v>6840</v>
+      </c>
+      <c r="C2187" s="3" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D2187" s="3" t="s">
+        <v>6841</v>
+      </c>
+      <c r="E2187" s="3" t="s">
+        <v>6842</v>
+      </c>
+      <c r="F2187" s="3">
+        <v>45926.34097222222</v>
+      </c>
+    </row>
+    <row r="2188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2188" s="4" t="s">
+        <v>6843</v>
+      </c>
+      <c r="B2188" s="3" t="s">
+        <v>6844</v>
+      </c>
+      <c r="C2188" s="3" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D2188" s="3" t="s">
+        <v>6845</v>
+      </c>
+      <c r="E2188" s="3" t="s">
+        <v>6846</v>
+      </c>
+      <c r="F2188" s="3">
+        <v>45926.32777777778</v>
+      </c>
+    </row>
+    <row r="2189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2189" s="4" t="s">
+        <v>6847</v>
+      </c>
+      <c r="B2189" s="3" t="s">
+        <v>6848</v>
+      </c>
+      <c r="C2189" s="3" t="s">
+        <v>3868</v>
+      </c>
+      <c r="D2189" s="3" t="s">
+        <v>2343</v>
+      </c>
+      <c r="E2189" s="3" t="s">
+        <v>6849</v>
+      </c>
+      <c r="F2189" s="3">
+        <v>45926.72013888889</v>
+      </c>
+    </row>
+    <row r="2190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2190" s="4" t="s">
+        <v>6850</v>
+      </c>
+      <c r="B2190" s="3" t="s">
+        <v>6851</v>
+      </c>
+      <c r="C2190" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2190" s="3" t="s">
+        <v>4142</v>
+      </c>
+      <c r="E2190" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2190" s="3">
+        <v>45926.50277777778</v>
+      </c>
+    </row>
+    <row r="2191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2191" s="4" t="s">
+        <v>6852</v>
+      </c>
+      <c r="B2191" s="3" t="s">
+        <v>6853</v>
+      </c>
+      <c r="C2191" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2191" s="3" t="s">
+        <v>2707</v>
+      </c>
+      <c r="E2191" s="3" t="s">
+        <v>6854</v>
+      </c>
+      <c r="F2191" s="3">
+        <v>45926.40486111111</v>
+      </c>
+    </row>
+    <row r="2192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2192" s="4" t="s">
+        <v>6855</v>
+      </c>
+      <c r="B2192" s="3" t="s">
+        <v>6856</v>
+      </c>
+      <c r="C2192" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2192" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="E2192" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2192" s="3">
+        <v>45926.33333333333</v>
+      </c>
+    </row>
+    <row r="2193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2193" s="4" t="s">
+        <v>6857</v>
+      </c>
+      <c r="B2193" s="3" t="s">
+        <v>6858</v>
+      </c>
+      <c r="C2193" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2193" s="3" t="s">
+        <v>1632</v>
+      </c>
+      <c r="E2193" s="3" t="s">
+        <v>6859</v>
+      </c>
+      <c r="F2193" s="3">
+        <v>45926.3</v>
+      </c>
+    </row>
+    <row r="2194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2194" s="4" t="s">
+        <v>6860</v>
+      </c>
+      <c r="B2194" s="3" t="s">
+        <v>6861</v>
+      </c>
+      <c r="C2194" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2194" s="3" t="s">
+        <v>1632</v>
+      </c>
+      <c r="E2194" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2194" s="3">
+        <v>45926.20625</v>
+      </c>
+    </row>
+    <row r="2195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2195" s="4" t="s">
+        <v>6862</v>
+      </c>
+      <c r="B2195" s="3" t="s">
+        <v>6863</v>
+      </c>
+      <c r="C2195" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2195" s="3" t="s">
+        <v>6864</v>
+      </c>
+      <c r="E2195" s="3" t="s">
+        <v>6865</v>
+      </c>
+      <c r="F2195" s="3">
+        <v>45925.790972222225</v>
+      </c>
+    </row>
+    <row r="2196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2196" s="4" t="s">
+        <v>6866</v>
+      </c>
+      <c r="B2196" s="3" t="s">
+        <v>6867</v>
+      </c>
+      <c r="C2196" s="3" t="s">
+        <v>4671</v>
+      </c>
+      <c r="D2196" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="E2196" s="3" t="s">
+        <v>6868</v>
+      </c>
+      <c r="F2196" s="3">
+        <v>45926.59236111111</v>
+      </c>
+    </row>
+    <row r="2197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2197" s="4" t="s">
+        <v>6869</v>
+      </c>
+      <c r="B2197" s="3" t="s">
+        <v>6870</v>
+      </c>
+      <c r="C2197" s="3" t="s">
+        <v>4671</v>
+      </c>
+      <c r="D2197" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="E2197" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2197" s="3">
+        <v>45926.33333333333</v>
+      </c>
+    </row>
+    <row r="2198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2198" s="4" t="s">
+        <v>6871</v>
+      </c>
+      <c r="B2198" s="3" t="s">
+        <v>6290</v>
+      </c>
+      <c r="C2198" s="3" t="s">
+        <v>4671</v>
+      </c>
+      <c r="D2198" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E2198" s="3" t="s">
+        <v>6872</v>
+      </c>
+      <c r="F2198" s="3">
+        <v>45926.330555555556</v>
+      </c>
+    </row>
+    <row r="2199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2199" s="4" t="s">
+        <v>6873</v>
+      </c>
+      <c r="B2199" s="3" t="s">
+        <v>6874</v>
+      </c>
+      <c r="C2199" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2199" s="3" t="s">
+        <v>1156</v>
+      </c>
+      <c r="E2199" s="3" t="s">
+        <v>6875</v>
+      </c>
+      <c r="F2199" s="3">
+        <v>45926.72222222222</v>
+      </c>
+    </row>
+    <row r="2200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2200" s="4" t="s">
+        <v>6876</v>
+      </c>
+      <c r="B2200" s="3" t="s">
+        <v>6877</v>
+      </c>
+      <c r="C2200" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2200" s="3" t="s">
+        <v>1430</v>
+      </c>
+      <c r="E2200" s="3" t="s">
+        <v>6878</v>
+      </c>
+      <c r="F2200" s="3">
+        <v>45926.38055555556</v>
+      </c>
+    </row>
+    <row r="2201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2201" s="4" t="s">
+        <v>6879</v>
+      </c>
+      <c r="B2201" s="3" t="s">
+        <v>6290</v>
+      </c>
+      <c r="C2201" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2201" s="3" t="s">
+        <v>6880</v>
+      </c>
+      <c r="E2201" s="3" t="s">
+        <v>6881</v>
+      </c>
+      <c r="F2201" s="3">
+        <v>45926.37430555555</v>
+      </c>
+    </row>
+    <row r="2202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2202" s="4" t="s">
+        <v>6882</v>
+      </c>
+      <c r="B2202" s="3" t="s">
+        <v>6883</v>
+      </c>
+      <c r="C2202" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2202" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="E2202" s="3" t="s">
+        <v>6884</v>
+      </c>
+      <c r="F2202" s="3">
+        <v>45926.32916666666</v>
+      </c>
+    </row>
+    <row r="2203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2203" s="4" t="s">
+        <v>6885</v>
+      </c>
+      <c r="B2203" s="3" t="s">
+        <v>6886</v>
+      </c>
+      <c r="C2203" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2203" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2203" s="3" t="s">
+        <v>6887</v>
+      </c>
+      <c r="F2203" s="3">
+        <v>45926.20416666666</v>
+      </c>
+    </row>
+    <row r="2204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2204" s="4" t="s">
+        <v>6888</v>
+      </c>
+      <c r="B2204" s="3" t="s">
+        <v>6889</v>
+      </c>
+      <c r="C2204" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2204" s="3" t="s">
+        <v>6890</v>
+      </c>
+      <c r="E2204" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2204" s="3">
+        <v>45926.42708333333</v>
+      </c>
+    </row>
+    <row r="2205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2205" s="4" t="s">
+        <v>6891</v>
+      </c>
+      <c r="B2205" s="3" t="s">
+        <v>6892</v>
+      </c>
+      <c r="C2205" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2205" s="3" t="s">
+        <v>5417</v>
+      </c>
+      <c r="E2205" s="3" t="s">
+        <v>5418</v>
+      </c>
+      <c r="F2205" s="3">
+        <v>45926.34027777778</v>
+      </c>
+    </row>
+    <row r="2206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2206" s="4" t="s">
+        <v>6893</v>
+      </c>
+      <c r="B2206" s="3" t="s">
+        <v>6894</v>
+      </c>
+      <c r="C2206" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2206" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2206" s="3" t="s">
+        <v>6895</v>
+      </c>
+      <c r="F2206" s="3">
+        <v>45926.524305555555</v>
+      </c>
+    </row>
+    <row r="2207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2207" s="4" t="s">
+        <v>6896</v>
+      </c>
+      <c r="B2207" s="3" t="s">
+        <v>6897</v>
+      </c>
+      <c r="C2207" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2207" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="E2207" s="3" t="s">
+        <v>6898</v>
+      </c>
+      <c r="F2207" s="3">
+        <v>45926.231944444444</v>
+      </c>
+    </row>
+    <row r="2208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2208" s="4" t="s">
+        <v>6899</v>
+      </c>
+      <c r="B2208" s="3" t="s">
+        <v>6900</v>
+      </c>
+      <c r="C2208" s="3" t="s">
+        <v>6133</v>
+      </c>
+      <c r="D2208" s="3" t="s">
+        <v>2248</v>
+      </c>
+      <c r="E2208" s="3" t="s">
+        <v>6901</v>
+      </c>
+      <c r="F2208" s="3">
+        <v>45926.23888888889</v>
+      </c>
+    </row>
+    <row r="2209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2209" s="4" t="s">
+        <v>6902</v>
+      </c>
+      <c r="B2209" s="3" t="s">
+        <v>6903</v>
+      </c>
+      <c r="C2209" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2209" s="3" t="s">
+        <v>4262</v>
+      </c>
+      <c r="E2209" s="3" t="s">
+        <v>6904</v>
+      </c>
+      <c r="F2209" s="3">
+        <v>45926.65902777778</v>
+      </c>
+    </row>
+    <row r="2210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2210" s="4" t="s">
+        <v>6905</v>
+      </c>
+      <c r="B2210" s="3" t="s">
+        <v>6906</v>
+      </c>
+      <c r="C2210" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2210" s="3" t="s">
+        <v>6327</v>
+      </c>
+      <c r="E2210" s="3" t="s">
+        <v>6907</v>
+      </c>
+      <c r="F2210" s="3">
+        <v>45926.569444444445</v>
+      </c>
+    </row>
+    <row r="2211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2211" s="4" t="s">
+        <v>6908</v>
+      </c>
+      <c r="B2211" s="3" t="s">
+        <v>1527</v>
+      </c>
+      <c r="C2211" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2211" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2211" s="3" t="s">
+        <v>6909</v>
+      </c>
+      <c r="F2211" s="3">
+        <v>45926.32430555555</v>
+      </c>
+    </row>
+    <row r="2212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2212" s="4" t="s">
+        <v>6910</v>
+      </c>
+      <c r="B2212" s="3" t="s">
+        <v>6911</v>
+      </c>
+      <c r="C2212" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2212" s="3" t="s">
+        <v>6912</v>
+      </c>
+      <c r="E2212" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2212" s="3">
+        <v>45925.68541666667</v>
+      </c>
+    </row>
+    <row r="2213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2213" s="4" t="s">
+        <v>6913</v>
+      </c>
+      <c r="B2213" s="3" t="s">
+        <v>6914</v>
+      </c>
+      <c r="C2213" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2213" s="3" t="s">
+        <v>6915</v>
+      </c>
+      <c r="E2213" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2213" s="3">
+        <v>45925.59861111111</v>
+      </c>
+    </row>
+    <row r="2214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2214" s="4" t="s">
+        <v>6916</v>
+      </c>
+      <c r="B2214" s="3" t="s">
+        <v>4123</v>
+      </c>
+      <c r="C2214" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2214" s="3" t="s">
+        <v>6917</v>
+      </c>
+      <c r="E2214" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2214" s="3">
+        <v>45926.82708333334</v>
       </c>
     </row>
   </sheetData>
@@ -67767,6 +69269,64 @@
     <hyperlink ref="A2154" r:id="rId2153"/>
     <hyperlink ref="A2155" r:id="rId2154"/>
     <hyperlink ref="A2156" r:id="rId2155"/>
+    <hyperlink ref="A2157" r:id="rId2156"/>
+    <hyperlink ref="A2158" r:id="rId2157"/>
+    <hyperlink ref="A2159" r:id="rId2158"/>
+    <hyperlink ref="A2160" r:id="rId2159"/>
+    <hyperlink ref="A2161" r:id="rId2160"/>
+    <hyperlink ref="A2162" r:id="rId2161"/>
+    <hyperlink ref="A2163" r:id="rId2162"/>
+    <hyperlink ref="A2164" r:id="rId2163"/>
+    <hyperlink ref="A2165" r:id="rId2164"/>
+    <hyperlink ref="A2166" r:id="rId2165"/>
+    <hyperlink ref="A2167" r:id="rId2166"/>
+    <hyperlink ref="A2168" r:id="rId2167"/>
+    <hyperlink ref="A2169" r:id="rId2168"/>
+    <hyperlink ref="A2170" r:id="rId2169"/>
+    <hyperlink ref="A2171" r:id="rId2170"/>
+    <hyperlink ref="A2172" r:id="rId2171"/>
+    <hyperlink ref="A2173" r:id="rId2172"/>
+    <hyperlink ref="A2174" r:id="rId2173"/>
+    <hyperlink ref="A2175" r:id="rId2174"/>
+    <hyperlink ref="A2176" r:id="rId2175"/>
+    <hyperlink ref="A2177" r:id="rId2176"/>
+    <hyperlink ref="A2178" r:id="rId2177"/>
+    <hyperlink ref="A2179" r:id="rId2178"/>
+    <hyperlink ref="A2180" r:id="rId2179"/>
+    <hyperlink ref="A2181" r:id="rId2180"/>
+    <hyperlink ref="A2182" r:id="rId2181"/>
+    <hyperlink ref="A2183" r:id="rId2182"/>
+    <hyperlink ref="A2184" r:id="rId2183"/>
+    <hyperlink ref="A2185" r:id="rId2184"/>
+    <hyperlink ref="A2186" r:id="rId2185"/>
+    <hyperlink ref="A2187" r:id="rId2186"/>
+    <hyperlink ref="A2188" r:id="rId2187"/>
+    <hyperlink ref="A2189" r:id="rId2188"/>
+    <hyperlink ref="A2190" r:id="rId2189"/>
+    <hyperlink ref="A2191" r:id="rId2190"/>
+    <hyperlink ref="A2192" r:id="rId2191"/>
+    <hyperlink ref="A2193" r:id="rId2192"/>
+    <hyperlink ref="A2194" r:id="rId2193"/>
+    <hyperlink ref="A2195" r:id="rId2194"/>
+    <hyperlink ref="A2196" r:id="rId2195"/>
+    <hyperlink ref="A2197" r:id="rId2196"/>
+    <hyperlink ref="A2198" r:id="rId2197"/>
+    <hyperlink ref="A2199" r:id="rId2198"/>
+    <hyperlink ref="A2200" r:id="rId2199"/>
+    <hyperlink ref="A2201" r:id="rId2200"/>
+    <hyperlink ref="A2202" r:id="rId2201"/>
+    <hyperlink ref="A2203" r:id="rId2202"/>
+    <hyperlink ref="A2204" r:id="rId2203"/>
+    <hyperlink ref="A2205" r:id="rId2204"/>
+    <hyperlink ref="A2206" r:id="rId2205"/>
+    <hyperlink ref="A2207" r:id="rId2206"/>
+    <hyperlink ref="A2208" r:id="rId2207"/>
+    <hyperlink ref="A2209" r:id="rId2208"/>
+    <hyperlink ref="A2210" r:id="rId2209"/>
+    <hyperlink ref="A2211" r:id="rId2210"/>
+    <hyperlink ref="A2212" r:id="rId2211"/>
+    <hyperlink ref="A2213" r:id="rId2212"/>
+    <hyperlink ref="A2214" r:id="rId2213"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Update lands data - 2025-09-30 12:21
</commit_message>
<xml_diff>
--- a/lands-scraped.xlsx
+++ b/lands-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11337" uniqueCount="7074">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11512" uniqueCount="7168">
   <si>
     <t>link</t>
   </si>
@@ -21240,6 +21240,288 @@
   </si>
   <si>
     <t>43 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/aluksne-and-reg/aluksne/cxnhd.html</t>
+  </si>
+  <si>
+    <t>1 000 € (2.50 €/m²)</t>
+  </si>
+  <si>
+    <t>36010392319002</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/bauska/agfco.html</t>
+  </si>
+  <si>
+    <t>39 500 € (11.29 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/bauska/gpijh.html</t>
+  </si>
+  <si>
+    <t>25 500 € (15.71 €/m²)</t>
+  </si>
+  <si>
+    <t>1623 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/cesis/enoli.html</t>
+  </si>
+  <si>
+    <t>15 000 € (8.23 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/cesis/bxddn.html</t>
+  </si>
+  <si>
+    <t>45 000 € (2.94 €/m²)</t>
+  </si>
+  <si>
+    <t>15312 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/daugavpils/gigkb.html</t>
+  </si>
+  <si>
+    <t>38 700 € (22.76 €/m²)</t>
+  </si>
+  <si>
+    <t>0.17 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jekabpils-and-reg/dunavas-pag/mmnjc.html</t>
+  </si>
+  <si>
+    <t>70 000 € (0.54 €/m²)</t>
+  </si>
+  <si>
+    <t>56540030006</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jelgava/ammei.html</t>
+  </si>
+  <si>
+    <t>105 000 € (0.58 €/m²)</t>
+  </si>
+  <si>
+    <t>54520030011</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kuldiga-and-reg/kuldiga/eexbj.html</t>
+  </si>
+  <si>
+    <t>36 500 € (25.19 €/m²)</t>
+  </si>
+  <si>
+    <t>1449 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/nicas-pag/gjxio.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/grobina/pedxb.html</t>
+  </si>
+  <si>
+    <t>45 000 € (35.89 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/grobinas-pag/adddj.html</t>
+  </si>
+  <si>
+    <t>18 500 € (5.28 €/m²)</t>
+  </si>
+  <si>
+    <t>3502 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/vergales-pag/mdlij.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/pavilosta/apnde.html</t>
+  </si>
+  <si>
+    <t>90 800 € (100 €/m²)</t>
+  </si>
+  <si>
+    <t>908 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ludza-and-reg/cirmas-pag/ijhkg.html</t>
+  </si>
+  <si>
+    <t>18 000 € (0.90 €/m²)</t>
+  </si>
+  <si>
+    <t>68500040128</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/madona-and-reg/madona/cepepe.html</t>
+  </si>
+  <si>
+    <t>70010010884</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ikskiles-l-t/ahfdp.html</t>
+  </si>
+  <si>
+    <t>35 500 € (5 €/m²)</t>
+  </si>
+  <si>
+    <t>7100 m²</t>
+  </si>
+  <si>
+    <t>74940100153</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/lauberes-pag/odfbd.html</t>
+  </si>
+  <si>
+    <t>32 000 € (0.47 €/m²)</t>
+  </si>
+  <si>
+    <t>67500 m²</t>
+  </si>
+  <si>
+    <t>74600050081</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ogre/cglce.html</t>
+  </si>
+  <si>
+    <t>34 900 € (22.89 €/m²)</t>
+  </si>
+  <si>
+    <t>1525 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/preili-and-reg/turku-pag/coxxd.html</t>
+  </si>
+  <si>
+    <t>76860070018</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/preili-and-reg/pelecu-pag/bdkddi.html</t>
+  </si>
+  <si>
+    <t>18 000 € (1.80 €/m²)</t>
+  </si>
+  <si>
+    <t>76440050003</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/rezekne/kgcge.html</t>
+  </si>
+  <si>
+    <t>55 000 € (25 €/m²)</t>
+  </si>
+  <si>
+    <t>21000030614</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/lendzu-pag/cfmml.html</t>
+  </si>
+  <si>
+    <t>23 000 € (0.42 €/m²)</t>
+  </si>
+  <si>
+    <t>5.45 ha.</t>
+  </si>
+  <si>
+    <t>78660050207</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/ozolaines-pag/afcjj.html</t>
+  </si>
+  <si>
+    <t>8 800 € (6.38 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/vilanu-pag/bmhed.html</t>
+  </si>
+  <si>
+    <t>75 000 € (0.50 €/m²)</t>
+  </si>
+  <si>
+    <t>78980090234</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/kaunatas-pag/adkbc.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/tumes-pag/afecf.html</t>
+  </si>
+  <si>
+    <t>90840020077</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/tumes-pag/hlkgh.html</t>
+  </si>
+  <si>
+    <t>90840040047</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/engures-pag/gemfc.html</t>
+  </si>
+  <si>
+    <t>37 000 € (15.05 €/m²)</t>
+  </si>
+  <si>
+    <t>2458 m²</t>
+  </si>
+  <si>
+    <t>9050 009 0184</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/zantes-pag/amdxl.html</t>
+  </si>
+  <si>
+    <t>27 000 € (0.48 €/m²)</t>
+  </si>
+  <si>
+    <t>90920020080</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valka-and-reg/smiltene/bxbnjg.html</t>
+  </si>
+  <si>
+    <t>30 000 € (20.39 €/m²)</t>
+  </si>
+  <si>
+    <t>1471 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/burtnieku-pag/jbfmo.html</t>
+  </si>
+  <si>
+    <t>48 000 € (1.07 €/m²)</t>
+  </si>
+  <si>
+    <t>44800 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/valmiera/bgiglp.html</t>
+  </si>
+  <si>
+    <t>17 800 € (22 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/valmiera/jhdli.html</t>
+  </si>
+  <si>
+    <t>337 000 € (99.97 €/m²)</t>
+  </si>
+  <si>
+    <t>3371 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/varves-pag/glndm.html</t>
+  </si>
+  <si>
+    <t>3 300 € (1.10 €/m²)</t>
+  </si>
+  <si>
+    <t>98840130230</t>
   </si>
 </sst>
 </file>
@@ -21675,7 +21957,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -21714,1042 +21996,702 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>6918</v>
+        <v>7074</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>6919</v>
+        <v>7075</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>8</v>
+        <v>243</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>6920</v>
+        <v>4239</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>6921</v>
+        <v>7076</v>
       </c>
       <c r="F2" s="3">
-        <v>45929.60486111111</v>
+        <v>45930.44305555556</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>6922</v>
+        <v>7077</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>6923</v>
+        <v>7078</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>419</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>111</v>
+        <v>2271</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>6924</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3">
-        <v>45929.54236111111</v>
+        <v>45930.34305555555</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>6925</v>
+        <v>7079</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>6926</v>
+        <v>7080</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>419</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>1430</v>
+        <v>7081</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>6927</v>
+        <v>10</v>
       </c>
       <c r="F4" s="3">
-        <v>45928.52222222222</v>
+        <v>45930.34305555555</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>6928</v>
+        <v>7082</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>6929</v>
+        <v>7083</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>419</v>
+        <v>772</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>6930</v>
+        <v>5999</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>6931</v>
+        <v>10</v>
       </c>
       <c r="F5" s="3">
-        <v>45927.55208333333</v>
+        <v>45930.37569444445</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>6932</v>
+        <v>7084</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>6933</v>
+        <v>7085</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>419</v>
+        <v>772</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>1632</v>
+        <v>7086</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="3">
-        <v>45927.54375</v>
+        <v>45930.37569444445</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>6934</v>
+        <v>7087</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>6935</v>
+        <v>7088</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>772</v>
+        <v>1218</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>6936</v>
+        <v>7089</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>6937</v>
+        <v>10</v>
       </c>
       <c r="F7" s="3">
-        <v>45929.57430555555</v>
+        <v>45930.57916666666</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>6938</v>
+        <v>7090</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>6939</v>
+        <v>7091</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>772</v>
+        <v>1733</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>6940</v>
+        <v>474</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>6941</v>
+        <v>7092</v>
       </c>
       <c r="F8" s="3">
-        <v>45929.57430555555</v>
+        <v>45929.75277777778</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>6942</v>
+        <v>7093</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>6943</v>
+        <v>7094</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>772</v>
+        <v>1929</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>77</v>
+        <v>294</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>6944</v>
+        <v>7095</v>
       </c>
       <c r="F9" s="3">
-        <v>45929.51944444445</v>
+        <v>45929.75277777778</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>6945</v>
+        <v>7096</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>6946</v>
+        <v>7097</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>772</v>
+        <v>2671</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>325</v>
+        <v>7098</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>992</v>
+        <v>10</v>
       </c>
       <c r="F10" s="3">
-        <v>45928.78194444445</v>
+        <v>45930.523611111115</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>6947</v>
+        <v>7099</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>6948</v>
+        <v>2849</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>772</v>
+        <v>2846</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>6949</v>
+        <v>2271</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>6950</v>
+        <v>10</v>
       </c>
       <c r="F11" s="3">
-        <v>45928.555555555555</v>
+        <v>45930.53194444445</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>6951</v>
+        <v>7100</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>6952</v>
+        <v>7101</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>772</v>
+        <v>2846</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>561</v>
+        <v>453</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>6953</v>
+        <v>10</v>
       </c>
       <c r="F12" s="3">
-        <v>45928.415972222225</v>
+        <v>45930.49791666667</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>6954</v>
+        <v>7102</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>6955</v>
+        <v>7103</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>1218</v>
+        <v>2846</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>6956</v>
+        <v>7104</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="3">
-        <v>45929.54791666666</v>
+        <v>45930.492361111115</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>6957</v>
+        <v>7105</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>6958</v>
+        <v>3967</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>1218</v>
+        <v>2846</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>6959</v>
+        <v>383</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>6960</v>
+        <v>10</v>
       </c>
       <c r="F14" s="3">
-        <v>45929.45138888889</v>
+        <v>45930.02847222222</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>6961</v>
+        <v>7106</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>6962</v>
+        <v>7107</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>1569</v>
+        <v>2846</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>6963</v>
+        <v>7108</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>6964</v>
+        <v>10</v>
       </c>
       <c r="F15" s="3">
-        <v>45929.632638888885</v>
+        <v>45929.92291666666</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>6965</v>
+        <v>7109</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>4426</v>
+        <v>7110</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>1929</v>
+        <v>3762</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>2896</v>
+        <v>171</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>6966</v>
+        <v>7111</v>
       </c>
       <c r="F16" s="3">
-        <v>45929.52013888889</v>
+        <v>45929.788194444445</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>6967</v>
+        <v>7112</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>6968</v>
+        <v>2828</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>1929</v>
+        <v>3868</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>6969</v>
+        <v>2829</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>6970</v>
+        <v>7113</v>
       </c>
       <c r="F17" s="3">
-        <v>45929.49791666667</v>
+        <v>45930.44583333333</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>6971</v>
+        <v>7114</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>2283</v>
+        <v>7115</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>1929</v>
+        <v>4034</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>2284</v>
+        <v>7116</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>2285</v>
+        <v>7117</v>
       </c>
       <c r="F18" s="3">
-        <v>45929.441666666666</v>
+        <v>45930.427777777775</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>6972</v>
+        <v>7118</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>6973</v>
+        <v>7119</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>1929</v>
+        <v>4034</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>171</v>
+        <v>7120</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>2261</v>
+        <v>7121</v>
       </c>
       <c r="F19" s="3">
-        <v>45929.3875</v>
+        <v>45930.39375</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>6974</v>
+        <v>7122</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>6975</v>
+        <v>7123</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>1929</v>
+        <v>4034</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>353</v>
+        <v>7124</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F20" s="3">
-        <v>45928.94305555556</v>
+        <v>45929.94861111111</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>6976</v>
+        <v>7125</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>6977</v>
+        <v>1692</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>1929</v>
+        <v>4671</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>6978</v>
+        <v>171</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>10</v>
+        <v>7126</v>
       </c>
       <c r="F21" s="3">
-        <v>45928.464583333334</v>
+        <v>45930.464583333334</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>6979</v>
+        <v>7127</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>6980</v>
+        <v>7128</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>2488</v>
+        <v>4671</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>201</v>
+        <v>32</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>6981</v>
+        <v>7129</v>
       </c>
       <c r="F22" s="3">
-        <v>45929.33333333333</v>
+        <v>45929.711805555555</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>6982</v>
+        <v>7130</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>6983</v>
+        <v>7131</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>2488</v>
+        <v>4770</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>32</v>
+        <v>4348</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>6984</v>
+        <v>7132</v>
       </c>
       <c r="F23" s="3">
-        <v>45928.802777777775</v>
+        <v>45930.46944444445</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>6985</v>
+        <v>7133</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>6986</v>
+        <v>7134</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>2488</v>
+        <v>4770</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>390</v>
+        <v>7135</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>6987</v>
+        <v>7136</v>
       </c>
       <c r="F24" s="3">
-        <v>45927.89722222222</v>
+        <v>45930.433333333334</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>6988</v>
+        <v>7137</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>6989</v>
+        <v>7138</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>3398</v>
+        <v>4770</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>3454</v>
+        <v>3702</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F25" s="3">
-        <v>45929.450694444444</v>
+        <v>45929.77083333333</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>6990</v>
+        <v>7139</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>6991</v>
+        <v>7140</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>3762</v>
+        <v>4770</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>6992</v>
+        <v>2191</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>6993</v>
+        <v>7141</v>
       </c>
       <c r="F26" s="3">
-        <v>45928.68611111111</v>
+        <v>45929.665972222225</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>6994</v>
+        <v>7142</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>6995</v>
+        <v>5131</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>3762</v>
+        <v>4770</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>6996</v>
+        <v>1430</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>10</v>
+        <v>5132</v>
       </c>
       <c r="F27" s="3">
-        <v>45928.54375</v>
+        <v>45929.65555555555</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>6997</v>
+        <v>7143</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>3761</v>
+        <v>2534</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>3762</v>
+        <v>5674</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>866</v>
+        <v>171</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>10</v>
+        <v>7144</v>
       </c>
       <c r="F28" s="3">
-        <v>45928.54375</v>
+        <v>45930.6125</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>6998</v>
+        <v>7145</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>6999</v>
+        <v>1187</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>4034</v>
+        <v>5674</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>32</v>
+        <v>201</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>7000</v>
+        <v>7146</v>
       </c>
       <c r="F29" s="3">
-        <v>45928.92569444445</v>
+        <v>45930.611805555556</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>7001</v>
+        <v>7147</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>7002</v>
+        <v>7148</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>4034</v>
+        <v>5674</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>6426</v>
+        <v>7149</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>10</v>
+        <v>7150</v>
       </c>
       <c r="F30" s="3">
-        <v>45928</v>
+        <v>45930.413194444445</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>7003</v>
+        <v>7151</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>7004</v>
+        <v>7152</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>4034</v>
+        <v>5674</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>2244</v>
+        <v>239</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>7005</v>
+        <v>7153</v>
       </c>
       <c r="F31" s="3">
-        <v>45927.89791666667</v>
+        <v>45929.888194444444</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>7006</v>
+        <v>7154</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>7007</v>
+        <v>7155</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>4034</v>
+        <v>6133</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>575</v>
+        <v>7156</v>
       </c>
       <c r="E32" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F32" s="3">
-        <v>45927.80972222222</v>
+        <v>45930.47777777778</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>7008</v>
+        <v>7157</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>7009</v>
+        <v>7158</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>4034</v>
+        <v>6207</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>7010</v>
+        <v>7159</v>
       </c>
       <c r="E33" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F33" s="3">
-        <v>45927.64166666666</v>
+        <v>45930.48055555555</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>7011</v>
+        <v>7160</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>403</v>
+        <v>7161</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>4770</v>
+        <v>6207</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>77</v>
+        <v>3097</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>7012</v>
+        <v>10</v>
       </c>
       <c r="F34" s="3">
-        <v>45928.80972222222</v>
+        <v>45930.47986111111</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>7013</v>
+        <v>7162</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>1989</v>
+        <v>7163</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>4770</v>
+        <v>6207</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>171</v>
+        <v>7164</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>7014</v>
+        <v>10</v>
       </c>
       <c r="F35" s="3">
-        <v>45928.808333333334</v>
+        <v>45930.476388888885</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>7015</v>
+        <v>7165</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>7016</v>
+        <v>7166</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>4770</v>
+        <v>6439</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>407</v>
+        <v>2538</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>7017</v>
+        <v>7167</v>
       </c>
       <c r="F36" s="3">
-        <v>45928.67638888889</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
-        <v>7018</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>7019</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>4770</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>2343</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>7020</v>
-      </c>
-      <c r="F37" s="3">
-        <v>45928.54375</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>7021</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>7022</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>4770</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>7023</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>7024</v>
-      </c>
-      <c r="F38" s="3">
-        <v>45927.59722222222</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>7025</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>4774</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>5147</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>561</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>7026</v>
-      </c>
-      <c r="F39" s="3">
-        <v>45929.60486111111</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>7027</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>7028</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>5266</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>4778</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>7029</v>
-      </c>
-      <c r="F40" s="3">
-        <v>45929.47430555556</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>7030</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>7031</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>5266</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>7032</v>
-      </c>
-      <c r="F41" s="3">
-        <v>45929.34583333333</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
-        <v>7033</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>7034</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>5266</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>2343</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>7035</v>
-      </c>
-      <c r="F42" s="3">
-        <v>45928.84722222222</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
-        <v>7036</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>3789</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>5674</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>3790</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>7037</v>
-      </c>
-      <c r="F43" s="3">
-        <v>45929.61319444445</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
-        <v>7038</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>7039</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>5674</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>7040</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>7041</v>
-      </c>
-      <c r="F44" s="3">
-        <v>45929.60763888889</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
-        <v>7042</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>7043</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>5674</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>7044</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>7045</v>
-      </c>
-      <c r="F45" s="3">
-        <v>45928.88402777778</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
-        <v>7046</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>7047</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>7048</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>7049</v>
-      </c>
-      <c r="F46" s="3">
-        <v>45929.60555555555</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
-        <v>7050</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>7051</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>7052</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>7053</v>
-      </c>
-      <c r="F47" s="3">
-        <v>45929.60555555555</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
-        <v>7054</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>7055</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>7056</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>7057</v>
-      </c>
-      <c r="F48" s="3">
-        <v>45929.60555555555</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
-        <v>7058</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>7059</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>7060</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>7061</v>
-      </c>
-      <c r="F49" s="3">
-        <v>45929.57291666667</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
-        <v>7062</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>323</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>325</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>7063</v>
-      </c>
-      <c r="F50" s="3">
-        <v>45929.40069444444</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
-        <v>7064</v>
-      </c>
-      <c r="B51" s="9" t="s">
-        <v>7065</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>7066</v>
-      </c>
-      <c r="F51" s="3">
-        <v>45928.99166666667</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
-        <v>7067</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>7068</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>7069</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>7070</v>
-      </c>
-      <c r="F52" s="3">
-        <v>45928.47430555556</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
-        <v>7071</v>
-      </c>
-      <c r="B53" s="9" t="s">
-        <v>7072</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>1194</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>7073</v>
-      </c>
-      <c r="E53" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F53" s="3">
-        <v>45928.39444444445</v>
+        <v>45929.75208333333</v>
       </c>
     </row>
   </sheetData>
@@ -22789,23 +22731,6 @@
     <hyperlink ref="A34" r:id="rId33"/>
     <hyperlink ref="A35" r:id="rId34"/>
     <hyperlink ref="A36" r:id="rId35"/>
-    <hyperlink ref="A37" r:id="rId36"/>
-    <hyperlink ref="A38" r:id="rId37"/>
-    <hyperlink ref="A39" r:id="rId38"/>
-    <hyperlink ref="A40" r:id="rId39"/>
-    <hyperlink ref="A41" r:id="rId40"/>
-    <hyperlink ref="A42" r:id="rId41"/>
-    <hyperlink ref="A43" r:id="rId42"/>
-    <hyperlink ref="A44" r:id="rId43"/>
-    <hyperlink ref="A45" r:id="rId44"/>
-    <hyperlink ref="A46" r:id="rId45"/>
-    <hyperlink ref="A47" r:id="rId46"/>
-    <hyperlink ref="A48" r:id="rId47"/>
-    <hyperlink ref="A49" r:id="rId48"/>
-    <hyperlink ref="A50" r:id="rId49"/>
-    <hyperlink ref="A51" r:id="rId50"/>
-    <hyperlink ref="A52" r:id="rId51"/>
-    <hyperlink ref="A53" r:id="rId52"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -22814,7 +22739,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2214"/>
+  <dimension ref="A1:F2266"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -67110,6 +67035,1046 @@
       </c>
       <c r="F2214" s="3">
         <v>45926.82708333334</v>
+      </c>
+    </row>
+    <row r="2215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2215" s="4" t="s">
+        <v>6918</v>
+      </c>
+      <c r="B2215" s="3" t="s">
+        <v>6919</v>
+      </c>
+      <c r="C2215" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2215" s="3" t="s">
+        <v>6920</v>
+      </c>
+      <c r="E2215" s="3" t="s">
+        <v>6921</v>
+      </c>
+      <c r="F2215" s="3">
+        <v>45929.60486111111</v>
+      </c>
+    </row>
+    <row r="2216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2216" s="4" t="s">
+        <v>6922</v>
+      </c>
+      <c r="B2216" s="3" t="s">
+        <v>6923</v>
+      </c>
+      <c r="C2216" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2216" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2216" s="3" t="s">
+        <v>6924</v>
+      </c>
+      <c r="F2216" s="3">
+        <v>45929.54236111111</v>
+      </c>
+    </row>
+    <row r="2217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2217" s="4" t="s">
+        <v>6925</v>
+      </c>
+      <c r="B2217" s="3" t="s">
+        <v>6926</v>
+      </c>
+      <c r="C2217" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2217" s="3" t="s">
+        <v>1430</v>
+      </c>
+      <c r="E2217" s="3" t="s">
+        <v>6927</v>
+      </c>
+      <c r="F2217" s="3">
+        <v>45928.52222222222</v>
+      </c>
+    </row>
+    <row r="2218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2218" s="4" t="s">
+        <v>6928</v>
+      </c>
+      <c r="B2218" s="3" t="s">
+        <v>6929</v>
+      </c>
+      <c r="C2218" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2218" s="3" t="s">
+        <v>6930</v>
+      </c>
+      <c r="E2218" s="3" t="s">
+        <v>6931</v>
+      </c>
+      <c r="F2218" s="3">
+        <v>45927.55208333333</v>
+      </c>
+    </row>
+    <row r="2219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2219" s="4" t="s">
+        <v>6932</v>
+      </c>
+      <c r="B2219" s="3" t="s">
+        <v>6933</v>
+      </c>
+      <c r="C2219" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2219" s="3" t="s">
+        <v>1632</v>
+      </c>
+      <c r="E2219" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2219" s="3">
+        <v>45927.54375</v>
+      </c>
+    </row>
+    <row r="2220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2220" s="4" t="s">
+        <v>6934</v>
+      </c>
+      <c r="B2220" s="3" t="s">
+        <v>6935</v>
+      </c>
+      <c r="C2220" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2220" s="3" t="s">
+        <v>6936</v>
+      </c>
+      <c r="E2220" s="3" t="s">
+        <v>6937</v>
+      </c>
+      <c r="F2220" s="3">
+        <v>45929.57430555555</v>
+      </c>
+    </row>
+    <row r="2221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2221" s="4" t="s">
+        <v>6938</v>
+      </c>
+      <c r="B2221" s="3" t="s">
+        <v>6939</v>
+      </c>
+      <c r="C2221" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2221" s="3" t="s">
+        <v>6940</v>
+      </c>
+      <c r="E2221" s="3" t="s">
+        <v>6941</v>
+      </c>
+      <c r="F2221" s="3">
+        <v>45929.57430555555</v>
+      </c>
+    </row>
+    <row r="2222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2222" s="4" t="s">
+        <v>6942</v>
+      </c>
+      <c r="B2222" s="3" t="s">
+        <v>6943</v>
+      </c>
+      <c r="C2222" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2222" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2222" s="3" t="s">
+        <v>6944</v>
+      </c>
+      <c r="F2222" s="3">
+        <v>45929.51944444445</v>
+      </c>
+    </row>
+    <row r="2223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2223" s="4" t="s">
+        <v>6945</v>
+      </c>
+      <c r="B2223" s="3" t="s">
+        <v>6946</v>
+      </c>
+      <c r="C2223" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2223" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2223" s="3" t="s">
+        <v>992</v>
+      </c>
+      <c r="F2223" s="3">
+        <v>45928.78194444445</v>
+      </c>
+    </row>
+    <row r="2224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2224" s="4" t="s">
+        <v>6947</v>
+      </c>
+      <c r="B2224" s="3" t="s">
+        <v>6948</v>
+      </c>
+      <c r="C2224" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2224" s="3" t="s">
+        <v>6949</v>
+      </c>
+      <c r="E2224" s="3" t="s">
+        <v>6950</v>
+      </c>
+      <c r="F2224" s="3">
+        <v>45928.555555555555</v>
+      </c>
+    </row>
+    <row r="2225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2225" s="4" t="s">
+        <v>6951</v>
+      </c>
+      <c r="B2225" s="3" t="s">
+        <v>6952</v>
+      </c>
+      <c r="C2225" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2225" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="E2225" s="3" t="s">
+        <v>6953</v>
+      </c>
+      <c r="F2225" s="3">
+        <v>45928.415972222225</v>
+      </c>
+    </row>
+    <row r="2226" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2226" s="4" t="s">
+        <v>6954</v>
+      </c>
+      <c r="B2226" s="3" t="s">
+        <v>6955</v>
+      </c>
+      <c r="C2226" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2226" s="3" t="s">
+        <v>6956</v>
+      </c>
+      <c r="E2226" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2226" s="3">
+        <v>45929.54791666666</v>
+      </c>
+    </row>
+    <row r="2227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2227" s="4" t="s">
+        <v>6957</v>
+      </c>
+      <c r="B2227" s="3" t="s">
+        <v>6958</v>
+      </c>
+      <c r="C2227" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2227" s="3" t="s">
+        <v>6959</v>
+      </c>
+      <c r="E2227" s="3" t="s">
+        <v>6960</v>
+      </c>
+      <c r="F2227" s="3">
+        <v>45929.45138888889</v>
+      </c>
+    </row>
+    <row r="2228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2228" s="4" t="s">
+        <v>6961</v>
+      </c>
+      <c r="B2228" s="3" t="s">
+        <v>6962</v>
+      </c>
+      <c r="C2228" s="3" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D2228" s="3" t="s">
+        <v>6963</v>
+      </c>
+      <c r="E2228" s="3" t="s">
+        <v>6964</v>
+      </c>
+      <c r="F2228" s="3">
+        <v>45929.632638888885</v>
+      </c>
+    </row>
+    <row r="2229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2229" s="4" t="s">
+        <v>6965</v>
+      </c>
+      <c r="B2229" s="3" t="s">
+        <v>4426</v>
+      </c>
+      <c r="C2229" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2229" s="3" t="s">
+        <v>2896</v>
+      </c>
+      <c r="E2229" s="3" t="s">
+        <v>6966</v>
+      </c>
+      <c r="F2229" s="3">
+        <v>45929.52013888889</v>
+      </c>
+    </row>
+    <row r="2230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2230" s="4" t="s">
+        <v>6967</v>
+      </c>
+      <c r="B2230" s="3" t="s">
+        <v>6968</v>
+      </c>
+      <c r="C2230" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2230" s="3" t="s">
+        <v>6969</v>
+      </c>
+      <c r="E2230" s="3" t="s">
+        <v>6970</v>
+      </c>
+      <c r="F2230" s="3">
+        <v>45929.49791666667</v>
+      </c>
+    </row>
+    <row r="2231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2231" s="4" t="s">
+        <v>6971</v>
+      </c>
+      <c r="B2231" s="3" t="s">
+        <v>2283</v>
+      </c>
+      <c r="C2231" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2231" s="3" t="s">
+        <v>2284</v>
+      </c>
+      <c r="E2231" s="3" t="s">
+        <v>2285</v>
+      </c>
+      <c r="F2231" s="3">
+        <v>45929.441666666666</v>
+      </c>
+    </row>
+    <row r="2232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2232" s="4" t="s">
+        <v>6972</v>
+      </c>
+      <c r="B2232" s="3" t="s">
+        <v>6973</v>
+      </c>
+      <c r="C2232" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2232" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2232" s="3" t="s">
+        <v>2261</v>
+      </c>
+      <c r="F2232" s="3">
+        <v>45929.3875</v>
+      </c>
+    </row>
+    <row r="2233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2233" s="4" t="s">
+        <v>6974</v>
+      </c>
+      <c r="B2233" s="3" t="s">
+        <v>6975</v>
+      </c>
+      <c r="C2233" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2233" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="E2233" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2233" s="3">
+        <v>45928.94305555556</v>
+      </c>
+    </row>
+    <row r="2234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2234" s="4" t="s">
+        <v>6976</v>
+      </c>
+      <c r="B2234" s="3" t="s">
+        <v>6977</v>
+      </c>
+      <c r="C2234" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2234" s="3" t="s">
+        <v>6978</v>
+      </c>
+      <c r="E2234" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2234" s="3">
+        <v>45928.464583333334</v>
+      </c>
+    </row>
+    <row r="2235" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2235" s="4" t="s">
+        <v>6979</v>
+      </c>
+      <c r="B2235" s="3" t="s">
+        <v>6980</v>
+      </c>
+      <c r="C2235" s="3" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D2235" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2235" s="3" t="s">
+        <v>6981</v>
+      </c>
+      <c r="F2235" s="3">
+        <v>45929.33333333333</v>
+      </c>
+    </row>
+    <row r="2236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2236" s="4" t="s">
+        <v>6982</v>
+      </c>
+      <c r="B2236" s="3" t="s">
+        <v>6983</v>
+      </c>
+      <c r="C2236" s="3" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D2236" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2236" s="3" t="s">
+        <v>6984</v>
+      </c>
+      <c r="F2236" s="3">
+        <v>45928.802777777775</v>
+      </c>
+    </row>
+    <row r="2237" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2237" s="4" t="s">
+        <v>6985</v>
+      </c>
+      <c r="B2237" s="3" t="s">
+        <v>6986</v>
+      </c>
+      <c r="C2237" s="3" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D2237" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="E2237" s="3" t="s">
+        <v>6987</v>
+      </c>
+      <c r="F2237" s="3">
+        <v>45927.89722222222</v>
+      </c>
+    </row>
+    <row r="2238" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2238" s="4" t="s">
+        <v>6988</v>
+      </c>
+      <c r="B2238" s="3" t="s">
+        <v>6989</v>
+      </c>
+      <c r="C2238" s="3" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D2238" s="3" t="s">
+        <v>3454</v>
+      </c>
+      <c r="E2238" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2238" s="3">
+        <v>45929.450694444444</v>
+      </c>
+    </row>
+    <row r="2239" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2239" s="4" t="s">
+        <v>6990</v>
+      </c>
+      <c r="B2239" s="3" t="s">
+        <v>6991</v>
+      </c>
+      <c r="C2239" s="3" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D2239" s="3" t="s">
+        <v>6992</v>
+      </c>
+      <c r="E2239" s="3" t="s">
+        <v>6993</v>
+      </c>
+      <c r="F2239" s="3">
+        <v>45928.68611111111</v>
+      </c>
+    </row>
+    <row r="2240" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2240" s="4" t="s">
+        <v>6994</v>
+      </c>
+      <c r="B2240" s="3" t="s">
+        <v>6995</v>
+      </c>
+      <c r="C2240" s="3" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D2240" s="3" t="s">
+        <v>6996</v>
+      </c>
+      <c r="E2240" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2240" s="3">
+        <v>45928.54375</v>
+      </c>
+    </row>
+    <row r="2241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2241" s="4" t="s">
+        <v>6997</v>
+      </c>
+      <c r="B2241" s="3" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C2241" s="3" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D2241" s="3" t="s">
+        <v>866</v>
+      </c>
+      <c r="E2241" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2241" s="3">
+        <v>45928.54375</v>
+      </c>
+    </row>
+    <row r="2242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2242" s="4" t="s">
+        <v>6998</v>
+      </c>
+      <c r="B2242" s="3" t="s">
+        <v>6999</v>
+      </c>
+      <c r="C2242" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2242" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2242" s="3" t="s">
+        <v>7000</v>
+      </c>
+      <c r="F2242" s="3">
+        <v>45928.92569444445</v>
+      </c>
+    </row>
+    <row r="2243" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2243" s="4" t="s">
+        <v>7001</v>
+      </c>
+      <c r="B2243" s="3" t="s">
+        <v>7002</v>
+      </c>
+      <c r="C2243" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2243" s="3" t="s">
+        <v>6426</v>
+      </c>
+      <c r="E2243" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2243" s="3">
+        <v>45928</v>
+      </c>
+    </row>
+    <row r="2244" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2244" s="4" t="s">
+        <v>7003</v>
+      </c>
+      <c r="B2244" s="3" t="s">
+        <v>7004</v>
+      </c>
+      <c r="C2244" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2244" s="3" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E2244" s="3" t="s">
+        <v>7005</v>
+      </c>
+      <c r="F2244" s="3">
+        <v>45927.89791666667</v>
+      </c>
+    </row>
+    <row r="2245" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2245" s="4" t="s">
+        <v>7006</v>
+      </c>
+      <c r="B2245" s="3" t="s">
+        <v>7007</v>
+      </c>
+      <c r="C2245" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2245" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="E2245" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2245" s="3">
+        <v>45927.80972222222</v>
+      </c>
+    </row>
+    <row r="2246" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2246" s="4" t="s">
+        <v>7008</v>
+      </c>
+      <c r="B2246" s="3" t="s">
+        <v>7009</v>
+      </c>
+      <c r="C2246" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2246" s="3" t="s">
+        <v>7010</v>
+      </c>
+      <c r="E2246" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2246" s="3">
+        <v>45927.64166666666</v>
+      </c>
+    </row>
+    <row r="2247" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2247" s="4" t="s">
+        <v>7011</v>
+      </c>
+      <c r="B2247" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="C2247" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2247" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2247" s="3" t="s">
+        <v>7012</v>
+      </c>
+      <c r="F2247" s="3">
+        <v>45928.80972222222</v>
+      </c>
+    </row>
+    <row r="2248" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2248" s="4" t="s">
+        <v>7013</v>
+      </c>
+      <c r="B2248" s="3" t="s">
+        <v>1989</v>
+      </c>
+      <c r="C2248" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2248" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2248" s="3" t="s">
+        <v>7014</v>
+      </c>
+      <c r="F2248" s="3">
+        <v>45928.808333333334</v>
+      </c>
+    </row>
+    <row r="2249" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2249" s="4" t="s">
+        <v>7015</v>
+      </c>
+      <c r="B2249" s="3" t="s">
+        <v>7016</v>
+      </c>
+      <c r="C2249" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2249" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="E2249" s="3" t="s">
+        <v>7017</v>
+      </c>
+      <c r="F2249" s="3">
+        <v>45928.67638888889</v>
+      </c>
+    </row>
+    <row r="2250" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2250" s="4" t="s">
+        <v>7018</v>
+      </c>
+      <c r="B2250" s="3" t="s">
+        <v>7019</v>
+      </c>
+      <c r="C2250" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2250" s="3" t="s">
+        <v>2343</v>
+      </c>
+      <c r="E2250" s="3" t="s">
+        <v>7020</v>
+      </c>
+      <c r="F2250" s="3">
+        <v>45928.54375</v>
+      </c>
+    </row>
+    <row r="2251" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2251" s="4" t="s">
+        <v>7021</v>
+      </c>
+      <c r="B2251" s="3" t="s">
+        <v>7022</v>
+      </c>
+      <c r="C2251" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2251" s="3" t="s">
+        <v>7023</v>
+      </c>
+      <c r="E2251" s="3" t="s">
+        <v>7024</v>
+      </c>
+      <c r="F2251" s="3">
+        <v>45927.59722222222</v>
+      </c>
+    </row>
+    <row r="2252" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2252" s="4" t="s">
+        <v>7025</v>
+      </c>
+      <c r="B2252" s="3" t="s">
+        <v>4774</v>
+      </c>
+      <c r="C2252" s="3" t="s">
+        <v>5147</v>
+      </c>
+      <c r="D2252" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="E2252" s="3" t="s">
+        <v>7026</v>
+      </c>
+      <c r="F2252" s="3">
+        <v>45929.60486111111</v>
+      </c>
+    </row>
+    <row r="2253" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2253" s="4" t="s">
+        <v>7027</v>
+      </c>
+      <c r="B2253" s="3" t="s">
+        <v>7028</v>
+      </c>
+      <c r="C2253" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2253" s="3" t="s">
+        <v>4778</v>
+      </c>
+      <c r="E2253" s="3" t="s">
+        <v>7029</v>
+      </c>
+      <c r="F2253" s="3">
+        <v>45929.47430555556</v>
+      </c>
+    </row>
+    <row r="2254" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2254" s="4" t="s">
+        <v>7030</v>
+      </c>
+      <c r="B2254" s="3" t="s">
+        <v>7031</v>
+      </c>
+      <c r="C2254" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2254" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2254" s="3" t="s">
+        <v>7032</v>
+      </c>
+      <c r="F2254" s="3">
+        <v>45929.34583333333</v>
+      </c>
+    </row>
+    <row r="2255" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2255" s="4" t="s">
+        <v>7033</v>
+      </c>
+      <c r="B2255" s="3" t="s">
+        <v>7034</v>
+      </c>
+      <c r="C2255" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2255" s="3" t="s">
+        <v>2343</v>
+      </c>
+      <c r="E2255" s="3" t="s">
+        <v>7035</v>
+      </c>
+      <c r="F2255" s="3">
+        <v>45928.84722222222</v>
+      </c>
+    </row>
+    <row r="2256" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2256" s="4" t="s">
+        <v>7036</v>
+      </c>
+      <c r="B2256" s="3" t="s">
+        <v>3789</v>
+      </c>
+      <c r="C2256" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2256" s="3" t="s">
+        <v>3790</v>
+      </c>
+      <c r="E2256" s="3" t="s">
+        <v>7037</v>
+      </c>
+      <c r="F2256" s="3">
+        <v>45929.61319444445</v>
+      </c>
+    </row>
+    <row r="2257" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2257" s="4" t="s">
+        <v>7038</v>
+      </c>
+      <c r="B2257" s="3" t="s">
+        <v>7039</v>
+      </c>
+      <c r="C2257" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2257" s="3" t="s">
+        <v>7040</v>
+      </c>
+      <c r="E2257" s="3" t="s">
+        <v>7041</v>
+      </c>
+      <c r="F2257" s="3">
+        <v>45929.60763888889</v>
+      </c>
+    </row>
+    <row r="2258" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2258" s="4" t="s">
+        <v>7042</v>
+      </c>
+      <c r="B2258" s="3" t="s">
+        <v>7043</v>
+      </c>
+      <c r="C2258" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2258" s="3" t="s">
+        <v>7044</v>
+      </c>
+      <c r="E2258" s="3" t="s">
+        <v>7045</v>
+      </c>
+      <c r="F2258" s="3">
+        <v>45928.88402777778</v>
+      </c>
+    </row>
+    <row r="2259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2259" s="4" t="s">
+        <v>7046</v>
+      </c>
+      <c r="B2259" s="3" t="s">
+        <v>7047</v>
+      </c>
+      <c r="C2259" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2259" s="3" t="s">
+        <v>7048</v>
+      </c>
+      <c r="E2259" s="3" t="s">
+        <v>7049</v>
+      </c>
+      <c r="F2259" s="3">
+        <v>45929.60555555555</v>
+      </c>
+    </row>
+    <row r="2260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2260" s="4" t="s">
+        <v>7050</v>
+      </c>
+      <c r="B2260" s="3" t="s">
+        <v>7051</v>
+      </c>
+      <c r="C2260" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2260" s="3" t="s">
+        <v>7052</v>
+      </c>
+      <c r="E2260" s="3" t="s">
+        <v>7053</v>
+      </c>
+      <c r="F2260" s="3">
+        <v>45929.60555555555</v>
+      </c>
+    </row>
+    <row r="2261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2261" s="4" t="s">
+        <v>7054</v>
+      </c>
+      <c r="B2261" s="3" t="s">
+        <v>7055</v>
+      </c>
+      <c r="C2261" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2261" s="3" t="s">
+        <v>7056</v>
+      </c>
+      <c r="E2261" s="3" t="s">
+        <v>7057</v>
+      </c>
+      <c r="F2261" s="3">
+        <v>45929.60555555555</v>
+      </c>
+    </row>
+    <row r="2262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2262" s="4" t="s">
+        <v>7058</v>
+      </c>
+      <c r="B2262" s="3" t="s">
+        <v>7059</v>
+      </c>
+      <c r="C2262" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2262" s="3" t="s">
+        <v>7060</v>
+      </c>
+      <c r="E2262" s="3" t="s">
+        <v>7061</v>
+      </c>
+      <c r="F2262" s="3">
+        <v>45929.57291666667</v>
+      </c>
+    </row>
+    <row r="2263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2263" s="4" t="s">
+        <v>7062</v>
+      </c>
+      <c r="B2263" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C2263" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2263" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2263" s="3" t="s">
+        <v>7063</v>
+      </c>
+      <c r="F2263" s="3">
+        <v>45929.40069444444</v>
+      </c>
+    </row>
+    <row r="2264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2264" s="4" t="s">
+        <v>7064</v>
+      </c>
+      <c r="B2264" s="3" t="s">
+        <v>7065</v>
+      </c>
+      <c r="C2264" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2264" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2264" s="3" t="s">
+        <v>7066</v>
+      </c>
+      <c r="F2264" s="3">
+        <v>45928.99166666667</v>
+      </c>
+    </row>
+    <row r="2265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2265" s="4" t="s">
+        <v>7067</v>
+      </c>
+      <c r="B2265" s="3" t="s">
+        <v>7068</v>
+      </c>
+      <c r="C2265" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2265" s="3" t="s">
+        <v>7069</v>
+      </c>
+      <c r="E2265" s="3" t="s">
+        <v>7070</v>
+      </c>
+      <c r="F2265" s="3">
+        <v>45928.47430555556</v>
+      </c>
+    </row>
+    <row r="2266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2266" s="4" t="s">
+        <v>7071</v>
+      </c>
+      <c r="B2266" s="3" t="s">
+        <v>7072</v>
+      </c>
+      <c r="C2266" s="3" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D2266" s="3" t="s">
+        <v>7073</v>
+      </c>
+      <c r="E2266" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2266" s="3">
+        <v>45928.39444444445</v>
       </c>
     </row>
   </sheetData>
@@ -69327,6 +70292,58 @@
     <hyperlink ref="A2212" r:id="rId2211"/>
     <hyperlink ref="A2213" r:id="rId2212"/>
     <hyperlink ref="A2214" r:id="rId2213"/>
+    <hyperlink ref="A2215" r:id="rId2214"/>
+    <hyperlink ref="A2216" r:id="rId2215"/>
+    <hyperlink ref="A2217" r:id="rId2216"/>
+    <hyperlink ref="A2218" r:id="rId2217"/>
+    <hyperlink ref="A2219" r:id="rId2218"/>
+    <hyperlink ref="A2220" r:id="rId2219"/>
+    <hyperlink ref="A2221" r:id="rId2220"/>
+    <hyperlink ref="A2222" r:id="rId2221"/>
+    <hyperlink ref="A2223" r:id="rId2222"/>
+    <hyperlink ref="A2224" r:id="rId2223"/>
+    <hyperlink ref="A2225" r:id="rId2224"/>
+    <hyperlink ref="A2226" r:id="rId2225"/>
+    <hyperlink ref="A2227" r:id="rId2226"/>
+    <hyperlink ref="A2228" r:id="rId2227"/>
+    <hyperlink ref="A2229" r:id="rId2228"/>
+    <hyperlink ref="A2230" r:id="rId2229"/>
+    <hyperlink ref="A2231" r:id="rId2230"/>
+    <hyperlink ref="A2232" r:id="rId2231"/>
+    <hyperlink ref="A2233" r:id="rId2232"/>
+    <hyperlink ref="A2234" r:id="rId2233"/>
+    <hyperlink ref="A2235" r:id="rId2234"/>
+    <hyperlink ref="A2236" r:id="rId2235"/>
+    <hyperlink ref="A2237" r:id="rId2236"/>
+    <hyperlink ref="A2238" r:id="rId2237"/>
+    <hyperlink ref="A2239" r:id="rId2238"/>
+    <hyperlink ref="A2240" r:id="rId2239"/>
+    <hyperlink ref="A2241" r:id="rId2240"/>
+    <hyperlink ref="A2242" r:id="rId2241"/>
+    <hyperlink ref="A2243" r:id="rId2242"/>
+    <hyperlink ref="A2244" r:id="rId2243"/>
+    <hyperlink ref="A2245" r:id="rId2244"/>
+    <hyperlink ref="A2246" r:id="rId2245"/>
+    <hyperlink ref="A2247" r:id="rId2246"/>
+    <hyperlink ref="A2248" r:id="rId2247"/>
+    <hyperlink ref="A2249" r:id="rId2248"/>
+    <hyperlink ref="A2250" r:id="rId2249"/>
+    <hyperlink ref="A2251" r:id="rId2250"/>
+    <hyperlink ref="A2252" r:id="rId2251"/>
+    <hyperlink ref="A2253" r:id="rId2252"/>
+    <hyperlink ref="A2254" r:id="rId2253"/>
+    <hyperlink ref="A2255" r:id="rId2254"/>
+    <hyperlink ref="A2256" r:id="rId2255"/>
+    <hyperlink ref="A2257" r:id="rId2256"/>
+    <hyperlink ref="A2258" r:id="rId2257"/>
+    <hyperlink ref="A2259" r:id="rId2258"/>
+    <hyperlink ref="A2260" r:id="rId2259"/>
+    <hyperlink ref="A2261" r:id="rId2260"/>
+    <hyperlink ref="A2262" r:id="rId2261"/>
+    <hyperlink ref="A2263" r:id="rId2262"/>
+    <hyperlink ref="A2264" r:id="rId2263"/>
+    <hyperlink ref="A2265" r:id="rId2264"/>
+    <hyperlink ref="A2266" r:id="rId2265"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Update lands data - 2025-10-01 12:21
</commit_message>
<xml_diff>
--- a/lands-scraped.xlsx
+++ b/lands-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11512" uniqueCount="7168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11647" uniqueCount="7239">
   <si>
     <t>link</t>
   </si>
@@ -21522,6 +21522,219 @@
   </si>
   <si>
     <t>98840130230</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/aizkraukle-and-reg/kokneses-pag/gecnp.html</t>
+  </si>
+  <si>
+    <t>12 000 € (0.69 €/m²)</t>
+  </si>
+  <si>
+    <t>17300 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/balvi-and-reg/balvi/jbxcl.html</t>
+  </si>
+  <si>
+    <t>2 100 € (1.24 €/m²)</t>
+  </si>
+  <si>
+    <t>1699 m²</t>
+  </si>
+  <si>
+    <t>38460030218</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/bauska/dnffn.html</t>
+  </si>
+  <si>
+    <t>54 000 € (28.24 €/m²)</t>
+  </si>
+  <si>
+    <t>1912 m²</t>
+  </si>
+  <si>
+    <t>40010050247</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/ligatne/inpnl.html</t>
+  </si>
+  <si>
+    <t>27 000 € (1 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jekabpils-and-reg/asares-pag/cfdnxg.html</t>
+  </si>
+  <si>
+    <t>56840050396</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jekabpils-and-reg/vipes-pag/fohig.html</t>
+  </si>
+  <si>
+    <t>47 500 € (0.68 €/m²)</t>
+  </si>
+  <si>
+    <t>56960060026</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jelgava/adhdj.html</t>
+  </si>
+  <si>
+    <t>49 500 € (17.68 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/kalnciems/aidcf.html</t>
+  </si>
+  <si>
+    <t>30 000 € (30 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kraslava-and-reg/andrupenes-pag/blxnm.html</t>
+  </si>
+  <si>
+    <t>6042 002 0073</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kraslava-and-reg/kastulinas-pag/ifhom.html</t>
+  </si>
+  <si>
+    <t>60720010327</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kuldiga-and-reg/kuldiga/ghjnj.html</t>
+  </si>
+  <si>
+    <t>20 500 € (14.49 €/m²)</t>
+  </si>
+  <si>
+    <t>1415 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/rucavas-pag/imdli.html</t>
+  </si>
+  <si>
+    <t>78 000 € (3.90 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/liepaja/hojmo.html</t>
+  </si>
+  <si>
+    <t>750 000 € (246.63 €/m²)</t>
+  </si>
+  <si>
+    <t>3041 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/nicas-pag/alxhn.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/limbadzi-and-reg/vidrizu-pag/dekdg.html</t>
+  </si>
+  <si>
+    <t>66840050273</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ludza-and-reg/nuksu-pag/ipdmd.html</t>
+  </si>
+  <si>
+    <t>40 500 € (0.41 €/m²)</t>
+  </si>
+  <si>
+    <t>6880 001 0530</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ikskile/ahlkm.html</t>
+  </si>
+  <si>
+    <t>149 160 € (30 €/m²)</t>
+  </si>
+  <si>
+    <t>4972 m²</t>
+  </si>
+  <si>
+    <t>74940150534</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/birzgales-pag/bgxhol.html</t>
+  </si>
+  <si>
+    <t>74440010144</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ikskiles-l-t/abghi.html</t>
+  </si>
+  <si>
+    <t>110 000 € (1.83 €/m²)</t>
+  </si>
+  <si>
+    <t>7494 004 0435</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/kegums/diolc.html</t>
+  </si>
+  <si>
+    <t>120 000 € (12 €/m²)</t>
+  </si>
+  <si>
+    <t>74840060007</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/lielvarde/gbhpo.html</t>
+  </si>
+  <si>
+    <t>29 999 € (1 €/m²)</t>
+  </si>
+  <si>
+    <t>74330020061</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/preili-and-reg/turku-pag/bcgfxb.html</t>
+  </si>
+  <si>
+    <t>40 000 € (0.36 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/preili-and-reg/rusonas-pag/fxeod.html</t>
+  </si>
+  <si>
+    <t>24 000 € (0.40 €/m²)</t>
+  </si>
+  <si>
+    <t>76700010148</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/luznavas-pag/ahkhn.html</t>
+  </si>
+  <si>
+    <t>78680050063</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/tumes-pag/afdic.html</t>
+  </si>
+  <si>
+    <t>400 000 € (0.50 €/m²)</t>
+  </si>
+  <si>
+    <t>80 ha.</t>
+  </si>
+  <si>
+    <t>90840020190</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/jaunsatu-pag/coohj.html</t>
+  </si>
+  <si>
+    <t>55 000 € (0.79 €/m²)</t>
+  </si>
+  <si>
+    <t>90580010336</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/ventspils/bxkjkk.html</t>
+  </si>
+  <si>
+    <t>35 000 € (23 €/m²)</t>
   </si>
 </sst>
 </file>
@@ -21957,7 +22170,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -21996,702 +22209,542 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>7074</v>
+        <v>7168</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>7075</v>
+        <v>7169</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>243</v>
+        <v>8</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>4239</v>
+        <v>7170</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>7076</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3">
-        <v>45930.44305555556</v>
+        <v>45931.55902777778</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>7077</v>
+        <v>7171</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>7078</v>
+        <v>7172</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>419</v>
+        <v>324</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>2271</v>
+        <v>7173</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>10</v>
+        <v>7174</v>
       </c>
       <c r="F3" s="3">
-        <v>45930.34305555555</v>
+        <v>45931.55972222222</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>7079</v>
+        <v>7175</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>7080</v>
+        <v>7176</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>419</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>7081</v>
+        <v>7177</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>10</v>
+        <v>7178</v>
       </c>
       <c r="F4" s="3">
-        <v>45930.34305555555</v>
+        <v>45931.33333333333</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>7082</v>
+        <v>7179</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>7083</v>
+        <v>7180</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>772</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>5999</v>
+        <v>5559</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="3">
-        <v>45930.37569444445</v>
+        <v>45931.6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>7084</v>
+        <v>7181</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>7085</v>
+        <v>6668</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>772</v>
+        <v>1733</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>7086</v>
+        <v>32</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>10</v>
+        <v>7182</v>
       </c>
       <c r="F6" s="3">
-        <v>45930.37569444445</v>
+        <v>45931.36458333333</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>7087</v>
+        <v>7183</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>7088</v>
+        <v>7184</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>1218</v>
+        <v>1733</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>7089</v>
+        <v>407</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>10</v>
+        <v>7185</v>
       </c>
       <c r="F7" s="3">
-        <v>45930.57916666666</v>
+        <v>45930.77986111111</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>7090</v>
+        <v>7186</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>7091</v>
+        <v>7187</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1733</v>
+        <v>1929</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>474</v>
+        <v>1651</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>7092</v>
+        <v>10</v>
       </c>
       <c r="F8" s="3">
-        <v>45929.75277777778</v>
+        <v>45931.47361111111</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>7093</v>
+        <v>7188</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>7094</v>
+        <v>7189</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>1929</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>294</v>
+        <v>677</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>7095</v>
+        <v>10</v>
       </c>
       <c r="F9" s="3">
-        <v>45929.75277777778</v>
+        <v>45930.95277777778</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>7096</v>
+        <v>7190</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>7097</v>
+        <v>5600</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>2671</v>
+        <v>2488</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>7098</v>
+        <v>353</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>10</v>
+        <v>7191</v>
       </c>
       <c r="F10" s="3">
-        <v>45930.523611111115</v>
+        <v>45930.78680555556</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>7099</v>
+        <v>7192</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>2849</v>
+        <v>702</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>2846</v>
+        <v>2488</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>2271</v>
+        <v>171</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>10</v>
+        <v>7193</v>
       </c>
       <c r="F11" s="3">
-        <v>45930.53194444445</v>
+        <v>45930.78611111111</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>7100</v>
+        <v>7194</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>7101</v>
+        <v>7195</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>2846</v>
+        <v>2671</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>453</v>
+        <v>7196</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F12" s="3">
-        <v>45930.49791666667</v>
+        <v>45931.53194444445</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>7102</v>
+        <v>7197</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>7103</v>
+        <v>7198</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>2846</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>7104</v>
+        <v>171</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="3">
-        <v>45930.492361111115</v>
+        <v>45931.5375</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>7105</v>
+        <v>7199</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>3967</v>
+        <v>7200</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>2846</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>383</v>
+        <v>7201</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="3">
-        <v>45930.02847222222</v>
+        <v>45930.73402777778</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>7106</v>
+        <v>7202</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>7107</v>
+        <v>1467</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>2846</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>7108</v>
+        <v>201</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F15" s="3">
-        <v>45929.92291666666</v>
+        <v>45930.65486111111</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>7109</v>
+        <v>7203</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>7110</v>
+        <v>1519</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>3762</v>
+        <v>3398</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>171</v>
+        <v>1588</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>7111</v>
+        <v>7204</v>
       </c>
       <c r="F16" s="3">
-        <v>45929.788194444445</v>
+        <v>45931.51736111111</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>7112</v>
+        <v>7205</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>2828</v>
+        <v>7206</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>3868</v>
+        <v>3762</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>2829</v>
+        <v>325</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>7113</v>
+        <v>7207</v>
       </c>
       <c r="F17" s="3">
-        <v>45930.44583333333</v>
+        <v>45930.77916666667</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>7114</v>
+        <v>7208</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>7115</v>
+        <v>7209</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>4034</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>7116</v>
+        <v>7210</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>7117</v>
+        <v>7211</v>
       </c>
       <c r="F18" s="3">
-        <v>45930.427777777775</v>
+        <v>45931.58263888889</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>7118</v>
+        <v>7212</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>7119</v>
+        <v>460</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>4034</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>7120</v>
+        <v>171</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>7121</v>
+        <v>7213</v>
       </c>
       <c r="F19" s="3">
-        <v>45930.39375</v>
+        <v>45931.45833333333</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>7122</v>
+        <v>7214</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>7123</v>
+        <v>7215</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>4034</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>7124</v>
+        <v>383</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>10</v>
+        <v>7216</v>
       </c>
       <c r="F20" s="3">
-        <v>45929.94861111111</v>
+        <v>45931.45277777778</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>7125</v>
+        <v>7217</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>1692</v>
+        <v>7218</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>4671</v>
+        <v>4034</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>171</v>
+        <v>32</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>7126</v>
+        <v>7219</v>
       </c>
       <c r="F21" s="3">
-        <v>45930.464583333334</v>
+        <v>45930.836111111115</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>7127</v>
+        <v>7220</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>7128</v>
+        <v>7221</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>4671</v>
+        <v>4034</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>32</v>
+        <v>201</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>7129</v>
+        <v>7222</v>
       </c>
       <c r="F22" s="3">
-        <v>45929.711805555555</v>
+        <v>45930.74722222222</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>7130</v>
+        <v>7223</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>7131</v>
+        <v>7224</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>4770</v>
+        <v>4671</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>4348</v>
+        <v>683</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>7132</v>
+        <v>10</v>
       </c>
       <c r="F23" s="3">
-        <v>45930.46944444445</v>
+        <v>45931.419444444444</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>7133</v>
+        <v>7225</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>7134</v>
+        <v>7226</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>4770</v>
+        <v>4671</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>7135</v>
+        <v>383</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>7136</v>
+        <v>7227</v>
       </c>
       <c r="F24" s="3">
-        <v>45930.433333333334</v>
+        <v>45931.33263888889</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>7137</v>
+        <v>7228</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>7138</v>
+        <v>3865</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>4770</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>3702</v>
+        <v>201</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>10</v>
+        <v>7229</v>
       </c>
       <c r="F25" s="3">
-        <v>45929.77083333333</v>
+        <v>45930.77986111111</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>7139</v>
+        <v>7230</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>7140</v>
+        <v>7231</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>4770</v>
+        <v>5674</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>2191</v>
+        <v>7232</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>7141</v>
+        <v>7233</v>
       </c>
       <c r="F26" s="3">
-        <v>45929.665972222225</v>
+        <v>45931.51458333334</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>7142</v>
+        <v>7234</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>5131</v>
+        <v>7235</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>4770</v>
+        <v>5674</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>1430</v>
+        <v>407</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>5132</v>
+        <v>7236</v>
       </c>
       <c r="F27" s="3">
-        <v>45929.65555555555</v>
+        <v>45931.430555555555</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>7143</v>
+        <v>7237</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>2534</v>
+        <v>7238</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>5674</v>
+        <v>6439</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>171</v>
+        <v>4539</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>7144</v>
+        <v>10</v>
       </c>
       <c r="F28" s="3">
-        <v>45930.6125</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
-        <v>7145</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>1187</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>5674</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>7146</v>
-      </c>
-      <c r="F29" s="3">
-        <v>45930.611805555556</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>7147</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>7148</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>5674</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>7149</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>7150</v>
-      </c>
-      <c r="F30" s="3">
-        <v>45930.413194444445</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>7151</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>7152</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>5674</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>7153</v>
-      </c>
-      <c r="F31" s="3">
-        <v>45929.888194444444</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>7154</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>7155</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>6133</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>7156</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="3">
-        <v>45930.47777777778</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>7157</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>7158</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>6207</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>7159</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" s="3">
-        <v>45930.48055555555</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>7160</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>7161</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>6207</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>3097</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34" s="3">
-        <v>45930.47986111111</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>7162</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>7163</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>6207</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>7164</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" s="3">
-        <v>45930.476388888885</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
-        <v>7165</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>7166</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>2538</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>7167</v>
-      </c>
-      <c r="F36" s="3">
-        <v>45929.75208333333</v>
+        <v>45930.67638888889</v>
       </c>
     </row>
   </sheetData>
@@ -22723,14 +22776,6 @@
     <hyperlink ref="A26" r:id="rId25"/>
     <hyperlink ref="A27" r:id="rId26"/>
     <hyperlink ref="A28" r:id="rId27"/>
-    <hyperlink ref="A29" r:id="rId28"/>
-    <hyperlink ref="A30" r:id="rId29"/>
-    <hyperlink ref="A31" r:id="rId30"/>
-    <hyperlink ref="A32" r:id="rId31"/>
-    <hyperlink ref="A33" r:id="rId32"/>
-    <hyperlink ref="A34" r:id="rId33"/>
-    <hyperlink ref="A35" r:id="rId34"/>
-    <hyperlink ref="A36" r:id="rId35"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -22739,7 +22784,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2266"/>
+  <dimension ref="A1:F2301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -68075,6 +68120,706 @@
       </c>
       <c r="F2266" s="3">
         <v>45928.39444444445</v>
+      </c>
+    </row>
+    <row r="2267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2267" s="4" t="s">
+        <v>7074</v>
+      </c>
+      <c r="B2267" s="3" t="s">
+        <v>7075</v>
+      </c>
+      <c r="C2267" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D2267" s="3" t="s">
+        <v>4239</v>
+      </c>
+      <c r="E2267" s="3" t="s">
+        <v>7076</v>
+      </c>
+      <c r="F2267" s="3">
+        <v>45930.44305555556</v>
+      </c>
+    </row>
+    <row r="2268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2268" s="4" t="s">
+        <v>7077</v>
+      </c>
+      <c r="B2268" s="3" t="s">
+        <v>7078</v>
+      </c>
+      <c r="C2268" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2268" s="3" t="s">
+        <v>2271</v>
+      </c>
+      <c r="E2268" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2268" s="3">
+        <v>45930.34305555555</v>
+      </c>
+    </row>
+    <row r="2269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2269" s="4" t="s">
+        <v>7079</v>
+      </c>
+      <c r="B2269" s="3" t="s">
+        <v>7080</v>
+      </c>
+      <c r="C2269" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2269" s="3" t="s">
+        <v>7081</v>
+      </c>
+      <c r="E2269" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2269" s="3">
+        <v>45930.34305555555</v>
+      </c>
+    </row>
+    <row r="2270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2270" s="4" t="s">
+        <v>7082</v>
+      </c>
+      <c r="B2270" s="3" t="s">
+        <v>7083</v>
+      </c>
+      <c r="C2270" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2270" s="3" t="s">
+        <v>5999</v>
+      </c>
+      <c r="E2270" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2270" s="3">
+        <v>45930.37569444445</v>
+      </c>
+    </row>
+    <row r="2271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2271" s="4" t="s">
+        <v>7084</v>
+      </c>
+      <c r="B2271" s="3" t="s">
+        <v>7085</v>
+      </c>
+      <c r="C2271" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2271" s="3" t="s">
+        <v>7086</v>
+      </c>
+      <c r="E2271" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2271" s="3">
+        <v>45930.37569444445</v>
+      </c>
+    </row>
+    <row r="2272" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2272" s="4" t="s">
+        <v>7087</v>
+      </c>
+      <c r="B2272" s="3" t="s">
+        <v>7088</v>
+      </c>
+      <c r="C2272" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2272" s="3" t="s">
+        <v>7089</v>
+      </c>
+      <c r="E2272" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2272" s="3">
+        <v>45930.57916666666</v>
+      </c>
+    </row>
+    <row r="2273" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2273" s="4" t="s">
+        <v>7090</v>
+      </c>
+      <c r="B2273" s="3" t="s">
+        <v>7091</v>
+      </c>
+      <c r="C2273" s="3" t="s">
+        <v>1733</v>
+      </c>
+      <c r="D2273" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="E2273" s="3" t="s">
+        <v>7092</v>
+      </c>
+      <c r="F2273" s="3">
+        <v>45929.75277777778</v>
+      </c>
+    </row>
+    <row r="2274" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2274" s="4" t="s">
+        <v>7093</v>
+      </c>
+      <c r="B2274" s="3" t="s">
+        <v>7094</v>
+      </c>
+      <c r="C2274" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2274" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="E2274" s="3" t="s">
+        <v>7095</v>
+      </c>
+      <c r="F2274" s="3">
+        <v>45929.75277777778</v>
+      </c>
+    </row>
+    <row r="2275" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2275" s="4" t="s">
+        <v>7096</v>
+      </c>
+      <c r="B2275" s="3" t="s">
+        <v>7097</v>
+      </c>
+      <c r="C2275" s="3" t="s">
+        <v>2671</v>
+      </c>
+      <c r="D2275" s="3" t="s">
+        <v>7098</v>
+      </c>
+      <c r="E2275" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2275" s="3">
+        <v>45930.523611111115</v>
+      </c>
+    </row>
+    <row r="2276" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2276" s="4" t="s">
+        <v>7099</v>
+      </c>
+      <c r="B2276" s="3" t="s">
+        <v>2849</v>
+      </c>
+      <c r="C2276" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2276" s="3" t="s">
+        <v>2271</v>
+      </c>
+      <c r="E2276" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2276" s="3">
+        <v>45930.53194444445</v>
+      </c>
+    </row>
+    <row r="2277" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2277" s="4" t="s">
+        <v>7100</v>
+      </c>
+      <c r="B2277" s="3" t="s">
+        <v>7101</v>
+      </c>
+      <c r="C2277" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2277" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="E2277" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2277" s="3">
+        <v>45930.49791666667</v>
+      </c>
+    </row>
+    <row r="2278" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2278" s="4" t="s">
+        <v>7102</v>
+      </c>
+      <c r="B2278" s="3" t="s">
+        <v>7103</v>
+      </c>
+      <c r="C2278" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2278" s="3" t="s">
+        <v>7104</v>
+      </c>
+      <c r="E2278" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2278" s="3">
+        <v>45930.492361111115</v>
+      </c>
+    </row>
+    <row r="2279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2279" s="4" t="s">
+        <v>7105</v>
+      </c>
+      <c r="B2279" s="3" t="s">
+        <v>3967</v>
+      </c>
+      <c r="C2279" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2279" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E2279" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2279" s="3">
+        <v>45930.02847222222</v>
+      </c>
+    </row>
+    <row r="2280" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2280" s="4" t="s">
+        <v>7106</v>
+      </c>
+      <c r="B2280" s="3" t="s">
+        <v>7107</v>
+      </c>
+      <c r="C2280" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2280" s="3" t="s">
+        <v>7108</v>
+      </c>
+      <c r="E2280" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2280" s="3">
+        <v>45929.92291666666</v>
+      </c>
+    </row>
+    <row r="2281" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2281" s="4" t="s">
+        <v>7109</v>
+      </c>
+      <c r="B2281" s="3" t="s">
+        <v>7110</v>
+      </c>
+      <c r="C2281" s="3" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D2281" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2281" s="3" t="s">
+        <v>7111</v>
+      </c>
+      <c r="F2281" s="3">
+        <v>45929.788194444445</v>
+      </c>
+    </row>
+    <row r="2282" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2282" s="4" t="s">
+        <v>7112</v>
+      </c>
+      <c r="B2282" s="3" t="s">
+        <v>2828</v>
+      </c>
+      <c r="C2282" s="3" t="s">
+        <v>3868</v>
+      </c>
+      <c r="D2282" s="3" t="s">
+        <v>2829</v>
+      </c>
+      <c r="E2282" s="3" t="s">
+        <v>7113</v>
+      </c>
+      <c r="F2282" s="3">
+        <v>45930.44583333333</v>
+      </c>
+    </row>
+    <row r="2283" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2283" s="4" t="s">
+        <v>7114</v>
+      </c>
+      <c r="B2283" s="3" t="s">
+        <v>7115</v>
+      </c>
+      <c r="C2283" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2283" s="3" t="s">
+        <v>7116</v>
+      </c>
+      <c r="E2283" s="3" t="s">
+        <v>7117</v>
+      </c>
+      <c r="F2283" s="3">
+        <v>45930.427777777775</v>
+      </c>
+    </row>
+    <row r="2284" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2284" s="4" t="s">
+        <v>7118</v>
+      </c>
+      <c r="B2284" s="3" t="s">
+        <v>7119</v>
+      </c>
+      <c r="C2284" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2284" s="3" t="s">
+        <v>7120</v>
+      </c>
+      <c r="E2284" s="3" t="s">
+        <v>7121</v>
+      </c>
+      <c r="F2284" s="3">
+        <v>45930.39375</v>
+      </c>
+    </row>
+    <row r="2285" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2285" s="4" t="s">
+        <v>7122</v>
+      </c>
+      <c r="B2285" s="3" t="s">
+        <v>7123</v>
+      </c>
+      <c r="C2285" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2285" s="3" t="s">
+        <v>7124</v>
+      </c>
+      <c r="E2285" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2285" s="3">
+        <v>45929.94861111111</v>
+      </c>
+    </row>
+    <row r="2286" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2286" s="4" t="s">
+        <v>7125</v>
+      </c>
+      <c r="B2286" s="3" t="s">
+        <v>1692</v>
+      </c>
+      <c r="C2286" s="3" t="s">
+        <v>4671</v>
+      </c>
+      <c r="D2286" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2286" s="3" t="s">
+        <v>7126</v>
+      </c>
+      <c r="F2286" s="3">
+        <v>45930.464583333334</v>
+      </c>
+    </row>
+    <row r="2287" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2287" s="4" t="s">
+        <v>7127</v>
+      </c>
+      <c r="B2287" s="3" t="s">
+        <v>7128</v>
+      </c>
+      <c r="C2287" s="3" t="s">
+        <v>4671</v>
+      </c>
+      <c r="D2287" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2287" s="3" t="s">
+        <v>7129</v>
+      </c>
+      <c r="F2287" s="3">
+        <v>45929.711805555555</v>
+      </c>
+    </row>
+    <row r="2288" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2288" s="4" t="s">
+        <v>7130</v>
+      </c>
+      <c r="B2288" s="3" t="s">
+        <v>7131</v>
+      </c>
+      <c r="C2288" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2288" s="3" t="s">
+        <v>4348</v>
+      </c>
+      <c r="E2288" s="3" t="s">
+        <v>7132</v>
+      </c>
+      <c r="F2288" s="3">
+        <v>45930.46944444445</v>
+      </c>
+    </row>
+    <row r="2289" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2289" s="4" t="s">
+        <v>7133</v>
+      </c>
+      <c r="B2289" s="3" t="s">
+        <v>7134</v>
+      </c>
+      <c r="C2289" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2289" s="3" t="s">
+        <v>7135</v>
+      </c>
+      <c r="E2289" s="3" t="s">
+        <v>7136</v>
+      </c>
+      <c r="F2289" s="3">
+        <v>45930.433333333334</v>
+      </c>
+    </row>
+    <row r="2290" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2290" s="4" t="s">
+        <v>7137</v>
+      </c>
+      <c r="B2290" s="3" t="s">
+        <v>7138</v>
+      </c>
+      <c r="C2290" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2290" s="3" t="s">
+        <v>3702</v>
+      </c>
+      <c r="E2290" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2290" s="3">
+        <v>45929.77083333333</v>
+      </c>
+    </row>
+    <row r="2291" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2291" s="4" t="s">
+        <v>7139</v>
+      </c>
+      <c r="B2291" s="3" t="s">
+        <v>7140</v>
+      </c>
+      <c r="C2291" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2291" s="3" t="s">
+        <v>2191</v>
+      </c>
+      <c r="E2291" s="3" t="s">
+        <v>7141</v>
+      </c>
+      <c r="F2291" s="3">
+        <v>45929.665972222225</v>
+      </c>
+    </row>
+    <row r="2292" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2292" s="4" t="s">
+        <v>7142</v>
+      </c>
+      <c r="B2292" s="3" t="s">
+        <v>5131</v>
+      </c>
+      <c r="C2292" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2292" s="3" t="s">
+        <v>1430</v>
+      </c>
+      <c r="E2292" s="3" t="s">
+        <v>5132</v>
+      </c>
+      <c r="F2292" s="3">
+        <v>45929.65555555555</v>
+      </c>
+    </row>
+    <row r="2293" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2293" s="4" t="s">
+        <v>7143</v>
+      </c>
+      <c r="B2293" s="3" t="s">
+        <v>2534</v>
+      </c>
+      <c r="C2293" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2293" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2293" s="3" t="s">
+        <v>7144</v>
+      </c>
+      <c r="F2293" s="3">
+        <v>45930.6125</v>
+      </c>
+    </row>
+    <row r="2294" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2294" s="4" t="s">
+        <v>7145</v>
+      </c>
+      <c r="B2294" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C2294" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2294" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2294" s="3" t="s">
+        <v>7146</v>
+      </c>
+      <c r="F2294" s="3">
+        <v>45930.611805555556</v>
+      </c>
+    </row>
+    <row r="2295" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2295" s="4" t="s">
+        <v>7147</v>
+      </c>
+      <c r="B2295" s="3" t="s">
+        <v>7148</v>
+      </c>
+      <c r="C2295" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2295" s="3" t="s">
+        <v>7149</v>
+      </c>
+      <c r="E2295" s="3" t="s">
+        <v>7150</v>
+      </c>
+      <c r="F2295" s="3">
+        <v>45930.413194444445</v>
+      </c>
+    </row>
+    <row r="2296" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2296" s="4" t="s">
+        <v>7151</v>
+      </c>
+      <c r="B2296" s="3" t="s">
+        <v>7152</v>
+      </c>
+      <c r="C2296" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2296" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E2296" s="3" t="s">
+        <v>7153</v>
+      </c>
+      <c r="F2296" s="3">
+        <v>45929.888194444444</v>
+      </c>
+    </row>
+    <row r="2297" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2297" s="4" t="s">
+        <v>7154</v>
+      </c>
+      <c r="B2297" s="3" t="s">
+        <v>7155</v>
+      </c>
+      <c r="C2297" s="3" t="s">
+        <v>6133</v>
+      </c>
+      <c r="D2297" s="3" t="s">
+        <v>7156</v>
+      </c>
+      <c r="E2297" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2297" s="3">
+        <v>45930.47777777778</v>
+      </c>
+    </row>
+    <row r="2298" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2298" s="4" t="s">
+        <v>7157</v>
+      </c>
+      <c r="B2298" s="3" t="s">
+        <v>7158</v>
+      </c>
+      <c r="C2298" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2298" s="3" t="s">
+        <v>7159</v>
+      </c>
+      <c r="E2298" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2298" s="3">
+        <v>45930.48055555555</v>
+      </c>
+    </row>
+    <row r="2299" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2299" s="4" t="s">
+        <v>7160</v>
+      </c>
+      <c r="B2299" s="3" t="s">
+        <v>7161</v>
+      </c>
+      <c r="C2299" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2299" s="3" t="s">
+        <v>3097</v>
+      </c>
+      <c r="E2299" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2299" s="3">
+        <v>45930.47986111111</v>
+      </c>
+    </row>
+    <row r="2300" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2300" s="4" t="s">
+        <v>7162</v>
+      </c>
+      <c r="B2300" s="3" t="s">
+        <v>7163</v>
+      </c>
+      <c r="C2300" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2300" s="3" t="s">
+        <v>7164</v>
+      </c>
+      <c r="E2300" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2300" s="3">
+        <v>45930.476388888885</v>
+      </c>
+    </row>
+    <row r="2301" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2301" s="4" t="s">
+        <v>7165</v>
+      </c>
+      <c r="B2301" s="3" t="s">
+        <v>7166</v>
+      </c>
+      <c r="C2301" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2301" s="3" t="s">
+        <v>2538</v>
+      </c>
+      <c r="E2301" s="3" t="s">
+        <v>7167</v>
+      </c>
+      <c r="F2301" s="3">
+        <v>45929.75208333333</v>
       </c>
     </row>
   </sheetData>
@@ -70344,6 +71089,41 @@
     <hyperlink ref="A2264" r:id="rId2263"/>
     <hyperlink ref="A2265" r:id="rId2264"/>
     <hyperlink ref="A2266" r:id="rId2265"/>
+    <hyperlink ref="A2267" r:id="rId2266"/>
+    <hyperlink ref="A2268" r:id="rId2267"/>
+    <hyperlink ref="A2269" r:id="rId2268"/>
+    <hyperlink ref="A2270" r:id="rId2269"/>
+    <hyperlink ref="A2271" r:id="rId2270"/>
+    <hyperlink ref="A2272" r:id="rId2271"/>
+    <hyperlink ref="A2273" r:id="rId2272"/>
+    <hyperlink ref="A2274" r:id="rId2273"/>
+    <hyperlink ref="A2275" r:id="rId2274"/>
+    <hyperlink ref="A2276" r:id="rId2275"/>
+    <hyperlink ref="A2277" r:id="rId2276"/>
+    <hyperlink ref="A2278" r:id="rId2277"/>
+    <hyperlink ref="A2279" r:id="rId2278"/>
+    <hyperlink ref="A2280" r:id="rId2279"/>
+    <hyperlink ref="A2281" r:id="rId2280"/>
+    <hyperlink ref="A2282" r:id="rId2281"/>
+    <hyperlink ref="A2283" r:id="rId2282"/>
+    <hyperlink ref="A2284" r:id="rId2283"/>
+    <hyperlink ref="A2285" r:id="rId2284"/>
+    <hyperlink ref="A2286" r:id="rId2285"/>
+    <hyperlink ref="A2287" r:id="rId2286"/>
+    <hyperlink ref="A2288" r:id="rId2287"/>
+    <hyperlink ref="A2289" r:id="rId2288"/>
+    <hyperlink ref="A2290" r:id="rId2289"/>
+    <hyperlink ref="A2291" r:id="rId2290"/>
+    <hyperlink ref="A2292" r:id="rId2291"/>
+    <hyperlink ref="A2293" r:id="rId2292"/>
+    <hyperlink ref="A2294" r:id="rId2293"/>
+    <hyperlink ref="A2295" r:id="rId2294"/>
+    <hyperlink ref="A2296" r:id="rId2295"/>
+    <hyperlink ref="A2297" r:id="rId2296"/>
+    <hyperlink ref="A2298" r:id="rId2297"/>
+    <hyperlink ref="A2299" r:id="rId2298"/>
+    <hyperlink ref="A2300" r:id="rId2299"/>
+    <hyperlink ref="A2301" r:id="rId2300"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Update lands data - 2025-10-02 12:19
</commit_message>
<xml_diff>
--- a/lands-scraped.xlsx
+++ b/lands-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11647" uniqueCount="7239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11777" uniqueCount="7318">
   <si>
     <t>link</t>
   </si>
@@ -21735,6 +21735,243 @@
   </si>
   <si>
     <t>35 000 € (23 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/dzerbenes-pag/hxedi.html</t>
+  </si>
+  <si>
+    <t>17 500 € (5.15 €/m²)</t>
+  </si>
+  <si>
+    <t>0.34 ha.</t>
+  </si>
+  <si>
+    <t>42500070401</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/daugavpils/cxfoi.html</t>
+  </si>
+  <si>
+    <t>23 000 € (21.32 €/m²)</t>
+  </si>
+  <si>
+    <t>1079 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/kalkunes-pag/dmlxf.html</t>
+  </si>
+  <si>
+    <t>34 000 € (0.37 €/m²)</t>
+  </si>
+  <si>
+    <t>9.31 ha.</t>
+  </si>
+  <si>
+    <t>44600010092</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/daugavpils/hcipl.html</t>
+  </si>
+  <si>
+    <t>44600020131, 33, 34</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/daugavpils/gihxo.html</t>
+  </si>
+  <si>
+    <t>3 000 € (2.03 €/m²)</t>
+  </si>
+  <si>
+    <t>1476 m²</t>
+  </si>
+  <si>
+    <t>05000040236</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/demenes-pag/efplp.html</t>
+  </si>
+  <si>
+    <t>35 600 € (0.36 €/m²)</t>
+  </si>
+  <si>
+    <t>44500010195</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jelgava/bdgig.html</t>
+  </si>
+  <si>
+    <t>30 000 € (17.22 €/m²)</t>
+  </si>
+  <si>
+    <t>1742 m²</t>
+  </si>
+  <si>
+    <t>09000030356</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/kalnciems/fhhlg.html</t>
+  </si>
+  <si>
+    <t>50 000 € (0.17 €/m²)</t>
+  </si>
+  <si>
+    <t>295600 m²</t>
+  </si>
+  <si>
+    <t>54310020501</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jelgava/bdnjgl.html</t>
+  </si>
+  <si>
+    <t>20 000 € (15.82 €/m²)</t>
+  </si>
+  <si>
+    <t>1264 m²</t>
+  </si>
+  <si>
+    <t>09000300401</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jelgava/agkxi.html</t>
+  </si>
+  <si>
+    <t>25 725 € (25 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jelgava/adijx.html</t>
+  </si>
+  <si>
+    <t>24 000 € (12.07 €/m²)</t>
+  </si>
+  <si>
+    <t>1989 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jaunsvirlaukas-pag/afelc.html</t>
+  </si>
+  <si>
+    <t>42 000 € (0.70 €/m²)</t>
+  </si>
+  <si>
+    <t>54920010017</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jelgava/aapdh.html</t>
+  </si>
+  <si>
+    <t>299 000 € (8.94 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kraslava-and-reg/kepovas-pag/hlebl.html</t>
+  </si>
+  <si>
+    <t>60800010005</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/liepaja/bxiiml.html</t>
+  </si>
+  <si>
+    <t>40 000 € (0.85 €/m²)</t>
+  </si>
+  <si>
+    <t>17000150061</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/limbadzi-and-reg/skultes-pag/bkkic.html</t>
+  </si>
+  <si>
+    <t>22 000 € (5.50 €/m²)</t>
+  </si>
+  <si>
+    <t>66760160003</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/limbadzi-and-reg/skultes-pag/hinng.html</t>
+  </si>
+  <si>
+    <t>21 900 € (18.23 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/limbadzi-and-reg/limbazi/bxnexi.html</t>
+  </si>
+  <si>
+    <t>15 580 € (12.98 €/m²)</t>
+  </si>
+  <si>
+    <t>66010020139</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ogre/bnfof.html</t>
+  </si>
+  <si>
+    <t>22 000 € (11 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/pusas-pag/jlepk.html</t>
+  </si>
+  <si>
+    <t>39 000 € (0.17 €/m²)</t>
+  </si>
+  <si>
+    <t>78800050079</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/rojas-pag/dxgjx.html</t>
+  </si>
+  <si>
+    <t>59 000 € (41.76 €/m²)</t>
+  </si>
+  <si>
+    <t>1413 m²</t>
+  </si>
+  <si>
+    <t>88820081304</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/rojas-pag/icnob.html</t>
+  </si>
+  <si>
+    <t>28 000 € (5.71 €/m²)</t>
+  </si>
+  <si>
+    <t>4900 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/tumes-pag/efgli.html</t>
+  </si>
+  <si>
+    <t>50 000 € (0.55 €/m²)</t>
+  </si>
+  <si>
+    <t>9.10 ha.</t>
+  </si>
+  <si>
+    <t>90840040188</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/kandava/kdiog.html</t>
+  </si>
+  <si>
+    <t>60 000 € (1.76 €/m²)</t>
+  </si>
+  <si>
+    <t>3.40 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valka-and-reg/valka/dpkmg.html</t>
+  </si>
+  <si>
+    <t>9 000 € (1.91 €/m²)</t>
+  </si>
+  <si>
+    <t>0.47 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/other/djxci.html</t>
+  </si>
+  <si>
+    <t>3 000 € (3 €/m²)</t>
   </si>
 </sst>
 </file>
@@ -22170,7 +22407,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -22209,542 +22446,522 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>7168</v>
+        <v>7239</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>7169</v>
+        <v>7240</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>8</v>
+        <v>772</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>7170</v>
+        <v>7241</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>10</v>
+        <v>7242</v>
       </c>
       <c r="F2" s="3">
-        <v>45931.55902777778</v>
+        <v>45931.80138888889</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>7171</v>
+        <v>7243</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>7172</v>
+        <v>7244</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>324</v>
+        <v>1218</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>7173</v>
+        <v>7245</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>7174</v>
+        <v>1295</v>
       </c>
       <c r="F3" s="3">
-        <v>45931.55972222222</v>
+        <v>45932.45694444445</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>7175</v>
+        <v>7246</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>7176</v>
+        <v>7247</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>419</v>
+        <v>1218</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>7177</v>
+        <v>7248</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>7178</v>
+        <v>7249</v>
       </c>
       <c r="F4" s="3">
-        <v>45931.33333333333</v>
+        <v>45932.419444444444</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>7179</v>
+        <v>7250</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>7180</v>
+        <v>2615</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>772</v>
+        <v>1218</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>5559</v>
+        <v>325</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>10</v>
+        <v>7251</v>
       </c>
       <c r="F5" s="3">
-        <v>45931.6</v>
+        <v>45931.902083333334</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>7181</v>
+        <v>7252</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>6668</v>
+        <v>7253</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1733</v>
+        <v>1218</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>32</v>
+        <v>7254</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>7182</v>
+        <v>7255</v>
       </c>
       <c r="F6" s="3">
-        <v>45931.36458333333</v>
+        <v>45931.902083333334</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>7183</v>
+        <v>7256</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>7184</v>
+        <v>7257</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>1733</v>
+        <v>1218</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>407</v>
+        <v>325</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>7185</v>
+        <v>7258</v>
       </c>
       <c r="F7" s="3">
-        <v>45930.77986111111</v>
+        <v>45931.67083333334</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>7186</v>
+        <v>7259</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>7187</v>
+        <v>7260</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>1929</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>1651</v>
+        <v>7261</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>10</v>
+        <v>7262</v>
       </c>
       <c r="F8" s="3">
-        <v>45931.47361111111</v>
+        <v>45932.43958333333</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>7188</v>
+        <v>7263</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>7189</v>
+        <v>7264</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>1929</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>677</v>
+        <v>7265</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>10</v>
+        <v>7266</v>
       </c>
       <c r="F9" s="3">
-        <v>45930.95277777778</v>
+        <v>45932.40486111111</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>7190</v>
+        <v>7267</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>5600</v>
+        <v>7268</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>2488</v>
+        <v>1929</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>353</v>
+        <v>7269</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>7191</v>
+        <v>7270</v>
       </c>
       <c r="F10" s="3">
-        <v>45930.78680555556</v>
+        <v>45932.27013888889</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>7192</v>
+        <v>7271</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>702</v>
+        <v>7272</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>2488</v>
+        <v>1929</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>171</v>
+        <v>5695</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>7193</v>
+        <v>10</v>
       </c>
       <c r="F11" s="3">
-        <v>45930.78611111111</v>
+        <v>45932.26666666666</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>7194</v>
+        <v>7273</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>7195</v>
+        <v>7274</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>2671</v>
+        <v>1929</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>7196</v>
+        <v>7275</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F12" s="3">
-        <v>45931.53194444445</v>
+        <v>45932.02291666667</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>7197</v>
+        <v>7276</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>7198</v>
+        <v>7277</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>2846</v>
+        <v>1929</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>171</v>
+        <v>383</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>10</v>
+        <v>7278</v>
       </c>
       <c r="F13" s="3">
-        <v>45931.5375</v>
+        <v>45931.70208333334</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>7199</v>
+        <v>7279</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>7200</v>
+        <v>7280</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>2846</v>
+        <v>1929</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>7201</v>
+        <v>2179</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>10</v>
+        <v>2180</v>
       </c>
       <c r="F14" s="3">
-        <v>45930.73402777778</v>
+        <v>45931.69097222222</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>7202</v>
+        <v>7281</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>1467</v>
+        <v>2609</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>2846</v>
+        <v>2488</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>201</v>
+        <v>407</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>10</v>
+        <v>7282</v>
       </c>
       <c r="F15" s="3">
-        <v>45930.65486111111</v>
+        <v>45932.47083333333</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>7203</v>
+        <v>7283</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>1519</v>
+        <v>7284</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>3398</v>
+        <v>2846</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>1588</v>
+        <v>365</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>7204</v>
+        <v>7285</v>
       </c>
       <c r="F16" s="3">
-        <v>45931.51736111111</v>
+        <v>45932.601388888885</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>7205</v>
+        <v>7286</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>7206</v>
+        <v>7287</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>3762</v>
+        <v>3398</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>325</v>
+        <v>149</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>7207</v>
+        <v>7288</v>
       </c>
       <c r="F17" s="3">
-        <v>45930.77916666667</v>
+        <v>45932.52986111111</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>7208</v>
+        <v>7289</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>7209</v>
+        <v>7290</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>4034</v>
+        <v>3398</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>7210</v>
+        <v>290</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>7211</v>
+        <v>10</v>
       </c>
       <c r="F18" s="3">
-        <v>45931.58263888889</v>
+        <v>45932.46597222222</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>7212</v>
+        <v>7291</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>460</v>
+        <v>7292</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>4034</v>
+        <v>3398</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>171</v>
+        <v>111</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>7213</v>
+        <v>7293</v>
       </c>
       <c r="F19" s="3">
-        <v>45931.45833333333</v>
+        <v>45931.90416666667</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>7214</v>
+        <v>7294</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>7215</v>
+        <v>7295</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>4034</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>383</v>
+        <v>317</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>7216</v>
+        <v>4511</v>
       </c>
       <c r="F20" s="3">
-        <v>45931.45277777778</v>
+        <v>45932.45</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>7217</v>
+        <v>7296</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>7218</v>
+        <v>7297</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>4034</v>
+        <v>4770</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>32</v>
+        <v>809</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>7219</v>
+        <v>7298</v>
       </c>
       <c r="F21" s="3">
-        <v>45930.836111111115</v>
+        <v>45931.87986111111</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>7220</v>
+        <v>7299</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>7221</v>
+        <v>7300</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>4034</v>
+        <v>5266</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>201</v>
+        <v>7301</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>7222</v>
+        <v>7302</v>
       </c>
       <c r="F22" s="3">
-        <v>45930.74722222222</v>
+        <v>45932.44305555556</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>7223</v>
+        <v>7303</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>7224</v>
+        <v>7304</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>4671</v>
+        <v>5266</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>683</v>
+        <v>7305</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F23" s="3">
-        <v>45931.419444444444</v>
+        <v>45931.660416666666</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>7225</v>
+        <v>7306</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>7226</v>
+        <v>7307</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>4671</v>
+        <v>5674</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>383</v>
+        <v>7308</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>7227</v>
+        <v>7309</v>
       </c>
       <c r="F24" s="3">
-        <v>45931.33263888889</v>
+        <v>45932.62222222222</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>7228</v>
+        <v>7310</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>3865</v>
+        <v>7311</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>4770</v>
+        <v>5674</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>201</v>
+        <v>7312</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>7229</v>
+        <v>10</v>
       </c>
       <c r="F25" s="3">
-        <v>45930.77986111111</v>
+        <v>45932.60208333333</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>7230</v>
+        <v>7313</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>7231</v>
+        <v>7314</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>5674</v>
+        <v>6133</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>7232</v>
+        <v>7315</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>7233</v>
+        <v>10</v>
       </c>
       <c r="F26" s="3">
-        <v>45931.51458333334</v>
+        <v>45931.75</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>7234</v>
+        <v>7316</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>7235</v>
+        <v>7317</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>5674</v>
+        <v>1194</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>407</v>
+        <v>71</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>7236</v>
+        <v>10</v>
       </c>
       <c r="F27" s="3">
-        <v>45931.430555555555</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>7237</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>7238</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>4539</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" s="3">
-        <v>45930.67638888889</v>
+        <v>45931.69236111111</v>
       </c>
     </row>
   </sheetData>
@@ -22775,7 +22992,6 @@
     <hyperlink ref="A25" r:id="rId24"/>
     <hyperlink ref="A26" r:id="rId25"/>
     <hyperlink ref="A27" r:id="rId26"/>
-    <hyperlink ref="A28" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -22784,7 +23000,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2301"/>
+  <dimension ref="A1:F2328"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -68820,6 +69036,546 @@
       </c>
       <c r="F2301" s="3">
         <v>45929.75208333333</v>
+      </c>
+    </row>
+    <row r="2302" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2302" s="4" t="s">
+        <v>7168</v>
+      </c>
+      <c r="B2302" s="3" t="s">
+        <v>7169</v>
+      </c>
+      <c r="C2302" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2302" s="3" t="s">
+        <v>7170</v>
+      </c>
+      <c r="E2302" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2302" s="3">
+        <v>45931.55902777778</v>
+      </c>
+    </row>
+    <row r="2303" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2303" s="4" t="s">
+        <v>7171</v>
+      </c>
+      <c r="B2303" s="3" t="s">
+        <v>7172</v>
+      </c>
+      <c r="C2303" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="D2303" s="3" t="s">
+        <v>7173</v>
+      </c>
+      <c r="E2303" s="3" t="s">
+        <v>7174</v>
+      </c>
+      <c r="F2303" s="3">
+        <v>45931.55972222222</v>
+      </c>
+    </row>
+    <row r="2304" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2304" s="4" t="s">
+        <v>7175</v>
+      </c>
+      <c r="B2304" s="3" t="s">
+        <v>7176</v>
+      </c>
+      <c r="C2304" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2304" s="3" t="s">
+        <v>7177</v>
+      </c>
+      <c r="E2304" s="3" t="s">
+        <v>7178</v>
+      </c>
+      <c r="F2304" s="3">
+        <v>45931.33333333333</v>
+      </c>
+    </row>
+    <row r="2305" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2305" s="4" t="s">
+        <v>7179</v>
+      </c>
+      <c r="B2305" s="3" t="s">
+        <v>7180</v>
+      </c>
+      <c r="C2305" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2305" s="3" t="s">
+        <v>5559</v>
+      </c>
+      <c r="E2305" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2305" s="3">
+        <v>45931.6</v>
+      </c>
+    </row>
+    <row r="2306" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2306" s="4" t="s">
+        <v>7181</v>
+      </c>
+      <c r="B2306" s="3" t="s">
+        <v>6668</v>
+      </c>
+      <c r="C2306" s="3" t="s">
+        <v>1733</v>
+      </c>
+      <c r="D2306" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2306" s="3" t="s">
+        <v>7182</v>
+      </c>
+      <c r="F2306" s="3">
+        <v>45931.36458333333</v>
+      </c>
+    </row>
+    <row r="2307" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2307" s="4" t="s">
+        <v>7183</v>
+      </c>
+      <c r="B2307" s="3" t="s">
+        <v>7184</v>
+      </c>
+      <c r="C2307" s="3" t="s">
+        <v>1733</v>
+      </c>
+      <c r="D2307" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="E2307" s="3" t="s">
+        <v>7185</v>
+      </c>
+      <c r="F2307" s="3">
+        <v>45930.77986111111</v>
+      </c>
+    </row>
+    <row r="2308" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2308" s="4" t="s">
+        <v>7186</v>
+      </c>
+      <c r="B2308" s="3" t="s">
+        <v>7187</v>
+      </c>
+      <c r="C2308" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2308" s="3" t="s">
+        <v>1651</v>
+      </c>
+      <c r="E2308" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2308" s="3">
+        <v>45931.47361111111</v>
+      </c>
+    </row>
+    <row r="2309" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2309" s="4" t="s">
+        <v>7188</v>
+      </c>
+      <c r="B2309" s="3" t="s">
+        <v>7189</v>
+      </c>
+      <c r="C2309" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2309" s="3" t="s">
+        <v>677</v>
+      </c>
+      <c r="E2309" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2309" s="3">
+        <v>45930.95277777778</v>
+      </c>
+    </row>
+    <row r="2310" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2310" s="4" t="s">
+        <v>7190</v>
+      </c>
+      <c r="B2310" s="3" t="s">
+        <v>5600</v>
+      </c>
+      <c r="C2310" s="3" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D2310" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="E2310" s="3" t="s">
+        <v>7191</v>
+      </c>
+      <c r="F2310" s="3">
+        <v>45930.78680555556</v>
+      </c>
+    </row>
+    <row r="2311" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2311" s="4" t="s">
+        <v>7192</v>
+      </c>
+      <c r="B2311" s="3" t="s">
+        <v>702</v>
+      </c>
+      <c r="C2311" s="3" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D2311" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2311" s="3" t="s">
+        <v>7193</v>
+      </c>
+      <c r="F2311" s="3">
+        <v>45930.78611111111</v>
+      </c>
+    </row>
+    <row r="2312" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2312" s="4" t="s">
+        <v>7194</v>
+      </c>
+      <c r="B2312" s="3" t="s">
+        <v>7195</v>
+      </c>
+      <c r="C2312" s="3" t="s">
+        <v>2671</v>
+      </c>
+      <c r="D2312" s="3" t="s">
+        <v>7196</v>
+      </c>
+      <c r="E2312" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2312" s="3">
+        <v>45931.53194444445</v>
+      </c>
+    </row>
+    <row r="2313" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2313" s="4" t="s">
+        <v>7197</v>
+      </c>
+      <c r="B2313" s="3" t="s">
+        <v>7198</v>
+      </c>
+      <c r="C2313" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2313" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2313" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2313" s="3">
+        <v>45931.5375</v>
+      </c>
+    </row>
+    <row r="2314" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2314" s="4" t="s">
+        <v>7199</v>
+      </c>
+      <c r="B2314" s="3" t="s">
+        <v>7200</v>
+      </c>
+      <c r="C2314" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2314" s="3" t="s">
+        <v>7201</v>
+      </c>
+      <c r="E2314" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2314" s="3">
+        <v>45930.73402777778</v>
+      </c>
+    </row>
+    <row r="2315" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2315" s="4" t="s">
+        <v>7202</v>
+      </c>
+      <c r="B2315" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="C2315" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2315" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2315" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2315" s="3">
+        <v>45930.65486111111</v>
+      </c>
+    </row>
+    <row r="2316" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2316" s="4" t="s">
+        <v>7203</v>
+      </c>
+      <c r="B2316" s="3" t="s">
+        <v>1519</v>
+      </c>
+      <c r="C2316" s="3" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D2316" s="3" t="s">
+        <v>1588</v>
+      </c>
+      <c r="E2316" s="3" t="s">
+        <v>7204</v>
+      </c>
+      <c r="F2316" s="3">
+        <v>45931.51736111111</v>
+      </c>
+    </row>
+    <row r="2317" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2317" s="4" t="s">
+        <v>7205</v>
+      </c>
+      <c r="B2317" s="3" t="s">
+        <v>7206</v>
+      </c>
+      <c r="C2317" s="3" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D2317" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2317" s="3" t="s">
+        <v>7207</v>
+      </c>
+      <c r="F2317" s="3">
+        <v>45930.77916666667</v>
+      </c>
+    </row>
+    <row r="2318" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2318" s="4" t="s">
+        <v>7208</v>
+      </c>
+      <c r="B2318" s="3" t="s">
+        <v>7209</v>
+      </c>
+      <c r="C2318" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2318" s="3" t="s">
+        <v>7210</v>
+      </c>
+      <c r="E2318" s="3" t="s">
+        <v>7211</v>
+      </c>
+      <c r="F2318" s="3">
+        <v>45931.58263888889</v>
+      </c>
+    </row>
+    <row r="2319" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2319" s="4" t="s">
+        <v>7212</v>
+      </c>
+      <c r="B2319" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="C2319" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2319" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2319" s="3" t="s">
+        <v>7213</v>
+      </c>
+      <c r="F2319" s="3">
+        <v>45931.45833333333</v>
+      </c>
+    </row>
+    <row r="2320" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2320" s="4" t="s">
+        <v>7214</v>
+      </c>
+      <c r="B2320" s="3" t="s">
+        <v>7215</v>
+      </c>
+      <c r="C2320" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2320" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E2320" s="3" t="s">
+        <v>7216</v>
+      </c>
+      <c r="F2320" s="3">
+        <v>45931.45277777778</v>
+      </c>
+    </row>
+    <row r="2321" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2321" s="4" t="s">
+        <v>7217</v>
+      </c>
+      <c r="B2321" s="3" t="s">
+        <v>7218</v>
+      </c>
+      <c r="C2321" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2321" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2321" s="3" t="s">
+        <v>7219</v>
+      </c>
+      <c r="F2321" s="3">
+        <v>45930.836111111115</v>
+      </c>
+    </row>
+    <row r="2322" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2322" s="4" t="s">
+        <v>7220</v>
+      </c>
+      <c r="B2322" s="3" t="s">
+        <v>7221</v>
+      </c>
+      <c r="C2322" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2322" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2322" s="3" t="s">
+        <v>7222</v>
+      </c>
+      <c r="F2322" s="3">
+        <v>45930.74722222222</v>
+      </c>
+    </row>
+    <row r="2323" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2323" s="4" t="s">
+        <v>7223</v>
+      </c>
+      <c r="B2323" s="3" t="s">
+        <v>7224</v>
+      </c>
+      <c r="C2323" s="3" t="s">
+        <v>4671</v>
+      </c>
+      <c r="D2323" s="3" t="s">
+        <v>683</v>
+      </c>
+      <c r="E2323" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2323" s="3">
+        <v>45931.419444444444</v>
+      </c>
+    </row>
+    <row r="2324" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2324" s="4" t="s">
+        <v>7225</v>
+      </c>
+      <c r="B2324" s="3" t="s">
+        <v>7226</v>
+      </c>
+      <c r="C2324" s="3" t="s">
+        <v>4671</v>
+      </c>
+      <c r="D2324" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E2324" s="3" t="s">
+        <v>7227</v>
+      </c>
+      <c r="F2324" s="3">
+        <v>45931.33263888889</v>
+      </c>
+    </row>
+    <row r="2325" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2325" s="4" t="s">
+        <v>7228</v>
+      </c>
+      <c r="B2325" s="3" t="s">
+        <v>3865</v>
+      </c>
+      <c r="C2325" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2325" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2325" s="3" t="s">
+        <v>7229</v>
+      </c>
+      <c r="F2325" s="3">
+        <v>45930.77986111111</v>
+      </c>
+    </row>
+    <row r="2326" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2326" s="4" t="s">
+        <v>7230</v>
+      </c>
+      <c r="B2326" s="3" t="s">
+        <v>7231</v>
+      </c>
+      <c r="C2326" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2326" s="3" t="s">
+        <v>7232</v>
+      </c>
+      <c r="E2326" s="3" t="s">
+        <v>7233</v>
+      </c>
+      <c r="F2326" s="3">
+        <v>45931.51458333334</v>
+      </c>
+    </row>
+    <row r="2327" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2327" s="4" t="s">
+        <v>7234</v>
+      </c>
+      <c r="B2327" s="3" t="s">
+        <v>7235</v>
+      </c>
+      <c r="C2327" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2327" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="E2327" s="3" t="s">
+        <v>7236</v>
+      </c>
+      <c r="F2327" s="3">
+        <v>45931.430555555555</v>
+      </c>
+    </row>
+    <row r="2328" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2328" s="4" t="s">
+        <v>7237</v>
+      </c>
+      <c r="B2328" s="3" t="s">
+        <v>7238</v>
+      </c>
+      <c r="C2328" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2328" s="3" t="s">
+        <v>4539</v>
+      </c>
+      <c r="E2328" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2328" s="3">
+        <v>45930.67638888889</v>
       </c>
     </row>
   </sheetData>
@@ -71124,6 +71880,33 @@
     <hyperlink ref="A2299" r:id="rId2298"/>
     <hyperlink ref="A2300" r:id="rId2299"/>
     <hyperlink ref="A2301" r:id="rId2300"/>
+    <hyperlink ref="A2302" r:id="rId2301"/>
+    <hyperlink ref="A2303" r:id="rId2302"/>
+    <hyperlink ref="A2304" r:id="rId2303"/>
+    <hyperlink ref="A2305" r:id="rId2304"/>
+    <hyperlink ref="A2306" r:id="rId2305"/>
+    <hyperlink ref="A2307" r:id="rId2306"/>
+    <hyperlink ref="A2308" r:id="rId2307"/>
+    <hyperlink ref="A2309" r:id="rId2308"/>
+    <hyperlink ref="A2310" r:id="rId2309"/>
+    <hyperlink ref="A2311" r:id="rId2310"/>
+    <hyperlink ref="A2312" r:id="rId2311"/>
+    <hyperlink ref="A2313" r:id="rId2312"/>
+    <hyperlink ref="A2314" r:id="rId2313"/>
+    <hyperlink ref="A2315" r:id="rId2314"/>
+    <hyperlink ref="A2316" r:id="rId2315"/>
+    <hyperlink ref="A2317" r:id="rId2316"/>
+    <hyperlink ref="A2318" r:id="rId2317"/>
+    <hyperlink ref="A2319" r:id="rId2318"/>
+    <hyperlink ref="A2320" r:id="rId2319"/>
+    <hyperlink ref="A2321" r:id="rId2320"/>
+    <hyperlink ref="A2322" r:id="rId2321"/>
+    <hyperlink ref="A2323" r:id="rId2322"/>
+    <hyperlink ref="A2324" r:id="rId2323"/>
+    <hyperlink ref="A2325" r:id="rId2324"/>
+    <hyperlink ref="A2326" r:id="rId2325"/>
+    <hyperlink ref="A2327" r:id="rId2326"/>
+    <hyperlink ref="A2328" r:id="rId2327"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Update lands data - 2025-10-03 12:19
</commit_message>
<xml_diff>
--- a/lands-scraped.xlsx
+++ b/lands-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11777" uniqueCount="7318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11922" uniqueCount="7398">
   <si>
     <t>link</t>
   </si>
@@ -21972,6 +21972,246 @@
   </si>
   <si>
     <t>3 000 € (3 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/aizkraukle-and-reg/aizkraukles/gnhnc.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/aizkraukle-and-reg/jaunjelgava/jkinp.html</t>
+  </si>
+  <si>
+    <t>44 755 € (21.31 €/m²)</t>
+  </si>
+  <si>
+    <t>32070021825</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/iecavas-nov/abbhi.html</t>
+  </si>
+  <si>
+    <t>40 000 € (1 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/raiskuma-pag/bclodp.html</t>
+  </si>
+  <si>
+    <t>14 000 € (11.17 €/m²)</t>
+  </si>
+  <si>
+    <t>1253 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/daugavpils/bfbpo.html</t>
+  </si>
+  <si>
+    <t>66 900 € (36.66 €/m²)</t>
+  </si>
+  <si>
+    <t>1825 m²</t>
+  </si>
+  <si>
+    <t>05000290049</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/naujenes-pag/hhpjb.html</t>
+  </si>
+  <si>
+    <t>44740060548</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/daugavpils/gpjmp.html</t>
+  </si>
+  <si>
+    <t>79 900 € (24.97 €/m²)</t>
+  </si>
+  <si>
+    <t>3200 m²</t>
+  </si>
+  <si>
+    <t>5000010838</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/dobele-and-reg/berzes-pag/ledlb.html</t>
+  </si>
+  <si>
+    <t>260 000 € (1.44 €/m²)</t>
+  </si>
+  <si>
+    <t>46520040033</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jekabpils-and-reg/rites-pag/cepjd.html</t>
+  </si>
+  <si>
+    <t>240 000 € (0.50 €/m²)</t>
+  </si>
+  <si>
+    <t>48 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kuldiga-and-reg/padures-pag/aedhe.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/nicas-pag/icfnm.html</t>
+  </si>
+  <si>
+    <t>50 000 € (2.63 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/liepaja/aaggn.html</t>
+  </si>
+  <si>
+    <t>75 000 € (50.30 €/m²)</t>
+  </si>
+  <si>
+    <t>1491 m²</t>
+  </si>
+  <si>
+    <t>17000120533</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/madona-and-reg/erglu-pag/ibnef.html</t>
+  </si>
+  <si>
+    <t>20 000 € (0.56 €/m²)</t>
+  </si>
+  <si>
+    <t>70540040075</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/krapes-pag/fcgpj.html</t>
+  </si>
+  <si>
+    <t>85 000 € (0.94 €/m²)</t>
+  </si>
+  <si>
+    <t>74520080031</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/rembates-pag/ccdnk.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/feimanu-pag/cmlkx.html</t>
+  </si>
+  <si>
+    <t>6 500 € (0.33 €/m²)</t>
+  </si>
+  <si>
+    <t>78520060182</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/vandzenes-pag/afoeo.html</t>
+  </si>
+  <si>
+    <t>31 500 € (0.55 €/m²)</t>
+  </si>
+  <si>
+    <t>5.68 ha.</t>
+  </si>
+  <si>
+    <t>88940040052</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/talsi/enijn.html</t>
+  </si>
+  <si>
+    <t>35 000 € (9.90 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/talsi/cdeep.html</t>
+  </si>
+  <si>
+    <t>17 000 € (12.14 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/pures-pag/aoiff.html</t>
+  </si>
+  <si>
+    <t>29 500 € (8.36 €/m²)</t>
+  </si>
+  <si>
+    <t>90740080404</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/tumes-pag/eeleb.html</t>
+  </si>
+  <si>
+    <t>15 999 € (4.85 €/m²)</t>
+  </si>
+  <si>
+    <t>90840080170</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/dzukstes-pag/aibdg.html</t>
+  </si>
+  <si>
+    <t>90480040128</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/engures-pag/clddn.html</t>
+  </si>
+  <si>
+    <t>36 450 € (14.58 €/m²)</t>
+  </si>
+  <si>
+    <t>90500050602</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/engures-pag/abhjo.html</t>
+  </si>
+  <si>
+    <t>36 980 € (14.79 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/engures-pag/dbbfh.html</t>
+  </si>
+  <si>
+    <t>58 230 € (11.88 €/m²)</t>
+  </si>
+  <si>
+    <t>0.49 ha.</t>
+  </si>
+  <si>
+    <t>90500051060</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/engures-pag/bpbbd.html</t>
+  </si>
+  <si>
+    <t>38 990 € (11.14 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valka-and-reg/blomes-pag/igkkj.html</t>
+  </si>
+  <si>
+    <t>70 000 € (1.33 €/m²)</t>
+  </si>
+  <si>
+    <t>5.26 ha.</t>
+  </si>
+  <si>
+    <t>94460040019</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valka-and-reg/brantu-pag/eeegb.html</t>
+  </si>
+  <si>
+    <t>35 000 € (1.19 €/m²)</t>
+  </si>
+  <si>
+    <t>29300 m²</t>
+  </si>
+  <si>
+    <t>94480020281</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/valmieras-pag/gjbcj.html</t>
+  </si>
+  <si>
+    <t>40 000 € (23.53 €/m²)</t>
+  </si>
+  <si>
+    <t>96900080695</t>
   </si>
 </sst>
 </file>
@@ -22407,7 +22647,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -22446,522 +22686,582 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>7239</v>
+        <v>7318</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>7240</v>
+        <v>70</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>772</v>
+        <v>8</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>7241</v>
+        <v>71</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>7242</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3">
-        <v>45931.80138888889</v>
+        <v>45932.90763888889</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>7243</v>
+        <v>7319</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>7244</v>
+        <v>7320</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1218</v>
+        <v>8</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>7245</v>
+        <v>3346</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>1295</v>
+        <v>7321</v>
       </c>
       <c r="F3" s="3">
-        <v>45932.45694444445</v>
+        <v>45932.80416666667</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>7246</v>
+        <v>7322</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>7247</v>
+        <v>7323</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>1218</v>
+        <v>419</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>7248</v>
+        <v>353</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>7249</v>
+        <v>10</v>
       </c>
       <c r="F4" s="3">
-        <v>45932.419444444444</v>
+        <v>45932.64583333333</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>7250</v>
+        <v>7324</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>2615</v>
+        <v>7325</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>1218</v>
+        <v>772</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>325</v>
+        <v>7326</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>7251</v>
+        <v>10</v>
       </c>
       <c r="F5" s="3">
-        <v>45931.902083333334</v>
+        <v>45933.44583333333</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>7252</v>
+        <v>7327</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>7253</v>
+        <v>7328</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>1218</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>7254</v>
+        <v>7329</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>7255</v>
+        <v>7330</v>
       </c>
       <c r="F6" s="3">
-        <v>45931.902083333334</v>
+        <v>45933.45416666666</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>7256</v>
+        <v>7331</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>7257</v>
+        <v>471</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>1218</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>325</v>
+        <v>32</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>7258</v>
+        <v>7332</v>
       </c>
       <c r="F7" s="3">
-        <v>45931.67083333334</v>
+        <v>45933.33333333333</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>7259</v>
+        <v>7333</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>7260</v>
+        <v>7334</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1929</v>
+        <v>1218</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>7261</v>
+        <v>7335</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>7262</v>
+        <v>7336</v>
       </c>
       <c r="F8" s="3">
-        <v>45932.43958333333</v>
+        <v>45932.70833333333</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>7263</v>
+        <v>7337</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>7264</v>
+        <v>7338</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>1929</v>
+        <v>1569</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>7265</v>
+        <v>294</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>7266</v>
+        <v>7339</v>
       </c>
       <c r="F9" s="3">
-        <v>45932.40486111111</v>
+        <v>45932.70347222222</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>7267</v>
+        <v>7340</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>7268</v>
+        <v>7341</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>1929</v>
+        <v>1733</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>7269</v>
+        <v>7342</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>7270</v>
+        <v>10</v>
       </c>
       <c r="F10" s="3">
-        <v>45932.27013888889</v>
+        <v>45933.399305555555</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>7271</v>
+        <v>7343</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>7272</v>
+        <v>4083</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>1929</v>
+        <v>2671</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>5695</v>
+        <v>201</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F11" s="3">
-        <v>45932.26666666666</v>
+        <v>45932.95763888889</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>7273</v>
+        <v>7344</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>7274</v>
+        <v>7345</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>1929</v>
+        <v>2846</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>7275</v>
+        <v>4365</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F12" s="3">
-        <v>45932.02291666667</v>
+        <v>45933.56875</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>7276</v>
+        <v>7346</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>7277</v>
+        <v>7347</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>1929</v>
+        <v>2846</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>383</v>
+        <v>7348</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>7278</v>
+        <v>7349</v>
       </c>
       <c r="F13" s="3">
-        <v>45931.70208333334</v>
+        <v>45932.71319444444</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>7279</v>
+        <v>7350</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>7280</v>
+        <v>7351</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>1929</v>
+        <v>3868</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>2179</v>
+        <v>2707</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>2180</v>
+        <v>7352</v>
       </c>
       <c r="F14" s="3">
-        <v>45931.69097222222</v>
+        <v>45933.631944444445</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>7281</v>
+        <v>7353</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>2609</v>
+        <v>7354</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>2488</v>
+        <v>4034</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>407</v>
+        <v>1430</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>7282</v>
+        <v>7355</v>
       </c>
       <c r="F15" s="3">
-        <v>45932.47083333333</v>
+        <v>45933.509722222225</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>7283</v>
+        <v>7356</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>7284</v>
+        <v>4426</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>2846</v>
+        <v>4034</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>365</v>
+        <v>55</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>7285</v>
+        <v>10</v>
       </c>
       <c r="F16" s="3">
-        <v>45932.601388888885</v>
+        <v>45932.711111111115</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>7286</v>
+        <v>7357</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>7287</v>
+        <v>7358</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>3398</v>
+        <v>4770</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>7288</v>
+        <v>7359</v>
       </c>
       <c r="F17" s="3">
-        <v>45932.52986111111</v>
+        <v>45933.51041666667</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>7289</v>
+        <v>7360</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>7290</v>
+        <v>7361</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>3398</v>
+        <v>5266</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>290</v>
+        <v>7362</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>10</v>
+        <v>7363</v>
       </c>
       <c r="F18" s="3">
-        <v>45932.46597222222</v>
+        <v>45933.51041666667</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>7291</v>
+        <v>7364</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>7292</v>
+        <v>7365</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>3398</v>
+        <v>5266</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>111</v>
+        <v>2847</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>7293</v>
+        <v>10</v>
       </c>
       <c r="F19" s="3">
-        <v>45931.90416666667</v>
+        <v>45932.81319444445</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>7294</v>
+        <v>7366</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>7295</v>
+        <v>7367</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>4034</v>
+        <v>5266</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>317</v>
+        <v>1259</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>4511</v>
+        <v>10</v>
       </c>
       <c r="F20" s="3">
-        <v>45932.45</v>
+        <v>45932.725</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>7296</v>
+        <v>7368</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>7297</v>
+        <v>7369</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>4770</v>
+        <v>5674</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>809</v>
+        <v>5954</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>7298</v>
+        <v>7370</v>
       </c>
       <c r="F21" s="3">
-        <v>45931.87986111111</v>
+        <v>45933.507638888885</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>7299</v>
+        <v>7371</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>7300</v>
+        <v>7372</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>5266</v>
+        <v>5674</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>7301</v>
+        <v>488</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>7302</v>
+        <v>7373</v>
       </c>
       <c r="F22" s="3">
-        <v>45932.44305555556</v>
+        <v>45933.393055555556</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>7303</v>
+        <v>7374</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>7304</v>
+        <v>1549</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>5266</v>
+        <v>5674</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>7305</v>
+        <v>32</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>10</v>
+        <v>7375</v>
       </c>
       <c r="F23" s="3">
-        <v>45931.660416666666</v>
+        <v>45933.33333333333</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>7306</v>
+        <v>7376</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>7307</v>
+        <v>7377</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>5674</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>7308</v>
+        <v>1632</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>7309</v>
+        <v>7378</v>
       </c>
       <c r="F24" s="3">
-        <v>45932.62222222222</v>
+        <v>45932.81388888889</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>7310</v>
+        <v>7379</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>7311</v>
+        <v>7380</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>5674</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>7312</v>
+        <v>1632</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>10</v>
+        <v>7378</v>
       </c>
       <c r="F25" s="3">
-        <v>45932.60208333333</v>
+        <v>45932.8125</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>7313</v>
+        <v>7381</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>7314</v>
+        <v>7382</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>6133</v>
+        <v>5674</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>7315</v>
+        <v>7383</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>10</v>
+        <v>7384</v>
       </c>
       <c r="F26" s="3">
-        <v>45931.75</v>
+        <v>45932.80902777778</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>7316</v>
+        <v>7385</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>7317</v>
+        <v>7386</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>1194</v>
+        <v>5674</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>71</v>
+        <v>2271</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>10</v>
+        <v>7384</v>
       </c>
       <c r="F27" s="3">
-        <v>45931.69236111111</v>
+        <v>45932.808333333334</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>7387</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>7388</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>6133</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>7389</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>7390</v>
+      </c>
+      <c r="F28" s="3">
+        <v>45933.60555555555</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>7391</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>7392</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>6133</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>7393</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>7394</v>
+      </c>
+      <c r="F29" s="3">
+        <v>45933.46527777778</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>7395</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>7396</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>7089</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>7397</v>
+      </c>
+      <c r="F30" s="3">
+        <v>45932.88611111111</v>
       </c>
     </row>
   </sheetData>
@@ -22992,6 +23292,9 @@
     <hyperlink ref="A25" r:id="rId24"/>
     <hyperlink ref="A26" r:id="rId25"/>
     <hyperlink ref="A27" r:id="rId26"/>
+    <hyperlink ref="A28" r:id="rId27"/>
+    <hyperlink ref="A29" r:id="rId28"/>
+    <hyperlink ref="A30" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -23000,7 +23303,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2328"/>
+  <dimension ref="A1:F2354"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -69576,6 +69879,526 @@
       </c>
       <c r="F2328" s="3">
         <v>45930.67638888889</v>
+      </c>
+    </row>
+    <row r="2329" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2329" s="4" t="s">
+        <v>7239</v>
+      </c>
+      <c r="B2329" s="3" t="s">
+        <v>7240</v>
+      </c>
+      <c r="C2329" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2329" s="3" t="s">
+        <v>7241</v>
+      </c>
+      <c r="E2329" s="3" t="s">
+        <v>7242</v>
+      </c>
+      <c r="F2329" s="3">
+        <v>45931.80138888889</v>
+      </c>
+    </row>
+    <row r="2330" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2330" s="4" t="s">
+        <v>7243</v>
+      </c>
+      <c r="B2330" s="3" t="s">
+        <v>7244</v>
+      </c>
+      <c r="C2330" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2330" s="3" t="s">
+        <v>7245</v>
+      </c>
+      <c r="E2330" s="3" t="s">
+        <v>1295</v>
+      </c>
+      <c r="F2330" s="3">
+        <v>45932.45694444445</v>
+      </c>
+    </row>
+    <row r="2331" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2331" s="4" t="s">
+        <v>7246</v>
+      </c>
+      <c r="B2331" s="3" t="s">
+        <v>7247</v>
+      </c>
+      <c r="C2331" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2331" s="3" t="s">
+        <v>7248</v>
+      </c>
+      <c r="E2331" s="3" t="s">
+        <v>7249</v>
+      </c>
+      <c r="F2331" s="3">
+        <v>45932.419444444444</v>
+      </c>
+    </row>
+    <row r="2332" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2332" s="4" t="s">
+        <v>7250</v>
+      </c>
+      <c r="B2332" s="3" t="s">
+        <v>2615</v>
+      </c>
+      <c r="C2332" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2332" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2332" s="3" t="s">
+        <v>7251</v>
+      </c>
+      <c r="F2332" s="3">
+        <v>45931.902083333334</v>
+      </c>
+    </row>
+    <row r="2333" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2333" s="4" t="s">
+        <v>7252</v>
+      </c>
+      <c r="B2333" s="3" t="s">
+        <v>7253</v>
+      </c>
+      <c r="C2333" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2333" s="3" t="s">
+        <v>7254</v>
+      </c>
+      <c r="E2333" s="3" t="s">
+        <v>7255</v>
+      </c>
+      <c r="F2333" s="3">
+        <v>45931.902083333334</v>
+      </c>
+    </row>
+    <row r="2334" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2334" s="4" t="s">
+        <v>7256</v>
+      </c>
+      <c r="B2334" s="3" t="s">
+        <v>7257</v>
+      </c>
+      <c r="C2334" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2334" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2334" s="3" t="s">
+        <v>7258</v>
+      </c>
+      <c r="F2334" s="3">
+        <v>45931.67083333334</v>
+      </c>
+    </row>
+    <row r="2335" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2335" s="4" t="s">
+        <v>7259</v>
+      </c>
+      <c r="B2335" s="3" t="s">
+        <v>7260</v>
+      </c>
+      <c r="C2335" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2335" s="3" t="s">
+        <v>7261</v>
+      </c>
+      <c r="E2335" s="3" t="s">
+        <v>7262</v>
+      </c>
+      <c r="F2335" s="3">
+        <v>45932.43958333333</v>
+      </c>
+    </row>
+    <row r="2336" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2336" s="4" t="s">
+        <v>7263</v>
+      </c>
+      <c r="B2336" s="3" t="s">
+        <v>7264</v>
+      </c>
+      <c r="C2336" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2336" s="3" t="s">
+        <v>7265</v>
+      </c>
+      <c r="E2336" s="3" t="s">
+        <v>7266</v>
+      </c>
+      <c r="F2336" s="3">
+        <v>45932.40486111111</v>
+      </c>
+    </row>
+    <row r="2337" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2337" s="4" t="s">
+        <v>7267</v>
+      </c>
+      <c r="B2337" s="3" t="s">
+        <v>7268</v>
+      </c>
+      <c r="C2337" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2337" s="3" t="s">
+        <v>7269</v>
+      </c>
+      <c r="E2337" s="3" t="s">
+        <v>7270</v>
+      </c>
+      <c r="F2337" s="3">
+        <v>45932.27013888889</v>
+      </c>
+    </row>
+    <row r="2338" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2338" s="4" t="s">
+        <v>7271</v>
+      </c>
+      <c r="B2338" s="3" t="s">
+        <v>7272</v>
+      </c>
+      <c r="C2338" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2338" s="3" t="s">
+        <v>5695</v>
+      </c>
+      <c r="E2338" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2338" s="3">
+        <v>45932.26666666666</v>
+      </c>
+    </row>
+    <row r="2339" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2339" s="4" t="s">
+        <v>7273</v>
+      </c>
+      <c r="B2339" s="3" t="s">
+        <v>7274</v>
+      </c>
+      <c r="C2339" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2339" s="3" t="s">
+        <v>7275</v>
+      </c>
+      <c r="E2339" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2339" s="3">
+        <v>45932.02291666667</v>
+      </c>
+    </row>
+    <row r="2340" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2340" s="4" t="s">
+        <v>7276</v>
+      </c>
+      <c r="B2340" s="3" t="s">
+        <v>7277</v>
+      </c>
+      <c r="C2340" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2340" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E2340" s="3" t="s">
+        <v>7278</v>
+      </c>
+      <c r="F2340" s="3">
+        <v>45931.70208333334</v>
+      </c>
+    </row>
+    <row r="2341" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2341" s="4" t="s">
+        <v>7279</v>
+      </c>
+      <c r="B2341" s="3" t="s">
+        <v>7280</v>
+      </c>
+      <c r="C2341" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2341" s="3" t="s">
+        <v>2179</v>
+      </c>
+      <c r="E2341" s="3" t="s">
+        <v>2180</v>
+      </c>
+      <c r="F2341" s="3">
+        <v>45931.69097222222</v>
+      </c>
+    </row>
+    <row r="2342" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2342" s="4" t="s">
+        <v>7281</v>
+      </c>
+      <c r="B2342" s="3" t="s">
+        <v>2609</v>
+      </c>
+      <c r="C2342" s="3" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D2342" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="E2342" s="3" t="s">
+        <v>7282</v>
+      </c>
+      <c r="F2342" s="3">
+        <v>45932.47083333333</v>
+      </c>
+    </row>
+    <row r="2343" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2343" s="4" t="s">
+        <v>7283</v>
+      </c>
+      <c r="B2343" s="3" t="s">
+        <v>7284</v>
+      </c>
+      <c r="C2343" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2343" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E2343" s="3" t="s">
+        <v>7285</v>
+      </c>
+      <c r="F2343" s="3">
+        <v>45932.601388888885</v>
+      </c>
+    </row>
+    <row r="2344" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2344" s="4" t="s">
+        <v>7286</v>
+      </c>
+      <c r="B2344" s="3" t="s">
+        <v>7287</v>
+      </c>
+      <c r="C2344" s="3" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D2344" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E2344" s="3" t="s">
+        <v>7288</v>
+      </c>
+      <c r="F2344" s="3">
+        <v>45932.52986111111</v>
+      </c>
+    </row>
+    <row r="2345" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2345" s="4" t="s">
+        <v>7289</v>
+      </c>
+      <c r="B2345" s="3" t="s">
+        <v>7290</v>
+      </c>
+      <c r="C2345" s="3" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D2345" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="E2345" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2345" s="3">
+        <v>45932.46597222222</v>
+      </c>
+    </row>
+    <row r="2346" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2346" s="4" t="s">
+        <v>7291</v>
+      </c>
+      <c r="B2346" s="3" t="s">
+        <v>7292</v>
+      </c>
+      <c r="C2346" s="3" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D2346" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2346" s="3" t="s">
+        <v>7293</v>
+      </c>
+      <c r="F2346" s="3">
+        <v>45931.90416666667</v>
+      </c>
+    </row>
+    <row r="2347" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2347" s="4" t="s">
+        <v>7294</v>
+      </c>
+      <c r="B2347" s="3" t="s">
+        <v>7295</v>
+      </c>
+      <c r="C2347" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2347" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E2347" s="3" t="s">
+        <v>4511</v>
+      </c>
+      <c r="F2347" s="3">
+        <v>45932.45</v>
+      </c>
+    </row>
+    <row r="2348" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2348" s="4" t="s">
+        <v>7296</v>
+      </c>
+      <c r="B2348" s="3" t="s">
+        <v>7297</v>
+      </c>
+      <c r="C2348" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2348" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="E2348" s="3" t="s">
+        <v>7298</v>
+      </c>
+      <c r="F2348" s="3">
+        <v>45931.87986111111</v>
+      </c>
+    </row>
+    <row r="2349" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2349" s="4" t="s">
+        <v>7299</v>
+      </c>
+      <c r="B2349" s="3" t="s">
+        <v>7300</v>
+      </c>
+      <c r="C2349" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2349" s="3" t="s">
+        <v>7301</v>
+      </c>
+      <c r="E2349" s="3" t="s">
+        <v>7302</v>
+      </c>
+      <c r="F2349" s="3">
+        <v>45932.44305555556</v>
+      </c>
+    </row>
+    <row r="2350" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2350" s="4" t="s">
+        <v>7303</v>
+      </c>
+      <c r="B2350" s="3" t="s">
+        <v>7304</v>
+      </c>
+      <c r="C2350" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2350" s="3" t="s">
+        <v>7305</v>
+      </c>
+      <c r="E2350" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2350" s="3">
+        <v>45931.660416666666</v>
+      </c>
+    </row>
+    <row r="2351" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2351" s="4" t="s">
+        <v>7306</v>
+      </c>
+      <c r="B2351" s="3" t="s">
+        <v>7307</v>
+      </c>
+      <c r="C2351" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2351" s="3" t="s">
+        <v>7308</v>
+      </c>
+      <c r="E2351" s="3" t="s">
+        <v>7309</v>
+      </c>
+      <c r="F2351" s="3">
+        <v>45932.62222222222</v>
+      </c>
+    </row>
+    <row r="2352" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2352" s="4" t="s">
+        <v>7310</v>
+      </c>
+      <c r="B2352" s="3" t="s">
+        <v>7311</v>
+      </c>
+      <c r="C2352" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2352" s="3" t="s">
+        <v>7312</v>
+      </c>
+      <c r="E2352" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2352" s="3">
+        <v>45932.60208333333</v>
+      </c>
+    </row>
+    <row r="2353" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2353" s="4" t="s">
+        <v>7313</v>
+      </c>
+      <c r="B2353" s="3" t="s">
+        <v>7314</v>
+      </c>
+      <c r="C2353" s="3" t="s">
+        <v>6133</v>
+      </c>
+      <c r="D2353" s="3" t="s">
+        <v>7315</v>
+      </c>
+      <c r="E2353" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2353" s="3">
+        <v>45931.75</v>
+      </c>
+    </row>
+    <row r="2354" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2354" s="4" t="s">
+        <v>7316</v>
+      </c>
+      <c r="B2354" s="3" t="s">
+        <v>7317</v>
+      </c>
+      <c r="C2354" s="3" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D2354" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2354" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2354" s="3">
+        <v>45931.69236111111</v>
       </c>
     </row>
   </sheetData>
@@ -71907,6 +72730,32 @@
     <hyperlink ref="A2326" r:id="rId2325"/>
     <hyperlink ref="A2327" r:id="rId2326"/>
     <hyperlink ref="A2328" r:id="rId2327"/>
+    <hyperlink ref="A2329" r:id="rId2328"/>
+    <hyperlink ref="A2330" r:id="rId2329"/>
+    <hyperlink ref="A2331" r:id="rId2330"/>
+    <hyperlink ref="A2332" r:id="rId2331"/>
+    <hyperlink ref="A2333" r:id="rId2332"/>
+    <hyperlink ref="A2334" r:id="rId2333"/>
+    <hyperlink ref="A2335" r:id="rId2334"/>
+    <hyperlink ref="A2336" r:id="rId2335"/>
+    <hyperlink ref="A2337" r:id="rId2336"/>
+    <hyperlink ref="A2338" r:id="rId2337"/>
+    <hyperlink ref="A2339" r:id="rId2338"/>
+    <hyperlink ref="A2340" r:id="rId2339"/>
+    <hyperlink ref="A2341" r:id="rId2340"/>
+    <hyperlink ref="A2342" r:id="rId2341"/>
+    <hyperlink ref="A2343" r:id="rId2342"/>
+    <hyperlink ref="A2344" r:id="rId2343"/>
+    <hyperlink ref="A2345" r:id="rId2344"/>
+    <hyperlink ref="A2346" r:id="rId2345"/>
+    <hyperlink ref="A2347" r:id="rId2346"/>
+    <hyperlink ref="A2348" r:id="rId2347"/>
+    <hyperlink ref="A2349" r:id="rId2348"/>
+    <hyperlink ref="A2350" r:id="rId2349"/>
+    <hyperlink ref="A2351" r:id="rId2350"/>
+    <hyperlink ref="A2352" r:id="rId2351"/>
+    <hyperlink ref="A2353" r:id="rId2352"/>
+    <hyperlink ref="A2354" r:id="rId2353"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Update lands data - 2025-10-06 12:21
</commit_message>
<xml_diff>
--- a/lands-scraped.xlsx
+++ b/lands-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11922" uniqueCount="7398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12242" uniqueCount="7578">
   <si>
     <t>link</t>
   </si>
@@ -22212,6 +22212,546 @@
   </si>
   <si>
     <t>96900080695</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/aizkraukle-and-reg/skriveru-pag/bgfbf.html</t>
+  </si>
+  <si>
+    <t>18 000 € (9.97 €/m²)</t>
+  </si>
+  <si>
+    <t>32820080175</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/aizkraukle-and-reg/klintaines-pag/alebo.html</t>
+  </si>
+  <si>
+    <t>20 000 € (0.57 €/m²)</t>
+  </si>
+  <si>
+    <t>32580090116</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/gailisu-pag/abifk.html</t>
+  </si>
+  <si>
+    <t>15 000 € (1.21 €/m²)</t>
+  </si>
+  <si>
+    <t>40600070179</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/vecumnieku-pag/anfgp.html</t>
+  </si>
+  <si>
+    <t>38 000 € (0.77 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/davinu-pag/joxfj.html</t>
+  </si>
+  <si>
+    <t>45 000 € (0.50 €/m²)</t>
+  </si>
+  <si>
+    <t>50560030040</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/davinu-pag/mhxco.html</t>
+  </si>
+  <si>
+    <t>35 000 € (0.70 €/m²)</t>
+  </si>
+  <si>
+    <t>40560030040</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/codes-pag/mhedn.html</t>
+  </si>
+  <si>
+    <t>16 730 € (0.70 €/m²)</t>
+  </si>
+  <si>
+    <t>2.39 ha.</t>
+  </si>
+  <si>
+    <t>40520050162</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/codes-pag/gfjcg.html</t>
+  </si>
+  <si>
+    <t>89 600 € (0.70 €/m²)</t>
+  </si>
+  <si>
+    <t>12.80 ha.</t>
+  </si>
+  <si>
+    <t>40520050015</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/davinu-pag/ekjmf.html</t>
+  </si>
+  <si>
+    <t>31 380 € (0.63 €/m²)</t>
+  </si>
+  <si>
+    <t>40560030110</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/iecavas-nov/hfdio.html</t>
+  </si>
+  <si>
+    <t>205 920 € (4.12 €/m²)</t>
+  </si>
+  <si>
+    <t>40640100080</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/iecavas-nov/gkckh.html</t>
+  </si>
+  <si>
+    <t>36 000 € (8.78 €/m²)</t>
+  </si>
+  <si>
+    <t>40640100697</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/rundales-pag/jmbib.html</t>
+  </si>
+  <si>
+    <t>10 000 € (5.75 €/m²)</t>
+  </si>
+  <si>
+    <t>1739 m²</t>
+  </si>
+  <si>
+    <t>40760060205</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/cesis/ahbnd.html</t>
+  </si>
+  <si>
+    <t>38 000 € (7.22 €/m²)</t>
+  </si>
+  <si>
+    <t>5261 m²</t>
+  </si>
+  <si>
+    <t>42010081009</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/vecpiebalgas-pag/cnkop.html</t>
+  </si>
+  <si>
+    <t>40 000 € (0.32 €/m²)</t>
+  </si>
+  <si>
+    <t>124000 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/dzerbenes-pag/jxcpd.html</t>
+  </si>
+  <si>
+    <t>8 000 € (0.73 €/m²)</t>
+  </si>
+  <si>
+    <t>10983 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/ligatnes-pag/gbgfi.html</t>
+  </si>
+  <si>
+    <t>280 000 € (0.62 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/laucesas-pag/clhke.html</t>
+  </si>
+  <si>
+    <t>69 700 € (0.37 €/m²)</t>
+  </si>
+  <si>
+    <t>44640010143</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/dobele-and-reg/auru-pag/aekxl.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jekabpils-and-reg/vipes-pag/cggdkx.html</t>
+  </si>
+  <si>
+    <t>38 000 € (0.95 €/m²)</t>
+  </si>
+  <si>
+    <t>56960050120</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jekabpils-and-reg/jekabpils/bceinl.html</t>
+  </si>
+  <si>
+    <t>11 000 € (10.47 €/m²)</t>
+  </si>
+  <si>
+    <t>1051 m²</t>
+  </si>
+  <si>
+    <t>56010022492</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/zalenieku-pag/abxgn.html</t>
+  </si>
+  <si>
+    <t>90 000 € (1.01 €/m²)</t>
+  </si>
+  <si>
+    <t>89200 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jelgava/bdomlm.html</t>
+  </si>
+  <si>
+    <t>85 000 € (10.71 €/m²)</t>
+  </si>
+  <si>
+    <t>7940 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/valgundes-nov/alxen.html</t>
+  </si>
+  <si>
+    <t>54860010024</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jelgava/hfhxd.html</t>
+  </si>
+  <si>
+    <t>140 000 € (4.92 €/m²)</t>
+  </si>
+  <si>
+    <t>28454 m²</t>
+  </si>
+  <si>
+    <t>0900 009 0207 /0257</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/valgundes-nov/aomoc.html</t>
+  </si>
+  <si>
+    <t>54860130601</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jelgava/engdj.html</t>
+  </si>
+  <si>
+    <t>35 000 € (13.41 €/m²)</t>
+  </si>
+  <si>
+    <t>2610 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/platones-pag/cnlpi.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/cenu-pag/cleff.html</t>
+  </si>
+  <si>
+    <t>29 500 € (2.95 €/m²)</t>
+  </si>
+  <si>
+    <t>54440050632</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/ciravas-pag/hkpnb.html</t>
+  </si>
+  <si>
+    <t>65 369 € (0.65 €/m²)</t>
+  </si>
+  <si>
+    <t>64480070048</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/liepaja/aaacm.html</t>
+  </si>
+  <si>
+    <t>43 000 € (64.76 €/m²)</t>
+  </si>
+  <si>
+    <t>664 m²</t>
+  </si>
+  <si>
+    <t>17000200458</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/nicas-pag/ajcbc.html</t>
+  </si>
+  <si>
+    <t>50 000 € (3.03 €/m²)</t>
+  </si>
+  <si>
+    <t>16500 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/otanku-pag/nlobd.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/limbadzi-and-reg/salacgriva/eokej.html</t>
+  </si>
+  <si>
+    <t>114 420 € (30 €/m²)</t>
+  </si>
+  <si>
+    <t>3814 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/limbadzi-and-reg/salacgriva/cichi.html</t>
+  </si>
+  <si>
+    <t>104 190 € (30 €/m²)</t>
+  </si>
+  <si>
+    <t>3473 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/limbadzi-and-reg/liepupes-pag/cfool.html</t>
+  </si>
+  <si>
+    <t>66600090598</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/madona-and-reg/cesvaine/hmnxm.html</t>
+  </si>
+  <si>
+    <t>13 000 € (0.41 €/m²)</t>
+  </si>
+  <si>
+    <t>3.20 ha.</t>
+  </si>
+  <si>
+    <t>70270100121</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/madona-and-reg/erglu-pag/cbceb.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/madona-and-reg/erglu-pag/hnhhe.html</t>
+  </si>
+  <si>
+    <t>33 000 € (0.45 €/m²)</t>
+  </si>
+  <si>
+    <t>70540040097</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/birzgales-pag/aodjh.html</t>
+  </si>
+  <si>
+    <t>15 555 € (6.22 €/m²)</t>
+  </si>
+  <si>
+    <t>7444 005 0478</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ikskiles-l-t/hpknp.html</t>
+  </si>
+  <si>
+    <t>32 000 € (8 €/m²)</t>
+  </si>
+  <si>
+    <t>74940080092</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ikskile/cimio.html</t>
+  </si>
+  <si>
+    <t>50 000 € (38.76 €/m²)</t>
+  </si>
+  <si>
+    <t>74940120644</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ikskile/ckoih.html</t>
+  </si>
+  <si>
+    <t>50 000 € (38.46 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/lielvarde/doopg.html</t>
+  </si>
+  <si>
+    <t>67 500 € (6.75 €/m²)</t>
+  </si>
+  <si>
+    <t>7433 002 0140</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/lielvarde/akxbg.html</t>
+  </si>
+  <si>
+    <t>45 000 € (16.69 €/m²)</t>
+  </si>
+  <si>
+    <t>2697 m²</t>
+  </si>
+  <si>
+    <t>74130020041</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ledmanes-pag/ajgbx.html</t>
+  </si>
+  <si>
+    <t>74640060147</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/keguma-l-t/nnfgx.html</t>
+  </si>
+  <si>
+    <t>74290040207</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/keguma-l-t/ncpxg.html</t>
+  </si>
+  <si>
+    <t>100 000 € (4.31 €/m²)</t>
+  </si>
+  <si>
+    <t>2.32 ha.</t>
+  </si>
+  <si>
+    <t>74290040208</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/keguma-l-t/ndnhm.html</t>
+  </si>
+  <si>
+    <t>74290040056</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/keguma-l-t/nebfc.html</t>
+  </si>
+  <si>
+    <t>74290040053</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/keguma-l-t/blpok.html</t>
+  </si>
+  <si>
+    <t>74290040108</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/preili-and-reg/livani/bbkphx.html</t>
+  </si>
+  <si>
+    <t>76520010121</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/preili-and-reg/jersikas-pag/beixc.html</t>
+  </si>
+  <si>
+    <t>10 000 € (1.99 €/m²)</t>
+  </si>
+  <si>
+    <t>5018 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/preili-and-reg/aglonas-pag/hihdk.html</t>
+  </si>
+  <si>
+    <t>97 000 € (2.89 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/ozolaines-pag/afdop.html</t>
+  </si>
+  <si>
+    <t>2 500 € (5.81 €/m²)</t>
+  </si>
+  <si>
+    <t>430 m²</t>
+  </si>
+  <si>
+    <t>78760010056</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/struzanu-pag/bxmjof.html</t>
+  </si>
+  <si>
+    <t>55 000 € (2.75 €/m²)</t>
+  </si>
+  <si>
+    <t>78500030311</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/rezekne/bfool.html</t>
+  </si>
+  <si>
+    <t>3 500 € (6.39 €/m²)</t>
+  </si>
+  <si>
+    <t>78960050461</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/griskanu-pag/fjdnl.html</t>
+  </si>
+  <si>
+    <t>78560010880</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/silmalas-pag/cfbjic.html</t>
+  </si>
+  <si>
+    <t>9 000 € (1 €/m²)</t>
+  </si>
+  <si>
+    <t>78880020199</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/silmalas-pag/beddgk.html</t>
+  </si>
+  <si>
+    <t>78880020284</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/mersraga-pag/aibef.html</t>
+  </si>
+  <si>
+    <t>30 000 € (3.37 €/m²)</t>
+  </si>
+  <si>
+    <t>8900 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/mersraga-pag/eccpi.html</t>
+  </si>
+  <si>
+    <t>13 000 € (5.19 €/m²)</t>
+  </si>
+  <si>
+    <t>2505 m²</t>
+  </si>
+  <si>
+    <t>88780030664</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/tukums/eeljf.html</t>
+  </si>
+  <si>
+    <t>27 000 € (28.18 €/m²)</t>
+  </si>
+  <si>
+    <t>958 m²</t>
+  </si>
+  <si>
+    <t>90010040801</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/kocenu-pag/ajlcm.html</t>
+  </si>
+  <si>
+    <t>21 900 € (1.10 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/targales-pag/hhpho.html</t>
+  </si>
+  <si>
+    <t>15 000 € (0.75 €/m²)</t>
   </si>
 </sst>
 </file>
@@ -22647,7 +23187,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -22686,582 +23226,1282 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>7318</v>
+        <v>7398</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>70</v>
+        <v>7399</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>71</v>
+        <v>1984</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>10</v>
+        <v>7400</v>
       </c>
       <c r="F2" s="3">
-        <v>45932.90763888889</v>
+        <v>45935.52569444444</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>7319</v>
+        <v>7401</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>7320</v>
+        <v>7402</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>3346</v>
+        <v>2284</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>7321</v>
+        <v>7403</v>
       </c>
       <c r="F3" s="3">
-        <v>45932.80416666667</v>
+        <v>45933.65902777778</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>7322</v>
+        <v>7404</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>7323</v>
+        <v>7405</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>419</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>353</v>
+        <v>6208</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>10</v>
+        <v>7406</v>
       </c>
       <c r="F4" s="3">
-        <v>45932.64583333333</v>
+        <v>45935.73055555555</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>7324</v>
+        <v>7407</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>7325</v>
+        <v>7408</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>772</v>
+        <v>419</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>7326</v>
+        <v>536</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>10</v>
+        <v>537</v>
       </c>
       <c r="F5" s="3">
-        <v>45933.44583333333</v>
+        <v>45935.49791666667</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>7327</v>
+        <v>7409</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>7328</v>
+        <v>7410</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1218</v>
+        <v>419</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>7329</v>
+        <v>1430</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>7330</v>
+        <v>7411</v>
       </c>
       <c r="F6" s="3">
-        <v>45933.45416666666</v>
+        <v>45935.481944444444</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>7331</v>
+        <v>7412</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>471</v>
+        <v>7413</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>1218</v>
+        <v>419</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>7332</v>
+        <v>7414</v>
       </c>
       <c r="F7" s="3">
-        <v>45933.33333333333</v>
+        <v>45935.475</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>7333</v>
+        <v>7415</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>7334</v>
+        <v>7416</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1218</v>
+        <v>419</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>7335</v>
+        <v>7417</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>7336</v>
+        <v>7418</v>
       </c>
       <c r="F8" s="3">
-        <v>45932.70833333333</v>
+        <v>45935.46736111111</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>7337</v>
+        <v>7419</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>7338</v>
+        <v>7420</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>1569</v>
+        <v>419</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>294</v>
+        <v>7421</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>7339</v>
+        <v>7422</v>
       </c>
       <c r="F9" s="3">
-        <v>45932.70347222222</v>
+        <v>45935.46319444444</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>7340</v>
+        <v>7423</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>7341</v>
+        <v>7424</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>1733</v>
+        <v>419</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>7342</v>
+        <v>77</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>10</v>
+        <v>7425</v>
       </c>
       <c r="F10" s="3">
-        <v>45933.399305555555</v>
+        <v>45935.45694444445</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>7343</v>
+        <v>7426</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>4083</v>
+        <v>7427</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>2671</v>
+        <v>419</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>201</v>
+        <v>77</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>10</v>
+        <v>7428</v>
       </c>
       <c r="F11" s="3">
-        <v>45932.95763888889</v>
+        <v>45934.58263888889</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>7344</v>
+        <v>7429</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>7345</v>
+        <v>7430</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>2846</v>
+        <v>419</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>4365</v>
+        <v>4468</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>10</v>
+        <v>7431</v>
       </c>
       <c r="F12" s="3">
-        <v>45933.56875</v>
+        <v>45933.86319444445</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>7346</v>
+        <v>7432</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>7347</v>
+        <v>7433</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>2846</v>
+        <v>419</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>7348</v>
+        <v>7434</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>7349</v>
+        <v>7435</v>
       </c>
       <c r="F13" s="3">
-        <v>45932.71319444444</v>
+        <v>45933.756944444445</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>7350</v>
+        <v>7436</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>7351</v>
+        <v>7437</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>3868</v>
+        <v>772</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>2707</v>
+        <v>7438</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>7352</v>
+        <v>7439</v>
       </c>
       <c r="F14" s="3">
-        <v>45933.631944444445</v>
+        <v>45934.7125</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>7353</v>
+        <v>7440</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>7354</v>
+        <v>7441</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>4034</v>
+        <v>772</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>1430</v>
+        <v>7442</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>7355</v>
+        <v>870</v>
       </c>
       <c r="F15" s="3">
-        <v>45933.509722222225</v>
+        <v>45934.5125</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>7356</v>
+        <v>7443</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>4426</v>
+        <v>7444</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>4034</v>
+        <v>772</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>55</v>
+        <v>7445</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F16" s="3">
-        <v>45932.711111111115</v>
+        <v>45934.464583333334</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>7357</v>
+        <v>7446</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>7358</v>
+        <v>7447</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>4770</v>
+        <v>772</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>171</v>
+        <v>1112</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>7359</v>
+        <v>1113</v>
       </c>
       <c r="F17" s="3">
-        <v>45933.51041666667</v>
+        <v>45934.41875</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>7360</v>
+        <v>7448</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>7361</v>
+        <v>7449</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>5266</v>
+        <v>1218</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>7362</v>
+        <v>1156</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>7363</v>
+        <v>7450</v>
       </c>
       <c r="F18" s="3">
-        <v>45933.51041666667</v>
+        <v>45933.66180555556</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>7364</v>
+        <v>7451</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>7365</v>
+        <v>830</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>5266</v>
+        <v>1569</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>2847</v>
+        <v>353</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F19" s="3">
-        <v>45932.81319444445</v>
+        <v>45936.59166666667</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>7366</v>
+        <v>7452</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>7367</v>
+        <v>7453</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>5266</v>
+        <v>1733</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>1259</v>
+        <v>353</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>10</v>
+        <v>7454</v>
       </c>
       <c r="F20" s="3">
-        <v>45932.725</v>
+        <v>45936.59027777778</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>7368</v>
+        <v>7455</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>7369</v>
+        <v>7456</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>5674</v>
+        <v>1733</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>5954</v>
+        <v>7457</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>7370</v>
+        <v>7458</v>
       </c>
       <c r="F21" s="3">
-        <v>45933.507638888885</v>
+        <v>45936.48888888889</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>7371</v>
+        <v>7459</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>7372</v>
+        <v>7460</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>5674</v>
+        <v>1929</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>488</v>
+        <v>7461</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>7373</v>
+        <v>10</v>
       </c>
       <c r="F22" s="3">
-        <v>45933.393055555556</v>
+        <v>45936.59027777778</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>7374</v>
+        <v>7462</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>1549</v>
+        <v>7463</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>5674</v>
+        <v>1929</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>32</v>
+        <v>7464</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>7375</v>
+        <v>10</v>
       </c>
       <c r="F23" s="3">
-        <v>45933.33333333333</v>
+        <v>45936.56458333333</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>7376</v>
+        <v>7465</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>7377</v>
+        <v>2838</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>5674</v>
+        <v>1929</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>1632</v>
+        <v>353</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>7378</v>
+        <v>7466</v>
       </c>
       <c r="F24" s="3">
-        <v>45932.81388888889</v>
+        <v>45936.48125</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>7379</v>
+        <v>7467</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>7380</v>
+        <v>7468</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>5674</v>
+        <v>1929</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>1632</v>
+        <v>7469</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>7378</v>
+        <v>7470</v>
       </c>
       <c r="F25" s="3">
-        <v>45932.8125</v>
+        <v>45935.856944444444</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>7381</v>
+        <v>7471</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>7382</v>
+        <v>2597</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>5674</v>
+        <v>1929</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>7383</v>
+        <v>171</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>7384</v>
+        <v>7472</v>
       </c>
       <c r="F26" s="3">
-        <v>45932.80902777778</v>
+        <v>45935.75277777778</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>7385</v>
+        <v>7473</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>7386</v>
+        <v>7474</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>5674</v>
+        <v>1929</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>2271</v>
+        <v>7475</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>7384</v>
+        <v>10</v>
       </c>
       <c r="F27" s="3">
-        <v>45932.808333333334</v>
+        <v>45934.444444444445</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>7387</v>
+        <v>7476</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>7388</v>
+        <v>4478</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>6133</v>
+        <v>1929</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>7389</v>
+        <v>561</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>7390</v>
+        <v>10</v>
       </c>
       <c r="F28" s="3">
-        <v>45933.60555555555</v>
+        <v>45934.361805555556</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>7391</v>
+        <v>7477</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>7392</v>
+        <v>7478</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>6133</v>
+        <v>1929</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>7393</v>
+        <v>32</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>7394</v>
+        <v>7479</v>
       </c>
       <c r="F29" s="3">
-        <v>45933.46527777778</v>
+        <v>45933.89583333333</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>7395</v>
+        <v>7480</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>7396</v>
+        <v>7481</v>
       </c>
       <c r="C30" s="9" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>7482</v>
+      </c>
+      <c r="F30" s="3">
+        <v>45936.601388888885</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>7483</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>7484</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>7485</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>7486</v>
+      </c>
+      <c r="F31" s="3">
+        <v>45936.47986111111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>7487</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>7488</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>7489</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="3">
+        <v>45936.30138888889</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>7490</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>7065</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="3">
+        <v>45935.535416666666</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>7491</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>7492</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>7493</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="3">
+        <v>45936.57986111111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>7494</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>7495</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>7496</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="3">
+        <v>45936.48333333334</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>7497</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>7498</v>
+      </c>
+      <c r="F36" s="3">
+        <v>45935.63125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>7499</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>7500</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>3868</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>7501</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>7502</v>
+      </c>
+      <c r="F37" s="3">
+        <v>45936.61597222222</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>7503</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>3979</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>3868</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>3980</v>
+      </c>
+      <c r="F38" s="3">
+        <v>45934.44097222222</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>7504</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>7505</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>3868</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>4006</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>7506</v>
+      </c>
+      <c r="F39" s="3">
+        <v>45933.64166666666</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>7507</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>7508</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>1632</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>7509</v>
+      </c>
+      <c r="F40" s="3">
+        <v>45935.94861111111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>7510</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>7511</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>7512</v>
+      </c>
+      <c r="F41" s="3">
+        <v>45935.88958333334</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>7513</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>7514</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>2059</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>7515</v>
+      </c>
+      <c r="F42" s="3">
+        <v>45935.65555555555</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>7516</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>7517</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>1006</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>4353</v>
+      </c>
+      <c r="F43" s="3">
+        <v>45935.648611111115</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>7518</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>7519</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>7520</v>
+      </c>
+      <c r="F44" s="3">
+        <v>45935.34375</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>7521</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>7522</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>7523</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>7524</v>
+      </c>
+      <c r="F45" s="3">
+        <v>45935.33472222222</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>7525</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>7526</v>
+      </c>
+      <c r="F46" s="3">
+        <v>45933.99930555555</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>7527</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>4478</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>7528</v>
+      </c>
+      <c r="F47" s="3">
+        <v>45933.84236111111</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>7529</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>7530</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>7531</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>7532</v>
+      </c>
+      <c r="F48" s="3">
+        <v>45933.836111111115</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>7533</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>7534</v>
+      </c>
+      <c r="F49" s="3">
+        <v>45933.820138888885</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>7535</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>3544</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>7536</v>
+      </c>
+      <c r="F50" s="3">
+        <v>45933.81527777778</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>7537</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>3544</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>7538</v>
+      </c>
+      <c r="F51" s="3">
+        <v>45933.808333333334</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>7539</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>4671</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>7540</v>
+      </c>
+      <c r="F52" s="3">
+        <v>45935.73333333334</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>7541</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>7542</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>4671</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>7543</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F53" s="3">
+        <v>45935.72430555556</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
+        <v>7544</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>7545</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>4671</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>4672</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" s="3">
+        <v>45933.763194444444</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>7546</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>7547</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>7548</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>7549</v>
+      </c>
+      <c r="F55" s="3">
+        <v>45935.73125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>7550</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>7551</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>7552</v>
+      </c>
+      <c r="F56" s="3">
+        <v>45934.85625</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
+        <v>7553</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>7554</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>6532</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>7555</v>
+      </c>
+      <c r="F57" s="3">
+        <v>45934.02986111111</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>7556</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>1943</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>7557</v>
+      </c>
+      <c r="F58" s="3">
+        <v>45933.896527777775</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
+        <v>7558</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>7559</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>3854</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>7560</v>
+      </c>
+      <c r="F59" s="3">
+        <v>45933.65486111111</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
+        <v>7561</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>4926</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>7562</v>
+      </c>
+      <c r="F60" s="3">
+        <v>45933.65416666667</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
+        <v>7563</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>7564</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>7565</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" s="3">
+        <v>45936.492361111115</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
+        <v>7566</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>7567</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>7568</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>7569</v>
+      </c>
+      <c r="F62" s="3">
+        <v>45933.79791666666</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
+        <v>7570</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>7571</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>7572</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>7573</v>
+      </c>
+      <c r="F63" s="3">
+        <v>45935.52083333333</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
+        <v>7574</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>7575</v>
+      </c>
+      <c r="C64" s="9" t="s">
         <v>6207</v>
       </c>
-      <c r="D30" s="9" t="s">
-        <v>7089</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>7397</v>
-      </c>
-      <c r="F30" s="3">
-        <v>45932.88611111111</v>
+      <c r="D64" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F64" s="3">
+        <v>45936.53958333333</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
+        <v>7576</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>7577</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F65" s="3">
+        <v>45934.54305555555</v>
       </c>
     </row>
   </sheetData>
@@ -23295,6 +24535,41 @@
     <hyperlink ref="A28" r:id="rId27"/>
     <hyperlink ref="A29" r:id="rId28"/>
     <hyperlink ref="A30" r:id="rId29"/>
+    <hyperlink ref="A31" r:id="rId30"/>
+    <hyperlink ref="A32" r:id="rId31"/>
+    <hyperlink ref="A33" r:id="rId32"/>
+    <hyperlink ref="A34" r:id="rId33"/>
+    <hyperlink ref="A35" r:id="rId34"/>
+    <hyperlink ref="A36" r:id="rId35"/>
+    <hyperlink ref="A37" r:id="rId36"/>
+    <hyperlink ref="A38" r:id="rId37"/>
+    <hyperlink ref="A39" r:id="rId38"/>
+    <hyperlink ref="A40" r:id="rId39"/>
+    <hyperlink ref="A41" r:id="rId40"/>
+    <hyperlink ref="A42" r:id="rId41"/>
+    <hyperlink ref="A43" r:id="rId42"/>
+    <hyperlink ref="A44" r:id="rId43"/>
+    <hyperlink ref="A45" r:id="rId44"/>
+    <hyperlink ref="A46" r:id="rId45"/>
+    <hyperlink ref="A47" r:id="rId46"/>
+    <hyperlink ref="A48" r:id="rId47"/>
+    <hyperlink ref="A49" r:id="rId48"/>
+    <hyperlink ref="A50" r:id="rId49"/>
+    <hyperlink ref="A51" r:id="rId50"/>
+    <hyperlink ref="A52" r:id="rId51"/>
+    <hyperlink ref="A53" r:id="rId52"/>
+    <hyperlink ref="A54" r:id="rId53"/>
+    <hyperlink ref="A55" r:id="rId54"/>
+    <hyperlink ref="A56" r:id="rId55"/>
+    <hyperlink ref="A57" r:id="rId56"/>
+    <hyperlink ref="A58" r:id="rId57"/>
+    <hyperlink ref="A59" r:id="rId58"/>
+    <hyperlink ref="A60" r:id="rId59"/>
+    <hyperlink ref="A61" r:id="rId60"/>
+    <hyperlink ref="A62" r:id="rId61"/>
+    <hyperlink ref="A63" r:id="rId62"/>
+    <hyperlink ref="A64" r:id="rId63"/>
+    <hyperlink ref="A65" r:id="rId64"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -23303,7 +24578,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2354"/>
+  <dimension ref="A1:F2383"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -70399,6 +71674,586 @@
       </c>
       <c r="F2354" s="3">
         <v>45931.69236111111</v>
+      </c>
+    </row>
+    <row r="2355" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2355" s="4" t="s">
+        <v>7318</v>
+      </c>
+      <c r="B2355" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2355" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2355" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2355" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2355" s="3">
+        <v>45932.90763888889</v>
+      </c>
+    </row>
+    <row r="2356" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2356" s="4" t="s">
+        <v>7319</v>
+      </c>
+      <c r="B2356" s="3" t="s">
+        <v>7320</v>
+      </c>
+      <c r="C2356" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2356" s="3" t="s">
+        <v>3346</v>
+      </c>
+      <c r="E2356" s="3" t="s">
+        <v>7321</v>
+      </c>
+      <c r="F2356" s="3">
+        <v>45932.80416666667</v>
+      </c>
+    </row>
+    <row r="2357" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2357" s="4" t="s">
+        <v>7322</v>
+      </c>
+      <c r="B2357" s="3" t="s">
+        <v>7323</v>
+      </c>
+      <c r="C2357" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2357" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="E2357" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2357" s="3">
+        <v>45932.64583333333</v>
+      </c>
+    </row>
+    <row r="2358" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2358" s="4" t="s">
+        <v>7324</v>
+      </c>
+      <c r="B2358" s="3" t="s">
+        <v>7325</v>
+      </c>
+      <c r="C2358" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2358" s="3" t="s">
+        <v>7326</v>
+      </c>
+      <c r="E2358" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2358" s="3">
+        <v>45933.44583333333</v>
+      </c>
+    </row>
+    <row r="2359" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2359" s="4" t="s">
+        <v>7327</v>
+      </c>
+      <c r="B2359" s="3" t="s">
+        <v>7328</v>
+      </c>
+      <c r="C2359" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2359" s="3" t="s">
+        <v>7329</v>
+      </c>
+      <c r="E2359" s="3" t="s">
+        <v>7330</v>
+      </c>
+      <c r="F2359" s="3">
+        <v>45933.45416666666</v>
+      </c>
+    </row>
+    <row r="2360" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2360" s="4" t="s">
+        <v>7331</v>
+      </c>
+      <c r="B2360" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="C2360" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2360" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2360" s="3" t="s">
+        <v>7332</v>
+      </c>
+      <c r="F2360" s="3">
+        <v>45933.33333333333</v>
+      </c>
+    </row>
+    <row r="2361" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2361" s="4" t="s">
+        <v>7333</v>
+      </c>
+      <c r="B2361" s="3" t="s">
+        <v>7334</v>
+      </c>
+      <c r="C2361" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2361" s="3" t="s">
+        <v>7335</v>
+      </c>
+      <c r="E2361" s="3" t="s">
+        <v>7336</v>
+      </c>
+      <c r="F2361" s="3">
+        <v>45932.70833333333</v>
+      </c>
+    </row>
+    <row r="2362" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2362" s="4" t="s">
+        <v>7337</v>
+      </c>
+      <c r="B2362" s="3" t="s">
+        <v>7338</v>
+      </c>
+      <c r="C2362" s="3" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D2362" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="E2362" s="3" t="s">
+        <v>7339</v>
+      </c>
+      <c r="F2362" s="3">
+        <v>45932.70347222222</v>
+      </c>
+    </row>
+    <row r="2363" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2363" s="4" t="s">
+        <v>7340</v>
+      </c>
+      <c r="B2363" s="3" t="s">
+        <v>7341</v>
+      </c>
+      <c r="C2363" s="3" t="s">
+        <v>1733</v>
+      </c>
+      <c r="D2363" s="3" t="s">
+        <v>7342</v>
+      </c>
+      <c r="E2363" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2363" s="3">
+        <v>45933.399305555555</v>
+      </c>
+    </row>
+    <row r="2364" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2364" s="4" t="s">
+        <v>7343</v>
+      </c>
+      <c r="B2364" s="3" t="s">
+        <v>4083</v>
+      </c>
+      <c r="C2364" s="3" t="s">
+        <v>2671</v>
+      </c>
+      <c r="D2364" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2364" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2364" s="3">
+        <v>45932.95763888889</v>
+      </c>
+    </row>
+    <row r="2365" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2365" s="4" t="s">
+        <v>7344</v>
+      </c>
+      <c r="B2365" s="3" t="s">
+        <v>7345</v>
+      </c>
+      <c r="C2365" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2365" s="3" t="s">
+        <v>4365</v>
+      </c>
+      <c r="E2365" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2365" s="3">
+        <v>45933.56875</v>
+      </c>
+    </row>
+    <row r="2366" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2366" s="4" t="s">
+        <v>7346</v>
+      </c>
+      <c r="B2366" s="3" t="s">
+        <v>7347</v>
+      </c>
+      <c r="C2366" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2366" s="3" t="s">
+        <v>7348</v>
+      </c>
+      <c r="E2366" s="3" t="s">
+        <v>7349</v>
+      </c>
+      <c r="F2366" s="3">
+        <v>45932.71319444444</v>
+      </c>
+    </row>
+    <row r="2367" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2367" s="4" t="s">
+        <v>7350</v>
+      </c>
+      <c r="B2367" s="3" t="s">
+        <v>7351</v>
+      </c>
+      <c r="C2367" s="3" t="s">
+        <v>3868</v>
+      </c>
+      <c r="D2367" s="3" t="s">
+        <v>2707</v>
+      </c>
+      <c r="E2367" s="3" t="s">
+        <v>7352</v>
+      </c>
+      <c r="F2367" s="3">
+        <v>45933.631944444445</v>
+      </c>
+    </row>
+    <row r="2368" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2368" s="4" t="s">
+        <v>7353</v>
+      </c>
+      <c r="B2368" s="3" t="s">
+        <v>7354</v>
+      </c>
+      <c r="C2368" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2368" s="3" t="s">
+        <v>1430</v>
+      </c>
+      <c r="E2368" s="3" t="s">
+        <v>7355</v>
+      </c>
+      <c r="F2368" s="3">
+        <v>45933.509722222225</v>
+      </c>
+    </row>
+    <row r="2369" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2369" s="4" t="s">
+        <v>7356</v>
+      </c>
+      <c r="B2369" s="3" t="s">
+        <v>4426</v>
+      </c>
+      <c r="C2369" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2369" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2369" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2369" s="3">
+        <v>45932.711111111115</v>
+      </c>
+    </row>
+    <row r="2370" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2370" s="4" t="s">
+        <v>7357</v>
+      </c>
+      <c r="B2370" s="3" t="s">
+        <v>7358</v>
+      </c>
+      <c r="C2370" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2370" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2370" s="3" t="s">
+        <v>7359</v>
+      </c>
+      <c r="F2370" s="3">
+        <v>45933.51041666667</v>
+      </c>
+    </row>
+    <row r="2371" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2371" s="4" t="s">
+        <v>7360</v>
+      </c>
+      <c r="B2371" s="3" t="s">
+        <v>7361</v>
+      </c>
+      <c r="C2371" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2371" s="3" t="s">
+        <v>7362</v>
+      </c>
+      <c r="E2371" s="3" t="s">
+        <v>7363</v>
+      </c>
+      <c r="F2371" s="3">
+        <v>45933.51041666667</v>
+      </c>
+    </row>
+    <row r="2372" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2372" s="4" t="s">
+        <v>7364</v>
+      </c>
+      <c r="B2372" s="3" t="s">
+        <v>7365</v>
+      </c>
+      <c r="C2372" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2372" s="3" t="s">
+        <v>2847</v>
+      </c>
+      <c r="E2372" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2372" s="3">
+        <v>45932.81319444445</v>
+      </c>
+    </row>
+    <row r="2373" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2373" s="4" t="s">
+        <v>7366</v>
+      </c>
+      <c r="B2373" s="3" t="s">
+        <v>7367</v>
+      </c>
+      <c r="C2373" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2373" s="3" t="s">
+        <v>1259</v>
+      </c>
+      <c r="E2373" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2373" s="3">
+        <v>45932.725</v>
+      </c>
+    </row>
+    <row r="2374" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2374" s="4" t="s">
+        <v>7368</v>
+      </c>
+      <c r="B2374" s="3" t="s">
+        <v>7369</v>
+      </c>
+      <c r="C2374" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2374" s="3" t="s">
+        <v>5954</v>
+      </c>
+      <c r="E2374" s="3" t="s">
+        <v>7370</v>
+      </c>
+      <c r="F2374" s="3">
+        <v>45933.507638888885</v>
+      </c>
+    </row>
+    <row r="2375" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2375" s="4" t="s">
+        <v>7371</v>
+      </c>
+      <c r="B2375" s="3" t="s">
+        <v>7372</v>
+      </c>
+      <c r="C2375" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2375" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="E2375" s="3" t="s">
+        <v>7373</v>
+      </c>
+      <c r="F2375" s="3">
+        <v>45933.393055555556</v>
+      </c>
+    </row>
+    <row r="2376" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2376" s="4" t="s">
+        <v>7374</v>
+      </c>
+      <c r="B2376" s="3" t="s">
+        <v>1549</v>
+      </c>
+      <c r="C2376" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2376" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2376" s="3" t="s">
+        <v>7375</v>
+      </c>
+      <c r="F2376" s="3">
+        <v>45933.33333333333</v>
+      </c>
+    </row>
+    <row r="2377" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2377" s="4" t="s">
+        <v>7376</v>
+      </c>
+      <c r="B2377" s="3" t="s">
+        <v>7377</v>
+      </c>
+      <c r="C2377" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2377" s="3" t="s">
+        <v>1632</v>
+      </c>
+      <c r="E2377" s="3" t="s">
+        <v>7378</v>
+      </c>
+      <c r="F2377" s="3">
+        <v>45932.81388888889</v>
+      </c>
+    </row>
+    <row r="2378" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2378" s="4" t="s">
+        <v>7379</v>
+      </c>
+      <c r="B2378" s="3" t="s">
+        <v>7380</v>
+      </c>
+      <c r="C2378" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2378" s="3" t="s">
+        <v>1632</v>
+      </c>
+      <c r="E2378" s="3" t="s">
+        <v>7378</v>
+      </c>
+      <c r="F2378" s="3">
+        <v>45932.8125</v>
+      </c>
+    </row>
+    <row r="2379" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2379" s="4" t="s">
+        <v>7381</v>
+      </c>
+      <c r="B2379" s="3" t="s">
+        <v>7382</v>
+      </c>
+      <c r="C2379" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2379" s="3" t="s">
+        <v>7383</v>
+      </c>
+      <c r="E2379" s="3" t="s">
+        <v>7384</v>
+      </c>
+      <c r="F2379" s="3">
+        <v>45932.80902777778</v>
+      </c>
+    </row>
+    <row r="2380" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2380" s="4" t="s">
+        <v>7385</v>
+      </c>
+      <c r="B2380" s="3" t="s">
+        <v>7386</v>
+      </c>
+      <c r="C2380" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2380" s="3" t="s">
+        <v>2271</v>
+      </c>
+      <c r="E2380" s="3" t="s">
+        <v>7384</v>
+      </c>
+      <c r="F2380" s="3">
+        <v>45932.808333333334</v>
+      </c>
+    </row>
+    <row r="2381" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2381" s="4" t="s">
+        <v>7387</v>
+      </c>
+      <c r="B2381" s="3" t="s">
+        <v>7388</v>
+      </c>
+      <c r="C2381" s="3" t="s">
+        <v>6133</v>
+      </c>
+      <c r="D2381" s="3" t="s">
+        <v>7389</v>
+      </c>
+      <c r="E2381" s="3" t="s">
+        <v>7390</v>
+      </c>
+      <c r="F2381" s="3">
+        <v>45933.60555555555</v>
+      </c>
+    </row>
+    <row r="2382" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2382" s="4" t="s">
+        <v>7391</v>
+      </c>
+      <c r="B2382" s="3" t="s">
+        <v>7392</v>
+      </c>
+      <c r="C2382" s="3" t="s">
+        <v>6133</v>
+      </c>
+      <c r="D2382" s="3" t="s">
+        <v>7393</v>
+      </c>
+      <c r="E2382" s="3" t="s">
+        <v>7394</v>
+      </c>
+      <c r="F2382" s="3">
+        <v>45933.46527777778</v>
+      </c>
+    </row>
+    <row r="2383" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2383" s="4" t="s">
+        <v>7395</v>
+      </c>
+      <c r="B2383" s="3" t="s">
+        <v>7396</v>
+      </c>
+      <c r="C2383" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2383" s="3" t="s">
+        <v>7089</v>
+      </c>
+      <c r="E2383" s="3" t="s">
+        <v>7397</v>
+      </c>
+      <c r="F2383" s="3">
+        <v>45932.88611111111</v>
       </c>
     </row>
   </sheetData>
@@ -72756,6 +74611,35 @@
     <hyperlink ref="A2352" r:id="rId2351"/>
     <hyperlink ref="A2353" r:id="rId2352"/>
     <hyperlink ref="A2354" r:id="rId2353"/>
+    <hyperlink ref="A2355" r:id="rId2354"/>
+    <hyperlink ref="A2356" r:id="rId2355"/>
+    <hyperlink ref="A2357" r:id="rId2356"/>
+    <hyperlink ref="A2358" r:id="rId2357"/>
+    <hyperlink ref="A2359" r:id="rId2358"/>
+    <hyperlink ref="A2360" r:id="rId2359"/>
+    <hyperlink ref="A2361" r:id="rId2360"/>
+    <hyperlink ref="A2362" r:id="rId2361"/>
+    <hyperlink ref="A2363" r:id="rId2362"/>
+    <hyperlink ref="A2364" r:id="rId2363"/>
+    <hyperlink ref="A2365" r:id="rId2364"/>
+    <hyperlink ref="A2366" r:id="rId2365"/>
+    <hyperlink ref="A2367" r:id="rId2366"/>
+    <hyperlink ref="A2368" r:id="rId2367"/>
+    <hyperlink ref="A2369" r:id="rId2368"/>
+    <hyperlink ref="A2370" r:id="rId2369"/>
+    <hyperlink ref="A2371" r:id="rId2370"/>
+    <hyperlink ref="A2372" r:id="rId2371"/>
+    <hyperlink ref="A2373" r:id="rId2372"/>
+    <hyperlink ref="A2374" r:id="rId2373"/>
+    <hyperlink ref="A2375" r:id="rId2374"/>
+    <hyperlink ref="A2376" r:id="rId2375"/>
+    <hyperlink ref="A2377" r:id="rId2376"/>
+    <hyperlink ref="A2378" r:id="rId2377"/>
+    <hyperlink ref="A2379" r:id="rId2378"/>
+    <hyperlink ref="A2380" r:id="rId2379"/>
+    <hyperlink ref="A2381" r:id="rId2380"/>
+    <hyperlink ref="A2382" r:id="rId2381"/>
+    <hyperlink ref="A2383" r:id="rId2382"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Update lands data - 2025-10-07 12:21
</commit_message>
<xml_diff>
--- a/lands-scraped.xlsx
+++ b/lands-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12242" uniqueCount="7578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12432" uniqueCount="7681">
   <si>
     <t>link</t>
   </si>
@@ -22752,6 +22752,315 @@
   </si>
   <si>
     <t>15 000 € (0.75 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/islices-pag/hcjlc.html</t>
+  </si>
+  <si>
+    <t>51 000 € (1.58 €/m²)</t>
+  </si>
+  <si>
+    <t>3.23 ha.</t>
+  </si>
+  <si>
+    <t>40680070034</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/iecavas-nov/aicgg.html</t>
+  </si>
+  <si>
+    <t>237 000 € (3.95 €/m²)</t>
+  </si>
+  <si>
+    <t>40640080089</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/vecsalienas-pag/mcnio.html</t>
+  </si>
+  <si>
+    <t>24 000 € (0.20 €/m²)</t>
+  </si>
+  <si>
+    <t>44960070002</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/medumu-pag/lxgbk.html</t>
+  </si>
+  <si>
+    <t>1 800 € (0.06 €/m²)</t>
+  </si>
+  <si>
+    <t>44720050224</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/daugavpils/afpok.html</t>
+  </si>
+  <si>
+    <t>15 500 € (10.33 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/naujenes-pag/kchge.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/daugavpils/goljo.html</t>
+  </si>
+  <si>
+    <t>8 000 € (26.06 €/m²)</t>
+  </si>
+  <si>
+    <t>307 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/dobele-and-reg/dobeles-pag/aibmk.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jekabpils-and-reg/vipes-pag/cggdnx.html</t>
+  </si>
+  <si>
+    <t>5696 005 0120</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/valgundes-nov/efdhb.html</t>
+  </si>
+  <si>
+    <t>16 500 € (3.30 €/m²)</t>
+  </si>
+  <si>
+    <t>54860030080</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jelgava/beopb.html</t>
+  </si>
+  <si>
+    <t>27 840 € (20 €/m²)</t>
+  </si>
+  <si>
+    <t>1392 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kraslava-and-reg/skaunes-pag/cfdnid.html</t>
+  </si>
+  <si>
+    <t>14 500 € (0.21 €/m²)</t>
+  </si>
+  <si>
+    <t>60920010147</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kuldiga-and-reg/kuldiga/ageif.html</t>
+  </si>
+  <si>
+    <t>11 000 € (5.50 €/m²)</t>
+  </si>
+  <si>
+    <t>62840050295</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kuldiga-and-reg/kuldiga/enijc.html</t>
+  </si>
+  <si>
+    <t>10 000 € (15.13 €/m²)</t>
+  </si>
+  <si>
+    <t>661 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/limbadzi-and-reg/skultes-pag/agfxd.html</t>
+  </si>
+  <si>
+    <t>55 000 € (3.82 €/m²)</t>
+  </si>
+  <si>
+    <t>1.44 ha.</t>
+  </si>
+  <si>
+    <t>66760134758</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ludza-and-reg/ciblas-pag/gixnm.html</t>
+  </si>
+  <si>
+    <t>71 000 € (0.34 €/m²)</t>
+  </si>
+  <si>
+    <t>208000 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/madona-and-reg/praulienas-pag/hmnxh.html</t>
+  </si>
+  <si>
+    <t>39 000 € (0.28 €/m²)</t>
+  </si>
+  <si>
+    <t>70860140243</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/keipenes-pag/ajnxe.html</t>
+  </si>
+  <si>
+    <t>49 500 € (0.99 €/m²)</t>
+  </si>
+  <si>
+    <t>74560070027</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/keipenes-pag/abpgm.html</t>
+  </si>
+  <si>
+    <t>74560050188</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ogresgala-pag/nkhox.html</t>
+  </si>
+  <si>
+    <t>22 000 € (16.20 €/m²)</t>
+  </si>
+  <si>
+    <t>74800040205</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ogresgala-pag/akcxf.html</t>
+  </si>
+  <si>
+    <t>18 000 € (15 €/m²)</t>
+  </si>
+  <si>
+    <t>74800040105</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ogre/ahjmh.html</t>
+  </si>
+  <si>
+    <t>28 000 € (12.96 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ikskiles-l-t/cckof.html</t>
+  </si>
+  <si>
+    <t>16 000 € (3.02 €/m²)</t>
+  </si>
+  <si>
+    <t>5300 m²</t>
+  </si>
+  <si>
+    <t>74940040237</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ledmanes-pag/afohp.html</t>
+  </si>
+  <si>
+    <t>74640060326</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/rojas-pag/ekgof.html</t>
+  </si>
+  <si>
+    <t>42 000 € (15 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/dundagas-pag/cgxpfd.html</t>
+  </si>
+  <si>
+    <t>95 000 € (0.30 €/m²)</t>
+  </si>
+  <si>
+    <t>88500180110</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/dundagas-pag/cggdlh.html</t>
+  </si>
+  <si>
+    <t>88500170119</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/dundagas-pag/cgxpfc.html</t>
+  </si>
+  <si>
+    <t>69 500 € (0.37 €/m²)</t>
+  </si>
+  <si>
+    <t>88500270070</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/lapmezciema-nov/eglnp.html</t>
+  </si>
+  <si>
+    <t>79 900 € (20.13 €/m²)</t>
+  </si>
+  <si>
+    <t>90660040397</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/semes-pag/fjdeo.html</t>
+  </si>
+  <si>
+    <t>80 800 € (0.80 €/m²)</t>
+  </si>
+  <si>
+    <t>90780010052</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/tukums/ajjxb.html</t>
+  </si>
+  <si>
+    <t>38 000 € (18.25 €/m²)</t>
+  </si>
+  <si>
+    <t>2082 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valka-and-reg/smiltenes-pag/khxed.html</t>
+  </si>
+  <si>
+    <t>94800040025</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valka-and-reg/smiltenes-pag/meicj.html</t>
+  </si>
+  <si>
+    <t>9 990 € (8.53 €/m²)</t>
+  </si>
+  <si>
+    <t>1171 m²</t>
+  </si>
+  <si>
+    <t>94800050382</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/kocenu-pag/coemb.html</t>
+  </si>
+  <si>
+    <t>34 000 € (8.10 €/m²)</t>
+  </si>
+  <si>
+    <t>4200 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/valmieras-pag/cgcdjp.html</t>
+  </si>
+  <si>
+    <t>32 500 € (0.54 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/valmieras-pag/cgcdkx.html</t>
+  </si>
+  <si>
+    <t>66 000 € (0.51 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/usmas-pag/adphx.html</t>
+  </si>
+  <si>
+    <t>205 000 € (6.61 €/m²)</t>
+  </si>
+  <si>
+    <t>98740040028</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/jurkalnes-pag/acenh.html</t>
+  </si>
+  <si>
+    <t>48 000 € (2.40 €/m²)</t>
   </si>
 </sst>
 </file>
@@ -23187,7 +23496,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -23226,1282 +23535,762 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>7398</v>
+        <v>7578</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>7399</v>
+        <v>7579</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>8</v>
+        <v>419</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>1984</v>
+        <v>7580</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>7400</v>
+        <v>7581</v>
       </c>
       <c r="F2" s="3">
-        <v>45935.52569444444</v>
+        <v>45937.424305555556</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>7401</v>
+        <v>7582</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>7402</v>
+        <v>7583</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>8</v>
+        <v>419</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>2284</v>
+        <v>383</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>7403</v>
+        <v>7584</v>
       </c>
       <c r="F3" s="3">
-        <v>45933.65902777778</v>
+        <v>45936.96527777778</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>7404</v>
+        <v>7585</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>7405</v>
+        <v>7586</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>419</v>
+        <v>1218</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>6208</v>
+        <v>146</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>7406</v>
+        <v>7587</v>
       </c>
       <c r="F4" s="3">
-        <v>45935.73055555555</v>
+        <v>45937.63611111111</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>7407</v>
+        <v>7588</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>7408</v>
+        <v>7589</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>419</v>
+        <v>1218</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>536</v>
+        <v>201</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>537</v>
+        <v>7590</v>
       </c>
       <c r="F5" s="3">
-        <v>45935.49791666667</v>
+        <v>45937.63055555556</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>7409</v>
+        <v>7591</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>7410</v>
+        <v>7592</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>419</v>
+        <v>1218</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>1430</v>
+        <v>985</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>7411</v>
+        <v>10</v>
       </c>
       <c r="F6" s="3">
-        <v>45935.481944444444</v>
+        <v>45937.51666666666</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>7412</v>
+        <v>7593</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>7413</v>
+        <v>2609</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>419</v>
+        <v>1218</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>77</v>
+        <v>407</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>7414</v>
+        <v>10</v>
       </c>
       <c r="F7" s="3">
-        <v>45935.475</v>
+        <v>45936.8375</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>7415</v>
+        <v>7594</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>7416</v>
+        <v>7595</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>419</v>
+        <v>1218</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>7417</v>
+        <v>7596</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>7418</v>
+        <v>10</v>
       </c>
       <c r="F8" s="3">
-        <v>45935.46736111111</v>
+        <v>45936.67152777778</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>7419</v>
+        <v>7597</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>7420</v>
+        <v>1183</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>419</v>
+        <v>1569</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>7421</v>
+        <v>171</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>7422</v>
+        <v>10</v>
       </c>
       <c r="F9" s="3">
-        <v>45935.46319444444</v>
+        <v>45937.41180555556</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>7423</v>
+        <v>7598</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>7424</v>
+        <v>7453</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>419</v>
+        <v>1733</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>77</v>
+        <v>353</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>7425</v>
+        <v>7599</v>
       </c>
       <c r="F10" s="3">
-        <v>45935.45694444445</v>
+        <v>45936.86041666666</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>7426</v>
+        <v>7600</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>7427</v>
+        <v>7601</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>419</v>
+        <v>1929</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>7428</v>
+        <v>7602</v>
       </c>
       <c r="F11" s="3">
-        <v>45934.58263888889</v>
+        <v>45937.58333333333</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>7429</v>
+        <v>7603</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>7430</v>
+        <v>7604</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>419</v>
+        <v>1929</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>4468</v>
+        <v>7605</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>7431</v>
+        <v>10</v>
       </c>
       <c r="F12" s="3">
-        <v>45933.86319444445</v>
+        <v>45937.535416666666</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>7432</v>
+        <v>7606</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>7433</v>
+        <v>7607</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>419</v>
+        <v>2488</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>7434</v>
+        <v>407</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>7435</v>
+        <v>7608</v>
       </c>
       <c r="F13" s="3">
-        <v>45933.756944444445</v>
+        <v>45937.63402777778</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>7436</v>
+        <v>7609</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>7437</v>
+        <v>7610</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>772</v>
+        <v>2671</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>7438</v>
+        <v>317</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>7439</v>
+        <v>7611</v>
       </c>
       <c r="F14" s="3">
-        <v>45934.7125</v>
+        <v>45937.56527777778</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>7440</v>
+        <v>7612</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>7441</v>
+        <v>7613</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>772</v>
+        <v>2671</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>7442</v>
+        <v>7614</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>870</v>
+        <v>10</v>
       </c>
       <c r="F15" s="3">
-        <v>45934.5125</v>
+        <v>45937.507638888885</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>7443</v>
+        <v>7615</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>7444</v>
+        <v>7616</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>772</v>
+        <v>3398</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>7445</v>
+        <v>7617</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>10</v>
+        <v>7618</v>
       </c>
       <c r="F16" s="3">
-        <v>45934.464583333334</v>
+        <v>45937.52986111111</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>7446</v>
+        <v>7619</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>7447</v>
+        <v>7620</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>772</v>
+        <v>3762</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>1112</v>
+        <v>7621</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>1113</v>
+        <v>10</v>
       </c>
       <c r="F17" s="3">
-        <v>45934.41875</v>
+        <v>45937.61458333333</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>7448</v>
+        <v>7622</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>7449</v>
+        <v>7623</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>1218</v>
+        <v>3868</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>1156</v>
+        <v>181</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>7450</v>
+        <v>7624</v>
       </c>
       <c r="F18" s="3">
-        <v>45933.66180555556</v>
+        <v>45937.63402777778</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>7451</v>
+        <v>7625</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>830</v>
+        <v>7626</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>1569</v>
+        <v>4034</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>353</v>
+        <v>77</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>10</v>
+        <v>7627</v>
       </c>
       <c r="F19" s="3">
-        <v>45936.59166666667</v>
+        <v>45937.63680555555</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>7452</v>
+        <v>7628</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>7453</v>
+        <v>2510</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>1733</v>
+        <v>4034</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>353</v>
+        <v>383</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>7454</v>
+        <v>7629</v>
       </c>
       <c r="F20" s="3">
-        <v>45936.59027777778</v>
+        <v>45937.63680555555</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>7455</v>
+        <v>7630</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>7456</v>
+        <v>7631</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>1733</v>
+        <v>4034</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>7457</v>
+        <v>442</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>7458</v>
+        <v>7632</v>
       </c>
       <c r="F21" s="3">
-        <v>45936.48888888889</v>
+        <v>45936.990277777775</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>7459</v>
+        <v>7633</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>7460</v>
+        <v>7634</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>1929</v>
+        <v>4034</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>7461</v>
+        <v>436</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>10</v>
+        <v>7635</v>
       </c>
       <c r="F22" s="3">
-        <v>45936.59027777778</v>
+        <v>45936.805555555555</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>7462</v>
+        <v>7636</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>7463</v>
+        <v>7637</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>1929</v>
+        <v>4034</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>7464</v>
+        <v>2723</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F23" s="3">
-        <v>45936.56458333333</v>
+        <v>45936.75486111111</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>7465</v>
+        <v>7638</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>2838</v>
+        <v>7639</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>1929</v>
+        <v>4034</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>353</v>
+        <v>7640</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>7466</v>
+        <v>7641</v>
       </c>
       <c r="F24" s="3">
-        <v>45936.48125</v>
+        <v>45936.69027777778</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>7467</v>
+        <v>7642</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>7468</v>
+        <v>471</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>1929</v>
+        <v>4034</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>7469</v>
+        <v>32</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>7470</v>
+        <v>7643</v>
       </c>
       <c r="F25" s="3">
-        <v>45935.856944444444</v>
+        <v>45936.67222222222</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>7471</v>
+        <v>7644</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>2597</v>
+        <v>7645</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>1929</v>
+        <v>5266</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>171</v>
+        <v>1651</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>7472</v>
+        <v>10</v>
       </c>
       <c r="F26" s="3">
-        <v>45935.75277777778</v>
+        <v>45937.57152777778</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>7473</v>
+        <v>7646</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>7474</v>
+        <v>7647</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>1929</v>
+        <v>5266</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>7475</v>
+        <v>1724</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>10</v>
+        <v>7648</v>
       </c>
       <c r="F27" s="3">
-        <v>45934.444444444445</v>
+        <v>45936.72986111111</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>7476</v>
+        <v>7649</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>4478</v>
+        <v>4954</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>1929</v>
+        <v>5266</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>561</v>
+        <v>407</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>10</v>
+        <v>7650</v>
       </c>
       <c r="F28" s="3">
-        <v>45934.361805555556</v>
+        <v>45936.72777777778</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>7477</v>
+        <v>7651</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>7478</v>
+        <v>7652</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>1929</v>
+        <v>5266</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>32</v>
+        <v>1156</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>7479</v>
+        <v>7653</v>
       </c>
       <c r="F29" s="3">
-        <v>45933.89583333333</v>
+        <v>45936.70625</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>7480</v>
+        <v>7654</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>7481</v>
+        <v>7655</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>2846</v>
+        <v>5674</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>325</v>
+        <v>6086</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>7482</v>
+        <v>7656</v>
       </c>
       <c r="F30" s="3">
-        <v>45936.601388888885</v>
+        <v>45937.425</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>7483</v>
+        <v>7657</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>7484</v>
+        <v>7658</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>2846</v>
+        <v>5674</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>7485</v>
+        <v>4888</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>7486</v>
+        <v>7659</v>
       </c>
       <c r="F31" s="3">
-        <v>45936.47986111111</v>
+        <v>45937.36041666666</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>7487</v>
+        <v>7660</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>7488</v>
+        <v>7661</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>2846</v>
+        <v>5674</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>7489</v>
+        <v>7662</v>
       </c>
       <c r="E32" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F32" s="3">
-        <v>45936.30138888889</v>
+        <v>45936.69305555556</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>7490</v>
+        <v>7663</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>7065</v>
+        <v>1387</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>2846</v>
+        <v>6133</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>32</v>
+        <v>353</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>10</v>
+        <v>7664</v>
       </c>
       <c r="F33" s="3">
-        <v>45935.535416666666</v>
+        <v>45937.632638888885</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>7491</v>
+        <v>7665</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>7492</v>
+        <v>7666</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>3398</v>
+        <v>6133</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>7493</v>
+        <v>7667</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>10</v>
+        <v>7668</v>
       </c>
       <c r="F34" s="3">
-        <v>45936.57986111111</v>
+        <v>45936.77986111111</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>7494</v>
+        <v>7669</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>7495</v>
+        <v>7670</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>3398</v>
+        <v>6207</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>7496</v>
+        <v>7671</v>
       </c>
       <c r="E35" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F35" s="3">
-        <v>45936.48333333334</v>
+        <v>45937.4875</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>7497</v>
+        <v>7672</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>1294</v>
+        <v>7673</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>3398</v>
+        <v>6207</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>205</v>
+        <v>383</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>7498</v>
+        <v>10</v>
       </c>
       <c r="F36" s="3">
-        <v>45935.63125</v>
+        <v>45936.70277777778</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>7499</v>
+        <v>7674</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>7500</v>
+        <v>7675</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>3868</v>
+        <v>6207</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>7501</v>
+        <v>474</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>7502</v>
+        <v>10</v>
       </c>
       <c r="F37" s="3">
-        <v>45936.61597222222</v>
+        <v>45936.70208333334</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>7503</v>
+        <v>7676</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>3979</v>
+        <v>7677</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>3868</v>
+        <v>6439</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>383</v>
+        <v>4546</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>3980</v>
+        <v>7678</v>
       </c>
       <c r="F38" s="3">
-        <v>45934.44097222222</v>
+        <v>45937.46597222222</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>7504</v>
+        <v>7679</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>7505</v>
+        <v>7680</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>3868</v>
+        <v>6439</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>4006</v>
+        <v>171</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>7506</v>
+        <v>10</v>
       </c>
       <c r="F39" s="3">
-        <v>45933.64166666666</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>7507</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>7508</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>1632</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>7509</v>
-      </c>
-      <c r="F40" s="3">
-        <v>45935.94861111111</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>7510</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>7511</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>7512</v>
-      </c>
-      <c r="F41" s="3">
-        <v>45935.88958333334</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
-        <v>7513</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>7514</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>2059</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>7515</v>
-      </c>
-      <c r="F42" s="3">
-        <v>45935.65555555555</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
-        <v>7516</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>7517</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>1006</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>4353</v>
-      </c>
-      <c r="F43" s="3">
-        <v>45935.648611111115</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
-        <v>7518</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>7519</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>7520</v>
-      </c>
-      <c r="F44" s="3">
-        <v>45935.34375</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
-        <v>7521</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>7522</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>7523</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>7524</v>
-      </c>
-      <c r="F45" s="3">
-        <v>45935.33472222222</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
-        <v>7525</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>471</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>7526</v>
-      </c>
-      <c r="F46" s="3">
-        <v>45933.99930555555</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
-        <v>7527</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>4478</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>7528</v>
-      </c>
-      <c r="F47" s="3">
-        <v>45933.84236111111</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
-        <v>7529</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>7530</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>7531</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>7532</v>
-      </c>
-      <c r="F48" s="3">
-        <v>45933.836111111115</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
-        <v>7533</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>7534</v>
-      </c>
-      <c r="F49" s="3">
-        <v>45933.820138888885</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
-        <v>7535</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>3544</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>7536</v>
-      </c>
-      <c r="F50" s="3">
-        <v>45933.81527777778</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
-        <v>7537</v>
-      </c>
-      <c r="B51" s="9" t="s">
-        <v>3544</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>7538</v>
-      </c>
-      <c r="F51" s="3">
-        <v>45933.808333333334</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
-        <v>7539</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>1100</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>4671</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>7540</v>
-      </c>
-      <c r="F52" s="3">
-        <v>45935.73333333334</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
-        <v>7541</v>
-      </c>
-      <c r="B53" s="9" t="s">
-        <v>7542</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>4671</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>7543</v>
-      </c>
-      <c r="E53" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F53" s="3">
-        <v>45935.72430555556</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="8" t="s">
-        <v>7544</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>7545</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>4671</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>4672</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F54" s="3">
-        <v>45933.763194444444</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
-        <v>7546</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>7547</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>4770</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>7548</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>7549</v>
-      </c>
-      <c r="F55" s="3">
-        <v>45935.73125</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
-        <v>7550</v>
-      </c>
-      <c r="B56" s="9" t="s">
-        <v>7551</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>4770</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>7552</v>
-      </c>
-      <c r="F56" s="3">
-        <v>45934.85625</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="8" t="s">
-        <v>7553</v>
-      </c>
-      <c r="B57" s="9" t="s">
-        <v>7554</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>4770</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>6532</v>
-      </c>
-      <c r="E57" s="9" t="s">
-        <v>7555</v>
-      </c>
-      <c r="F57" s="3">
-        <v>45934.02986111111</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="8" t="s">
-        <v>7556</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>1943</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>4770</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>7557</v>
-      </c>
-      <c r="F58" s="3">
-        <v>45933.896527777775</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
-        <v>7558</v>
-      </c>
-      <c r="B59" s="9" t="s">
-        <v>7559</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>4770</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>3854</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>7560</v>
-      </c>
-      <c r="F59" s="3">
-        <v>45933.65486111111</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="8" t="s">
-        <v>7561</v>
-      </c>
-      <c r="B60" s="9" t="s">
-        <v>4926</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>4770</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>7562</v>
-      </c>
-      <c r="F60" s="3">
-        <v>45933.65416666667</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="8" t="s">
-        <v>7563</v>
-      </c>
-      <c r="B61" s="9" t="s">
-        <v>7564</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>5266</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>7565</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F61" s="3">
-        <v>45936.492361111115</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="8" t="s">
-        <v>7566</v>
-      </c>
-      <c r="B62" s="9" t="s">
-        <v>7567</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>5266</v>
-      </c>
-      <c r="D62" s="9" t="s">
-        <v>7568</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>7569</v>
-      </c>
-      <c r="F62" s="3">
-        <v>45933.79791666666</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="8" t="s">
-        <v>7570</v>
-      </c>
-      <c r="B63" s="9" t="s">
-        <v>7571</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>5674</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>7572</v>
-      </c>
-      <c r="E63" s="9" t="s">
-        <v>7573</v>
-      </c>
-      <c r="F63" s="3">
-        <v>45935.52083333333</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="8" t="s">
-        <v>7574</v>
-      </c>
-      <c r="B64" s="9" t="s">
-        <v>7575</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>6207</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F64" s="3">
-        <v>45936.53958333333</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="8" t="s">
-        <v>7576</v>
-      </c>
-      <c r="B65" s="9" t="s">
-        <v>7577</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F65" s="3">
-        <v>45934.54305555555</v>
+        <v>45936.88888888889</v>
       </c>
     </row>
   </sheetData>
@@ -24544,32 +24333,6 @@
     <hyperlink ref="A37" r:id="rId36"/>
     <hyperlink ref="A38" r:id="rId37"/>
     <hyperlink ref="A39" r:id="rId38"/>
-    <hyperlink ref="A40" r:id="rId39"/>
-    <hyperlink ref="A41" r:id="rId40"/>
-    <hyperlink ref="A42" r:id="rId41"/>
-    <hyperlink ref="A43" r:id="rId42"/>
-    <hyperlink ref="A44" r:id="rId43"/>
-    <hyperlink ref="A45" r:id="rId44"/>
-    <hyperlink ref="A46" r:id="rId45"/>
-    <hyperlink ref="A47" r:id="rId46"/>
-    <hyperlink ref="A48" r:id="rId47"/>
-    <hyperlink ref="A49" r:id="rId48"/>
-    <hyperlink ref="A50" r:id="rId49"/>
-    <hyperlink ref="A51" r:id="rId50"/>
-    <hyperlink ref="A52" r:id="rId51"/>
-    <hyperlink ref="A53" r:id="rId52"/>
-    <hyperlink ref="A54" r:id="rId53"/>
-    <hyperlink ref="A55" r:id="rId54"/>
-    <hyperlink ref="A56" r:id="rId55"/>
-    <hyperlink ref="A57" r:id="rId56"/>
-    <hyperlink ref="A58" r:id="rId57"/>
-    <hyperlink ref="A59" r:id="rId58"/>
-    <hyperlink ref="A60" r:id="rId59"/>
-    <hyperlink ref="A61" r:id="rId60"/>
-    <hyperlink ref="A62" r:id="rId61"/>
-    <hyperlink ref="A63" r:id="rId62"/>
-    <hyperlink ref="A64" r:id="rId63"/>
-    <hyperlink ref="A65" r:id="rId64"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -24578,7 +24341,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2383"/>
+  <dimension ref="A1:F2447"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -72254,6 +72017,1286 @@
       </c>
       <c r="F2383" s="3">
         <v>45932.88611111111</v>
+      </c>
+    </row>
+    <row r="2384" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2384" s="4" t="s">
+        <v>7398</v>
+      </c>
+      <c r="B2384" s="3" t="s">
+        <v>7399</v>
+      </c>
+      <c r="C2384" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2384" s="3" t="s">
+        <v>1984</v>
+      </c>
+      <c r="E2384" s="3" t="s">
+        <v>7400</v>
+      </c>
+      <c r="F2384" s="3">
+        <v>45935.52569444444</v>
+      </c>
+    </row>
+    <row r="2385" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2385" s="4" t="s">
+        <v>7401</v>
+      </c>
+      <c r="B2385" s="3" t="s">
+        <v>7402</v>
+      </c>
+      <c r="C2385" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2385" s="3" t="s">
+        <v>2284</v>
+      </c>
+      <c r="E2385" s="3" t="s">
+        <v>7403</v>
+      </c>
+      <c r="F2385" s="3">
+        <v>45933.65902777778</v>
+      </c>
+    </row>
+    <row r="2386" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2386" s="4" t="s">
+        <v>7404</v>
+      </c>
+      <c r="B2386" s="3" t="s">
+        <v>7405</v>
+      </c>
+      <c r="C2386" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2386" s="3" t="s">
+        <v>6208</v>
+      </c>
+      <c r="E2386" s="3" t="s">
+        <v>7406</v>
+      </c>
+      <c r="F2386" s="3">
+        <v>45935.73055555555</v>
+      </c>
+    </row>
+    <row r="2387" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2387" s="4" t="s">
+        <v>7407</v>
+      </c>
+      <c r="B2387" s="3" t="s">
+        <v>7408</v>
+      </c>
+      <c r="C2387" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2387" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="E2387" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="F2387" s="3">
+        <v>45935.49791666667</v>
+      </c>
+    </row>
+    <row r="2388" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2388" s="4" t="s">
+        <v>7409</v>
+      </c>
+      <c r="B2388" s="3" t="s">
+        <v>7410</v>
+      </c>
+      <c r="C2388" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2388" s="3" t="s">
+        <v>1430</v>
+      </c>
+      <c r="E2388" s="3" t="s">
+        <v>7411</v>
+      </c>
+      <c r="F2388" s="3">
+        <v>45935.481944444444</v>
+      </c>
+    </row>
+    <row r="2389" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2389" s="4" t="s">
+        <v>7412</v>
+      </c>
+      <c r="B2389" s="3" t="s">
+        <v>7413</v>
+      </c>
+      <c r="C2389" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2389" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2389" s="3" t="s">
+        <v>7414</v>
+      </c>
+      <c r="F2389" s="3">
+        <v>45935.475</v>
+      </c>
+    </row>
+    <row r="2390" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2390" s="4" t="s">
+        <v>7415</v>
+      </c>
+      <c r="B2390" s="3" t="s">
+        <v>7416</v>
+      </c>
+      <c r="C2390" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2390" s="3" t="s">
+        <v>7417</v>
+      </c>
+      <c r="E2390" s="3" t="s">
+        <v>7418</v>
+      </c>
+      <c r="F2390" s="3">
+        <v>45935.46736111111</v>
+      </c>
+    </row>
+    <row r="2391" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2391" s="4" t="s">
+        <v>7419</v>
+      </c>
+      <c r="B2391" s="3" t="s">
+        <v>7420</v>
+      </c>
+      <c r="C2391" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2391" s="3" t="s">
+        <v>7421</v>
+      </c>
+      <c r="E2391" s="3" t="s">
+        <v>7422</v>
+      </c>
+      <c r="F2391" s="3">
+        <v>45935.46319444444</v>
+      </c>
+    </row>
+    <row r="2392" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2392" s="4" t="s">
+        <v>7423</v>
+      </c>
+      <c r="B2392" s="3" t="s">
+        <v>7424</v>
+      </c>
+      <c r="C2392" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2392" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2392" s="3" t="s">
+        <v>7425</v>
+      </c>
+      <c r="F2392" s="3">
+        <v>45935.45694444445</v>
+      </c>
+    </row>
+    <row r="2393" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2393" s="4" t="s">
+        <v>7426</v>
+      </c>
+      <c r="B2393" s="3" t="s">
+        <v>7427</v>
+      </c>
+      <c r="C2393" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2393" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2393" s="3" t="s">
+        <v>7428</v>
+      </c>
+      <c r="F2393" s="3">
+        <v>45934.58263888889</v>
+      </c>
+    </row>
+    <row r="2394" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2394" s="4" t="s">
+        <v>7429</v>
+      </c>
+      <c r="B2394" s="3" t="s">
+        <v>7430</v>
+      </c>
+      <c r="C2394" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2394" s="3" t="s">
+        <v>4468</v>
+      </c>
+      <c r="E2394" s="3" t="s">
+        <v>7431</v>
+      </c>
+      <c r="F2394" s="3">
+        <v>45933.86319444445</v>
+      </c>
+    </row>
+    <row r="2395" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2395" s="4" t="s">
+        <v>7432</v>
+      </c>
+      <c r="B2395" s="3" t="s">
+        <v>7433</v>
+      </c>
+      <c r="C2395" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2395" s="3" t="s">
+        <v>7434</v>
+      </c>
+      <c r="E2395" s="3" t="s">
+        <v>7435</v>
+      </c>
+      <c r="F2395" s="3">
+        <v>45933.756944444445</v>
+      </c>
+    </row>
+    <row r="2396" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2396" s="4" t="s">
+        <v>7436</v>
+      </c>
+      <c r="B2396" s="3" t="s">
+        <v>7437</v>
+      </c>
+      <c r="C2396" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2396" s="3" t="s">
+        <v>7438</v>
+      </c>
+      <c r="E2396" s="3" t="s">
+        <v>7439</v>
+      </c>
+      <c r="F2396" s="3">
+        <v>45934.7125</v>
+      </c>
+    </row>
+    <row r="2397" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2397" s="4" t="s">
+        <v>7440</v>
+      </c>
+      <c r="B2397" s="3" t="s">
+        <v>7441</v>
+      </c>
+      <c r="C2397" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2397" s="3" t="s">
+        <v>7442</v>
+      </c>
+      <c r="E2397" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="F2397" s="3">
+        <v>45934.5125</v>
+      </c>
+    </row>
+    <row r="2398" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2398" s="4" t="s">
+        <v>7443</v>
+      </c>
+      <c r="B2398" s="3" t="s">
+        <v>7444</v>
+      </c>
+      <c r="C2398" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2398" s="3" t="s">
+        <v>7445</v>
+      </c>
+      <c r="E2398" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2398" s="3">
+        <v>45934.464583333334</v>
+      </c>
+    </row>
+    <row r="2399" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2399" s="4" t="s">
+        <v>7446</v>
+      </c>
+      <c r="B2399" s="3" t="s">
+        <v>7447</v>
+      </c>
+      <c r="C2399" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2399" s="3" t="s">
+        <v>1112</v>
+      </c>
+      <c r="E2399" s="3" t="s">
+        <v>1113</v>
+      </c>
+      <c r="F2399" s="3">
+        <v>45934.41875</v>
+      </c>
+    </row>
+    <row r="2400" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2400" s="4" t="s">
+        <v>7448</v>
+      </c>
+      <c r="B2400" s="3" t="s">
+        <v>7449</v>
+      </c>
+      <c r="C2400" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2400" s="3" t="s">
+        <v>1156</v>
+      </c>
+      <c r="E2400" s="3" t="s">
+        <v>7450</v>
+      </c>
+      <c r="F2400" s="3">
+        <v>45933.66180555556</v>
+      </c>
+    </row>
+    <row r="2401" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2401" s="4" t="s">
+        <v>7451</v>
+      </c>
+      <c r="B2401" s="3" t="s">
+        <v>830</v>
+      </c>
+      <c r="C2401" s="3" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D2401" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="E2401" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2401" s="3">
+        <v>45936.59166666667</v>
+      </c>
+    </row>
+    <row r="2402" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2402" s="4" t="s">
+        <v>7452</v>
+      </c>
+      <c r="B2402" s="3" t="s">
+        <v>7453</v>
+      </c>
+      <c r="C2402" s="3" t="s">
+        <v>1733</v>
+      </c>
+      <c r="D2402" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="E2402" s="3" t="s">
+        <v>7454</v>
+      </c>
+      <c r="F2402" s="3">
+        <v>45936.59027777778</v>
+      </c>
+    </row>
+    <row r="2403" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2403" s="4" t="s">
+        <v>7455</v>
+      </c>
+      <c r="B2403" s="3" t="s">
+        <v>7456</v>
+      </c>
+      <c r="C2403" s="3" t="s">
+        <v>1733</v>
+      </c>
+      <c r="D2403" s="3" t="s">
+        <v>7457</v>
+      </c>
+      <c r="E2403" s="3" t="s">
+        <v>7458</v>
+      </c>
+      <c r="F2403" s="3">
+        <v>45936.48888888889</v>
+      </c>
+    </row>
+    <row r="2404" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2404" s="4" t="s">
+        <v>7459</v>
+      </c>
+      <c r="B2404" s="3" t="s">
+        <v>7460</v>
+      </c>
+      <c r="C2404" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2404" s="3" t="s">
+        <v>7461</v>
+      </c>
+      <c r="E2404" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2404" s="3">
+        <v>45936.59027777778</v>
+      </c>
+    </row>
+    <row r="2405" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2405" s="4" t="s">
+        <v>7462</v>
+      </c>
+      <c r="B2405" s="3" t="s">
+        <v>7463</v>
+      </c>
+      <c r="C2405" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2405" s="3" t="s">
+        <v>7464</v>
+      </c>
+      <c r="E2405" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2405" s="3">
+        <v>45936.56458333333</v>
+      </c>
+    </row>
+    <row r="2406" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2406" s="4" t="s">
+        <v>7465</v>
+      </c>
+      <c r="B2406" s="3" t="s">
+        <v>2838</v>
+      </c>
+      <c r="C2406" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2406" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="E2406" s="3" t="s">
+        <v>7466</v>
+      </c>
+      <c r="F2406" s="3">
+        <v>45936.48125</v>
+      </c>
+    </row>
+    <row r="2407" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2407" s="4" t="s">
+        <v>7467</v>
+      </c>
+      <c r="B2407" s="3" t="s">
+        <v>7468</v>
+      </c>
+      <c r="C2407" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2407" s="3" t="s">
+        <v>7469</v>
+      </c>
+      <c r="E2407" s="3" t="s">
+        <v>7470</v>
+      </c>
+      <c r="F2407" s="3">
+        <v>45935.856944444444</v>
+      </c>
+    </row>
+    <row r="2408" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2408" s="4" t="s">
+        <v>7471</v>
+      </c>
+      <c r="B2408" s="3" t="s">
+        <v>2597</v>
+      </c>
+      <c r="C2408" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2408" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2408" s="3" t="s">
+        <v>7472</v>
+      </c>
+      <c r="F2408" s="3">
+        <v>45935.75277777778</v>
+      </c>
+    </row>
+    <row r="2409" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2409" s="4" t="s">
+        <v>7473</v>
+      </c>
+      <c r="B2409" s="3" t="s">
+        <v>7474</v>
+      </c>
+      <c r="C2409" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2409" s="3" t="s">
+        <v>7475</v>
+      </c>
+      <c r="E2409" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2409" s="3">
+        <v>45934.444444444445</v>
+      </c>
+    </row>
+    <row r="2410" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2410" s="4" t="s">
+        <v>7476</v>
+      </c>
+      <c r="B2410" s="3" t="s">
+        <v>4478</v>
+      </c>
+      <c r="C2410" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2410" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="E2410" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2410" s="3">
+        <v>45934.361805555556</v>
+      </c>
+    </row>
+    <row r="2411" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2411" s="4" t="s">
+        <v>7477</v>
+      </c>
+      <c r="B2411" s="3" t="s">
+        <v>7478</v>
+      </c>
+      <c r="C2411" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2411" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2411" s="3" t="s">
+        <v>7479</v>
+      </c>
+      <c r="F2411" s="3">
+        <v>45933.89583333333</v>
+      </c>
+    </row>
+    <row r="2412" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2412" s="4" t="s">
+        <v>7480</v>
+      </c>
+      <c r="B2412" s="3" t="s">
+        <v>7481</v>
+      </c>
+      <c r="C2412" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2412" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2412" s="3" t="s">
+        <v>7482</v>
+      </c>
+      <c r="F2412" s="3">
+        <v>45936.601388888885</v>
+      </c>
+    </row>
+    <row r="2413" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2413" s="4" t="s">
+        <v>7483</v>
+      </c>
+      <c r="B2413" s="3" t="s">
+        <v>7484</v>
+      </c>
+      <c r="C2413" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2413" s="3" t="s">
+        <v>7485</v>
+      </c>
+      <c r="E2413" s="3" t="s">
+        <v>7486</v>
+      </c>
+      <c r="F2413" s="3">
+        <v>45936.47986111111</v>
+      </c>
+    </row>
+    <row r="2414" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2414" s="4" t="s">
+        <v>7487</v>
+      </c>
+      <c r="B2414" s="3" t="s">
+        <v>7488</v>
+      </c>
+      <c r="C2414" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2414" s="3" t="s">
+        <v>7489</v>
+      </c>
+      <c r="E2414" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2414" s="3">
+        <v>45936.30138888889</v>
+      </c>
+    </row>
+    <row r="2415" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2415" s="4" t="s">
+        <v>7490</v>
+      </c>
+      <c r="B2415" s="3" t="s">
+        <v>7065</v>
+      </c>
+      <c r="C2415" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2415" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2415" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2415" s="3">
+        <v>45935.535416666666</v>
+      </c>
+    </row>
+    <row r="2416" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2416" s="4" t="s">
+        <v>7491</v>
+      </c>
+      <c r="B2416" s="3" t="s">
+        <v>7492</v>
+      </c>
+      <c r="C2416" s="3" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D2416" s="3" t="s">
+        <v>7493</v>
+      </c>
+      <c r="E2416" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2416" s="3">
+        <v>45936.57986111111</v>
+      </c>
+    </row>
+    <row r="2417" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2417" s="4" t="s">
+        <v>7494</v>
+      </c>
+      <c r="B2417" s="3" t="s">
+        <v>7495</v>
+      </c>
+      <c r="C2417" s="3" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D2417" s="3" t="s">
+        <v>7496</v>
+      </c>
+      <c r="E2417" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2417" s="3">
+        <v>45936.48333333334</v>
+      </c>
+    </row>
+    <row r="2418" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2418" s="4" t="s">
+        <v>7497</v>
+      </c>
+      <c r="B2418" s="3" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C2418" s="3" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D2418" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E2418" s="3" t="s">
+        <v>7498</v>
+      </c>
+      <c r="F2418" s="3">
+        <v>45935.63125</v>
+      </c>
+    </row>
+    <row r="2419" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2419" s="4" t="s">
+        <v>7499</v>
+      </c>
+      <c r="B2419" s="3" t="s">
+        <v>7500</v>
+      </c>
+      <c r="C2419" s="3" t="s">
+        <v>3868</v>
+      </c>
+      <c r="D2419" s="3" t="s">
+        <v>7501</v>
+      </c>
+      <c r="E2419" s="3" t="s">
+        <v>7502</v>
+      </c>
+      <c r="F2419" s="3">
+        <v>45936.61597222222</v>
+      </c>
+    </row>
+    <row r="2420" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2420" s="4" t="s">
+        <v>7503</v>
+      </c>
+      <c r="B2420" s="3" t="s">
+        <v>3979</v>
+      </c>
+      <c r="C2420" s="3" t="s">
+        <v>3868</v>
+      </c>
+      <c r="D2420" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E2420" s="3" t="s">
+        <v>3980</v>
+      </c>
+      <c r="F2420" s="3">
+        <v>45934.44097222222</v>
+      </c>
+    </row>
+    <row r="2421" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2421" s="4" t="s">
+        <v>7504</v>
+      </c>
+      <c r="B2421" s="3" t="s">
+        <v>7505</v>
+      </c>
+      <c r="C2421" s="3" t="s">
+        <v>3868</v>
+      </c>
+      <c r="D2421" s="3" t="s">
+        <v>4006</v>
+      </c>
+      <c r="E2421" s="3" t="s">
+        <v>7506</v>
+      </c>
+      <c r="F2421" s="3">
+        <v>45933.64166666666</v>
+      </c>
+    </row>
+    <row r="2422" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2422" s="4" t="s">
+        <v>7507</v>
+      </c>
+      <c r="B2422" s="3" t="s">
+        <v>7508</v>
+      </c>
+      <c r="C2422" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2422" s="3" t="s">
+        <v>1632</v>
+      </c>
+      <c r="E2422" s="3" t="s">
+        <v>7509</v>
+      </c>
+      <c r="F2422" s="3">
+        <v>45935.94861111111</v>
+      </c>
+    </row>
+    <row r="2423" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2423" s="4" t="s">
+        <v>7510</v>
+      </c>
+      <c r="B2423" s="3" t="s">
+        <v>7511</v>
+      </c>
+      <c r="C2423" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2423" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E2423" s="3" t="s">
+        <v>7512</v>
+      </c>
+      <c r="F2423" s="3">
+        <v>45935.88958333334</v>
+      </c>
+    </row>
+    <row r="2424" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2424" s="4" t="s">
+        <v>7513</v>
+      </c>
+      <c r="B2424" s="3" t="s">
+        <v>7514</v>
+      </c>
+      <c r="C2424" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2424" s="3" t="s">
+        <v>2059</v>
+      </c>
+      <c r="E2424" s="3" t="s">
+        <v>7515</v>
+      </c>
+      <c r="F2424" s="3">
+        <v>45935.65555555555</v>
+      </c>
+    </row>
+    <row r="2425" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2425" s="4" t="s">
+        <v>7516</v>
+      </c>
+      <c r="B2425" s="3" t="s">
+        <v>7517</v>
+      </c>
+      <c r="C2425" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2425" s="3" t="s">
+        <v>1006</v>
+      </c>
+      <c r="E2425" s="3" t="s">
+        <v>4353</v>
+      </c>
+      <c r="F2425" s="3">
+        <v>45935.648611111115</v>
+      </c>
+    </row>
+    <row r="2426" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2426" s="4" t="s">
+        <v>7518</v>
+      </c>
+      <c r="B2426" s="3" t="s">
+        <v>7519</v>
+      </c>
+      <c r="C2426" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2426" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2426" s="3" t="s">
+        <v>7520</v>
+      </c>
+      <c r="F2426" s="3">
+        <v>45935.34375</v>
+      </c>
+    </row>
+    <row r="2427" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2427" s="4" t="s">
+        <v>7521</v>
+      </c>
+      <c r="B2427" s="3" t="s">
+        <v>7522</v>
+      </c>
+      <c r="C2427" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2427" s="3" t="s">
+        <v>7523</v>
+      </c>
+      <c r="E2427" s="3" t="s">
+        <v>7524</v>
+      </c>
+      <c r="F2427" s="3">
+        <v>45935.33472222222</v>
+      </c>
+    </row>
+    <row r="2428" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2428" s="4" t="s">
+        <v>7525</v>
+      </c>
+      <c r="B2428" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="C2428" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2428" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2428" s="3" t="s">
+        <v>7526</v>
+      </c>
+      <c r="F2428" s="3">
+        <v>45933.99930555555</v>
+      </c>
+    </row>
+    <row r="2429" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2429" s="4" t="s">
+        <v>7527</v>
+      </c>
+      <c r="B2429" s="3" t="s">
+        <v>4478</v>
+      </c>
+      <c r="C2429" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2429" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2429" s="3" t="s">
+        <v>7528</v>
+      </c>
+      <c r="F2429" s="3">
+        <v>45933.84236111111</v>
+      </c>
+    </row>
+    <row r="2430" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2430" s="4" t="s">
+        <v>7529</v>
+      </c>
+      <c r="B2430" s="3" t="s">
+        <v>7530</v>
+      </c>
+      <c r="C2430" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2430" s="3" t="s">
+        <v>7531</v>
+      </c>
+      <c r="E2430" s="3" t="s">
+        <v>7532</v>
+      </c>
+      <c r="F2430" s="3">
+        <v>45933.836111111115</v>
+      </c>
+    </row>
+    <row r="2431" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2431" s="4" t="s">
+        <v>7533</v>
+      </c>
+      <c r="B2431" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2431" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2431" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2431" s="3" t="s">
+        <v>7534</v>
+      </c>
+      <c r="F2431" s="3">
+        <v>45933.820138888885</v>
+      </c>
+    </row>
+    <row r="2432" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2432" s="4" t="s">
+        <v>7535</v>
+      </c>
+      <c r="B2432" s="3" t="s">
+        <v>3544</v>
+      </c>
+      <c r="C2432" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2432" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2432" s="3" t="s">
+        <v>7536</v>
+      </c>
+      <c r="F2432" s="3">
+        <v>45933.81527777778</v>
+      </c>
+    </row>
+    <row r="2433" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2433" s="4" t="s">
+        <v>7537</v>
+      </c>
+      <c r="B2433" s="3" t="s">
+        <v>3544</v>
+      </c>
+      <c r="C2433" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2433" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2433" s="3" t="s">
+        <v>7538</v>
+      </c>
+      <c r="F2433" s="3">
+        <v>45933.808333333334</v>
+      </c>
+    </row>
+    <row r="2434" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2434" s="4" t="s">
+        <v>7539</v>
+      </c>
+      <c r="B2434" s="3" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C2434" s="3" t="s">
+        <v>4671</v>
+      </c>
+      <c r="D2434" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2434" s="3" t="s">
+        <v>7540</v>
+      </c>
+      <c r="F2434" s="3">
+        <v>45935.73333333334</v>
+      </c>
+    </row>
+    <row r="2435" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2435" s="4" t="s">
+        <v>7541</v>
+      </c>
+      <c r="B2435" s="3" t="s">
+        <v>7542</v>
+      </c>
+      <c r="C2435" s="3" t="s">
+        <v>4671</v>
+      </c>
+      <c r="D2435" s="3" t="s">
+        <v>7543</v>
+      </c>
+      <c r="E2435" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2435" s="3">
+        <v>45935.72430555556</v>
+      </c>
+    </row>
+    <row r="2436" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2436" s="4" t="s">
+        <v>7544</v>
+      </c>
+      <c r="B2436" s="3" t="s">
+        <v>7545</v>
+      </c>
+      <c r="C2436" s="3" t="s">
+        <v>4671</v>
+      </c>
+      <c r="D2436" s="3" t="s">
+        <v>4672</v>
+      </c>
+      <c r="E2436" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2436" s="3">
+        <v>45933.763194444444</v>
+      </c>
+    </row>
+    <row r="2437" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2437" s="4" t="s">
+        <v>7546</v>
+      </c>
+      <c r="B2437" s="3" t="s">
+        <v>7547</v>
+      </c>
+      <c r="C2437" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2437" s="3" t="s">
+        <v>7548</v>
+      </c>
+      <c r="E2437" s="3" t="s">
+        <v>7549</v>
+      </c>
+      <c r="F2437" s="3">
+        <v>45935.73125</v>
+      </c>
+    </row>
+    <row r="2438" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2438" s="4" t="s">
+        <v>7550</v>
+      </c>
+      <c r="B2438" s="3" t="s">
+        <v>7551</v>
+      </c>
+      <c r="C2438" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2438" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2438" s="3" t="s">
+        <v>7552</v>
+      </c>
+      <c r="F2438" s="3">
+        <v>45934.85625</v>
+      </c>
+    </row>
+    <row r="2439" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2439" s="4" t="s">
+        <v>7553</v>
+      </c>
+      <c r="B2439" s="3" t="s">
+        <v>7554</v>
+      </c>
+      <c r="C2439" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2439" s="3" t="s">
+        <v>6532</v>
+      </c>
+      <c r="E2439" s="3" t="s">
+        <v>7555</v>
+      </c>
+      <c r="F2439" s="3">
+        <v>45934.02986111111</v>
+      </c>
+    </row>
+    <row r="2440" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2440" s="4" t="s">
+        <v>7556</v>
+      </c>
+      <c r="B2440" s="3" t="s">
+        <v>1943</v>
+      </c>
+      <c r="C2440" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2440" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2440" s="3" t="s">
+        <v>7557</v>
+      </c>
+      <c r="F2440" s="3">
+        <v>45933.896527777775</v>
+      </c>
+    </row>
+    <row r="2441" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2441" s="4" t="s">
+        <v>7558</v>
+      </c>
+      <c r="B2441" s="3" t="s">
+        <v>7559</v>
+      </c>
+      <c r="C2441" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2441" s="3" t="s">
+        <v>3854</v>
+      </c>
+      <c r="E2441" s="3" t="s">
+        <v>7560</v>
+      </c>
+      <c r="F2441" s="3">
+        <v>45933.65486111111</v>
+      </c>
+    </row>
+    <row r="2442" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2442" s="4" t="s">
+        <v>7561</v>
+      </c>
+      <c r="B2442" s="3" t="s">
+        <v>4926</v>
+      </c>
+      <c r="C2442" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2442" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2442" s="3" t="s">
+        <v>7562</v>
+      </c>
+      <c r="F2442" s="3">
+        <v>45933.65416666667</v>
+      </c>
+    </row>
+    <row r="2443" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2443" s="4" t="s">
+        <v>7563</v>
+      </c>
+      <c r="B2443" s="3" t="s">
+        <v>7564</v>
+      </c>
+      <c r="C2443" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2443" s="3" t="s">
+        <v>7565</v>
+      </c>
+      <c r="E2443" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2443" s="3">
+        <v>45936.492361111115</v>
+      </c>
+    </row>
+    <row r="2444" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2444" s="4" t="s">
+        <v>7566</v>
+      </c>
+      <c r="B2444" s="3" t="s">
+        <v>7567</v>
+      </c>
+      <c r="C2444" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2444" s="3" t="s">
+        <v>7568</v>
+      </c>
+      <c r="E2444" s="3" t="s">
+        <v>7569</v>
+      </c>
+      <c r="F2444" s="3">
+        <v>45933.79791666666</v>
+      </c>
+    </row>
+    <row r="2445" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2445" s="4" t="s">
+        <v>7570</v>
+      </c>
+      <c r="B2445" s="3" t="s">
+        <v>7571</v>
+      </c>
+      <c r="C2445" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2445" s="3" t="s">
+        <v>7572</v>
+      </c>
+      <c r="E2445" s="3" t="s">
+        <v>7573</v>
+      </c>
+      <c r="F2445" s="3">
+        <v>45935.52083333333</v>
+      </c>
+    </row>
+    <row r="2446" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2446" s="4" t="s">
+        <v>7574</v>
+      </c>
+      <c r="B2446" s="3" t="s">
+        <v>7575</v>
+      </c>
+      <c r="C2446" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2446" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2446" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2446" s="3">
+        <v>45936.53958333333</v>
+      </c>
+    </row>
+    <row r="2447" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2447" s="4" t="s">
+        <v>7576</v>
+      </c>
+      <c r="B2447" s="3" t="s">
+        <v>7577</v>
+      </c>
+      <c r="C2447" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2447" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2447" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2447" s="3">
+        <v>45934.54305555555</v>
       </c>
     </row>
   </sheetData>
@@ -74640,6 +75683,70 @@
     <hyperlink ref="A2381" r:id="rId2380"/>
     <hyperlink ref="A2382" r:id="rId2381"/>
     <hyperlink ref="A2383" r:id="rId2382"/>
+    <hyperlink ref="A2384" r:id="rId2383"/>
+    <hyperlink ref="A2385" r:id="rId2384"/>
+    <hyperlink ref="A2386" r:id="rId2385"/>
+    <hyperlink ref="A2387" r:id="rId2386"/>
+    <hyperlink ref="A2388" r:id="rId2387"/>
+    <hyperlink ref="A2389" r:id="rId2388"/>
+    <hyperlink ref="A2390" r:id="rId2389"/>
+    <hyperlink ref="A2391" r:id="rId2390"/>
+    <hyperlink ref="A2392" r:id="rId2391"/>
+    <hyperlink ref="A2393" r:id="rId2392"/>
+    <hyperlink ref="A2394" r:id="rId2393"/>
+    <hyperlink ref="A2395" r:id="rId2394"/>
+    <hyperlink ref="A2396" r:id="rId2395"/>
+    <hyperlink ref="A2397" r:id="rId2396"/>
+    <hyperlink ref="A2398" r:id="rId2397"/>
+    <hyperlink ref="A2399" r:id="rId2398"/>
+    <hyperlink ref="A2400" r:id="rId2399"/>
+    <hyperlink ref="A2401" r:id="rId2400"/>
+    <hyperlink ref="A2402" r:id="rId2401"/>
+    <hyperlink ref="A2403" r:id="rId2402"/>
+    <hyperlink ref="A2404" r:id="rId2403"/>
+    <hyperlink ref="A2405" r:id="rId2404"/>
+    <hyperlink ref="A2406" r:id="rId2405"/>
+    <hyperlink ref="A2407" r:id="rId2406"/>
+    <hyperlink ref="A2408" r:id="rId2407"/>
+    <hyperlink ref="A2409" r:id="rId2408"/>
+    <hyperlink ref="A2410" r:id="rId2409"/>
+    <hyperlink ref="A2411" r:id="rId2410"/>
+    <hyperlink ref="A2412" r:id="rId2411"/>
+    <hyperlink ref="A2413" r:id="rId2412"/>
+    <hyperlink ref="A2414" r:id="rId2413"/>
+    <hyperlink ref="A2415" r:id="rId2414"/>
+    <hyperlink ref="A2416" r:id="rId2415"/>
+    <hyperlink ref="A2417" r:id="rId2416"/>
+    <hyperlink ref="A2418" r:id="rId2417"/>
+    <hyperlink ref="A2419" r:id="rId2418"/>
+    <hyperlink ref="A2420" r:id="rId2419"/>
+    <hyperlink ref="A2421" r:id="rId2420"/>
+    <hyperlink ref="A2422" r:id="rId2421"/>
+    <hyperlink ref="A2423" r:id="rId2422"/>
+    <hyperlink ref="A2424" r:id="rId2423"/>
+    <hyperlink ref="A2425" r:id="rId2424"/>
+    <hyperlink ref="A2426" r:id="rId2425"/>
+    <hyperlink ref="A2427" r:id="rId2426"/>
+    <hyperlink ref="A2428" r:id="rId2427"/>
+    <hyperlink ref="A2429" r:id="rId2428"/>
+    <hyperlink ref="A2430" r:id="rId2429"/>
+    <hyperlink ref="A2431" r:id="rId2430"/>
+    <hyperlink ref="A2432" r:id="rId2431"/>
+    <hyperlink ref="A2433" r:id="rId2432"/>
+    <hyperlink ref="A2434" r:id="rId2433"/>
+    <hyperlink ref="A2435" r:id="rId2434"/>
+    <hyperlink ref="A2436" r:id="rId2435"/>
+    <hyperlink ref="A2437" r:id="rId2436"/>
+    <hyperlink ref="A2438" r:id="rId2437"/>
+    <hyperlink ref="A2439" r:id="rId2438"/>
+    <hyperlink ref="A2440" r:id="rId2439"/>
+    <hyperlink ref="A2441" r:id="rId2440"/>
+    <hyperlink ref="A2442" r:id="rId2441"/>
+    <hyperlink ref="A2443" r:id="rId2442"/>
+    <hyperlink ref="A2444" r:id="rId2443"/>
+    <hyperlink ref="A2445" r:id="rId2444"/>
+    <hyperlink ref="A2446" r:id="rId2445"/>
+    <hyperlink ref="A2447" r:id="rId2446"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Update lands data - 2025-10-08 12:21
</commit_message>
<xml_diff>
--- a/lands-scraped.xlsx
+++ b/lands-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12432" uniqueCount="7681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12537" uniqueCount="7741">
   <si>
     <t>link</t>
   </si>
@@ -23061,6 +23061,186 @@
   </si>
   <si>
     <t>48 000 € (2.40 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/drabesu-pag/ipclk.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/medumu-pag/enlcf.html</t>
+  </si>
+  <si>
+    <t>5 500 € (0.28 €/m²)</t>
+  </si>
+  <si>
+    <t>44720080260</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jekabpils-and-reg/mezares-pag/pdnhd.html</t>
+  </si>
+  <si>
+    <t>14 000 € (0.36 €/m²)</t>
+  </si>
+  <si>
+    <t>3.90 ha.</t>
+  </si>
+  <si>
+    <t>56760060029</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jelgava/fxfdk.html</t>
+  </si>
+  <si>
+    <t>31 000 € (28.89 €/m²)</t>
+  </si>
+  <si>
+    <t>1073 m²</t>
+  </si>
+  <si>
+    <t>0900 021 0580</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kraslava-and-reg/asunes-pag/abfjk.html</t>
+  </si>
+  <si>
+    <t>110 000 € (0.26 €/m²)</t>
+  </si>
+  <si>
+    <t>60460010003</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kraslava-and-reg/ezernieku-pag/jnfnj.html</t>
+  </si>
+  <si>
+    <t>60560020053</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/limbadzi-and-reg/liepupes-pag/hoihb.html</t>
+  </si>
+  <si>
+    <t>36 000 € (2 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/limbadzi-and-reg/skultes-pag/abnop.html</t>
+  </si>
+  <si>
+    <t>130 000 € (4.33 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/limbadzi-and-reg/aloja/bckhcc.html</t>
+  </si>
+  <si>
+    <t>9 500 € (2.88 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/limbadzi-and-reg/salacgriva/fjhnd.html</t>
+  </si>
+  <si>
+    <t>67 800 € (25 €/m²)</t>
+  </si>
+  <si>
+    <t>2712 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ogre/adgxk.html</t>
+  </si>
+  <si>
+    <t>50 000 € (27.06 €/m²)</t>
+  </si>
+  <si>
+    <t>1848 m²</t>
+  </si>
+  <si>
+    <t>74800051031</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ogresgala-pag/ioxjh.html</t>
+  </si>
+  <si>
+    <t>28 000 € (8 €/m²)</t>
+  </si>
+  <si>
+    <t>74800040557</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ogre/cdnoj.html</t>
+  </si>
+  <si>
+    <t>450 000 € (3.95 €/m²)</t>
+  </si>
+  <si>
+    <t>11.40 ha.</t>
+  </si>
+  <si>
+    <t>7401 003 0286</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/preili-and-reg/aglonas-pag/agfjf.html</t>
+  </si>
+  <si>
+    <t>32 000 € (0.34 €/m²)</t>
+  </si>
+  <si>
+    <t>76420050060</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/ozolaines-pag/bdjpoh.html</t>
+  </si>
+  <si>
+    <t>20 000 € (0.91 €/m²)</t>
+  </si>
+  <si>
+    <t>2.19 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/rezekne/nenmh.html</t>
+  </si>
+  <si>
+    <t>33 800 € (4.96 €/m²)</t>
+  </si>
+  <si>
+    <t>6809 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/jaunsatu-pag/fgkbh.html</t>
+  </si>
+  <si>
+    <t>31 000 € (1.03 €/m²)</t>
+  </si>
+  <si>
+    <t>90580050034</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/konu-pag/ahbjm.html</t>
+  </si>
+  <si>
+    <t>77 500 € (0.53 €/m²)</t>
+  </si>
+  <si>
+    <t>14.50 ha.</t>
+  </si>
+  <si>
+    <t>96660040280</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/valmiera/hobom.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/valmiera/aeooc.html</t>
+  </si>
+  <si>
+    <t>46 000 € (26.88 €/m²)</t>
+  </si>
+  <si>
+    <t>1711 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/valmiera/aghgx.html</t>
+  </si>
+  <si>
+    <t>390 000 € (111.11 €/m²)</t>
+  </si>
+  <si>
+    <t>3510 m²</t>
   </si>
 </sst>
 </file>
@@ -23496,7 +23676,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -23535,762 +23715,422 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>7578</v>
+        <v>7681</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>7579</v>
+        <v>915</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>419</v>
+        <v>772</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>7580</v>
+        <v>171</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>7581</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3">
-        <v>45937.424305555556</v>
+        <v>45937.79305555555</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>7582</v>
+        <v>7682</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>7583</v>
+        <v>7683</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>419</v>
+        <v>1218</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>383</v>
+        <v>171</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>7584</v>
+        <v>7684</v>
       </c>
       <c r="F3" s="3">
-        <v>45936.96527777778</v>
+        <v>45938.63402777778</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>7585</v>
+        <v>7685</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>7586</v>
+        <v>7686</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>1218</v>
+        <v>1733</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>146</v>
+        <v>7687</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>7587</v>
+        <v>7688</v>
       </c>
       <c r="F4" s="3">
-        <v>45937.63611111111</v>
+        <v>45938.44305555556</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>7588</v>
+        <v>7689</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>7589</v>
+        <v>7690</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>1218</v>
+        <v>1929</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>201</v>
+        <v>7691</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>7590</v>
+        <v>7692</v>
       </c>
       <c r="F5" s="3">
-        <v>45937.63055555556</v>
+        <v>45938.4</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>7591</v>
+        <v>7693</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>7592</v>
+        <v>7694</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1218</v>
+        <v>2488</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>985</v>
+        <v>4276</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>10</v>
+        <v>7695</v>
       </c>
       <c r="F6" s="3">
-        <v>45937.51666666666</v>
+        <v>45937.73541666666</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>7593</v>
+        <v>7696</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>2609</v>
+        <v>426</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>1218</v>
+        <v>2488</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>407</v>
+        <v>353</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>10</v>
+        <v>7697</v>
       </c>
       <c r="F7" s="3">
-        <v>45936.8375</v>
+        <v>45937.66458333333</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>7594</v>
+        <v>7698</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>7595</v>
+        <v>7699</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1218</v>
+        <v>3398</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>7596</v>
+        <v>4254</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="3">
-        <v>45936.67152777778</v>
+        <v>45938.54166666667</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>7597</v>
+        <v>7700</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>1183</v>
+        <v>7701</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>1569</v>
+        <v>3398</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>10</v>
+        <v>7618</v>
       </c>
       <c r="F9" s="3">
-        <v>45937.41180555556</v>
+        <v>45938.53055555555</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>7598</v>
+        <v>7702</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>7453</v>
+        <v>7703</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>1733</v>
+        <v>3398</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>353</v>
+        <v>488</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>7599</v>
+        <v>10</v>
       </c>
       <c r="F10" s="3">
-        <v>45936.86041666666</v>
+        <v>45938.48541666666</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>7600</v>
+        <v>7704</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>7601</v>
+        <v>7705</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>1929</v>
+        <v>3398</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>55</v>
+        <v>7706</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>7602</v>
+        <v>10</v>
       </c>
       <c r="F11" s="3">
-        <v>45937.58333333333</v>
+        <v>45938.37152777778</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>7603</v>
+        <v>7707</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>7604</v>
+        <v>7708</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>1929</v>
+        <v>4034</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>7605</v>
+        <v>7709</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>10</v>
+        <v>7710</v>
       </c>
       <c r="F12" s="3">
-        <v>45937.535416666666</v>
+        <v>45938.62013888889</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>7606</v>
+        <v>7711</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>7607</v>
+        <v>7712</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>2488</v>
+        <v>4034</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>407</v>
+        <v>2271</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>7608</v>
+        <v>7713</v>
       </c>
       <c r="F13" s="3">
-        <v>45937.63402777778</v>
+        <v>45938.41527777778</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>7609</v>
+        <v>7714</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>7610</v>
+        <v>7715</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>2671</v>
+        <v>4034</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>317</v>
+        <v>7716</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>7611</v>
+        <v>7717</v>
       </c>
       <c r="F14" s="3">
-        <v>45937.56527777778</v>
+        <v>45937.80138888889</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>7612</v>
+        <v>7718</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>7613</v>
+        <v>7719</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>2671</v>
+        <v>4671</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>7614</v>
+        <v>2522</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>10</v>
+        <v>7720</v>
       </c>
       <c r="F15" s="3">
-        <v>45937.507638888885</v>
+        <v>45937.89097222222</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>7615</v>
+        <v>7721</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>7616</v>
+        <v>7722</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>3398</v>
+        <v>4770</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>7617</v>
+        <v>7723</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>7618</v>
+        <v>10</v>
       </c>
       <c r="F16" s="3">
-        <v>45937.52986111111</v>
+        <v>45938.6</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>7619</v>
+        <v>7724</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>7620</v>
+        <v>7725</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>3762</v>
+        <v>4770</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>7621</v>
+        <v>7726</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F17" s="3">
-        <v>45937.61458333333</v>
+        <v>45937.7375</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>7622</v>
+        <v>7727</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>7623</v>
+        <v>7728</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>3868</v>
+        <v>5674</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>7624</v>
+        <v>7729</v>
       </c>
       <c r="F18" s="3">
-        <v>45937.63402777778</v>
+        <v>45938.45694444445</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>7625</v>
+        <v>7730</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>7626</v>
+        <v>7731</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>4034</v>
+        <v>6207</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>77</v>
+        <v>7732</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>7627</v>
+        <v>7733</v>
       </c>
       <c r="F19" s="3">
-        <v>45937.63680555555</v>
+        <v>45938.44652777778</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>7628</v>
+        <v>7734</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>2510</v>
+        <v>6223</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>4034</v>
+        <v>6207</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>383</v>
+        <v>2271</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>7629</v>
+        <v>10</v>
       </c>
       <c r="F20" s="3">
-        <v>45937.63680555555</v>
+        <v>45937.87430555555</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>7630</v>
+        <v>7735</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>7631</v>
+        <v>7736</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>4034</v>
+        <v>6207</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>442</v>
+        <v>7737</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>7632</v>
+        <v>10</v>
       </c>
       <c r="F21" s="3">
-        <v>45936.990277777775</v>
+        <v>45937.79583333334</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>7633</v>
+        <v>7738</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>7634</v>
+        <v>7739</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>4034</v>
+        <v>6207</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>436</v>
+        <v>7740</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>7635</v>
+        <v>10</v>
       </c>
       <c r="F22" s="3">
-        <v>45936.805555555555</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>7636</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>7637</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>2723</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="3">
-        <v>45936.75486111111</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>7638</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>7639</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>7640</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>7641</v>
-      </c>
-      <c r="F24" s="3">
-        <v>45936.69027777778</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>7642</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>471</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>7643</v>
-      </c>
-      <c r="F25" s="3">
-        <v>45936.67222222222</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>7644</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>7645</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>5266</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>1651</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" s="3">
-        <v>45937.57152777778</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>7646</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>7647</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>5266</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>1724</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>7648</v>
-      </c>
-      <c r="F27" s="3">
-        <v>45936.72986111111</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>7649</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>4954</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>5266</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>407</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>7650</v>
-      </c>
-      <c r="F28" s="3">
-        <v>45936.72777777778</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
-        <v>7651</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>7652</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>5266</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>1156</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>7653</v>
-      </c>
-      <c r="F29" s="3">
-        <v>45936.70625</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>7654</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>7655</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>5674</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>6086</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>7656</v>
-      </c>
-      <c r="F30" s="3">
-        <v>45937.425</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>7657</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>7658</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>5674</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>4888</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>7659</v>
-      </c>
-      <c r="F31" s="3">
-        <v>45937.36041666666</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>7660</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>7661</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>5674</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>7662</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="3">
-        <v>45936.69305555556</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>7663</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>1387</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>6133</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>353</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>7664</v>
-      </c>
-      <c r="F33" s="3">
-        <v>45937.632638888885</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>7665</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>7666</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>6133</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>7667</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>7668</v>
-      </c>
-      <c r="F34" s="3">
-        <v>45936.77986111111</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>7669</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>7670</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>6207</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>7671</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" s="3">
-        <v>45937.4875</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
-        <v>7672</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>7673</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>6207</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>383</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" s="3">
-        <v>45936.70277777778</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
-        <v>7674</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>7675</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>6207</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>474</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F37" s="3">
-        <v>45936.70208333334</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>7676</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>7677</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>4546</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>7678</v>
-      </c>
-      <c r="F38" s="3">
-        <v>45937.46597222222</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>7679</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>7680</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F39" s="3">
-        <v>45936.88888888889</v>
+        <v>45937.65347222222</v>
       </c>
     </row>
   </sheetData>
@@ -24316,23 +24156,6 @@
     <hyperlink ref="A20" r:id="rId19"/>
     <hyperlink ref="A21" r:id="rId20"/>
     <hyperlink ref="A22" r:id="rId21"/>
-    <hyperlink ref="A23" r:id="rId22"/>
-    <hyperlink ref="A24" r:id="rId23"/>
-    <hyperlink ref="A25" r:id="rId24"/>
-    <hyperlink ref="A26" r:id="rId25"/>
-    <hyperlink ref="A27" r:id="rId26"/>
-    <hyperlink ref="A28" r:id="rId27"/>
-    <hyperlink ref="A29" r:id="rId28"/>
-    <hyperlink ref="A30" r:id="rId29"/>
-    <hyperlink ref="A31" r:id="rId30"/>
-    <hyperlink ref="A32" r:id="rId31"/>
-    <hyperlink ref="A33" r:id="rId32"/>
-    <hyperlink ref="A34" r:id="rId33"/>
-    <hyperlink ref="A35" r:id="rId34"/>
-    <hyperlink ref="A36" r:id="rId35"/>
-    <hyperlink ref="A37" r:id="rId36"/>
-    <hyperlink ref="A38" r:id="rId37"/>
-    <hyperlink ref="A39" r:id="rId38"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -24341,7 +24164,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2447"/>
+  <dimension ref="A1:F2485"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -73297,6 +73120,766 @@
       </c>
       <c r="F2447" s="3">
         <v>45934.54305555555</v>
+      </c>
+    </row>
+    <row r="2448" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2448" s="4" t="s">
+        <v>7578</v>
+      </c>
+      <c r="B2448" s="3" t="s">
+        <v>7579</v>
+      </c>
+      <c r="C2448" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2448" s="3" t="s">
+        <v>7580</v>
+      </c>
+      <c r="E2448" s="3" t="s">
+        <v>7581</v>
+      </c>
+      <c r="F2448" s="3">
+        <v>45937.424305555556</v>
+      </c>
+    </row>
+    <row r="2449" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2449" s="4" t="s">
+        <v>7582</v>
+      </c>
+      <c r="B2449" s="3" t="s">
+        <v>7583</v>
+      </c>
+      <c r="C2449" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2449" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E2449" s="3" t="s">
+        <v>7584</v>
+      </c>
+      <c r="F2449" s="3">
+        <v>45936.96527777778</v>
+      </c>
+    </row>
+    <row r="2450" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2450" s="4" t="s">
+        <v>7585</v>
+      </c>
+      <c r="B2450" s="3" t="s">
+        <v>7586</v>
+      </c>
+      <c r="C2450" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2450" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2450" s="3" t="s">
+        <v>7587</v>
+      </c>
+      <c r="F2450" s="3">
+        <v>45937.63611111111</v>
+      </c>
+    </row>
+    <row r="2451" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2451" s="4" t="s">
+        <v>7588</v>
+      </c>
+      <c r="B2451" s="3" t="s">
+        <v>7589</v>
+      </c>
+      <c r="C2451" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2451" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2451" s="3" t="s">
+        <v>7590</v>
+      </c>
+      <c r="F2451" s="3">
+        <v>45937.63055555556</v>
+      </c>
+    </row>
+    <row r="2452" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2452" s="4" t="s">
+        <v>7591</v>
+      </c>
+      <c r="B2452" s="3" t="s">
+        <v>7592</v>
+      </c>
+      <c r="C2452" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2452" s="3" t="s">
+        <v>985</v>
+      </c>
+      <c r="E2452" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2452" s="3">
+        <v>45937.51666666666</v>
+      </c>
+    </row>
+    <row r="2453" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2453" s="4" t="s">
+        <v>7593</v>
+      </c>
+      <c r="B2453" s="3" t="s">
+        <v>2609</v>
+      </c>
+      <c r="C2453" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2453" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="E2453" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2453" s="3">
+        <v>45936.8375</v>
+      </c>
+    </row>
+    <row r="2454" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2454" s="4" t="s">
+        <v>7594</v>
+      </c>
+      <c r="B2454" s="3" t="s">
+        <v>7595</v>
+      </c>
+      <c r="C2454" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2454" s="3" t="s">
+        <v>7596</v>
+      </c>
+      <c r="E2454" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2454" s="3">
+        <v>45936.67152777778</v>
+      </c>
+    </row>
+    <row r="2455" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2455" s="4" t="s">
+        <v>7597</v>
+      </c>
+      <c r="B2455" s="3" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C2455" s="3" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D2455" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2455" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2455" s="3">
+        <v>45937.41180555556</v>
+      </c>
+    </row>
+    <row r="2456" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2456" s="4" t="s">
+        <v>7598</v>
+      </c>
+      <c r="B2456" s="3" t="s">
+        <v>7453</v>
+      </c>
+      <c r="C2456" s="3" t="s">
+        <v>1733</v>
+      </c>
+      <c r="D2456" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="E2456" s="3" t="s">
+        <v>7599</v>
+      </c>
+      <c r="F2456" s="3">
+        <v>45936.86041666666</v>
+      </c>
+    </row>
+    <row r="2457" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2457" s="4" t="s">
+        <v>7600</v>
+      </c>
+      <c r="B2457" s="3" t="s">
+        <v>7601</v>
+      </c>
+      <c r="C2457" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2457" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2457" s="3" t="s">
+        <v>7602</v>
+      </c>
+      <c r="F2457" s="3">
+        <v>45937.58333333333</v>
+      </c>
+    </row>
+    <row r="2458" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2458" s="4" t="s">
+        <v>7603</v>
+      </c>
+      <c r="B2458" s="3" t="s">
+        <v>7604</v>
+      </c>
+      <c r="C2458" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2458" s="3" t="s">
+        <v>7605</v>
+      </c>
+      <c r="E2458" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2458" s="3">
+        <v>45937.535416666666</v>
+      </c>
+    </row>
+    <row r="2459" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2459" s="4" t="s">
+        <v>7606</v>
+      </c>
+      <c r="B2459" s="3" t="s">
+        <v>7607</v>
+      </c>
+      <c r="C2459" s="3" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D2459" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="E2459" s="3" t="s">
+        <v>7608</v>
+      </c>
+      <c r="F2459" s="3">
+        <v>45937.63402777778</v>
+      </c>
+    </row>
+    <row r="2460" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2460" s="4" t="s">
+        <v>7609</v>
+      </c>
+      <c r="B2460" s="3" t="s">
+        <v>7610</v>
+      </c>
+      <c r="C2460" s="3" t="s">
+        <v>2671</v>
+      </c>
+      <c r="D2460" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E2460" s="3" t="s">
+        <v>7611</v>
+      </c>
+      <c r="F2460" s="3">
+        <v>45937.56527777778</v>
+      </c>
+    </row>
+    <row r="2461" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2461" s="4" t="s">
+        <v>7612</v>
+      </c>
+      <c r="B2461" s="3" t="s">
+        <v>7613</v>
+      </c>
+      <c r="C2461" s="3" t="s">
+        <v>2671</v>
+      </c>
+      <c r="D2461" s="3" t="s">
+        <v>7614</v>
+      </c>
+      <c r="E2461" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2461" s="3">
+        <v>45937.507638888885</v>
+      </c>
+    </row>
+    <row r="2462" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2462" s="4" t="s">
+        <v>7615</v>
+      </c>
+      <c r="B2462" s="3" t="s">
+        <v>7616</v>
+      </c>
+      <c r="C2462" s="3" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D2462" s="3" t="s">
+        <v>7617</v>
+      </c>
+      <c r="E2462" s="3" t="s">
+        <v>7618</v>
+      </c>
+      <c r="F2462" s="3">
+        <v>45937.52986111111</v>
+      </c>
+    </row>
+    <row r="2463" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2463" s="4" t="s">
+        <v>7619</v>
+      </c>
+      <c r="B2463" s="3" t="s">
+        <v>7620</v>
+      </c>
+      <c r="C2463" s="3" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D2463" s="3" t="s">
+        <v>7621</v>
+      </c>
+      <c r="E2463" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2463" s="3">
+        <v>45937.61458333333</v>
+      </c>
+    </row>
+    <row r="2464" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2464" s="4" t="s">
+        <v>7622</v>
+      </c>
+      <c r="B2464" s="3" t="s">
+        <v>7623</v>
+      </c>
+      <c r="C2464" s="3" t="s">
+        <v>3868</v>
+      </c>
+      <c r="D2464" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2464" s="3" t="s">
+        <v>7624</v>
+      </c>
+      <c r="F2464" s="3">
+        <v>45937.63402777778</v>
+      </c>
+    </row>
+    <row r="2465" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2465" s="4" t="s">
+        <v>7625</v>
+      </c>
+      <c r="B2465" s="3" t="s">
+        <v>7626</v>
+      </c>
+      <c r="C2465" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2465" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2465" s="3" t="s">
+        <v>7627</v>
+      </c>
+      <c r="F2465" s="3">
+        <v>45937.63680555555</v>
+      </c>
+    </row>
+    <row r="2466" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2466" s="4" t="s">
+        <v>7628</v>
+      </c>
+      <c r="B2466" s="3" t="s">
+        <v>2510</v>
+      </c>
+      <c r="C2466" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2466" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E2466" s="3" t="s">
+        <v>7629</v>
+      </c>
+      <c r="F2466" s="3">
+        <v>45937.63680555555</v>
+      </c>
+    </row>
+    <row r="2467" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2467" s="4" t="s">
+        <v>7630</v>
+      </c>
+      <c r="B2467" s="3" t="s">
+        <v>7631</v>
+      </c>
+      <c r="C2467" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2467" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="E2467" s="3" t="s">
+        <v>7632</v>
+      </c>
+      <c r="F2467" s="3">
+        <v>45936.990277777775</v>
+      </c>
+    </row>
+    <row r="2468" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2468" s="4" t="s">
+        <v>7633</v>
+      </c>
+      <c r="B2468" s="3" t="s">
+        <v>7634</v>
+      </c>
+      <c r="C2468" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2468" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="E2468" s="3" t="s">
+        <v>7635</v>
+      </c>
+      <c r="F2468" s="3">
+        <v>45936.805555555555</v>
+      </c>
+    </row>
+    <row r="2469" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2469" s="4" t="s">
+        <v>7636</v>
+      </c>
+      <c r="B2469" s="3" t="s">
+        <v>7637</v>
+      </c>
+      <c r="C2469" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2469" s="3" t="s">
+        <v>2723</v>
+      </c>
+      <c r="E2469" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2469" s="3">
+        <v>45936.75486111111</v>
+      </c>
+    </row>
+    <row r="2470" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2470" s="4" t="s">
+        <v>7638</v>
+      </c>
+      <c r="B2470" s="3" t="s">
+        <v>7639</v>
+      </c>
+      <c r="C2470" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2470" s="3" t="s">
+        <v>7640</v>
+      </c>
+      <c r="E2470" s="3" t="s">
+        <v>7641</v>
+      </c>
+      <c r="F2470" s="3">
+        <v>45936.69027777778</v>
+      </c>
+    </row>
+    <row r="2471" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2471" s="4" t="s">
+        <v>7642</v>
+      </c>
+      <c r="B2471" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="C2471" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2471" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2471" s="3" t="s">
+        <v>7643</v>
+      </c>
+      <c r="F2471" s="3">
+        <v>45936.67222222222</v>
+      </c>
+    </row>
+    <row r="2472" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2472" s="4" t="s">
+        <v>7644</v>
+      </c>
+      <c r="B2472" s="3" t="s">
+        <v>7645</v>
+      </c>
+      <c r="C2472" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2472" s="3" t="s">
+        <v>1651</v>
+      </c>
+      <c r="E2472" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2472" s="3">
+        <v>45937.57152777778</v>
+      </c>
+    </row>
+    <row r="2473" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2473" s="4" t="s">
+        <v>7646</v>
+      </c>
+      <c r="B2473" s="3" t="s">
+        <v>7647</v>
+      </c>
+      <c r="C2473" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2473" s="3" t="s">
+        <v>1724</v>
+      </c>
+      <c r="E2473" s="3" t="s">
+        <v>7648</v>
+      </c>
+      <c r="F2473" s="3">
+        <v>45936.72986111111</v>
+      </c>
+    </row>
+    <row r="2474" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2474" s="4" t="s">
+        <v>7649</v>
+      </c>
+      <c r="B2474" s="3" t="s">
+        <v>4954</v>
+      </c>
+      <c r="C2474" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2474" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="E2474" s="3" t="s">
+        <v>7650</v>
+      </c>
+      <c r="F2474" s="3">
+        <v>45936.72777777778</v>
+      </c>
+    </row>
+    <row r="2475" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2475" s="4" t="s">
+        <v>7651</v>
+      </c>
+      <c r="B2475" s="3" t="s">
+        <v>7652</v>
+      </c>
+      <c r="C2475" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2475" s="3" t="s">
+        <v>1156</v>
+      </c>
+      <c r="E2475" s="3" t="s">
+        <v>7653</v>
+      </c>
+      <c r="F2475" s="3">
+        <v>45936.70625</v>
+      </c>
+    </row>
+    <row r="2476" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2476" s="4" t="s">
+        <v>7654</v>
+      </c>
+      <c r="B2476" s="3" t="s">
+        <v>7655</v>
+      </c>
+      <c r="C2476" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2476" s="3" t="s">
+        <v>6086</v>
+      </c>
+      <c r="E2476" s="3" t="s">
+        <v>7656</v>
+      </c>
+      <c r="F2476" s="3">
+        <v>45937.425</v>
+      </c>
+    </row>
+    <row r="2477" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2477" s="4" t="s">
+        <v>7657</v>
+      </c>
+      <c r="B2477" s="3" t="s">
+        <v>7658</v>
+      </c>
+      <c r="C2477" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2477" s="3" t="s">
+        <v>4888</v>
+      </c>
+      <c r="E2477" s="3" t="s">
+        <v>7659</v>
+      </c>
+      <c r="F2477" s="3">
+        <v>45937.36041666666</v>
+      </c>
+    </row>
+    <row r="2478" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2478" s="4" t="s">
+        <v>7660</v>
+      </c>
+      <c r="B2478" s="3" t="s">
+        <v>7661</v>
+      </c>
+      <c r="C2478" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2478" s="3" t="s">
+        <v>7662</v>
+      </c>
+      <c r="E2478" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2478" s="3">
+        <v>45936.69305555556</v>
+      </c>
+    </row>
+    <row r="2479" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2479" s="4" t="s">
+        <v>7663</v>
+      </c>
+      <c r="B2479" s="3" t="s">
+        <v>1387</v>
+      </c>
+      <c r="C2479" s="3" t="s">
+        <v>6133</v>
+      </c>
+      <c r="D2479" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="E2479" s="3" t="s">
+        <v>7664</v>
+      </c>
+      <c r="F2479" s="3">
+        <v>45937.632638888885</v>
+      </c>
+    </row>
+    <row r="2480" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2480" s="4" t="s">
+        <v>7665</v>
+      </c>
+      <c r="B2480" s="3" t="s">
+        <v>7666</v>
+      </c>
+      <c r="C2480" s="3" t="s">
+        <v>6133</v>
+      </c>
+      <c r="D2480" s="3" t="s">
+        <v>7667</v>
+      </c>
+      <c r="E2480" s="3" t="s">
+        <v>7668</v>
+      </c>
+      <c r="F2480" s="3">
+        <v>45936.77986111111</v>
+      </c>
+    </row>
+    <row r="2481" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2481" s="4" t="s">
+        <v>7669</v>
+      </c>
+      <c r="B2481" s="3" t="s">
+        <v>7670</v>
+      </c>
+      <c r="C2481" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2481" s="3" t="s">
+        <v>7671</v>
+      </c>
+      <c r="E2481" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2481" s="3">
+        <v>45937.4875</v>
+      </c>
+    </row>
+    <row r="2482" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2482" s="4" t="s">
+        <v>7672</v>
+      </c>
+      <c r="B2482" s="3" t="s">
+        <v>7673</v>
+      </c>
+      <c r="C2482" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2482" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E2482" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2482" s="3">
+        <v>45936.70277777778</v>
+      </c>
+    </row>
+    <row r="2483" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2483" s="4" t="s">
+        <v>7674</v>
+      </c>
+      <c r="B2483" s="3" t="s">
+        <v>7675</v>
+      </c>
+      <c r="C2483" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2483" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="E2483" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2483" s="3">
+        <v>45936.70208333334</v>
+      </c>
+    </row>
+    <row r="2484" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2484" s="4" t="s">
+        <v>7676</v>
+      </c>
+      <c r="B2484" s="3" t="s">
+        <v>7677</v>
+      </c>
+      <c r="C2484" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2484" s="3" t="s">
+        <v>4546</v>
+      </c>
+      <c r="E2484" s="3" t="s">
+        <v>7678</v>
+      </c>
+      <c r="F2484" s="3">
+        <v>45937.46597222222</v>
+      </c>
+    </row>
+    <row r="2485" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2485" s="4" t="s">
+        <v>7679</v>
+      </c>
+      <c r="B2485" s="3" t="s">
+        <v>7680</v>
+      </c>
+      <c r="C2485" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2485" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2485" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2485" s="3">
+        <v>45936.88888888889</v>
       </c>
     </row>
   </sheetData>
@@ -75747,6 +76330,44 @@
     <hyperlink ref="A2445" r:id="rId2444"/>
     <hyperlink ref="A2446" r:id="rId2445"/>
     <hyperlink ref="A2447" r:id="rId2446"/>
+    <hyperlink ref="A2448" r:id="rId2447"/>
+    <hyperlink ref="A2449" r:id="rId2448"/>
+    <hyperlink ref="A2450" r:id="rId2449"/>
+    <hyperlink ref="A2451" r:id="rId2450"/>
+    <hyperlink ref="A2452" r:id="rId2451"/>
+    <hyperlink ref="A2453" r:id="rId2452"/>
+    <hyperlink ref="A2454" r:id="rId2453"/>
+    <hyperlink ref="A2455" r:id="rId2454"/>
+    <hyperlink ref="A2456" r:id="rId2455"/>
+    <hyperlink ref="A2457" r:id="rId2456"/>
+    <hyperlink ref="A2458" r:id="rId2457"/>
+    <hyperlink ref="A2459" r:id="rId2458"/>
+    <hyperlink ref="A2460" r:id="rId2459"/>
+    <hyperlink ref="A2461" r:id="rId2460"/>
+    <hyperlink ref="A2462" r:id="rId2461"/>
+    <hyperlink ref="A2463" r:id="rId2462"/>
+    <hyperlink ref="A2464" r:id="rId2463"/>
+    <hyperlink ref="A2465" r:id="rId2464"/>
+    <hyperlink ref="A2466" r:id="rId2465"/>
+    <hyperlink ref="A2467" r:id="rId2466"/>
+    <hyperlink ref="A2468" r:id="rId2467"/>
+    <hyperlink ref="A2469" r:id="rId2468"/>
+    <hyperlink ref="A2470" r:id="rId2469"/>
+    <hyperlink ref="A2471" r:id="rId2470"/>
+    <hyperlink ref="A2472" r:id="rId2471"/>
+    <hyperlink ref="A2473" r:id="rId2472"/>
+    <hyperlink ref="A2474" r:id="rId2473"/>
+    <hyperlink ref="A2475" r:id="rId2474"/>
+    <hyperlink ref="A2476" r:id="rId2475"/>
+    <hyperlink ref="A2477" r:id="rId2476"/>
+    <hyperlink ref="A2478" r:id="rId2477"/>
+    <hyperlink ref="A2479" r:id="rId2478"/>
+    <hyperlink ref="A2480" r:id="rId2479"/>
+    <hyperlink ref="A2481" r:id="rId2480"/>
+    <hyperlink ref="A2482" r:id="rId2481"/>
+    <hyperlink ref="A2483" r:id="rId2482"/>
+    <hyperlink ref="A2484" r:id="rId2483"/>
+    <hyperlink ref="A2485" r:id="rId2484"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Update lands data - 2025-10-09 12:20
</commit_message>
<xml_diff>
--- a/lands-scraped.xlsx
+++ b/lands-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12537" uniqueCount="7741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12637" uniqueCount="7796">
   <si>
     <t>link</t>
   </si>
@@ -23241,6 +23241,171 @@
   </si>
   <si>
     <t>3510 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/aizkraukle-and-reg/staburaga-pag/agelf.html</t>
+  </si>
+  <si>
+    <t>21 500 € (1.08 €/m²)</t>
+  </si>
+  <si>
+    <t>32840020237</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/balvi-and-reg/balvi/fnfbj.html</t>
+  </si>
+  <si>
+    <t>11 000 € (9.22 €/m²)</t>
+  </si>
+  <si>
+    <t>1193 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/nitaures-pag/gdigf.html</t>
+  </si>
+  <si>
+    <t>148 800 € (0.40 €/m²)</t>
+  </si>
+  <si>
+    <t>37.10 ha.</t>
+  </si>
+  <si>
+    <t>42680050081</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/malinovas-pag/bdpmek.html</t>
+  </si>
+  <si>
+    <t>29 500 € (0.33 €/m²)</t>
+  </si>
+  <si>
+    <t>4470 004 0139</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/daugavpils/ixifp.html</t>
+  </si>
+  <si>
+    <t>12 500 € (2.37 €/m²)</t>
+  </si>
+  <si>
+    <t>5277 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/dobele-and-reg/penkules-pag/iicio.html</t>
+  </si>
+  <si>
+    <t>145 600 € (0.80 €/m²)</t>
+  </si>
+  <si>
+    <t>18.20 ha.</t>
+  </si>
+  <si>
+    <t>46840040044</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jekabpils-and-reg/other/nbmem.html</t>
+  </si>
+  <si>
+    <t>569600200900</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jekabpils-and-reg/asares-pag/cggfbj.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/valgundes-nov/cjhxl.html</t>
+  </si>
+  <si>
+    <t>49 000 € (7 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/valgundes-nov/bxiipg.html</t>
+  </si>
+  <si>
+    <t>60 000 € (6.06 €/m²)</t>
+  </si>
+  <si>
+    <t>0.99 ha.</t>
+  </si>
+  <si>
+    <t>54860040183</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kuldiga-and-reg/kuldiga/cgdbxx.html</t>
+  </si>
+  <si>
+    <t>22 000 € (22 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/grobinas-pag/pglmf.html</t>
+  </si>
+  <si>
+    <t>16 500 € (4.34 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/jumpravas-pag/aacfj.html</t>
+  </si>
+  <si>
+    <t>12 000 € (0.66 €/m²)</t>
+  </si>
+  <si>
+    <t>74480050137</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/lielvarde/agkpm.html</t>
+  </si>
+  <si>
+    <t>34 340 € (17 €/m²)</t>
+  </si>
+  <si>
+    <t>74130010733</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/preili-and-reg/livani/bbhhlg.html</t>
+  </si>
+  <si>
+    <t>35 000 € (1.61 €/m²)</t>
+  </si>
+  <si>
+    <t>21714 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/sakstagala-pag/hmixc.html</t>
+  </si>
+  <si>
+    <t>1 500 € (0.15 €/m²)</t>
+  </si>
+  <si>
+    <t>78860010190</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/rojas-pag/hldkh.html</t>
+  </si>
+  <si>
+    <t>85 000 € (28.28 €/m²)</t>
+  </si>
+  <si>
+    <t>8882 010 0341</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/mersraga-pag/ihcfn.html</t>
+  </si>
+  <si>
+    <t>39 000 € (0.93 €/m²)</t>
+  </si>
+  <si>
+    <t>88780030397</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/varves-pag/flgmo.html</t>
+  </si>
+  <si>
+    <t>40 000 € (0.67 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/varves-pag/hjmkb.html</t>
+  </si>
+  <si>
+    <t>11 000 € (1.57 €/m²)</t>
   </si>
 </sst>
 </file>
@@ -23676,7 +23841,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -23715,422 +23880,402 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>7681</v>
+        <v>7741</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>915</v>
+        <v>7742</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>772</v>
+        <v>8</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>171</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>10</v>
+        <v>7743</v>
       </c>
       <c r="F2" s="3">
-        <v>45937.79305555555</v>
+        <v>45938.879166666666</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>7682</v>
+        <v>7744</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>7683</v>
+        <v>7745</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1218</v>
+        <v>324</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>171</v>
+        <v>7746</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>7684</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3">
-        <v>45938.63402777778</v>
+        <v>45938.8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>7685</v>
+        <v>7747</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>7686</v>
+        <v>7748</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>1733</v>
+        <v>772</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>7687</v>
+        <v>7749</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>7688</v>
+        <v>7750</v>
       </c>
       <c r="F4" s="3">
-        <v>45938.44305555556</v>
+        <v>45939.035416666666</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>7689</v>
+        <v>7751</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>7690</v>
+        <v>7752</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>1929</v>
+        <v>1218</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>7691</v>
+        <v>1430</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>7692</v>
+        <v>7753</v>
       </c>
       <c r="F5" s="3">
-        <v>45938.4</v>
+        <v>45939.60972222222</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>7693</v>
+        <v>7754</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>7694</v>
+        <v>7755</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>2488</v>
+        <v>1218</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>4276</v>
+        <v>7756</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>7695</v>
+        <v>10</v>
       </c>
       <c r="F6" s="3">
-        <v>45937.73541666666</v>
+        <v>45939.50208333333</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>7696</v>
+        <v>7757</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>426</v>
+        <v>7758</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>2488</v>
+        <v>1569</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>353</v>
+        <v>7759</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>7697</v>
+        <v>7760</v>
       </c>
       <c r="F7" s="3">
-        <v>45937.66458333333</v>
+        <v>45939.569444444445</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>7698</v>
+        <v>7761</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>7699</v>
+        <v>5125</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>3398</v>
+        <v>1733</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>4254</v>
+        <v>383</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>10</v>
+        <v>7762</v>
       </c>
       <c r="F8" s="3">
-        <v>45938.54166666667</v>
+        <v>45939.59097222222</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>7700</v>
+        <v>7763</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>7701</v>
+        <v>1614</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>3398</v>
+        <v>1733</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>201</v>
+        <v>32</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>7618</v>
+        <v>7182</v>
       </c>
       <c r="F9" s="3">
-        <v>45938.53055555555</v>
+        <v>45938.7125</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>7702</v>
+        <v>7764</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>7703</v>
+        <v>7765</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>3398</v>
+        <v>1929</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>488</v>
+        <v>9</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="3">
-        <v>45938.48541666666</v>
+        <v>45939.56111111111</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>7704</v>
+        <v>7766</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>7705</v>
+        <v>7767</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>3398</v>
+        <v>1929</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>7706</v>
+        <v>7768</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>10</v>
+        <v>7769</v>
       </c>
       <c r="F11" s="3">
-        <v>45938.37152777778</v>
+        <v>45938.88333333333</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>7707</v>
+        <v>7770</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>7708</v>
+        <v>7771</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>4034</v>
+        <v>2671</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>7709</v>
+        <v>71</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>7710</v>
+        <v>10</v>
       </c>
       <c r="F12" s="3">
-        <v>45938.62013888889</v>
+        <v>45938.93680555555</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>7711</v>
+        <v>7772</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>7712</v>
+        <v>7773</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>4034</v>
+        <v>2846</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>2271</v>
+        <v>1054</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>7713</v>
+        <v>10</v>
       </c>
       <c r="F13" s="3">
-        <v>45938.41527777778</v>
+        <v>45939.48958333333</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>7714</v>
+        <v>7774</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>7715</v>
+        <v>7775</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>4034</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>7716</v>
+        <v>4358</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>7717</v>
+        <v>7776</v>
       </c>
       <c r="F14" s="3">
-        <v>45937.80138888889</v>
+        <v>45939.339583333334</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>7718</v>
+        <v>7777</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>7719</v>
+        <v>7778</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>4671</v>
+        <v>4034</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>2522</v>
+        <v>484</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>7720</v>
+        <v>7779</v>
       </c>
       <c r="F15" s="3">
-        <v>45937.89097222222</v>
+        <v>45938.68958333333</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>7721</v>
+        <v>7780</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>7722</v>
+        <v>7781</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>4770</v>
+        <v>4671</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>7723</v>
+        <v>7782</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>10</v>
+        <v>7540</v>
       </c>
       <c r="F16" s="3">
-        <v>45938.6</v>
+        <v>45938.78472222222</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>7724</v>
+        <v>7783</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>7725</v>
+        <v>7784</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>4770</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>7726</v>
+        <v>32</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>10</v>
+        <v>7785</v>
       </c>
       <c r="F17" s="3">
-        <v>45937.7375</v>
+        <v>45939.54513888889</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>7727</v>
+        <v>7786</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>7728</v>
+        <v>7787</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>5674</v>
+        <v>5266</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>201</v>
+        <v>593</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>7729</v>
+        <v>7788</v>
       </c>
       <c r="F18" s="3">
-        <v>45938.45694444445</v>
+        <v>45938.86875</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>7730</v>
+        <v>7789</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>7731</v>
+        <v>7790</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>6207</v>
+        <v>5266</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>7732</v>
+        <v>4882</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>7733</v>
+        <v>7791</v>
       </c>
       <c r="F19" s="3">
-        <v>45938.44652777778</v>
+        <v>45938.68402777778</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>7734</v>
+        <v>7792</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>6223</v>
+        <v>7793</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>6207</v>
+        <v>6439</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>2271</v>
+        <v>383</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F20" s="3">
-        <v>45937.87430555555</v>
+        <v>45939.44097222222</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>7735</v>
+        <v>7794</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>7736</v>
+        <v>7795</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>6207</v>
+        <v>6439</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>7737</v>
+        <v>9</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F21" s="3">
-        <v>45937.79583333334</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>7738</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>7739</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>6207</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>7740</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="3">
-        <v>45937.65347222222</v>
+        <v>45939.44097222222</v>
       </c>
     </row>
   </sheetData>
@@ -24155,7 +24300,6 @@
     <hyperlink ref="A19" r:id="rId18"/>
     <hyperlink ref="A20" r:id="rId19"/>
     <hyperlink ref="A21" r:id="rId20"/>
-    <hyperlink ref="A22" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -24164,7 +24308,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2485"/>
+  <dimension ref="A1:F2506"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -73880,6 +74024,426 @@
       </c>
       <c r="F2485" s="3">
         <v>45936.88888888889</v>
+      </c>
+    </row>
+    <row r="2486" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2486" s="4" t="s">
+        <v>7681</v>
+      </c>
+      <c r="B2486" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="C2486" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2486" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2486" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2486" s="3">
+        <v>45937.79305555555</v>
+      </c>
+    </row>
+    <row r="2487" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2487" s="4" t="s">
+        <v>7682</v>
+      </c>
+      <c r="B2487" s="3" t="s">
+        <v>7683</v>
+      </c>
+      <c r="C2487" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2487" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2487" s="3" t="s">
+        <v>7684</v>
+      </c>
+      <c r="F2487" s="3">
+        <v>45938.63402777778</v>
+      </c>
+    </row>
+    <row r="2488" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2488" s="4" t="s">
+        <v>7685</v>
+      </c>
+      <c r="B2488" s="3" t="s">
+        <v>7686</v>
+      </c>
+      <c r="C2488" s="3" t="s">
+        <v>1733</v>
+      </c>
+      <c r="D2488" s="3" t="s">
+        <v>7687</v>
+      </c>
+      <c r="E2488" s="3" t="s">
+        <v>7688</v>
+      </c>
+      <c r="F2488" s="3">
+        <v>45938.44305555556</v>
+      </c>
+    </row>
+    <row r="2489" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2489" s="4" t="s">
+        <v>7689</v>
+      </c>
+      <c r="B2489" s="3" t="s">
+        <v>7690</v>
+      </c>
+      <c r="C2489" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2489" s="3" t="s">
+        <v>7691</v>
+      </c>
+      <c r="E2489" s="3" t="s">
+        <v>7692</v>
+      </c>
+      <c r="F2489" s="3">
+        <v>45938.4</v>
+      </c>
+    </row>
+    <row r="2490" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2490" s="4" t="s">
+        <v>7693</v>
+      </c>
+      <c r="B2490" s="3" t="s">
+        <v>7694</v>
+      </c>
+      <c r="C2490" s="3" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D2490" s="3" t="s">
+        <v>4276</v>
+      </c>
+      <c r="E2490" s="3" t="s">
+        <v>7695</v>
+      </c>
+      <c r="F2490" s="3">
+        <v>45937.73541666666</v>
+      </c>
+    </row>
+    <row r="2491" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2491" s="4" t="s">
+        <v>7696</v>
+      </c>
+      <c r="B2491" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="C2491" s="3" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D2491" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="E2491" s="3" t="s">
+        <v>7697</v>
+      </c>
+      <c r="F2491" s="3">
+        <v>45937.66458333333</v>
+      </c>
+    </row>
+    <row r="2492" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2492" s="4" t="s">
+        <v>7698</v>
+      </c>
+      <c r="B2492" s="3" t="s">
+        <v>7699</v>
+      </c>
+      <c r="C2492" s="3" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D2492" s="3" t="s">
+        <v>4254</v>
+      </c>
+      <c r="E2492" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2492" s="3">
+        <v>45938.54166666667</v>
+      </c>
+    </row>
+    <row r="2493" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2493" s="4" t="s">
+        <v>7700</v>
+      </c>
+      <c r="B2493" s="3" t="s">
+        <v>7701</v>
+      </c>
+      <c r="C2493" s="3" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D2493" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2493" s="3" t="s">
+        <v>7618</v>
+      </c>
+      <c r="F2493" s="3">
+        <v>45938.53055555555</v>
+      </c>
+    </row>
+    <row r="2494" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2494" s="4" t="s">
+        <v>7702</v>
+      </c>
+      <c r="B2494" s="3" t="s">
+        <v>7703</v>
+      </c>
+      <c r="C2494" s="3" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D2494" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="E2494" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2494" s="3">
+        <v>45938.48541666666</v>
+      </c>
+    </row>
+    <row r="2495" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2495" s="4" t="s">
+        <v>7704</v>
+      </c>
+      <c r="B2495" s="3" t="s">
+        <v>7705</v>
+      </c>
+      <c r="C2495" s="3" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D2495" s="3" t="s">
+        <v>7706</v>
+      </c>
+      <c r="E2495" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2495" s="3">
+        <v>45938.37152777778</v>
+      </c>
+    </row>
+    <row r="2496" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2496" s="4" t="s">
+        <v>7707</v>
+      </c>
+      <c r="B2496" s="3" t="s">
+        <v>7708</v>
+      </c>
+      <c r="C2496" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2496" s="3" t="s">
+        <v>7709</v>
+      </c>
+      <c r="E2496" s="3" t="s">
+        <v>7710</v>
+      </c>
+      <c r="F2496" s="3">
+        <v>45938.62013888889</v>
+      </c>
+    </row>
+    <row r="2497" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2497" s="4" t="s">
+        <v>7711</v>
+      </c>
+      <c r="B2497" s="3" t="s">
+        <v>7712</v>
+      </c>
+      <c r="C2497" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2497" s="3" t="s">
+        <v>2271</v>
+      </c>
+      <c r="E2497" s="3" t="s">
+        <v>7713</v>
+      </c>
+      <c r="F2497" s="3">
+        <v>45938.41527777778</v>
+      </c>
+    </row>
+    <row r="2498" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2498" s="4" t="s">
+        <v>7714</v>
+      </c>
+      <c r="B2498" s="3" t="s">
+        <v>7715</v>
+      </c>
+      <c r="C2498" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2498" s="3" t="s">
+        <v>7716</v>
+      </c>
+      <c r="E2498" s="3" t="s">
+        <v>7717</v>
+      </c>
+      <c r="F2498" s="3">
+        <v>45937.80138888889</v>
+      </c>
+    </row>
+    <row r="2499" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2499" s="4" t="s">
+        <v>7718</v>
+      </c>
+      <c r="B2499" s="3" t="s">
+        <v>7719</v>
+      </c>
+      <c r="C2499" s="3" t="s">
+        <v>4671</v>
+      </c>
+      <c r="D2499" s="3" t="s">
+        <v>2522</v>
+      </c>
+      <c r="E2499" s="3" t="s">
+        <v>7720</v>
+      </c>
+      <c r="F2499" s="3">
+        <v>45937.89097222222</v>
+      </c>
+    </row>
+    <row r="2500" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2500" s="4" t="s">
+        <v>7721</v>
+      </c>
+      <c r="B2500" s="3" t="s">
+        <v>7722</v>
+      </c>
+      <c r="C2500" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2500" s="3" t="s">
+        <v>7723</v>
+      </c>
+      <c r="E2500" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2500" s="3">
+        <v>45938.6</v>
+      </c>
+    </row>
+    <row r="2501" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2501" s="4" t="s">
+        <v>7724</v>
+      </c>
+      <c r="B2501" s="3" t="s">
+        <v>7725</v>
+      </c>
+      <c r="C2501" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2501" s="3" t="s">
+        <v>7726</v>
+      </c>
+      <c r="E2501" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2501" s="3">
+        <v>45937.7375</v>
+      </c>
+    </row>
+    <row r="2502" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2502" s="4" t="s">
+        <v>7727</v>
+      </c>
+      <c r="B2502" s="3" t="s">
+        <v>7728</v>
+      </c>
+      <c r="C2502" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2502" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2502" s="3" t="s">
+        <v>7729</v>
+      </c>
+      <c r="F2502" s="3">
+        <v>45938.45694444445</v>
+      </c>
+    </row>
+    <row r="2503" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2503" s="4" t="s">
+        <v>7730</v>
+      </c>
+      <c r="B2503" s="3" t="s">
+        <v>7731</v>
+      </c>
+      <c r="C2503" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2503" s="3" t="s">
+        <v>7732</v>
+      </c>
+      <c r="E2503" s="3" t="s">
+        <v>7733</v>
+      </c>
+      <c r="F2503" s="3">
+        <v>45938.44652777778</v>
+      </c>
+    </row>
+    <row r="2504" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2504" s="4" t="s">
+        <v>7734</v>
+      </c>
+      <c r="B2504" s="3" t="s">
+        <v>6223</v>
+      </c>
+      <c r="C2504" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2504" s="3" t="s">
+        <v>2271</v>
+      </c>
+      <c r="E2504" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2504" s="3">
+        <v>45937.87430555555</v>
+      </c>
+    </row>
+    <row r="2505" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2505" s="4" t="s">
+        <v>7735</v>
+      </c>
+      <c r="B2505" s="3" t="s">
+        <v>7736</v>
+      </c>
+      <c r="C2505" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2505" s="3" t="s">
+        <v>7737</v>
+      </c>
+      <c r="E2505" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2505" s="3">
+        <v>45937.79583333334</v>
+      </c>
+    </row>
+    <row r="2506" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2506" s="4" t="s">
+        <v>7738</v>
+      </c>
+      <c r="B2506" s="3" t="s">
+        <v>7739</v>
+      </c>
+      <c r="C2506" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2506" s="3" t="s">
+        <v>7740</v>
+      </c>
+      <c r="E2506" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2506" s="3">
+        <v>45937.65347222222</v>
       </c>
     </row>
   </sheetData>
@@ -76368,6 +76932,27 @@
     <hyperlink ref="A2483" r:id="rId2482"/>
     <hyperlink ref="A2484" r:id="rId2483"/>
     <hyperlink ref="A2485" r:id="rId2484"/>
+    <hyperlink ref="A2486" r:id="rId2485"/>
+    <hyperlink ref="A2487" r:id="rId2486"/>
+    <hyperlink ref="A2488" r:id="rId2487"/>
+    <hyperlink ref="A2489" r:id="rId2488"/>
+    <hyperlink ref="A2490" r:id="rId2489"/>
+    <hyperlink ref="A2491" r:id="rId2490"/>
+    <hyperlink ref="A2492" r:id="rId2491"/>
+    <hyperlink ref="A2493" r:id="rId2492"/>
+    <hyperlink ref="A2494" r:id="rId2493"/>
+    <hyperlink ref="A2495" r:id="rId2494"/>
+    <hyperlink ref="A2496" r:id="rId2495"/>
+    <hyperlink ref="A2497" r:id="rId2496"/>
+    <hyperlink ref="A2498" r:id="rId2497"/>
+    <hyperlink ref="A2499" r:id="rId2498"/>
+    <hyperlink ref="A2500" r:id="rId2499"/>
+    <hyperlink ref="A2501" r:id="rId2500"/>
+    <hyperlink ref="A2502" r:id="rId2501"/>
+    <hyperlink ref="A2503" r:id="rId2502"/>
+    <hyperlink ref="A2504" r:id="rId2503"/>
+    <hyperlink ref="A2505" r:id="rId2504"/>
+    <hyperlink ref="A2506" r:id="rId2505"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Update lands data - 2025-10-10 12:21
</commit_message>
<xml_diff>
--- a/lands-scraped.xlsx
+++ b/lands-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12637" uniqueCount="7796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12767" uniqueCount="7867">
   <si>
     <t>link</t>
   </si>
@@ -23406,6 +23406,219 @@
   </si>
   <si>
     <t>11 000 € (1.57 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/aizkraukle-and-reg/pilskalnes-pag/egnib.html</t>
+  </si>
+  <si>
+    <t>75 000 € (0.37 €/m²)</t>
+  </si>
+  <si>
+    <t>20.30 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/iecavas-nov/ajmkj.html</t>
+  </si>
+  <si>
+    <t>26 460 € (7 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/rundales-pag/jgmkp.html</t>
+  </si>
+  <si>
+    <t>40760060215</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/barbeles-pag/knxfn.html</t>
+  </si>
+  <si>
+    <t>20 000 € (2.74 €/m²)</t>
+  </si>
+  <si>
+    <t>40440030092</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/barbeles-pag/kcofd.html</t>
+  </si>
+  <si>
+    <t>15 000 € (1.25 €/m²)</t>
+  </si>
+  <si>
+    <t>40440030036</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/drustu-pag/eflpf.html</t>
+  </si>
+  <si>
+    <t>91 200 € (0.38 €/m²)</t>
+  </si>
+  <si>
+    <t>4276 011 0045</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/cesis/agpio.html</t>
+  </si>
+  <si>
+    <t>185 000 € (18.48 €/m²)</t>
+  </si>
+  <si>
+    <t>10011 m²</t>
+  </si>
+  <si>
+    <t>42010040416</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/drabesu-pag/amkmi.html</t>
+  </si>
+  <si>
+    <t>260 000 € (0.81 €/m²)</t>
+  </si>
+  <si>
+    <t>42460020118</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/daugavpils/dpnjg.html</t>
+  </si>
+  <si>
+    <t>30 000 € (9.09 €/m²)</t>
+  </si>
+  <si>
+    <t>05000200087</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jekabpils-and-reg/dunavas-pag/mkjii.html</t>
+  </si>
+  <si>
+    <t>56540080085</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/vilces-pag/agbmi.html</t>
+  </si>
+  <si>
+    <t>4 000 € (1.48 €/m²)</t>
+  </si>
+  <si>
+    <t>54900020050</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kraslava-and-reg/udrisu-pag/fcjhf.html</t>
+  </si>
+  <si>
+    <t>38 750 € (0.24 €/m²)</t>
+  </si>
+  <si>
+    <t>60960040168</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kraslava-and-reg/udrisu-pag/abbpp.html</t>
+  </si>
+  <si>
+    <t>37 500 € (0.25 €/m²)</t>
+  </si>
+  <si>
+    <t>60960040167</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kraslava-and-reg/kaplavas-pag/acgmn.html</t>
+  </si>
+  <si>
+    <t>130 000 € (0.26 €/m²)</t>
+  </si>
+  <si>
+    <t>60700090260</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kuldiga-and-reg/kuldiga/ajmbc.html</t>
+  </si>
+  <si>
+    <t>29 000 € (24.13 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kuldiga-and-reg/kurmales-pag/imhpd.html</t>
+  </si>
+  <si>
+    <t>11 000 € (2.16 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/grobinas-pag/ddfgx.html</t>
+  </si>
+  <si>
+    <t>17 000 € (24.29 €/m²)</t>
+  </si>
+  <si>
+    <t>64760021880</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/nicas-pag/aaepn.html</t>
+  </si>
+  <si>
+    <t>49 900 € (0.71 €/m²)</t>
+  </si>
+  <si>
+    <t>64780040059</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/madona-and-reg/liezeres-pag/fedco.html</t>
+  </si>
+  <si>
+    <t>50 000 € (0.25 €/m²)</t>
+  </si>
+  <si>
+    <t>70680090038</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/rezekne/bigpi.html</t>
+  </si>
+  <si>
+    <t>31 777 € (3.15 €/m²)</t>
+  </si>
+  <si>
+    <t>10080 m²</t>
+  </si>
+  <si>
+    <t>21000030456</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/saldus-and-reg/saldus-pag/hifci.html</t>
+  </si>
+  <si>
+    <t>84860020501</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/abavas-pag/ipbgn.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/laucienes-pag/hihlh.html</t>
+  </si>
+  <si>
+    <t>125 000 € (0.78 €/m²)</t>
+  </si>
+  <si>
+    <t>88700170001</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/gibulu-pag/emilb.html</t>
+  </si>
+  <si>
+    <t>19 000 € (0.70 €/m²)</t>
+  </si>
+  <si>
+    <t>88540090004</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/valmiera/bdllmn.html</t>
+  </si>
+  <si>
+    <t>80 000 € (6.35 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/ventspils/idndg.html</t>
+  </si>
+  <si>
+    <t>70 000 € (58.58 €/m²)</t>
+  </si>
+  <si>
+    <t>27000041312</t>
   </si>
 </sst>
 </file>
@@ -23841,7 +24054,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -23880,402 +24093,522 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>7741</v>
+        <v>7796</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>7742</v>
+        <v>7797</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>171</v>
+        <v>7798</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>7743</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3">
-        <v>45938.879166666666</v>
+        <v>45940.56597222222</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>7744</v>
+        <v>7799</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>7745</v>
+        <v>7800</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>324</v>
+        <v>419</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>7746</v>
+        <v>642</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="3">
-        <v>45938.8</v>
+        <v>45940.50902777778</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>7747</v>
+        <v>7801</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>7748</v>
+        <v>1100</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>772</v>
+        <v>419</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>7749</v>
+        <v>171</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>7750</v>
+        <v>7802</v>
       </c>
       <c r="F4" s="3">
-        <v>45939.035416666666</v>
+        <v>45940.347916666666</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>7751</v>
+        <v>7803</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>7752</v>
+        <v>7804</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>1218</v>
+        <v>419</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>1430</v>
+        <v>6354</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>7753</v>
+        <v>7805</v>
       </c>
       <c r="F5" s="3">
-        <v>45939.60972222222</v>
+        <v>45939.72083333333</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>7754</v>
+        <v>7806</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>7755</v>
+        <v>7807</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1218</v>
+        <v>419</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>7756</v>
+        <v>967</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>10</v>
+        <v>7808</v>
       </c>
       <c r="F6" s="3">
-        <v>45939.50208333333</v>
+        <v>45939.71875</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>7757</v>
+        <v>7809</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>7758</v>
+        <v>7810</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>1569</v>
+        <v>772</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>7759</v>
+        <v>189</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>7760</v>
+        <v>7811</v>
       </c>
       <c r="F7" s="3">
-        <v>45939.569444444445</v>
+        <v>45940.60277777778</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>7761</v>
+        <v>7812</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>5125</v>
+        <v>7813</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1733</v>
+        <v>772</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>383</v>
+        <v>7814</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>7762</v>
+        <v>7815</v>
       </c>
       <c r="F8" s="3">
-        <v>45939.59097222222</v>
+        <v>45940.49652777778</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>7763</v>
+        <v>7816</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>1614</v>
+        <v>7817</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>1733</v>
+        <v>772</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>32</v>
+        <v>1724</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>7182</v>
+        <v>7818</v>
       </c>
       <c r="F9" s="3">
-        <v>45938.7125</v>
+        <v>45940.370833333334</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>7764</v>
+        <v>7819</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>7765</v>
+        <v>7820</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>1929</v>
+        <v>1218</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>9</v>
+        <v>488</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>10</v>
+        <v>7821</v>
       </c>
       <c r="F10" s="3">
-        <v>45939.56111111111</v>
+        <v>45939.80208333333</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>7766</v>
+        <v>7822</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>7767</v>
+        <v>5392</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>1929</v>
+        <v>1733</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>7768</v>
+        <v>171</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>7769</v>
+        <v>7823</v>
       </c>
       <c r="F11" s="3">
-        <v>45938.88333333333</v>
+        <v>45940.58194444445</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>7770</v>
+        <v>7824</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>7771</v>
+        <v>7825</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>2671</v>
+        <v>1929</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>71</v>
+        <v>1655</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>10</v>
+        <v>7826</v>
       </c>
       <c r="F12" s="3">
-        <v>45938.93680555555</v>
+        <v>45939.69930555555</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>7772</v>
+        <v>7827</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>7773</v>
+        <v>7828</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>2846</v>
+        <v>2488</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>1054</v>
+        <v>575</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>10</v>
+        <v>7829</v>
       </c>
       <c r="F13" s="3">
-        <v>45939.48958333333</v>
+        <v>45940.55625</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>7774</v>
+        <v>7830</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>7775</v>
+        <v>7831</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>4034</v>
+        <v>2488</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>4358</v>
+        <v>2191</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>7776</v>
+        <v>7832</v>
       </c>
       <c r="F14" s="3">
-        <v>45939.339583333334</v>
+        <v>45940.554861111115</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>7777</v>
+        <v>7833</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>7778</v>
+        <v>7834</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>4034</v>
+        <v>2488</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>484</v>
+        <v>3916</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>7779</v>
+        <v>7835</v>
       </c>
       <c r="F15" s="3">
-        <v>45938.68958333333</v>
+        <v>45939.78402777778</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>7780</v>
+        <v>7836</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>7781</v>
+        <v>7837</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>4671</v>
+        <v>2671</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>7782</v>
+        <v>4197</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>7540</v>
+        <v>10</v>
       </c>
       <c r="F16" s="3">
-        <v>45938.78472222222</v>
+        <v>45940.56597222222</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>7783</v>
+        <v>7838</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>7784</v>
+        <v>7839</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>4770</v>
+        <v>2671</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>32</v>
+        <v>3368</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>7785</v>
+        <v>10</v>
       </c>
       <c r="F17" s="3">
-        <v>45939.54513888889</v>
+        <v>45940.34722222222</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>7786</v>
+        <v>7840</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>7787</v>
+        <v>7841</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>5266</v>
+        <v>2846</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>593</v>
+        <v>3349</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>7788</v>
+        <v>7842</v>
       </c>
       <c r="F18" s="3">
-        <v>45938.86875</v>
+        <v>45940.447222222225</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>7789</v>
+        <v>7843</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>7790</v>
+        <v>7844</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>5266</v>
+        <v>2846</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>4882</v>
+        <v>407</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>7791</v>
+        <v>7845</v>
       </c>
       <c r="F19" s="3">
-        <v>45938.68402777778</v>
+        <v>45939.68819444445</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>7792</v>
+        <v>7846</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>7793</v>
+        <v>7847</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>6439</v>
+        <v>3868</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>383</v>
+        <v>645</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>10</v>
+        <v>7848</v>
       </c>
       <c r="F20" s="3">
-        <v>45939.44097222222</v>
+        <v>45940.63680555555</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>7794</v>
+        <v>7849</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>7795</v>
+        <v>7850</v>
       </c>
       <c r="C21" s="9" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>7851</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>7852</v>
+      </c>
+      <c r="F21" s="3">
+        <v>45940.55694444444</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>7853</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>3810</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>5147</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>411</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>7854</v>
+      </c>
+      <c r="F22" s="3">
+        <v>45939.70833333333</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>7855</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>1878</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>1430</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="3">
+        <v>45939.87361111111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>7856</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>7857</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>575</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>7858</v>
+      </c>
+      <c r="F24" s="3">
+        <v>45939.78125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>7859</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>7860</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>5559</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>7861</v>
+      </c>
+      <c r="F25" s="3">
+        <v>45939.74513888889</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>7862</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>7863</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>1940</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="3">
+        <v>45939.84236111111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>7864</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>7865</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>6439</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="3">
-        <v>45939.44097222222</v>
+      <c r="D27" s="9" t="s">
+        <v>3124</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>7866</v>
+      </c>
+      <c r="F27" s="3">
+        <v>45939.65694444445</v>
       </c>
     </row>
   </sheetData>
@@ -24300,6 +24633,12 @@
     <hyperlink ref="A19" r:id="rId18"/>
     <hyperlink ref="A20" r:id="rId19"/>
     <hyperlink ref="A21" r:id="rId20"/>
+    <hyperlink ref="A22" r:id="rId21"/>
+    <hyperlink ref="A23" r:id="rId22"/>
+    <hyperlink ref="A24" r:id="rId23"/>
+    <hyperlink ref="A25" r:id="rId24"/>
+    <hyperlink ref="A26" r:id="rId25"/>
+    <hyperlink ref="A27" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -24308,7 +24647,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2506"/>
+  <dimension ref="A1:F2526"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -74444,6 +74783,406 @@
       </c>
       <c r="F2506" s="3">
         <v>45937.65347222222</v>
+      </c>
+    </row>
+    <row r="2507" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2507" s="4" t="s">
+        <v>7741</v>
+      </c>
+      <c r="B2507" s="3" t="s">
+        <v>7742</v>
+      </c>
+      <c r="C2507" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2507" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2507" s="3" t="s">
+        <v>7743</v>
+      </c>
+      <c r="F2507" s="3">
+        <v>45938.879166666666</v>
+      </c>
+    </row>
+    <row r="2508" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2508" s="4" t="s">
+        <v>7744</v>
+      </c>
+      <c r="B2508" s="3" t="s">
+        <v>7745</v>
+      </c>
+      <c r="C2508" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="D2508" s="3" t="s">
+        <v>7746</v>
+      </c>
+      <c r="E2508" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2508" s="3">
+        <v>45938.8</v>
+      </c>
+    </row>
+    <row r="2509" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2509" s="4" t="s">
+        <v>7747</v>
+      </c>
+      <c r="B2509" s="3" t="s">
+        <v>7748</v>
+      </c>
+      <c r="C2509" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2509" s="3" t="s">
+        <v>7749</v>
+      </c>
+      <c r="E2509" s="3" t="s">
+        <v>7750</v>
+      </c>
+      <c r="F2509" s="3">
+        <v>45939.035416666666</v>
+      </c>
+    </row>
+    <row r="2510" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2510" s="4" t="s">
+        <v>7751</v>
+      </c>
+      <c r="B2510" s="3" t="s">
+        <v>7752</v>
+      </c>
+      <c r="C2510" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2510" s="3" t="s">
+        <v>1430</v>
+      </c>
+      <c r="E2510" s="3" t="s">
+        <v>7753</v>
+      </c>
+      <c r="F2510" s="3">
+        <v>45939.60972222222</v>
+      </c>
+    </row>
+    <row r="2511" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2511" s="4" t="s">
+        <v>7754</v>
+      </c>
+      <c r="B2511" s="3" t="s">
+        <v>7755</v>
+      </c>
+      <c r="C2511" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2511" s="3" t="s">
+        <v>7756</v>
+      </c>
+      <c r="E2511" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2511" s="3">
+        <v>45939.50208333333</v>
+      </c>
+    </row>
+    <row r="2512" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2512" s="4" t="s">
+        <v>7757</v>
+      </c>
+      <c r="B2512" s="3" t="s">
+        <v>7758</v>
+      </c>
+      <c r="C2512" s="3" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D2512" s="3" t="s">
+        <v>7759</v>
+      </c>
+      <c r="E2512" s="3" t="s">
+        <v>7760</v>
+      </c>
+      <c r="F2512" s="3">
+        <v>45939.569444444445</v>
+      </c>
+    </row>
+    <row r="2513" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2513" s="4" t="s">
+        <v>7761</v>
+      </c>
+      <c r="B2513" s="3" t="s">
+        <v>5125</v>
+      </c>
+      <c r="C2513" s="3" t="s">
+        <v>1733</v>
+      </c>
+      <c r="D2513" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E2513" s="3" t="s">
+        <v>7762</v>
+      </c>
+      <c r="F2513" s="3">
+        <v>45939.59097222222</v>
+      </c>
+    </row>
+    <row r="2514" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2514" s="4" t="s">
+        <v>7763</v>
+      </c>
+      <c r="B2514" s="3" t="s">
+        <v>1614</v>
+      </c>
+      <c r="C2514" s="3" t="s">
+        <v>1733</v>
+      </c>
+      <c r="D2514" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2514" s="3" t="s">
+        <v>7182</v>
+      </c>
+      <c r="F2514" s="3">
+        <v>45938.7125</v>
+      </c>
+    </row>
+    <row r="2515" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2515" s="4" t="s">
+        <v>7764</v>
+      </c>
+      <c r="B2515" s="3" t="s">
+        <v>7765</v>
+      </c>
+      <c r="C2515" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2515" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2515" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2515" s="3">
+        <v>45939.56111111111</v>
+      </c>
+    </row>
+    <row r="2516" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2516" s="4" t="s">
+        <v>7766</v>
+      </c>
+      <c r="B2516" s="3" t="s">
+        <v>7767</v>
+      </c>
+      <c r="C2516" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2516" s="3" t="s">
+        <v>7768</v>
+      </c>
+      <c r="E2516" s="3" t="s">
+        <v>7769</v>
+      </c>
+      <c r="F2516" s="3">
+        <v>45938.88333333333</v>
+      </c>
+    </row>
+    <row r="2517" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2517" s="4" t="s">
+        <v>7770</v>
+      </c>
+      <c r="B2517" s="3" t="s">
+        <v>7771</v>
+      </c>
+      <c r="C2517" s="3" t="s">
+        <v>2671</v>
+      </c>
+      <c r="D2517" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2517" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2517" s="3">
+        <v>45938.93680555555</v>
+      </c>
+    </row>
+    <row r="2518" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2518" s="4" t="s">
+        <v>7772</v>
+      </c>
+      <c r="B2518" s="3" t="s">
+        <v>7773</v>
+      </c>
+      <c r="C2518" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2518" s="3" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E2518" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2518" s="3">
+        <v>45939.48958333333</v>
+      </c>
+    </row>
+    <row r="2519" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2519" s="4" t="s">
+        <v>7774</v>
+      </c>
+      <c r="B2519" s="3" t="s">
+        <v>7775</v>
+      </c>
+      <c r="C2519" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2519" s="3" t="s">
+        <v>4358</v>
+      </c>
+      <c r="E2519" s="3" t="s">
+        <v>7776</v>
+      </c>
+      <c r="F2519" s="3">
+        <v>45939.339583333334</v>
+      </c>
+    </row>
+    <row r="2520" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2520" s="4" t="s">
+        <v>7777</v>
+      </c>
+      <c r="B2520" s="3" t="s">
+        <v>7778</v>
+      </c>
+      <c r="C2520" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2520" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="E2520" s="3" t="s">
+        <v>7779</v>
+      </c>
+      <c r="F2520" s="3">
+        <v>45938.68958333333</v>
+      </c>
+    </row>
+    <row r="2521" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2521" s="4" t="s">
+        <v>7780</v>
+      </c>
+      <c r="B2521" s="3" t="s">
+        <v>7781</v>
+      </c>
+      <c r="C2521" s="3" t="s">
+        <v>4671</v>
+      </c>
+      <c r="D2521" s="3" t="s">
+        <v>7782</v>
+      </c>
+      <c r="E2521" s="3" t="s">
+        <v>7540</v>
+      </c>
+      <c r="F2521" s="3">
+        <v>45938.78472222222</v>
+      </c>
+    </row>
+    <row r="2522" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2522" s="4" t="s">
+        <v>7783</v>
+      </c>
+      <c r="B2522" s="3" t="s">
+        <v>7784</v>
+      </c>
+      <c r="C2522" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2522" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2522" s="3" t="s">
+        <v>7785</v>
+      </c>
+      <c r="F2522" s="3">
+        <v>45939.54513888889</v>
+      </c>
+    </row>
+    <row r="2523" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2523" s="4" t="s">
+        <v>7786</v>
+      </c>
+      <c r="B2523" s="3" t="s">
+        <v>7787</v>
+      </c>
+      <c r="C2523" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2523" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="E2523" s="3" t="s">
+        <v>7788</v>
+      </c>
+      <c r="F2523" s="3">
+        <v>45938.86875</v>
+      </c>
+    </row>
+    <row r="2524" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2524" s="4" t="s">
+        <v>7789</v>
+      </c>
+      <c r="B2524" s="3" t="s">
+        <v>7790</v>
+      </c>
+      <c r="C2524" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2524" s="3" t="s">
+        <v>4882</v>
+      </c>
+      <c r="E2524" s="3" t="s">
+        <v>7791</v>
+      </c>
+      <c r="F2524" s="3">
+        <v>45938.68402777778</v>
+      </c>
+    </row>
+    <row r="2525" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2525" s="4" t="s">
+        <v>7792</v>
+      </c>
+      <c r="B2525" s="3" t="s">
+        <v>7793</v>
+      </c>
+      <c r="C2525" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2525" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E2525" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2525" s="3">
+        <v>45939.44097222222</v>
+      </c>
+    </row>
+    <row r="2526" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2526" s="4" t="s">
+        <v>7794</v>
+      </c>
+      <c r="B2526" s="3" t="s">
+        <v>7795</v>
+      </c>
+      <c r="C2526" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2526" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2526" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2526" s="3">
+        <v>45939.44097222222</v>
       </c>
     </row>
   </sheetData>
@@ -76953,6 +77692,26 @@
     <hyperlink ref="A2504" r:id="rId2503"/>
     <hyperlink ref="A2505" r:id="rId2504"/>
     <hyperlink ref="A2506" r:id="rId2505"/>
+    <hyperlink ref="A2507" r:id="rId2506"/>
+    <hyperlink ref="A2508" r:id="rId2507"/>
+    <hyperlink ref="A2509" r:id="rId2508"/>
+    <hyperlink ref="A2510" r:id="rId2509"/>
+    <hyperlink ref="A2511" r:id="rId2510"/>
+    <hyperlink ref="A2512" r:id="rId2511"/>
+    <hyperlink ref="A2513" r:id="rId2512"/>
+    <hyperlink ref="A2514" r:id="rId2513"/>
+    <hyperlink ref="A2515" r:id="rId2514"/>
+    <hyperlink ref="A2516" r:id="rId2515"/>
+    <hyperlink ref="A2517" r:id="rId2516"/>
+    <hyperlink ref="A2518" r:id="rId2517"/>
+    <hyperlink ref="A2519" r:id="rId2518"/>
+    <hyperlink ref="A2520" r:id="rId2519"/>
+    <hyperlink ref="A2521" r:id="rId2520"/>
+    <hyperlink ref="A2522" r:id="rId2521"/>
+    <hyperlink ref="A2523" r:id="rId2522"/>
+    <hyperlink ref="A2524" r:id="rId2523"/>
+    <hyperlink ref="A2525" r:id="rId2524"/>
+    <hyperlink ref="A2526" r:id="rId2525"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Update lands data - 2025-10-13 12:21
</commit_message>
<xml_diff>
--- a/lands-scraped.xlsx
+++ b/lands-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12767" uniqueCount="7867">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13112" uniqueCount="8066">
   <si>
     <t>link</t>
   </si>
@@ -23619,6 +23619,603 @@
   </si>
   <si>
     <t>27000041312</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/aluksne-and-reg/aluksne/cfkco.html</t>
+  </si>
+  <si>
+    <t>37 920 € (0.43 €/m²)</t>
+  </si>
+  <si>
+    <t>8.91 ha.</t>
+  </si>
+  <si>
+    <t>36560030236</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/balvi-and-reg/balvu-pag/oebgl.html</t>
+  </si>
+  <si>
+    <t>7 000 € (4.52 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/iecavas-nov/ddhgf.html</t>
+  </si>
+  <si>
+    <t>40640070119</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/stelpes-pag/fjpoh.html</t>
+  </si>
+  <si>
+    <t>10 000 € (0.80 €/m²)</t>
+  </si>
+  <si>
+    <t>1.25 ha.</t>
+  </si>
+  <si>
+    <t>40840010302</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/priekulu-pag/bddcnx.html</t>
+  </si>
+  <si>
+    <t>35 000 € (17.50 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/raunas-pag/dolhm.html</t>
+  </si>
+  <si>
+    <t>20 000 € (0.37 €/m²)</t>
+  </si>
+  <si>
+    <t>54600 m²</t>
+  </si>
+  <si>
+    <t>42760030164</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/amatas-pag/bxemex.html</t>
+  </si>
+  <si>
+    <t>42420050206</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/visku-pag/nfgpd.html</t>
+  </si>
+  <si>
+    <t>46 000 € (0.33 €/m²)</t>
+  </si>
+  <si>
+    <t>44980010228</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/daugavpils/agdnb.html</t>
+  </si>
+  <si>
+    <t>15 000 € (1.30 €/m²)</t>
+  </si>
+  <si>
+    <t>11580 m²</t>
+  </si>
+  <si>
+    <t>05000141901</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/daugavpils/cxnnd.html</t>
+  </si>
+  <si>
+    <t>50 000 € (58.34 €/m²)</t>
+  </si>
+  <si>
+    <t>857 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/tabores-pag/fjnpi.html</t>
+  </si>
+  <si>
+    <t>3 500 € (3.50 €/m²)</t>
+  </si>
+  <si>
+    <t>44920030070</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/dobele-and-reg/auru-pag/cggdd.html</t>
+  </si>
+  <si>
+    <t>19 000 € (29.83 €/m²)</t>
+  </si>
+  <si>
+    <t>637 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/dobele-and-reg/dobele/adjgb.html</t>
+  </si>
+  <si>
+    <t>43 074 € (18 €/m²)</t>
+  </si>
+  <si>
+    <t>2393 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/gulbene-and-reg/stamerienas-pag/iojbe.html</t>
+  </si>
+  <si>
+    <t>40 000 € (0.57 €/m²)</t>
+  </si>
+  <si>
+    <t>50880080170</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/gulbene-and-reg/stradu-pag/blpjh.html</t>
+  </si>
+  <si>
+    <t>18 500 € (0.93 €/m²)</t>
+  </si>
+  <si>
+    <t>50900040048</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/valgundes-nov/dmbhd.html</t>
+  </si>
+  <si>
+    <t>69 000 € (0.69 €/m²)</t>
+  </si>
+  <si>
+    <t>54860100218</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/livberzes-pag/cjfxc.html</t>
+  </si>
+  <si>
+    <t>54620101006</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/valgundes-nov/ahhke.html</t>
+  </si>
+  <si>
+    <t>76 200 € (15 €/m²)</t>
+  </si>
+  <si>
+    <t>5080 m²</t>
+  </si>
+  <si>
+    <t>54860040248</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jaunsvirlaukas-pag/abcbd.html</t>
+  </si>
+  <si>
+    <t>54560030099</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/valgundes-nov/belid.html</t>
+  </si>
+  <si>
+    <t>42 000 € (0.76 €/m²)</t>
+  </si>
+  <si>
+    <t>5.53 ha.</t>
+  </si>
+  <si>
+    <t>54860060075</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kuldiga-and-reg/rendas-pag/djioh.html</t>
+  </si>
+  <si>
+    <t>39 000 € (1.03 €/m²)</t>
+  </si>
+  <si>
+    <t>62800070442</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kuldiga-and-reg/kuldiga/cgdehi.html</t>
+  </si>
+  <si>
+    <t>13 900 € (23.17 €/m²)</t>
+  </si>
+  <si>
+    <t>62010340255</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kuldiga-and-reg/kuldiga/cgggif.html</t>
+  </si>
+  <si>
+    <t>130 000 € (28.20 €/m²)</t>
+  </si>
+  <si>
+    <t>4610 m²</t>
+  </si>
+  <si>
+    <t>62010160014</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kuldiga-and-reg/kuldiga/akpjo.html</t>
+  </si>
+  <si>
+    <t>88 000 € (49.11 €/m²)</t>
+  </si>
+  <si>
+    <t>1792 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/grobina/cknjx.html</t>
+  </si>
+  <si>
+    <t>135 000 € (20.30 €/m²)</t>
+  </si>
+  <si>
+    <t>6649 m²</t>
+  </si>
+  <si>
+    <t>64090020004</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/nicas-pag/nhoii.html</t>
+  </si>
+  <si>
+    <t>155 000 € (7.75 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/nicas-pag/egepo.html</t>
+  </si>
+  <si>
+    <t>38 000 € (1.21 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/rucavas-pag/bixjc.html</t>
+  </si>
+  <si>
+    <t>95 000 € (19 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/limbadzi-and-reg/salacgrivas-l-t/ddenj.html</t>
+  </si>
+  <si>
+    <t>66720070785</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/limbadzi-and-reg/salacgriva/bngbke.html</t>
+  </si>
+  <si>
+    <t>26 000 € (21.67 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ludza-and-reg/lidumnieku-pag/ihdix.html</t>
+  </si>
+  <si>
+    <t>20 000 € (0.42 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/madona-and-reg/madona/bllpf.html</t>
+  </si>
+  <si>
+    <t>100 000 € (1.43 €/m²)</t>
+  </si>
+  <si>
+    <t>70900080105</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/madona-and-reg/kalsnavas-pag/jjgbf.html</t>
+  </si>
+  <si>
+    <t>5 000 € (0.20 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/madona-and-reg/sarkanu-pag/akpon.html</t>
+  </si>
+  <si>
+    <t>60 000 € (0.86 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/madona-and-reg/laudonas-pag/mhdkx.html</t>
+  </si>
+  <si>
+    <t>216 300 € (0.70 €/m²)</t>
+  </si>
+  <si>
+    <t>70860180041</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ikskiles-l-t/dkpkm.html</t>
+  </si>
+  <si>
+    <t>75 600 € (3.50 €/m²)</t>
+  </si>
+  <si>
+    <t>74940040083</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ikskile/fhdhb.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ogresgala-pag/dphox.html</t>
+  </si>
+  <si>
+    <t>61 000 € (3.05 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/jumpravas-pag/ajhmd.html</t>
+  </si>
+  <si>
+    <t>31 000 € (1.83 €/m²)</t>
+  </si>
+  <si>
+    <t>16931 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/jumpravas-pag/bloekd.html</t>
+  </si>
+  <si>
+    <t>6 000 € (0.38 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/preili-and-reg/jersikas-pag/ahdkx.html</t>
+  </si>
+  <si>
+    <t>60 000 € (0.36 €/m²)</t>
+  </si>
+  <si>
+    <t>16.89 ha.</t>
+  </si>
+  <si>
+    <t>76520020399</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/rezekne/ahdlo.html</t>
+  </si>
+  <si>
+    <t>2 800 € (4.67 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/audrinu-pag/kcoxx.html</t>
+  </si>
+  <si>
+    <t>44 500 € (0.41 €/m²)</t>
+  </si>
+  <si>
+    <t>78420020046</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/saldus-and-reg/saldus/ibjlg.html</t>
+  </si>
+  <si>
+    <t>52 465 € (15.96 €/m²)</t>
+  </si>
+  <si>
+    <t>3287 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/mersraga-pag/fbbmb.html</t>
+  </si>
+  <si>
+    <t>28 500 € (8.85 €/m²)</t>
+  </si>
+  <si>
+    <t>3220 m²</t>
+  </si>
+  <si>
+    <t>88940060056</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/mersraga-pag/cgbxe.html</t>
+  </si>
+  <si>
+    <t>150 000 € (18.21 €/m²)</t>
+  </si>
+  <si>
+    <t>8238 m²</t>
+  </si>
+  <si>
+    <t>88780010253</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/lapmezciema-nov/cnopo.html</t>
+  </si>
+  <si>
+    <t>99 000 € (85.34 €/m²)</t>
+  </si>
+  <si>
+    <t>1160 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/engures-pag/bcgek.html</t>
+  </si>
+  <si>
+    <t>54 000 € (25.91 €/m²)</t>
+  </si>
+  <si>
+    <t>2084 m²</t>
+  </si>
+  <si>
+    <t>90500051146</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/tukums/adgpb.html</t>
+  </si>
+  <si>
+    <t>31 500 € (16.94 €/m²)</t>
+  </si>
+  <si>
+    <t>1860 m²</t>
+  </si>
+  <si>
+    <t>90010010586</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/tukums/ixmkj.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/tumes-pag/afecd.html</t>
+  </si>
+  <si>
+    <t>90840030066</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/tukums/ixifn.html</t>
+  </si>
+  <si>
+    <t>29 500 € (12.29 €/m²)</t>
+  </si>
+  <si>
+    <t>90820080408</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/tukums/ixigh.html</t>
+  </si>
+  <si>
+    <t>59 500 € (8.94 €/m²)</t>
+  </si>
+  <si>
+    <t>6652 m²</t>
+  </si>
+  <si>
+    <t>90820080402</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/pures-pag/gpmil.html</t>
+  </si>
+  <si>
+    <t>350 000 € (0.63 €/m²)</t>
+  </si>
+  <si>
+    <t>90740010020</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/engures-pag/eopxp.html</t>
+  </si>
+  <si>
+    <t>60 000 € (26.09 €/m²)</t>
+  </si>
+  <si>
+    <t>90500060259</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valka-and-reg/smiltene/nekcg.html</t>
+  </si>
+  <si>
+    <t>30 000 € (2.14 €/m²)</t>
+  </si>
+  <si>
+    <t>94800030295</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/valmiera/bgigjn.html</t>
+  </si>
+  <si>
+    <t>96010020601</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/kauguru-pag/bomoe.html</t>
+  </si>
+  <si>
+    <t>9 000 € (12.23 €/m²)</t>
+  </si>
+  <si>
+    <t>736 m²</t>
+  </si>
+  <si>
+    <t>96620020378</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/ventspils/bxxfgh.html</t>
+  </si>
+  <si>
+    <t>10 000 € (11.01 €/m²)</t>
+  </si>
+  <si>
+    <t>27000252439</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/varves-pag/lllkl.html</t>
+  </si>
+  <si>
+    <t>90 000 € (0.75 €/m²)</t>
+  </si>
+  <si>
+    <t>9884 005 0016</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/jurkalnes-pag/cpfke.html</t>
+  </si>
+  <si>
+    <t>26 000 € (0.65 €/m²)</t>
+  </si>
+  <si>
+    <t>9850 001 0250</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/jurkalnes-pag/npgkc.html</t>
+  </si>
+  <si>
+    <t>76 000 € (0.63 €/m²)</t>
+  </si>
+  <si>
+    <t>9850 001 0121</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/uzavas-pag/nmxkj.html</t>
+  </si>
+  <si>
+    <t>28 000 € (0.70 €/m²)</t>
+  </si>
+  <si>
+    <t>9878 002 0055</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/uzavas-pag/bfnom.html</t>
+  </si>
+  <si>
+    <t>85 000 € (0.77 €/m²)</t>
+  </si>
+  <si>
+    <t>9878 002 0063</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/varves-pag/lngdj.html</t>
+  </si>
+  <si>
+    <t>280 000 € (0.73 €/m²)</t>
+  </si>
+  <si>
+    <t>38.20 ha.</t>
+  </si>
+  <si>
+    <t>9884 006 0020</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/varves-pag/illxf.html</t>
+  </si>
+  <si>
+    <t>155 000 € (0.74 €/m²)</t>
+  </si>
+  <si>
+    <t>9884 006 0031</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/varves-pag/elgxd.html</t>
+  </si>
+  <si>
+    <t>140 000 € (0.67 €/m²)</t>
+  </si>
+  <si>
+    <t>9884 006 0005</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/ventspils/bcedb.html</t>
+  </si>
+  <si>
+    <t>9 500 € (5.72 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/ventspils/bmogh.html</t>
+  </si>
+  <si>
+    <t>84 000 € (5.25 €/m²)</t>
+  </si>
+  <si>
+    <t>16000 m²</t>
   </si>
 </sst>
 </file>
@@ -24054,7 +24651,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -24093,50 +24690,50 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>7796</v>
+        <v>7867</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>7797</v>
+        <v>7868</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>8</v>
+        <v>243</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>7798</v>
+        <v>7869</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>10</v>
+        <v>7870</v>
       </c>
       <c r="F2" s="3">
-        <v>45940.56597222222</v>
+        <v>45941.43680555555</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>7799</v>
+        <v>7871</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>7800</v>
+        <v>7872</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>419</v>
+        <v>324</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>642</v>
+        <v>5410</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="3">
-        <v>45940.50902777778</v>
+        <v>45941.81319444445</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>7801</v>
+        <v>7873</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>1100</v>
+        <v>3215</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>419</v>
@@ -24145,470 +24742,1330 @@
         <v>171</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>7802</v>
+        <v>7874</v>
       </c>
       <c r="F4" s="3">
-        <v>45940.347916666666</v>
+        <v>45943.45347222222</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>7803</v>
+        <v>7875</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>7804</v>
+        <v>7876</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>419</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>6354</v>
+        <v>7877</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>7805</v>
+        <v>7878</v>
       </c>
       <c r="F5" s="3">
-        <v>45939.72083333333</v>
+        <v>45940.69930555555</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>7806</v>
+        <v>7879</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>7807</v>
+        <v>7880</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>419</v>
+        <v>772</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>967</v>
+        <v>317</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>7808</v>
+        <v>10</v>
       </c>
       <c r="F6" s="3">
-        <v>45939.71875</v>
+        <v>45942.95208333334</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>7809</v>
+        <v>7881</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>7810</v>
+        <v>7882</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>772</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>189</v>
+        <v>7883</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>7811</v>
+        <v>7884</v>
       </c>
       <c r="F7" s="3">
-        <v>45940.60277777778</v>
+        <v>45942.44583333333</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>7812</v>
+        <v>7885</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>7813</v>
+        <v>2906</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>772</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>7814</v>
+        <v>32</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>7815</v>
+        <v>7886</v>
       </c>
       <c r="F8" s="3">
-        <v>45940.49652777778</v>
+        <v>45941.40486111111</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>7816</v>
+        <v>7887</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>7817</v>
+        <v>7888</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>772</v>
+        <v>1218</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>1724</v>
+        <v>181</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>7818</v>
+        <v>7889</v>
       </c>
       <c r="F9" s="3">
-        <v>45940.370833333334</v>
+        <v>45943.62361111111</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>7819</v>
+        <v>7890</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>7820</v>
+        <v>7891</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>1218</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>488</v>
+        <v>7892</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>7821</v>
+        <v>7893</v>
       </c>
       <c r="F10" s="3">
-        <v>45939.80208333333</v>
+        <v>45943.52222222222</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>7822</v>
+        <v>7894</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>5392</v>
+        <v>7895</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>1733</v>
+        <v>1218</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>171</v>
+        <v>7896</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>7823</v>
+        <v>10</v>
       </c>
       <c r="F11" s="3">
-        <v>45940.58194444445</v>
+        <v>45943.429861111115</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>7824</v>
+        <v>7897</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>7825</v>
+        <v>7898</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>1929</v>
+        <v>1218</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>1655</v>
+        <v>71</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>7826</v>
+        <v>7899</v>
       </c>
       <c r="F12" s="3">
-        <v>45939.69930555555</v>
+        <v>45940.63888888889</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>7827</v>
+        <v>7900</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>7828</v>
+        <v>7901</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>2488</v>
+        <v>1569</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>575</v>
+        <v>7902</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>7829</v>
+        <v>10</v>
       </c>
       <c r="F13" s="3">
-        <v>45940.55625</v>
+        <v>45943.54166666667</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>7830</v>
+        <v>7903</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>7831</v>
+        <v>7904</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>2488</v>
+        <v>1569</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>2191</v>
+        <v>7905</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>7832</v>
+        <v>10</v>
       </c>
       <c r="F14" s="3">
-        <v>45940.554861111115</v>
+        <v>45942.74722222222</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>7833</v>
+        <v>7906</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>7834</v>
+        <v>7907</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>2488</v>
+        <v>1671</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>3916</v>
+        <v>407</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>7835</v>
+        <v>7908</v>
       </c>
       <c r="F15" s="3">
-        <v>45939.78402777778</v>
+        <v>45942.80069444445</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>7836</v>
+        <v>7909</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>7837</v>
+        <v>7910</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>2671</v>
+        <v>1671</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>4197</v>
+        <v>171</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>10</v>
+        <v>7911</v>
       </c>
       <c r="F16" s="3">
-        <v>45940.56597222222</v>
+        <v>45941.91875</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>7838</v>
+        <v>7912</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>7839</v>
+        <v>7913</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>2671</v>
+        <v>1929</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>3368</v>
+        <v>325</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>10</v>
+        <v>7914</v>
       </c>
       <c r="F17" s="3">
-        <v>45940.34722222222</v>
+        <v>45943.42291666666</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>7840</v>
+        <v>7915</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>7841</v>
+        <v>511</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>2846</v>
+        <v>1929</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>3349</v>
+        <v>9</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>7842</v>
+        <v>7916</v>
       </c>
       <c r="F18" s="3">
-        <v>45940.447222222225</v>
+        <v>45943.419444444444</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>7843</v>
+        <v>7917</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>7844</v>
+        <v>7918</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>2846</v>
+        <v>1929</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>407</v>
+        <v>7919</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>7845</v>
+        <v>7920</v>
       </c>
       <c r="F19" s="3">
-        <v>45939.68819444445</v>
+        <v>45942.81597222222</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>7846</v>
+        <v>7921</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>7847</v>
+        <v>7235</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>3868</v>
+        <v>1929</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>645</v>
+        <v>407</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>7848</v>
+        <v>7922</v>
       </c>
       <c r="F20" s="3">
-        <v>45940.63680555555</v>
+        <v>45942.79027777778</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>7849</v>
+        <v>7923</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>7850</v>
+        <v>7924</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>4770</v>
+        <v>1929</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>7851</v>
+        <v>7925</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>7852</v>
+        <v>7926</v>
       </c>
       <c r="F21" s="3">
-        <v>45940.55694444444</v>
+        <v>45941.77083333333</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>7853</v>
+        <v>7927</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>3810</v>
+        <v>7928</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>5147</v>
+        <v>2671</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>411</v>
+        <v>2224</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>7854</v>
+        <v>7929</v>
       </c>
       <c r="F22" s="3">
-        <v>45939.70833333333</v>
+        <v>45942.575</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>7855</v>
+        <v>7930</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>1878</v>
+        <v>7931</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>5266</v>
+        <v>2671</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>1430</v>
+        <v>596</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>10</v>
+        <v>7932</v>
       </c>
       <c r="F23" s="3">
-        <v>45939.87361111111</v>
+        <v>45942.535416666666</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>7856</v>
+        <v>7933</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>7857</v>
+        <v>7934</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>5266</v>
+        <v>2671</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>575</v>
+        <v>7935</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>7858</v>
+        <v>7936</v>
       </c>
       <c r="F24" s="3">
-        <v>45939.78125</v>
+        <v>45940.78472222222</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>7859</v>
+        <v>7937</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>7860</v>
+        <v>7938</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>5266</v>
+        <v>2671</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>5559</v>
+        <v>7939</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>7861</v>
+        <v>10</v>
       </c>
       <c r="F25" s="3">
-        <v>45939.74513888889</v>
+        <v>45940.72986111111</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>7862</v>
+        <v>7940</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>7863</v>
+        <v>7941</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>6207</v>
+        <v>2846</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>1940</v>
+        <v>7942</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>10</v>
+        <v>7943</v>
       </c>
       <c r="F26" s="3">
-        <v>45939.84236111111</v>
+        <v>45943.558333333334</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>7864</v>
+        <v>7944</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>7865</v>
+        <v>7945</v>
       </c>
       <c r="C27" s="9" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="3">
+        <v>45941.825</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>7946</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>7947</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>3414</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="3">
+        <v>45940.72916666667</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>7948</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>7949</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="3">
+        <v>45940.66458333333</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>7950</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>956</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>7951</v>
+      </c>
+      <c r="F30" s="3">
+        <v>45943.36944444444</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>7952</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>7953</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="3">
+        <v>45940.69236111111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>7954</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>7955</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="3">
+        <v>45942.86319444445</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>7956</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>7957</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>3868</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>7958</v>
+      </c>
+      <c r="F33" s="3">
+        <v>45943.61944444444</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>7959</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>7960</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>3868</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>4362</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="3">
+        <v>45943.42152777778</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>7961</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>7962</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>3868</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="3">
+        <v>45942.84097222222</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>7963</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>7964</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>3868</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>5973</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>7965</v>
+      </c>
+      <c r="F36" s="3">
+        <v>45941.71875</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>7966</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>7967</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>5880</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>7968</v>
+      </c>
+      <c r="F37" s="3">
+        <v>45943.42569444445</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>7969</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>4178</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="3">
+        <v>45943.365277777775</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>7970</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>7971</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="3">
+        <v>45943.32638888889</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>7972</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>7973</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>7974</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="3">
+        <v>45942.67222222222</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>7975</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>7976</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>3772</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="3">
+        <v>45941.92638888889</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>7977</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>7978</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>4671</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>7979</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>7980</v>
+      </c>
+      <c r="F42" s="3">
+        <v>45943.44375</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>7981</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>7982</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="3">
+        <v>45942.8125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>7983</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>7984</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>4632</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>7985</v>
+      </c>
+      <c r="F44" s="3">
+        <v>45942.7625</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>7986</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>7987</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>5147</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>7988</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" s="3">
+        <v>45942.57083333333</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>7989</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>7990</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>7991</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>7992</v>
+      </c>
+      <c r="F46" s="3">
+        <v>45943.40416666667</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>7993</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>7994</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>7995</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>7996</v>
+      </c>
+      <c r="F47" s="3">
+        <v>45940.72152777778</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>7997</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>7998</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>7999</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" s="3">
+        <v>45943.63611111111</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>8000</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>8001</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>8002</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>8003</v>
+      </c>
+      <c r="F49" s="3">
+        <v>45943.62013888889</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>8004</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>8005</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>8006</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>8007</v>
+      </c>
+      <c r="F50" s="3">
+        <v>45943.40416666667</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>8008</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>5900</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>5901</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>5902</v>
+      </c>
+      <c r="F51" s="3">
+        <v>45942.618055555555</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>8009</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>897</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>8010</v>
+      </c>
+      <c r="F52" s="3">
+        <v>45942.527083333334</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>8011</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>8012</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>5309</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>8013</v>
+      </c>
+      <c r="F53" s="3">
+        <v>45941.87361111111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
+        <v>8014</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>8015</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>8016</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>8017</v>
+      </c>
+      <c r="F54" s="3">
+        <v>45941.81805555556</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>8018</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>8019</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>8020</v>
+      </c>
+      <c r="F55" s="3">
+        <v>45941.79583333334</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>8021</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>8022</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>8023</v>
+      </c>
+      <c r="F56" s="3">
+        <v>45940.98333333334</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
+        <v>8024</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>8025</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>6133</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>1535</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>8026</v>
+      </c>
+      <c r="F57" s="3">
+        <v>45941.71527777778</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>8027</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>6410</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>6411</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>8028</v>
+      </c>
+      <c r="F58" s="3">
+        <v>45943.580555555556</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
+        <v>8029</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>8030</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>8031</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>8032</v>
+      </c>
+      <c r="F59" s="3">
+        <v>45941.48888888889</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
+        <v>8033</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>8034</v>
+      </c>
+      <c r="C60" s="9" t="s">
         <v>6439</v>
       </c>
-      <c r="D27" s="9" t="s">
-        <v>3124</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>7866</v>
-      </c>
-      <c r="F27" s="3">
-        <v>45939.65694444445</v>
+      <c r="D60" s="9" t="s">
+        <v>7108</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>8035</v>
+      </c>
+      <c r="F60" s="3">
+        <v>45943.575694444444</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
+        <v>8036</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>8037</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>8038</v>
+      </c>
+      <c r="F61" s="3">
+        <v>45943.51527777778</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
+        <v>8039</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>8040</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>8041</v>
+      </c>
+      <c r="F62" s="3">
+        <v>45943.50833333333</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
+        <v>8042</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>8043</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>8044</v>
+      </c>
+      <c r="F63" s="3">
+        <v>45943.506944444445</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
+        <v>8045</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>8046</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>8047</v>
+      </c>
+      <c r="F64" s="3">
+        <v>45943.50625</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
+        <v>8048</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>8049</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>683</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>8050</v>
+      </c>
+      <c r="F65" s="3">
+        <v>45943.50347222222</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
+        <v>8051</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>8052</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>8053</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>8054</v>
+      </c>
+      <c r="F66" s="3">
+        <v>45943.50277777778</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="8" t="s">
+        <v>8055</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>8056</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>1709</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>8057</v>
+      </c>
+      <c r="F67" s="3">
+        <v>45943.49861111111</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
+        <v>8058</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>8059</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>1709</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>8060</v>
+      </c>
+      <c r="F68" s="3">
+        <v>45943.49375</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="8" t="s">
+        <v>8061</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>8062</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>6473</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" s="3">
+        <v>45942.683333333334</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="8" t="s">
+        <v>8063</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>8064</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>8065</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" s="3">
+        <v>45941.54166666667</v>
       </c>
     </row>
   </sheetData>
@@ -24639,6 +26096,49 @@
     <hyperlink ref="A25" r:id="rId24"/>
     <hyperlink ref="A26" r:id="rId25"/>
     <hyperlink ref="A27" r:id="rId26"/>
+    <hyperlink ref="A28" r:id="rId27"/>
+    <hyperlink ref="A29" r:id="rId28"/>
+    <hyperlink ref="A30" r:id="rId29"/>
+    <hyperlink ref="A31" r:id="rId30"/>
+    <hyperlink ref="A32" r:id="rId31"/>
+    <hyperlink ref="A33" r:id="rId32"/>
+    <hyperlink ref="A34" r:id="rId33"/>
+    <hyperlink ref="A35" r:id="rId34"/>
+    <hyperlink ref="A36" r:id="rId35"/>
+    <hyperlink ref="A37" r:id="rId36"/>
+    <hyperlink ref="A38" r:id="rId37"/>
+    <hyperlink ref="A39" r:id="rId38"/>
+    <hyperlink ref="A40" r:id="rId39"/>
+    <hyperlink ref="A41" r:id="rId40"/>
+    <hyperlink ref="A42" r:id="rId41"/>
+    <hyperlink ref="A43" r:id="rId42"/>
+    <hyperlink ref="A44" r:id="rId43"/>
+    <hyperlink ref="A45" r:id="rId44"/>
+    <hyperlink ref="A46" r:id="rId45"/>
+    <hyperlink ref="A47" r:id="rId46"/>
+    <hyperlink ref="A48" r:id="rId47"/>
+    <hyperlink ref="A49" r:id="rId48"/>
+    <hyperlink ref="A50" r:id="rId49"/>
+    <hyperlink ref="A51" r:id="rId50"/>
+    <hyperlink ref="A52" r:id="rId51"/>
+    <hyperlink ref="A53" r:id="rId52"/>
+    <hyperlink ref="A54" r:id="rId53"/>
+    <hyperlink ref="A55" r:id="rId54"/>
+    <hyperlink ref="A56" r:id="rId55"/>
+    <hyperlink ref="A57" r:id="rId56"/>
+    <hyperlink ref="A58" r:id="rId57"/>
+    <hyperlink ref="A59" r:id="rId58"/>
+    <hyperlink ref="A60" r:id="rId59"/>
+    <hyperlink ref="A61" r:id="rId60"/>
+    <hyperlink ref="A62" r:id="rId61"/>
+    <hyperlink ref="A63" r:id="rId62"/>
+    <hyperlink ref="A64" r:id="rId63"/>
+    <hyperlink ref="A65" r:id="rId64"/>
+    <hyperlink ref="A66" r:id="rId65"/>
+    <hyperlink ref="A67" r:id="rId66"/>
+    <hyperlink ref="A68" r:id="rId67"/>
+    <hyperlink ref="A69" r:id="rId68"/>
+    <hyperlink ref="A70" r:id="rId69"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -24647,7 +26147,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2526"/>
+  <dimension ref="A1:F2552"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -75183,6 +76683,526 @@
       </c>
       <c r="F2526" s="3">
         <v>45939.44097222222</v>
+      </c>
+    </row>
+    <row r="2527" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2527" s="4" t="s">
+        <v>7796</v>
+      </c>
+      <c r="B2527" s="3" t="s">
+        <v>7797</v>
+      </c>
+      <c r="C2527" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2527" s="3" t="s">
+        <v>7798</v>
+      </c>
+      <c r="E2527" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2527" s="3">
+        <v>45940.56597222222</v>
+      </c>
+    </row>
+    <row r="2528" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2528" s="4" t="s">
+        <v>7799</v>
+      </c>
+      <c r="B2528" s="3" t="s">
+        <v>7800</v>
+      </c>
+      <c r="C2528" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2528" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="E2528" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2528" s="3">
+        <v>45940.50902777778</v>
+      </c>
+    </row>
+    <row r="2529" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2529" s="4" t="s">
+        <v>7801</v>
+      </c>
+      <c r="B2529" s="3" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C2529" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2529" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2529" s="3" t="s">
+        <v>7802</v>
+      </c>
+      <c r="F2529" s="3">
+        <v>45940.347916666666</v>
+      </c>
+    </row>
+    <row r="2530" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2530" s="4" t="s">
+        <v>7803</v>
+      </c>
+      <c r="B2530" s="3" t="s">
+        <v>7804</v>
+      </c>
+      <c r="C2530" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2530" s="3" t="s">
+        <v>6354</v>
+      </c>
+      <c r="E2530" s="3" t="s">
+        <v>7805</v>
+      </c>
+      <c r="F2530" s="3">
+        <v>45939.72083333333</v>
+      </c>
+    </row>
+    <row r="2531" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2531" s="4" t="s">
+        <v>7806</v>
+      </c>
+      <c r="B2531" s="3" t="s">
+        <v>7807</v>
+      </c>
+      <c r="C2531" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2531" s="3" t="s">
+        <v>967</v>
+      </c>
+      <c r="E2531" s="3" t="s">
+        <v>7808</v>
+      </c>
+      <c r="F2531" s="3">
+        <v>45939.71875</v>
+      </c>
+    </row>
+    <row r="2532" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2532" s="4" t="s">
+        <v>7809</v>
+      </c>
+      <c r="B2532" s="3" t="s">
+        <v>7810</v>
+      </c>
+      <c r="C2532" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2532" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2532" s="3" t="s">
+        <v>7811</v>
+      </c>
+      <c r="F2532" s="3">
+        <v>45940.60277777778</v>
+      </c>
+    </row>
+    <row r="2533" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2533" s="4" t="s">
+        <v>7812</v>
+      </c>
+      <c r="B2533" s="3" t="s">
+        <v>7813</v>
+      </c>
+      <c r="C2533" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2533" s="3" t="s">
+        <v>7814</v>
+      </c>
+      <c r="E2533" s="3" t="s">
+        <v>7815</v>
+      </c>
+      <c r="F2533" s="3">
+        <v>45940.49652777778</v>
+      </c>
+    </row>
+    <row r="2534" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2534" s="4" t="s">
+        <v>7816</v>
+      </c>
+      <c r="B2534" s="3" t="s">
+        <v>7817</v>
+      </c>
+      <c r="C2534" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2534" s="3" t="s">
+        <v>1724</v>
+      </c>
+      <c r="E2534" s="3" t="s">
+        <v>7818</v>
+      </c>
+      <c r="F2534" s="3">
+        <v>45940.370833333334</v>
+      </c>
+    </row>
+    <row r="2535" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2535" s="4" t="s">
+        <v>7819</v>
+      </c>
+      <c r="B2535" s="3" t="s">
+        <v>7820</v>
+      </c>
+      <c r="C2535" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2535" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="E2535" s="3" t="s">
+        <v>7821</v>
+      </c>
+      <c r="F2535" s="3">
+        <v>45939.80208333333</v>
+      </c>
+    </row>
+    <row r="2536" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2536" s="4" t="s">
+        <v>7822</v>
+      </c>
+      <c r="B2536" s="3" t="s">
+        <v>5392</v>
+      </c>
+      <c r="C2536" s="3" t="s">
+        <v>1733</v>
+      </c>
+      <c r="D2536" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2536" s="3" t="s">
+        <v>7823</v>
+      </c>
+      <c r="F2536" s="3">
+        <v>45940.58194444445</v>
+      </c>
+    </row>
+    <row r="2537" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2537" s="4" t="s">
+        <v>7824</v>
+      </c>
+      <c r="B2537" s="3" t="s">
+        <v>7825</v>
+      </c>
+      <c r="C2537" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2537" s="3" t="s">
+        <v>1655</v>
+      </c>
+      <c r="E2537" s="3" t="s">
+        <v>7826</v>
+      </c>
+      <c r="F2537" s="3">
+        <v>45939.69930555555</v>
+      </c>
+    </row>
+    <row r="2538" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2538" s="4" t="s">
+        <v>7827</v>
+      </c>
+      <c r="B2538" s="3" t="s">
+        <v>7828</v>
+      </c>
+      <c r="C2538" s="3" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D2538" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="E2538" s="3" t="s">
+        <v>7829</v>
+      </c>
+      <c r="F2538" s="3">
+        <v>45940.55625</v>
+      </c>
+    </row>
+    <row r="2539" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2539" s="4" t="s">
+        <v>7830</v>
+      </c>
+      <c r="B2539" s="3" t="s">
+        <v>7831</v>
+      </c>
+      <c r="C2539" s="3" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D2539" s="3" t="s">
+        <v>2191</v>
+      </c>
+      <c r="E2539" s="3" t="s">
+        <v>7832</v>
+      </c>
+      <c r="F2539" s="3">
+        <v>45940.554861111115</v>
+      </c>
+    </row>
+    <row r="2540" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2540" s="4" t="s">
+        <v>7833</v>
+      </c>
+      <c r="B2540" s="3" t="s">
+        <v>7834</v>
+      </c>
+      <c r="C2540" s="3" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D2540" s="3" t="s">
+        <v>3916</v>
+      </c>
+      <c r="E2540" s="3" t="s">
+        <v>7835</v>
+      </c>
+      <c r="F2540" s="3">
+        <v>45939.78402777778</v>
+      </c>
+    </row>
+    <row r="2541" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2541" s="4" t="s">
+        <v>7836</v>
+      </c>
+      <c r="B2541" s="3" t="s">
+        <v>7837</v>
+      </c>
+      <c r="C2541" s="3" t="s">
+        <v>2671</v>
+      </c>
+      <c r="D2541" s="3" t="s">
+        <v>4197</v>
+      </c>
+      <c r="E2541" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2541" s="3">
+        <v>45940.56597222222</v>
+      </c>
+    </row>
+    <row r="2542" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2542" s="4" t="s">
+        <v>7838</v>
+      </c>
+      <c r="B2542" s="3" t="s">
+        <v>7839</v>
+      </c>
+      <c r="C2542" s="3" t="s">
+        <v>2671</v>
+      </c>
+      <c r="D2542" s="3" t="s">
+        <v>3368</v>
+      </c>
+      <c r="E2542" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2542" s="3">
+        <v>45940.34722222222</v>
+      </c>
+    </row>
+    <row r="2543" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2543" s="4" t="s">
+        <v>7840</v>
+      </c>
+      <c r="B2543" s="3" t="s">
+        <v>7841</v>
+      </c>
+      <c r="C2543" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2543" s="3" t="s">
+        <v>3349</v>
+      </c>
+      <c r="E2543" s="3" t="s">
+        <v>7842</v>
+      </c>
+      <c r="F2543" s="3">
+        <v>45940.447222222225</v>
+      </c>
+    </row>
+    <row r="2544" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2544" s="4" t="s">
+        <v>7843</v>
+      </c>
+      <c r="B2544" s="3" t="s">
+        <v>7844</v>
+      </c>
+      <c r="C2544" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2544" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="E2544" s="3" t="s">
+        <v>7845</v>
+      </c>
+      <c r="F2544" s="3">
+        <v>45939.68819444445</v>
+      </c>
+    </row>
+    <row r="2545" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2545" s="4" t="s">
+        <v>7846</v>
+      </c>
+      <c r="B2545" s="3" t="s">
+        <v>7847</v>
+      </c>
+      <c r="C2545" s="3" t="s">
+        <v>3868</v>
+      </c>
+      <c r="D2545" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="E2545" s="3" t="s">
+        <v>7848</v>
+      </c>
+      <c r="F2545" s="3">
+        <v>45940.63680555555</v>
+      </c>
+    </row>
+    <row r="2546" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2546" s="4" t="s">
+        <v>7849</v>
+      </c>
+      <c r="B2546" s="3" t="s">
+        <v>7850</v>
+      </c>
+      <c r="C2546" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2546" s="3" t="s">
+        <v>7851</v>
+      </c>
+      <c r="E2546" s="3" t="s">
+        <v>7852</v>
+      </c>
+      <c r="F2546" s="3">
+        <v>45940.55694444444</v>
+      </c>
+    </row>
+    <row r="2547" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2547" s="4" t="s">
+        <v>7853</v>
+      </c>
+      <c r="B2547" s="3" t="s">
+        <v>3810</v>
+      </c>
+      <c r="C2547" s="3" t="s">
+        <v>5147</v>
+      </c>
+      <c r="D2547" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="E2547" s="3" t="s">
+        <v>7854</v>
+      </c>
+      <c r="F2547" s="3">
+        <v>45939.70833333333</v>
+      </c>
+    </row>
+    <row r="2548" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2548" s="4" t="s">
+        <v>7855</v>
+      </c>
+      <c r="B2548" s="3" t="s">
+        <v>1878</v>
+      </c>
+      <c r="C2548" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2548" s="3" t="s">
+        <v>1430</v>
+      </c>
+      <c r="E2548" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2548" s="3">
+        <v>45939.87361111111</v>
+      </c>
+    </row>
+    <row r="2549" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2549" s="4" t="s">
+        <v>7856</v>
+      </c>
+      <c r="B2549" s="3" t="s">
+        <v>7857</v>
+      </c>
+      <c r="C2549" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2549" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="E2549" s="3" t="s">
+        <v>7858</v>
+      </c>
+      <c r="F2549" s="3">
+        <v>45939.78125</v>
+      </c>
+    </row>
+    <row r="2550" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2550" s="4" t="s">
+        <v>7859</v>
+      </c>
+      <c r="B2550" s="3" t="s">
+        <v>7860</v>
+      </c>
+      <c r="C2550" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2550" s="3" t="s">
+        <v>5559</v>
+      </c>
+      <c r="E2550" s="3" t="s">
+        <v>7861</v>
+      </c>
+      <c r="F2550" s="3">
+        <v>45939.74513888889</v>
+      </c>
+    </row>
+    <row r="2551" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2551" s="4" t="s">
+        <v>7862</v>
+      </c>
+      <c r="B2551" s="3" t="s">
+        <v>7863</v>
+      </c>
+      <c r="C2551" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2551" s="3" t="s">
+        <v>1940</v>
+      </c>
+      <c r="E2551" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2551" s="3">
+        <v>45939.84236111111</v>
+      </c>
+    </row>
+    <row r="2552" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2552" s="4" t="s">
+        <v>7864</v>
+      </c>
+      <c r="B2552" s="3" t="s">
+        <v>7865</v>
+      </c>
+      <c r="C2552" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2552" s="3" t="s">
+        <v>3124</v>
+      </c>
+      <c r="E2552" s="3" t="s">
+        <v>7866</v>
+      </c>
+      <c r="F2552" s="3">
+        <v>45939.65694444445</v>
       </c>
     </row>
   </sheetData>
@@ -77712,6 +79732,32 @@
     <hyperlink ref="A2524" r:id="rId2523"/>
     <hyperlink ref="A2525" r:id="rId2524"/>
     <hyperlink ref="A2526" r:id="rId2525"/>
+    <hyperlink ref="A2527" r:id="rId2526"/>
+    <hyperlink ref="A2528" r:id="rId2527"/>
+    <hyperlink ref="A2529" r:id="rId2528"/>
+    <hyperlink ref="A2530" r:id="rId2529"/>
+    <hyperlink ref="A2531" r:id="rId2530"/>
+    <hyperlink ref="A2532" r:id="rId2531"/>
+    <hyperlink ref="A2533" r:id="rId2532"/>
+    <hyperlink ref="A2534" r:id="rId2533"/>
+    <hyperlink ref="A2535" r:id="rId2534"/>
+    <hyperlink ref="A2536" r:id="rId2535"/>
+    <hyperlink ref="A2537" r:id="rId2536"/>
+    <hyperlink ref="A2538" r:id="rId2537"/>
+    <hyperlink ref="A2539" r:id="rId2538"/>
+    <hyperlink ref="A2540" r:id="rId2539"/>
+    <hyperlink ref="A2541" r:id="rId2540"/>
+    <hyperlink ref="A2542" r:id="rId2541"/>
+    <hyperlink ref="A2543" r:id="rId2542"/>
+    <hyperlink ref="A2544" r:id="rId2543"/>
+    <hyperlink ref="A2545" r:id="rId2544"/>
+    <hyperlink ref="A2546" r:id="rId2545"/>
+    <hyperlink ref="A2547" r:id="rId2546"/>
+    <hyperlink ref="A2548" r:id="rId2547"/>
+    <hyperlink ref="A2549" r:id="rId2548"/>
+    <hyperlink ref="A2550" r:id="rId2549"/>
+    <hyperlink ref="A2551" r:id="rId2550"/>
+    <hyperlink ref="A2552" r:id="rId2551"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Update lands data - 2025-10-14 12:22
</commit_message>
<xml_diff>
--- a/lands-scraped.xlsx
+++ b/lands-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13112" uniqueCount="8066">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13262" uniqueCount="8142">
   <si>
     <t>link</t>
   </si>
@@ -24216,6 +24216,234 @@
   </si>
   <si>
     <t>16000 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/aizkraukle-and-reg/serenes-pag/heoog.html</t>
+  </si>
+  <si>
+    <t>45 000 € (1.41 €/m²)</t>
+  </si>
+  <si>
+    <t>3280 002 0101</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/iecavas-nov/ejmph.html</t>
+  </si>
+  <si>
+    <t>28 000 € (0.98 €/m²)</t>
+  </si>
+  <si>
+    <t>2.85 ha.</t>
+  </si>
+  <si>
+    <t>40640130172</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/iecavas-nov/hxbge.html</t>
+  </si>
+  <si>
+    <t>12 000 € (0.99 €/m²)</t>
+  </si>
+  <si>
+    <t>1.21 ha.</t>
+  </si>
+  <si>
+    <t>40640040243</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/drabesu-pag/jbpbb.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/raiskuma-pag/gpkgd.html</t>
+  </si>
+  <si>
+    <t>27 500 € (0.92 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/liksnas-pag/ahkgh.html</t>
+  </si>
+  <si>
+    <t>3 500 € (0.52 €/m²)</t>
+  </si>
+  <si>
+    <t>0.67 ha.</t>
+  </si>
+  <si>
+    <t>44680040284</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/dobele-and-reg/naudites-pag/hjpeo.html</t>
+  </si>
+  <si>
+    <t>46800050060</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/dobele-and-reg/krimunu-pag/agfln.html</t>
+  </si>
+  <si>
+    <t>32 000 € (1.02 €/m²)</t>
+  </si>
+  <si>
+    <t>46720060086</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jekabpils-and-reg/jekabpils/cxjpk.html</t>
+  </si>
+  <si>
+    <t>5670 008 0419</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jelgava/giegn.html</t>
+  </si>
+  <si>
+    <t>119 000 € (11.90 €/m²)</t>
+  </si>
+  <si>
+    <t>0900 012 0033</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/svetes-pag/ahkpn.html</t>
+  </si>
+  <si>
+    <t>43 000 € (4.77 €/m²)</t>
+  </si>
+  <si>
+    <t>9020 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/kalnciems/mghkc.html</t>
+  </si>
+  <si>
+    <t>85 000 € (69.50 €/m²)</t>
+  </si>
+  <si>
+    <t>1223 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kraslava-and-reg/kalniesu-pag/npehc.html</t>
+  </si>
+  <si>
+    <t>9 000 € (0.27 €/m²)</t>
+  </si>
+  <si>
+    <t>3.30 ha.</t>
+  </si>
+  <si>
+    <t>60680010366</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/liepaja/bbjdch.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/limbadzi-and-reg/limbazi/bxknjn.html</t>
+  </si>
+  <si>
+    <t>97 000 € (57.60 €/m²)</t>
+  </si>
+  <si>
+    <t>1684 m²</t>
+  </si>
+  <si>
+    <t>6601 007 0125</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ikskiles-l-t/fcxkn.html</t>
+  </si>
+  <si>
+    <t>74940040420</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/madlienas-pag/dfpjx.html</t>
+  </si>
+  <si>
+    <t>74680100047</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ikskiles-l-t/agnek.html</t>
+  </si>
+  <si>
+    <t>19 000 € (3.77 €/m²)</t>
+  </si>
+  <si>
+    <t>5034 m²</t>
+  </si>
+  <si>
+    <t>74940050179</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/lielvarde/dphok.html</t>
+  </si>
+  <si>
+    <t>27 000 € (14.78 €/m²)</t>
+  </si>
+  <si>
+    <t>74130021017</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ogresgala-pag/aemof.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/griskanu-pag/cilej.html</t>
+  </si>
+  <si>
+    <t>50 000 € (15.25 €/m²)</t>
+  </si>
+  <si>
+    <t>3279 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/rojas-pag/hkgjb.html</t>
+  </si>
+  <si>
+    <t>46 608 € (12 €/m²)</t>
+  </si>
+  <si>
+    <t>3884 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/talsi/amlpo.html</t>
+  </si>
+  <si>
+    <t>88010110034</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/laidzes-pag/jbcmg.html</t>
+  </si>
+  <si>
+    <t>65 000 € (1.30 €/m²)</t>
+  </si>
+  <si>
+    <t>8868 012 0054</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/kolkas-pag/fjkxx.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/lapmezciema-nov/hgxxn.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/kandava/noepx.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/vecates-pag/fpogh.html</t>
+  </si>
+  <si>
+    <t>96920020100</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/kauguru-pag/cfbli.html</t>
+  </si>
+  <si>
+    <t>172 900 € (20 €/m²)</t>
+  </si>
+  <si>
+    <t>8645 m²</t>
+  </si>
+  <si>
+    <t>96620020790</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/usmas-pag/bgfeo.html</t>
   </si>
 </sst>
 </file>
@@ -24651,7 +24879,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -24690,1382 +24918,602 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>7867</v>
+        <v>8066</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>7868</v>
+        <v>8067</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>243</v>
+        <v>8</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>7869</v>
+        <v>7501</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>7870</v>
+        <v>8068</v>
       </c>
       <c r="F2" s="3">
-        <v>45941.43680555555</v>
+        <v>45943.79791666666</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>7871</v>
+        <v>8069</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>7872</v>
+        <v>8070</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>324</v>
+        <v>419</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>5410</v>
+        <v>8071</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>10</v>
+        <v>8072</v>
       </c>
       <c r="F3" s="3">
-        <v>45941.81319444445</v>
+        <v>45943.986805555556</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>7873</v>
+        <v>8073</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>3215</v>
+        <v>8074</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>419</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>171</v>
+        <v>8075</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>7874</v>
+        <v>8076</v>
       </c>
       <c r="F4" s="3">
-        <v>45943.45347222222</v>
+        <v>45943.89513888889</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>7875</v>
+        <v>8077</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>7876</v>
+        <v>905</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>419</v>
+        <v>772</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>7877</v>
+        <v>906</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>7878</v>
+        <v>907</v>
       </c>
       <c r="F5" s="3">
-        <v>45940.69930555555</v>
+        <v>45944.55208333333</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>7879</v>
+        <v>8078</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>7880</v>
+        <v>8079</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>772</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>317</v>
+        <v>201</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="3">
-        <v>45942.95208333334</v>
+        <v>45943.85972222222</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>7881</v>
+        <v>8080</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>7882</v>
+        <v>8081</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>772</v>
+        <v>1218</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>7883</v>
+        <v>8082</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>7884</v>
+        <v>8083</v>
       </c>
       <c r="F7" s="3">
-        <v>45942.44583333333</v>
+        <v>45943.8375</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>7885</v>
+        <v>8084</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>2906</v>
+        <v>306</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>772</v>
+        <v>1569</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>32</v>
+        <v>201</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>7886</v>
+        <v>8085</v>
       </c>
       <c r="F8" s="3">
-        <v>45941.40486111111</v>
+        <v>45944.32916666666</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>7887</v>
+        <v>8086</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>7888</v>
+        <v>8087</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>1218</v>
+        <v>1569</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>181</v>
+        <v>3414</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>7889</v>
+        <v>8088</v>
       </c>
       <c r="F9" s="3">
-        <v>45943.62361111111</v>
+        <v>45943.65694444445</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>7890</v>
+        <v>8089</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>7891</v>
+        <v>331</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>1218</v>
+        <v>1733</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>7892</v>
+        <v>561</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>7893</v>
+        <v>8090</v>
       </c>
       <c r="F10" s="3">
-        <v>45943.52222222222</v>
+        <v>45944.57708333334</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>7894</v>
+        <v>8091</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>7895</v>
+        <v>8092</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>1218</v>
+        <v>1929</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>7896</v>
+        <v>561</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>10</v>
+        <v>8093</v>
       </c>
       <c r="F11" s="3">
-        <v>45943.429861111115</v>
+        <v>45944.58472222222</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>7897</v>
+        <v>8094</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>7898</v>
+        <v>8095</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>1218</v>
+        <v>1929</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>71</v>
+        <v>8096</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>7899</v>
+        <v>10</v>
       </c>
       <c r="F12" s="3">
-        <v>45940.63888888889</v>
+        <v>45944.45833333333</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>7900</v>
+        <v>8097</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>7901</v>
+        <v>8098</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>1569</v>
+        <v>1929</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>7902</v>
+        <v>8099</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="3">
-        <v>45943.54166666667</v>
+        <v>45944.444444444445</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>7903</v>
+        <v>8100</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>7904</v>
+        <v>8101</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>1569</v>
+        <v>2488</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>7905</v>
+        <v>8102</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>10</v>
+        <v>8103</v>
       </c>
       <c r="F14" s="3">
-        <v>45942.74722222222</v>
+        <v>45944.45</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>7906</v>
+        <v>8104</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>7907</v>
+        <v>3082</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>1671</v>
+        <v>2846</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>407</v>
+        <v>3083</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>7908</v>
+        <v>10</v>
       </c>
       <c r="F15" s="3">
-        <v>45942.80069444445</v>
+        <v>45943.743055555555</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>7909</v>
+        <v>8105</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>7910</v>
+        <v>8106</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>1671</v>
+        <v>3398</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>171</v>
+        <v>8107</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>7911</v>
+        <v>8108</v>
       </c>
       <c r="F16" s="3">
-        <v>45941.91875</v>
+        <v>45944.584027777775</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>7912</v>
+        <v>8109</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>7913</v>
+        <v>4429</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>1929</v>
+        <v>4034</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>325</v>
+        <v>55</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>7914</v>
+        <v>8110</v>
       </c>
       <c r="F17" s="3">
-        <v>45943.42291666666</v>
+        <v>45944.53472222222</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>7915</v>
+        <v>8111</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>511</v>
+        <v>2710</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>1929</v>
+        <v>4034</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>9</v>
+        <v>474</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>7916</v>
+        <v>8112</v>
       </c>
       <c r="F18" s="3">
-        <v>45943.419444444444</v>
+        <v>45944.52986111111</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>7917</v>
+        <v>8113</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>7918</v>
+        <v>8114</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>1929</v>
+        <v>4034</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>7919</v>
+        <v>8115</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>7920</v>
+        <v>8116</v>
       </c>
       <c r="F19" s="3">
-        <v>45942.81597222222</v>
+        <v>45944.45277777778</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>7921</v>
+        <v>8117</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>7235</v>
+        <v>8118</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>1929</v>
+        <v>4034</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>407</v>
+        <v>2166</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>7922</v>
+        <v>8119</v>
       </c>
       <c r="F20" s="3">
-        <v>45942.79027777778</v>
+        <v>45944.43541666667</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>7923</v>
+        <v>8120</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>7924</v>
+        <v>4774</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>1929</v>
+        <v>4034</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>7925</v>
+        <v>32</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>7926</v>
+        <v>10</v>
       </c>
       <c r="F21" s="3">
-        <v>45941.77083333333</v>
+        <v>45943.853472222225</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>7927</v>
+        <v>8121</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>7928</v>
+        <v>8122</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>2671</v>
+        <v>4770</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>2224</v>
+        <v>8123</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>7929</v>
+        <v>10</v>
       </c>
       <c r="F22" s="3">
-        <v>45942.575</v>
+        <v>45943.77638888889</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>7930</v>
+        <v>8124</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>7931</v>
+        <v>8125</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>2671</v>
+        <v>5266</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>596</v>
+        <v>8126</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>7932</v>
+        <v>10</v>
       </c>
       <c r="F23" s="3">
-        <v>45942.535416666666</v>
+        <v>45944.61111111111</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>7933</v>
+        <v>8127</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>7934</v>
+        <v>2804</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>2671</v>
+        <v>5266</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>7935</v>
+        <v>201</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>7936</v>
+        <v>8128</v>
       </c>
       <c r="F24" s="3">
-        <v>45940.78472222222</v>
+        <v>45944.58541666667</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>7937</v>
+        <v>8129</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>7938</v>
+        <v>8130</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>2671</v>
+        <v>5266</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>7939</v>
+        <v>77</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>10</v>
+        <v>8131</v>
       </c>
       <c r="F25" s="3">
-        <v>45940.72986111111</v>
+        <v>45944.46805555555</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>7940</v>
+        <v>8132</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>7941</v>
+        <v>5359</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>2846</v>
+        <v>5266</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>7942</v>
+        <v>5360</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>7943</v>
+        <v>5361</v>
       </c>
       <c r="F26" s="3">
-        <v>45943.558333333334</v>
+        <v>45943.85486111111</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>7944</v>
+        <v>8133</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>7945</v>
+        <v>5886</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>2846</v>
+        <v>5674</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>171</v>
+        <v>2446</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>10</v>
+        <v>5887</v>
       </c>
       <c r="F27" s="3">
-        <v>45941.825</v>
+        <v>45944.41111111111</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>7946</v>
+        <v>8134</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>7947</v>
+        <v>5627</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>2846</v>
+        <v>5674</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>3414</v>
+        <v>1632</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F28" s="3">
-        <v>45940.72916666667</v>
+        <v>45943.804861111115</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>7948</v>
+        <v>8135</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>7949</v>
+        <v>2615</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>2846</v>
+        <v>6207</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>55</v>
+        <v>325</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>10</v>
+        <v>8136</v>
       </c>
       <c r="F29" s="3">
-        <v>45940.66458333333</v>
+        <v>45943.853472222225</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>7950</v>
+        <v>8137</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>956</v>
+        <v>8138</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>3398</v>
+        <v>6207</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>201</v>
+        <v>8139</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>7951</v>
+        <v>8140</v>
       </c>
       <c r="F30" s="3">
-        <v>45943.36944444444</v>
+        <v>45943.683333333334</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>7952</v>
+        <v>8141</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>7953</v>
+        <v>5870</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>3398</v>
+        <v>6439</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>436</v>
+        <v>383</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F31" s="3">
-        <v>45940.69236111111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>7954</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>7955</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="3">
-        <v>45942.86319444445</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>7956</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>7957</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>3868</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>407</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>7958</v>
-      </c>
-      <c r="F33" s="3">
-        <v>45943.61944444444</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>7959</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>7960</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>3868</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>4362</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34" s="3">
-        <v>45943.42152777778</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>7961</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>7962</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>3868</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>407</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" s="3">
-        <v>45942.84097222222</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
-        <v>7963</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>7964</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>3868</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>5973</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>7965</v>
-      </c>
-      <c r="F36" s="3">
-        <v>45941.71875</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
-        <v>7966</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>7967</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>5880</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>7968</v>
-      </c>
-      <c r="F37" s="3">
-        <v>45943.42569444445</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>7969</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>4178</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F38" s="3">
-        <v>45943.365277777775</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>7970</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>7971</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F39" s="3">
-        <v>45943.32638888889</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>7972</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>7973</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>7974</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F40" s="3">
-        <v>45942.67222222222</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>7975</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>7976</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>3772</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F41" s="3">
-        <v>45941.92638888889</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
-        <v>7977</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>7978</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>4671</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>7979</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>7980</v>
-      </c>
-      <c r="F42" s="3">
-        <v>45943.44375</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
-        <v>7981</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>7982</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>4770</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>596</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F43" s="3">
-        <v>45942.8125</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
-        <v>7983</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>7984</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>4770</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>4632</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>7985</v>
-      </c>
-      <c r="F44" s="3">
-        <v>45942.7625</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
-        <v>7986</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>7987</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>5147</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>7988</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F45" s="3">
-        <v>45942.57083333333</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
-        <v>7989</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>7990</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>5266</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>7991</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>7992</v>
-      </c>
-      <c r="F46" s="3">
-        <v>45943.40416666667</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
-        <v>7993</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>7994</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>5266</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>7995</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>7996</v>
-      </c>
-      <c r="F47" s="3">
-        <v>45940.72152777778</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
-        <v>7997</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>7998</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>5674</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>7999</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F48" s="3">
-        <v>45943.63611111111</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
-        <v>8000</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>8001</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>5674</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>8002</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>8003</v>
-      </c>
-      <c r="F49" s="3">
-        <v>45943.62013888889</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
-        <v>8004</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>8005</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>5674</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>8006</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>8007</v>
-      </c>
-      <c r="F50" s="3">
-        <v>45943.40416666667</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
-        <v>8008</v>
-      </c>
-      <c r="B51" s="9" t="s">
-        <v>5900</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>5674</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>5901</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>5902</v>
-      </c>
-      <c r="F51" s="3">
-        <v>45942.618055555555</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
-        <v>8009</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>897</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>5674</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>436</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>8010</v>
-      </c>
-      <c r="F52" s="3">
-        <v>45942.527083333334</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
-        <v>8011</v>
-      </c>
-      <c r="B53" s="9" t="s">
-        <v>8012</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>5674</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>5309</v>
-      </c>
-      <c r="E53" s="9" t="s">
-        <v>8013</v>
-      </c>
-      <c r="F53" s="3">
-        <v>45941.87361111111</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="8" t="s">
-        <v>8014</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>8015</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>5674</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>8016</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>8017</v>
-      </c>
-      <c r="F54" s="3">
-        <v>45941.81805555556</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
-        <v>8018</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>8019</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>5674</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>342</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>8020</v>
-      </c>
-      <c r="F55" s="3">
-        <v>45941.79583333334</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
-        <v>8021</v>
-      </c>
-      <c r="B56" s="9" t="s">
-        <v>8022</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>5674</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>8023</v>
-      </c>
-      <c r="F56" s="3">
-        <v>45940.98333333334</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="8" t="s">
-        <v>8024</v>
-      </c>
-      <c r="B57" s="9" t="s">
-        <v>8025</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>6133</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>1535</v>
-      </c>
-      <c r="E57" s="9" t="s">
-        <v>8026</v>
-      </c>
-      <c r="F57" s="3">
-        <v>45941.71527777778</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="8" t="s">
-        <v>8027</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>6410</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>6207</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>6411</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>8028</v>
-      </c>
-      <c r="F58" s="3">
-        <v>45943.580555555556</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
-        <v>8029</v>
-      </c>
-      <c r="B59" s="9" t="s">
-        <v>8030</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>6207</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>8031</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>8032</v>
-      </c>
-      <c r="F59" s="3">
-        <v>45941.48888888889</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="8" t="s">
-        <v>8033</v>
-      </c>
-      <c r="B60" s="9" t="s">
-        <v>8034</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>7108</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>8035</v>
-      </c>
-      <c r="F60" s="3">
-        <v>45943.575694444444</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="8" t="s">
-        <v>8036</v>
-      </c>
-      <c r="B61" s="9" t="s">
-        <v>8037</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>8038</v>
-      </c>
-      <c r="F61" s="3">
-        <v>45943.51527777778</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="8" t="s">
-        <v>8039</v>
-      </c>
-      <c r="B62" s="9" t="s">
-        <v>8040</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D62" s="9" t="s">
-        <v>353</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>8041</v>
-      </c>
-      <c r="F62" s="3">
-        <v>45943.50833333333</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="8" t="s">
-        <v>8042</v>
-      </c>
-      <c r="B63" s="9" t="s">
-        <v>8043</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="E63" s="9" t="s">
-        <v>8044</v>
-      </c>
-      <c r="F63" s="3">
-        <v>45943.506944444445</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="8" t="s">
-        <v>8045</v>
-      </c>
-      <c r="B64" s="9" t="s">
-        <v>8046</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>353</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>8047</v>
-      </c>
-      <c r="F64" s="3">
-        <v>45943.50625</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="8" t="s">
-        <v>8048</v>
-      </c>
-      <c r="B65" s="9" t="s">
-        <v>8049</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>683</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>8050</v>
-      </c>
-      <c r="F65" s="3">
-        <v>45943.50347222222</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="8" t="s">
-        <v>8051</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>8052</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>8053</v>
-      </c>
-      <c r="E66" s="9" t="s">
-        <v>8054</v>
-      </c>
-      <c r="F66" s="3">
-        <v>45943.50277777778</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="8" t="s">
-        <v>8055</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>8056</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>1709</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>8057</v>
-      </c>
-      <c r="F67" s="3">
-        <v>45943.49861111111</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="8" t="s">
-        <v>8058</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>8059</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D68" s="9" t="s">
-        <v>1709</v>
-      </c>
-      <c r="E68" s="9" t="s">
-        <v>8060</v>
-      </c>
-      <c r="F68" s="3">
-        <v>45943.49375</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="8" t="s">
-        <v>8061</v>
-      </c>
-      <c r="B69" s="9" t="s">
-        <v>8062</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D69" s="9" t="s">
-        <v>6473</v>
-      </c>
-      <c r="E69" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F69" s="3">
-        <v>45942.683333333334</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="8" t="s">
-        <v>8063</v>
-      </c>
-      <c r="B70" s="9" t="s">
-        <v>8064</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>8065</v>
-      </c>
-      <c r="E70" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F70" s="3">
-        <v>45941.54166666667</v>
+        <v>45943.85972222222</v>
       </c>
     </row>
   </sheetData>
@@ -26100,45 +25548,6 @@
     <hyperlink ref="A29" r:id="rId28"/>
     <hyperlink ref="A30" r:id="rId29"/>
     <hyperlink ref="A31" r:id="rId30"/>
-    <hyperlink ref="A32" r:id="rId31"/>
-    <hyperlink ref="A33" r:id="rId32"/>
-    <hyperlink ref="A34" r:id="rId33"/>
-    <hyperlink ref="A35" r:id="rId34"/>
-    <hyperlink ref="A36" r:id="rId35"/>
-    <hyperlink ref="A37" r:id="rId36"/>
-    <hyperlink ref="A38" r:id="rId37"/>
-    <hyperlink ref="A39" r:id="rId38"/>
-    <hyperlink ref="A40" r:id="rId39"/>
-    <hyperlink ref="A41" r:id="rId40"/>
-    <hyperlink ref="A42" r:id="rId41"/>
-    <hyperlink ref="A43" r:id="rId42"/>
-    <hyperlink ref="A44" r:id="rId43"/>
-    <hyperlink ref="A45" r:id="rId44"/>
-    <hyperlink ref="A46" r:id="rId45"/>
-    <hyperlink ref="A47" r:id="rId46"/>
-    <hyperlink ref="A48" r:id="rId47"/>
-    <hyperlink ref="A49" r:id="rId48"/>
-    <hyperlink ref="A50" r:id="rId49"/>
-    <hyperlink ref="A51" r:id="rId50"/>
-    <hyperlink ref="A52" r:id="rId51"/>
-    <hyperlink ref="A53" r:id="rId52"/>
-    <hyperlink ref="A54" r:id="rId53"/>
-    <hyperlink ref="A55" r:id="rId54"/>
-    <hyperlink ref="A56" r:id="rId55"/>
-    <hyperlink ref="A57" r:id="rId56"/>
-    <hyperlink ref="A58" r:id="rId57"/>
-    <hyperlink ref="A59" r:id="rId58"/>
-    <hyperlink ref="A60" r:id="rId59"/>
-    <hyperlink ref="A61" r:id="rId60"/>
-    <hyperlink ref="A62" r:id="rId61"/>
-    <hyperlink ref="A63" r:id="rId62"/>
-    <hyperlink ref="A64" r:id="rId63"/>
-    <hyperlink ref="A65" r:id="rId64"/>
-    <hyperlink ref="A66" r:id="rId65"/>
-    <hyperlink ref="A67" r:id="rId66"/>
-    <hyperlink ref="A68" r:id="rId67"/>
-    <hyperlink ref="A69" r:id="rId68"/>
-    <hyperlink ref="A70" r:id="rId69"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -26147,7 +25556,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2552"/>
+  <dimension ref="A1:F2621"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -77203,6 +76612,1386 @@
       </c>
       <c r="F2552" s="3">
         <v>45939.65694444445</v>
+      </c>
+    </row>
+    <row r="2553" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2553" s="4" t="s">
+        <v>7867</v>
+      </c>
+      <c r="B2553" s="3" t="s">
+        <v>7868</v>
+      </c>
+      <c r="C2553" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D2553" s="3" t="s">
+        <v>7869</v>
+      </c>
+      <c r="E2553" s="3" t="s">
+        <v>7870</v>
+      </c>
+      <c r="F2553" s="3">
+        <v>45941.43680555555</v>
+      </c>
+    </row>
+    <row r="2554" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2554" s="4" t="s">
+        <v>7871</v>
+      </c>
+      <c r="B2554" s="3" t="s">
+        <v>7872</v>
+      </c>
+      <c r="C2554" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="D2554" s="3" t="s">
+        <v>5410</v>
+      </c>
+      <c r="E2554" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2554" s="3">
+        <v>45941.81319444445</v>
+      </c>
+    </row>
+    <row r="2555" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2555" s="4" t="s">
+        <v>7873</v>
+      </c>
+      <c r="B2555" s="3" t="s">
+        <v>3215</v>
+      </c>
+      <c r="C2555" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2555" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2555" s="3" t="s">
+        <v>7874</v>
+      </c>
+      <c r="F2555" s="3">
+        <v>45943.45347222222</v>
+      </c>
+    </row>
+    <row r="2556" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2556" s="4" t="s">
+        <v>7875</v>
+      </c>
+      <c r="B2556" s="3" t="s">
+        <v>7876</v>
+      </c>
+      <c r="C2556" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2556" s="3" t="s">
+        <v>7877</v>
+      </c>
+      <c r="E2556" s="3" t="s">
+        <v>7878</v>
+      </c>
+      <c r="F2556" s="3">
+        <v>45940.69930555555</v>
+      </c>
+    </row>
+    <row r="2557" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2557" s="4" t="s">
+        <v>7879</v>
+      </c>
+      <c r="B2557" s="3" t="s">
+        <v>7880</v>
+      </c>
+      <c r="C2557" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2557" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E2557" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2557" s="3">
+        <v>45942.95208333334</v>
+      </c>
+    </row>
+    <row r="2558" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2558" s="4" t="s">
+        <v>7881</v>
+      </c>
+      <c r="B2558" s="3" t="s">
+        <v>7882</v>
+      </c>
+      <c r="C2558" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2558" s="3" t="s">
+        <v>7883</v>
+      </c>
+      <c r="E2558" s="3" t="s">
+        <v>7884</v>
+      </c>
+      <c r="F2558" s="3">
+        <v>45942.44583333333</v>
+      </c>
+    </row>
+    <row r="2559" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2559" s="4" t="s">
+        <v>7885</v>
+      </c>
+      <c r="B2559" s="3" t="s">
+        <v>2906</v>
+      </c>
+      <c r="C2559" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2559" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2559" s="3" t="s">
+        <v>7886</v>
+      </c>
+      <c r="F2559" s="3">
+        <v>45941.40486111111</v>
+      </c>
+    </row>
+    <row r="2560" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2560" s="4" t="s">
+        <v>7887</v>
+      </c>
+      <c r="B2560" s="3" t="s">
+        <v>7888</v>
+      </c>
+      <c r="C2560" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2560" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2560" s="3" t="s">
+        <v>7889</v>
+      </c>
+      <c r="F2560" s="3">
+        <v>45943.62361111111</v>
+      </c>
+    </row>
+    <row r="2561" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2561" s="4" t="s">
+        <v>7890</v>
+      </c>
+      <c r="B2561" s="3" t="s">
+        <v>7891</v>
+      </c>
+      <c r="C2561" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2561" s="3" t="s">
+        <v>7892</v>
+      </c>
+      <c r="E2561" s="3" t="s">
+        <v>7893</v>
+      </c>
+      <c r="F2561" s="3">
+        <v>45943.52222222222</v>
+      </c>
+    </row>
+    <row r="2562" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2562" s="4" t="s">
+        <v>7894</v>
+      </c>
+      <c r="B2562" s="3" t="s">
+        <v>7895</v>
+      </c>
+      <c r="C2562" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2562" s="3" t="s">
+        <v>7896</v>
+      </c>
+      <c r="E2562" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2562" s="3">
+        <v>45943.429861111115</v>
+      </c>
+    </row>
+    <row r="2563" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2563" s="4" t="s">
+        <v>7897</v>
+      </c>
+      <c r="B2563" s="3" t="s">
+        <v>7898</v>
+      </c>
+      <c r="C2563" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2563" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2563" s="3" t="s">
+        <v>7899</v>
+      </c>
+      <c r="F2563" s="3">
+        <v>45940.63888888889</v>
+      </c>
+    </row>
+    <row r="2564" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2564" s="4" t="s">
+        <v>7900</v>
+      </c>
+      <c r="B2564" s="3" t="s">
+        <v>7901</v>
+      </c>
+      <c r="C2564" s="3" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D2564" s="3" t="s">
+        <v>7902</v>
+      </c>
+      <c r="E2564" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2564" s="3">
+        <v>45943.54166666667</v>
+      </c>
+    </row>
+    <row r="2565" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2565" s="4" t="s">
+        <v>7903</v>
+      </c>
+      <c r="B2565" s="3" t="s">
+        <v>7904</v>
+      </c>
+      <c r="C2565" s="3" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D2565" s="3" t="s">
+        <v>7905</v>
+      </c>
+      <c r="E2565" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2565" s="3">
+        <v>45942.74722222222</v>
+      </c>
+    </row>
+    <row r="2566" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2566" s="4" t="s">
+        <v>7906</v>
+      </c>
+      <c r="B2566" s="3" t="s">
+        <v>7907</v>
+      </c>
+      <c r="C2566" s="3" t="s">
+        <v>1671</v>
+      </c>
+      <c r="D2566" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="E2566" s="3" t="s">
+        <v>7908</v>
+      </c>
+      <c r="F2566" s="3">
+        <v>45942.80069444445</v>
+      </c>
+    </row>
+    <row r="2567" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2567" s="4" t="s">
+        <v>7909</v>
+      </c>
+      <c r="B2567" s="3" t="s">
+        <v>7910</v>
+      </c>
+      <c r="C2567" s="3" t="s">
+        <v>1671</v>
+      </c>
+      <c r="D2567" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2567" s="3" t="s">
+        <v>7911</v>
+      </c>
+      <c r="F2567" s="3">
+        <v>45941.91875</v>
+      </c>
+    </row>
+    <row r="2568" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2568" s="4" t="s">
+        <v>7912</v>
+      </c>
+      <c r="B2568" s="3" t="s">
+        <v>7913</v>
+      </c>
+      <c r="C2568" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2568" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2568" s="3" t="s">
+        <v>7914</v>
+      </c>
+      <c r="F2568" s="3">
+        <v>45943.42291666666</v>
+      </c>
+    </row>
+    <row r="2569" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2569" s="4" t="s">
+        <v>7915</v>
+      </c>
+      <c r="B2569" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="C2569" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2569" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2569" s="3" t="s">
+        <v>7916</v>
+      </c>
+      <c r="F2569" s="3">
+        <v>45943.419444444444</v>
+      </c>
+    </row>
+    <row r="2570" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2570" s="4" t="s">
+        <v>7917</v>
+      </c>
+      <c r="B2570" s="3" t="s">
+        <v>7918</v>
+      </c>
+      <c r="C2570" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2570" s="3" t="s">
+        <v>7919</v>
+      </c>
+      <c r="E2570" s="3" t="s">
+        <v>7920</v>
+      </c>
+      <c r="F2570" s="3">
+        <v>45942.81597222222</v>
+      </c>
+    </row>
+    <row r="2571" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2571" s="4" t="s">
+        <v>7921</v>
+      </c>
+      <c r="B2571" s="3" t="s">
+        <v>7235</v>
+      </c>
+      <c r="C2571" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2571" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="E2571" s="3" t="s">
+        <v>7922</v>
+      </c>
+      <c r="F2571" s="3">
+        <v>45942.79027777778</v>
+      </c>
+    </row>
+    <row r="2572" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2572" s="4" t="s">
+        <v>7923</v>
+      </c>
+      <c r="B2572" s="3" t="s">
+        <v>7924</v>
+      </c>
+      <c r="C2572" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2572" s="3" t="s">
+        <v>7925</v>
+      </c>
+      <c r="E2572" s="3" t="s">
+        <v>7926</v>
+      </c>
+      <c r="F2572" s="3">
+        <v>45941.77083333333</v>
+      </c>
+    </row>
+    <row r="2573" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2573" s="4" t="s">
+        <v>7927</v>
+      </c>
+      <c r="B2573" s="3" t="s">
+        <v>7928</v>
+      </c>
+      <c r="C2573" s="3" t="s">
+        <v>2671</v>
+      </c>
+      <c r="D2573" s="3" t="s">
+        <v>2224</v>
+      </c>
+      <c r="E2573" s="3" t="s">
+        <v>7929</v>
+      </c>
+      <c r="F2573" s="3">
+        <v>45942.575</v>
+      </c>
+    </row>
+    <row r="2574" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2574" s="4" t="s">
+        <v>7930</v>
+      </c>
+      <c r="B2574" s="3" t="s">
+        <v>7931</v>
+      </c>
+      <c r="C2574" s="3" t="s">
+        <v>2671</v>
+      </c>
+      <c r="D2574" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="E2574" s="3" t="s">
+        <v>7932</v>
+      </c>
+      <c r="F2574" s="3">
+        <v>45942.535416666666</v>
+      </c>
+    </row>
+    <row r="2575" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2575" s="4" t="s">
+        <v>7933</v>
+      </c>
+      <c r="B2575" s="3" t="s">
+        <v>7934</v>
+      </c>
+      <c r="C2575" s="3" t="s">
+        <v>2671</v>
+      </c>
+      <c r="D2575" s="3" t="s">
+        <v>7935</v>
+      </c>
+      <c r="E2575" s="3" t="s">
+        <v>7936</v>
+      </c>
+      <c r="F2575" s="3">
+        <v>45940.78472222222</v>
+      </c>
+    </row>
+    <row r="2576" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2576" s="4" t="s">
+        <v>7937</v>
+      </c>
+      <c r="B2576" s="3" t="s">
+        <v>7938</v>
+      </c>
+      <c r="C2576" s="3" t="s">
+        <v>2671</v>
+      </c>
+      <c r="D2576" s="3" t="s">
+        <v>7939</v>
+      </c>
+      <c r="E2576" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2576" s="3">
+        <v>45940.72986111111</v>
+      </c>
+    </row>
+    <row r="2577" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2577" s="4" t="s">
+        <v>7940</v>
+      </c>
+      <c r="B2577" s="3" t="s">
+        <v>7941</v>
+      </c>
+      <c r="C2577" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2577" s="3" t="s">
+        <v>7942</v>
+      </c>
+      <c r="E2577" s="3" t="s">
+        <v>7943</v>
+      </c>
+      <c r="F2577" s="3">
+        <v>45943.558333333334</v>
+      </c>
+    </row>
+    <row r="2578" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2578" s="4" t="s">
+        <v>7944</v>
+      </c>
+      <c r="B2578" s="3" t="s">
+        <v>7945</v>
+      </c>
+      <c r="C2578" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2578" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2578" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2578" s="3">
+        <v>45941.825</v>
+      </c>
+    </row>
+    <row r="2579" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2579" s="4" t="s">
+        <v>7946</v>
+      </c>
+      <c r="B2579" s="3" t="s">
+        <v>7947</v>
+      </c>
+      <c r="C2579" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2579" s="3" t="s">
+        <v>3414</v>
+      </c>
+      <c r="E2579" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2579" s="3">
+        <v>45940.72916666667</v>
+      </c>
+    </row>
+    <row r="2580" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2580" s="4" t="s">
+        <v>7948</v>
+      </c>
+      <c r="B2580" s="3" t="s">
+        <v>7949</v>
+      </c>
+      <c r="C2580" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2580" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2580" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2580" s="3">
+        <v>45940.66458333333</v>
+      </c>
+    </row>
+    <row r="2581" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2581" s="4" t="s">
+        <v>7950</v>
+      </c>
+      <c r="B2581" s="3" t="s">
+        <v>956</v>
+      </c>
+      <c r="C2581" s="3" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D2581" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2581" s="3" t="s">
+        <v>7951</v>
+      </c>
+      <c r="F2581" s="3">
+        <v>45943.36944444444</v>
+      </c>
+    </row>
+    <row r="2582" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2582" s="4" t="s">
+        <v>7952</v>
+      </c>
+      <c r="B2582" s="3" t="s">
+        <v>7953</v>
+      </c>
+      <c r="C2582" s="3" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D2582" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="E2582" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2582" s="3">
+        <v>45940.69236111111</v>
+      </c>
+    </row>
+    <row r="2583" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2583" s="4" t="s">
+        <v>7954</v>
+      </c>
+      <c r="B2583" s="3" t="s">
+        <v>7955</v>
+      </c>
+      <c r="C2583" s="3" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D2583" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="E2583" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2583" s="3">
+        <v>45942.86319444445</v>
+      </c>
+    </row>
+    <row r="2584" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2584" s="4" t="s">
+        <v>7956</v>
+      </c>
+      <c r="B2584" s="3" t="s">
+        <v>7957</v>
+      </c>
+      <c r="C2584" s="3" t="s">
+        <v>3868</v>
+      </c>
+      <c r="D2584" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="E2584" s="3" t="s">
+        <v>7958</v>
+      </c>
+      <c r="F2584" s="3">
+        <v>45943.61944444444</v>
+      </c>
+    </row>
+    <row r="2585" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2585" s="4" t="s">
+        <v>7959</v>
+      </c>
+      <c r="B2585" s="3" t="s">
+        <v>7960</v>
+      </c>
+      <c r="C2585" s="3" t="s">
+        <v>3868</v>
+      </c>
+      <c r="D2585" s="3" t="s">
+        <v>4362</v>
+      </c>
+      <c r="E2585" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2585" s="3">
+        <v>45943.42152777778</v>
+      </c>
+    </row>
+    <row r="2586" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2586" s="4" t="s">
+        <v>7961</v>
+      </c>
+      <c r="B2586" s="3" t="s">
+        <v>7962</v>
+      </c>
+      <c r="C2586" s="3" t="s">
+        <v>3868</v>
+      </c>
+      <c r="D2586" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="E2586" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2586" s="3">
+        <v>45942.84097222222</v>
+      </c>
+    </row>
+    <row r="2587" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2587" s="4" t="s">
+        <v>7963</v>
+      </c>
+      <c r="B2587" s="3" t="s">
+        <v>7964</v>
+      </c>
+      <c r="C2587" s="3" t="s">
+        <v>3868</v>
+      </c>
+      <c r="D2587" s="3" t="s">
+        <v>5973</v>
+      </c>
+      <c r="E2587" s="3" t="s">
+        <v>7965</v>
+      </c>
+      <c r="F2587" s="3">
+        <v>45941.71875</v>
+      </c>
+    </row>
+    <row r="2588" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2588" s="4" t="s">
+        <v>7966</v>
+      </c>
+      <c r="B2588" s="3" t="s">
+        <v>7967</v>
+      </c>
+      <c r="C2588" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2588" s="3" t="s">
+        <v>5880</v>
+      </c>
+      <c r="E2588" s="3" t="s">
+        <v>7968</v>
+      </c>
+      <c r="F2588" s="3">
+        <v>45943.42569444445</v>
+      </c>
+    </row>
+    <row r="2589" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2589" s="4" t="s">
+        <v>7969</v>
+      </c>
+      <c r="B2589" s="3" t="s">
+        <v>4178</v>
+      </c>
+      <c r="C2589" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2589" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2589" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2589" s="3">
+        <v>45943.365277777775</v>
+      </c>
+    </row>
+    <row r="2590" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2590" s="4" t="s">
+        <v>7970</v>
+      </c>
+      <c r="B2590" s="3" t="s">
+        <v>7971</v>
+      </c>
+      <c r="C2590" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2590" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2590" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2590" s="3">
+        <v>45943.32638888889</v>
+      </c>
+    </row>
+    <row r="2591" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2591" s="4" t="s">
+        <v>7972</v>
+      </c>
+      <c r="B2591" s="3" t="s">
+        <v>7973</v>
+      </c>
+      <c r="C2591" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2591" s="3" t="s">
+        <v>7974</v>
+      </c>
+      <c r="E2591" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2591" s="3">
+        <v>45942.67222222222</v>
+      </c>
+    </row>
+    <row r="2592" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2592" s="4" t="s">
+        <v>7975</v>
+      </c>
+      <c r="B2592" s="3" t="s">
+        <v>7976</v>
+      </c>
+      <c r="C2592" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2592" s="3" t="s">
+        <v>3772</v>
+      </c>
+      <c r="E2592" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2592" s="3">
+        <v>45941.92638888889</v>
+      </c>
+    </row>
+    <row r="2593" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2593" s="4" t="s">
+        <v>7977</v>
+      </c>
+      <c r="B2593" s="3" t="s">
+        <v>7978</v>
+      </c>
+      <c r="C2593" s="3" t="s">
+        <v>4671</v>
+      </c>
+      <c r="D2593" s="3" t="s">
+        <v>7979</v>
+      </c>
+      <c r="E2593" s="3" t="s">
+        <v>7980</v>
+      </c>
+      <c r="F2593" s="3">
+        <v>45943.44375</v>
+      </c>
+    </row>
+    <row r="2594" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2594" s="4" t="s">
+        <v>7981</v>
+      </c>
+      <c r="B2594" s="3" t="s">
+        <v>7982</v>
+      </c>
+      <c r="C2594" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2594" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="E2594" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2594" s="3">
+        <v>45942.8125</v>
+      </c>
+    </row>
+    <row r="2595" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2595" s="4" t="s">
+        <v>7983</v>
+      </c>
+      <c r="B2595" s="3" t="s">
+        <v>7984</v>
+      </c>
+      <c r="C2595" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2595" s="3" t="s">
+        <v>4632</v>
+      </c>
+      <c r="E2595" s="3" t="s">
+        <v>7985</v>
+      </c>
+      <c r="F2595" s="3">
+        <v>45942.7625</v>
+      </c>
+    </row>
+    <row r="2596" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2596" s="4" t="s">
+        <v>7986</v>
+      </c>
+      <c r="B2596" s="3" t="s">
+        <v>7987</v>
+      </c>
+      <c r="C2596" s="3" t="s">
+        <v>5147</v>
+      </c>
+      <c r="D2596" s="3" t="s">
+        <v>7988</v>
+      </c>
+      <c r="E2596" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2596" s="3">
+        <v>45942.57083333333</v>
+      </c>
+    </row>
+    <row r="2597" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2597" s="4" t="s">
+        <v>7989</v>
+      </c>
+      <c r="B2597" s="3" t="s">
+        <v>7990</v>
+      </c>
+      <c r="C2597" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2597" s="3" t="s">
+        <v>7991</v>
+      </c>
+      <c r="E2597" s="3" t="s">
+        <v>7992</v>
+      </c>
+      <c r="F2597" s="3">
+        <v>45943.40416666667</v>
+      </c>
+    </row>
+    <row r="2598" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2598" s="4" t="s">
+        <v>7993</v>
+      </c>
+      <c r="B2598" s="3" t="s">
+        <v>7994</v>
+      </c>
+      <c r="C2598" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2598" s="3" t="s">
+        <v>7995</v>
+      </c>
+      <c r="E2598" s="3" t="s">
+        <v>7996</v>
+      </c>
+      <c r="F2598" s="3">
+        <v>45940.72152777778</v>
+      </c>
+    </row>
+    <row r="2599" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2599" s="4" t="s">
+        <v>7997</v>
+      </c>
+      <c r="B2599" s="3" t="s">
+        <v>7998</v>
+      </c>
+      <c r="C2599" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2599" s="3" t="s">
+        <v>7999</v>
+      </c>
+      <c r="E2599" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2599" s="3">
+        <v>45943.63611111111</v>
+      </c>
+    </row>
+    <row r="2600" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2600" s="4" t="s">
+        <v>8000</v>
+      </c>
+      <c r="B2600" s="3" t="s">
+        <v>8001</v>
+      </c>
+      <c r="C2600" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2600" s="3" t="s">
+        <v>8002</v>
+      </c>
+      <c r="E2600" s="3" t="s">
+        <v>8003</v>
+      </c>
+      <c r="F2600" s="3">
+        <v>45943.62013888889</v>
+      </c>
+    </row>
+    <row r="2601" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2601" s="4" t="s">
+        <v>8004</v>
+      </c>
+      <c r="B2601" s="3" t="s">
+        <v>8005</v>
+      </c>
+      <c r="C2601" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2601" s="3" t="s">
+        <v>8006</v>
+      </c>
+      <c r="E2601" s="3" t="s">
+        <v>8007</v>
+      </c>
+      <c r="F2601" s="3">
+        <v>45943.40416666667</v>
+      </c>
+    </row>
+    <row r="2602" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2602" s="4" t="s">
+        <v>8008</v>
+      </c>
+      <c r="B2602" s="3" t="s">
+        <v>5900</v>
+      </c>
+      <c r="C2602" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2602" s="3" t="s">
+        <v>5901</v>
+      </c>
+      <c r="E2602" s="3" t="s">
+        <v>5902</v>
+      </c>
+      <c r="F2602" s="3">
+        <v>45942.618055555555</v>
+      </c>
+    </row>
+    <row r="2603" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2603" s="4" t="s">
+        <v>8009</v>
+      </c>
+      <c r="B2603" s="3" t="s">
+        <v>897</v>
+      </c>
+      <c r="C2603" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2603" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="E2603" s="3" t="s">
+        <v>8010</v>
+      </c>
+      <c r="F2603" s="3">
+        <v>45942.527083333334</v>
+      </c>
+    </row>
+    <row r="2604" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2604" s="4" t="s">
+        <v>8011</v>
+      </c>
+      <c r="B2604" s="3" t="s">
+        <v>8012</v>
+      </c>
+      <c r="C2604" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2604" s="3" t="s">
+        <v>5309</v>
+      </c>
+      <c r="E2604" s="3" t="s">
+        <v>8013</v>
+      </c>
+      <c r="F2604" s="3">
+        <v>45941.87361111111</v>
+      </c>
+    </row>
+    <row r="2605" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2605" s="4" t="s">
+        <v>8014</v>
+      </c>
+      <c r="B2605" s="3" t="s">
+        <v>8015</v>
+      </c>
+      <c r="C2605" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2605" s="3" t="s">
+        <v>8016</v>
+      </c>
+      <c r="E2605" s="3" t="s">
+        <v>8017</v>
+      </c>
+      <c r="F2605" s="3">
+        <v>45941.81805555556</v>
+      </c>
+    </row>
+    <row r="2606" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2606" s="4" t="s">
+        <v>8018</v>
+      </c>
+      <c r="B2606" s="3" t="s">
+        <v>8019</v>
+      </c>
+      <c r="C2606" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2606" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="E2606" s="3" t="s">
+        <v>8020</v>
+      </c>
+      <c r="F2606" s="3">
+        <v>45941.79583333334</v>
+      </c>
+    </row>
+    <row r="2607" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2607" s="4" t="s">
+        <v>8021</v>
+      </c>
+      <c r="B2607" s="3" t="s">
+        <v>8022</v>
+      </c>
+      <c r="C2607" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2607" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2607" s="3" t="s">
+        <v>8023</v>
+      </c>
+      <c r="F2607" s="3">
+        <v>45940.98333333334</v>
+      </c>
+    </row>
+    <row r="2608" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2608" s="4" t="s">
+        <v>8024</v>
+      </c>
+      <c r="B2608" s="3" t="s">
+        <v>8025</v>
+      </c>
+      <c r="C2608" s="3" t="s">
+        <v>6133</v>
+      </c>
+      <c r="D2608" s="3" t="s">
+        <v>1535</v>
+      </c>
+      <c r="E2608" s="3" t="s">
+        <v>8026</v>
+      </c>
+      <c r="F2608" s="3">
+        <v>45941.71527777778</v>
+      </c>
+    </row>
+    <row r="2609" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2609" s="4" t="s">
+        <v>8027</v>
+      </c>
+      <c r="B2609" s="3" t="s">
+        <v>6410</v>
+      </c>
+      <c r="C2609" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2609" s="3" t="s">
+        <v>6411</v>
+      </c>
+      <c r="E2609" s="3" t="s">
+        <v>8028</v>
+      </c>
+      <c r="F2609" s="3">
+        <v>45943.580555555556</v>
+      </c>
+    </row>
+    <row r="2610" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2610" s="4" t="s">
+        <v>8029</v>
+      </c>
+      <c r="B2610" s="3" t="s">
+        <v>8030</v>
+      </c>
+      <c r="C2610" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2610" s="3" t="s">
+        <v>8031</v>
+      </c>
+      <c r="E2610" s="3" t="s">
+        <v>8032</v>
+      </c>
+      <c r="F2610" s="3">
+        <v>45941.48888888889</v>
+      </c>
+    </row>
+    <row r="2611" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2611" s="4" t="s">
+        <v>8033</v>
+      </c>
+      <c r="B2611" s="3" t="s">
+        <v>8034</v>
+      </c>
+      <c r="C2611" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2611" s="3" t="s">
+        <v>7108</v>
+      </c>
+      <c r="E2611" s="3" t="s">
+        <v>8035</v>
+      </c>
+      <c r="F2611" s="3">
+        <v>45943.575694444444</v>
+      </c>
+    </row>
+    <row r="2612" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2612" s="4" t="s">
+        <v>8036</v>
+      </c>
+      <c r="B2612" s="3" t="s">
+        <v>8037</v>
+      </c>
+      <c r="C2612" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2612" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2612" s="3" t="s">
+        <v>8038</v>
+      </c>
+      <c r="F2612" s="3">
+        <v>45943.51527777778</v>
+      </c>
+    </row>
+    <row r="2613" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2613" s="4" t="s">
+        <v>8039</v>
+      </c>
+      <c r="B2613" s="3" t="s">
+        <v>8040</v>
+      </c>
+      <c r="C2613" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2613" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="E2613" s="3" t="s">
+        <v>8041</v>
+      </c>
+      <c r="F2613" s="3">
+        <v>45943.50833333333</v>
+      </c>
+    </row>
+    <row r="2614" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2614" s="4" t="s">
+        <v>8042</v>
+      </c>
+      <c r="B2614" s="3" t="s">
+        <v>8043</v>
+      </c>
+      <c r="C2614" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2614" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2614" s="3" t="s">
+        <v>8044</v>
+      </c>
+      <c r="F2614" s="3">
+        <v>45943.506944444445</v>
+      </c>
+    </row>
+    <row r="2615" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2615" s="4" t="s">
+        <v>8045</v>
+      </c>
+      <c r="B2615" s="3" t="s">
+        <v>8046</v>
+      </c>
+      <c r="C2615" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2615" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="E2615" s="3" t="s">
+        <v>8047</v>
+      </c>
+      <c r="F2615" s="3">
+        <v>45943.50625</v>
+      </c>
+    </row>
+    <row r="2616" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2616" s="4" t="s">
+        <v>8048</v>
+      </c>
+      <c r="B2616" s="3" t="s">
+        <v>8049</v>
+      </c>
+      <c r="C2616" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2616" s="3" t="s">
+        <v>683</v>
+      </c>
+      <c r="E2616" s="3" t="s">
+        <v>8050</v>
+      </c>
+      <c r="F2616" s="3">
+        <v>45943.50347222222</v>
+      </c>
+    </row>
+    <row r="2617" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2617" s="4" t="s">
+        <v>8051</v>
+      </c>
+      <c r="B2617" s="3" t="s">
+        <v>8052</v>
+      </c>
+      <c r="C2617" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2617" s="3" t="s">
+        <v>8053</v>
+      </c>
+      <c r="E2617" s="3" t="s">
+        <v>8054</v>
+      </c>
+      <c r="F2617" s="3">
+        <v>45943.50277777778</v>
+      </c>
+    </row>
+    <row r="2618" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2618" s="4" t="s">
+        <v>8055</v>
+      </c>
+      <c r="B2618" s="3" t="s">
+        <v>8056</v>
+      </c>
+      <c r="C2618" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2618" s="3" t="s">
+        <v>1709</v>
+      </c>
+      <c r="E2618" s="3" t="s">
+        <v>8057</v>
+      </c>
+      <c r="F2618" s="3">
+        <v>45943.49861111111</v>
+      </c>
+    </row>
+    <row r="2619" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2619" s="4" t="s">
+        <v>8058</v>
+      </c>
+      <c r="B2619" s="3" t="s">
+        <v>8059</v>
+      </c>
+      <c r="C2619" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2619" s="3" t="s">
+        <v>1709</v>
+      </c>
+      <c r="E2619" s="3" t="s">
+        <v>8060</v>
+      </c>
+      <c r="F2619" s="3">
+        <v>45943.49375</v>
+      </c>
+    </row>
+    <row r="2620" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2620" s="4" t="s">
+        <v>8061</v>
+      </c>
+      <c r="B2620" s="3" t="s">
+        <v>8062</v>
+      </c>
+      <c r="C2620" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2620" s="3" t="s">
+        <v>6473</v>
+      </c>
+      <c r="E2620" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2620" s="3">
+        <v>45942.683333333334</v>
+      </c>
+    </row>
+    <row r="2621" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2621" s="4" t="s">
+        <v>8063</v>
+      </c>
+      <c r="B2621" s="3" t="s">
+        <v>8064</v>
+      </c>
+      <c r="C2621" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2621" s="3" t="s">
+        <v>8065</v>
+      </c>
+      <c r="E2621" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2621" s="3">
+        <v>45941.54166666667</v>
       </c>
     </row>
   </sheetData>
@@ -79758,6 +80547,75 @@
     <hyperlink ref="A2550" r:id="rId2549"/>
     <hyperlink ref="A2551" r:id="rId2550"/>
     <hyperlink ref="A2552" r:id="rId2551"/>
+    <hyperlink ref="A2553" r:id="rId2552"/>
+    <hyperlink ref="A2554" r:id="rId2553"/>
+    <hyperlink ref="A2555" r:id="rId2554"/>
+    <hyperlink ref="A2556" r:id="rId2555"/>
+    <hyperlink ref="A2557" r:id="rId2556"/>
+    <hyperlink ref="A2558" r:id="rId2557"/>
+    <hyperlink ref="A2559" r:id="rId2558"/>
+    <hyperlink ref="A2560" r:id="rId2559"/>
+    <hyperlink ref="A2561" r:id="rId2560"/>
+    <hyperlink ref="A2562" r:id="rId2561"/>
+    <hyperlink ref="A2563" r:id="rId2562"/>
+    <hyperlink ref="A2564" r:id="rId2563"/>
+    <hyperlink ref="A2565" r:id="rId2564"/>
+    <hyperlink ref="A2566" r:id="rId2565"/>
+    <hyperlink ref="A2567" r:id="rId2566"/>
+    <hyperlink ref="A2568" r:id="rId2567"/>
+    <hyperlink ref="A2569" r:id="rId2568"/>
+    <hyperlink ref="A2570" r:id="rId2569"/>
+    <hyperlink ref="A2571" r:id="rId2570"/>
+    <hyperlink ref="A2572" r:id="rId2571"/>
+    <hyperlink ref="A2573" r:id="rId2572"/>
+    <hyperlink ref="A2574" r:id="rId2573"/>
+    <hyperlink ref="A2575" r:id="rId2574"/>
+    <hyperlink ref="A2576" r:id="rId2575"/>
+    <hyperlink ref="A2577" r:id="rId2576"/>
+    <hyperlink ref="A2578" r:id="rId2577"/>
+    <hyperlink ref="A2579" r:id="rId2578"/>
+    <hyperlink ref="A2580" r:id="rId2579"/>
+    <hyperlink ref="A2581" r:id="rId2580"/>
+    <hyperlink ref="A2582" r:id="rId2581"/>
+    <hyperlink ref="A2583" r:id="rId2582"/>
+    <hyperlink ref="A2584" r:id="rId2583"/>
+    <hyperlink ref="A2585" r:id="rId2584"/>
+    <hyperlink ref="A2586" r:id="rId2585"/>
+    <hyperlink ref="A2587" r:id="rId2586"/>
+    <hyperlink ref="A2588" r:id="rId2587"/>
+    <hyperlink ref="A2589" r:id="rId2588"/>
+    <hyperlink ref="A2590" r:id="rId2589"/>
+    <hyperlink ref="A2591" r:id="rId2590"/>
+    <hyperlink ref="A2592" r:id="rId2591"/>
+    <hyperlink ref="A2593" r:id="rId2592"/>
+    <hyperlink ref="A2594" r:id="rId2593"/>
+    <hyperlink ref="A2595" r:id="rId2594"/>
+    <hyperlink ref="A2596" r:id="rId2595"/>
+    <hyperlink ref="A2597" r:id="rId2596"/>
+    <hyperlink ref="A2598" r:id="rId2597"/>
+    <hyperlink ref="A2599" r:id="rId2598"/>
+    <hyperlink ref="A2600" r:id="rId2599"/>
+    <hyperlink ref="A2601" r:id="rId2600"/>
+    <hyperlink ref="A2602" r:id="rId2601"/>
+    <hyperlink ref="A2603" r:id="rId2602"/>
+    <hyperlink ref="A2604" r:id="rId2603"/>
+    <hyperlink ref="A2605" r:id="rId2604"/>
+    <hyperlink ref="A2606" r:id="rId2605"/>
+    <hyperlink ref="A2607" r:id="rId2606"/>
+    <hyperlink ref="A2608" r:id="rId2607"/>
+    <hyperlink ref="A2609" r:id="rId2608"/>
+    <hyperlink ref="A2610" r:id="rId2609"/>
+    <hyperlink ref="A2611" r:id="rId2610"/>
+    <hyperlink ref="A2612" r:id="rId2611"/>
+    <hyperlink ref="A2613" r:id="rId2612"/>
+    <hyperlink ref="A2614" r:id="rId2613"/>
+    <hyperlink ref="A2615" r:id="rId2614"/>
+    <hyperlink ref="A2616" r:id="rId2615"/>
+    <hyperlink ref="A2617" r:id="rId2616"/>
+    <hyperlink ref="A2618" r:id="rId2617"/>
+    <hyperlink ref="A2619" r:id="rId2618"/>
+    <hyperlink ref="A2620" r:id="rId2619"/>
+    <hyperlink ref="A2621" r:id="rId2620"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Update lands data - 2025-10-15 12:22
</commit_message>
<xml_diff>
--- a/lands-scraped.xlsx
+++ b/lands-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13262" uniqueCount="8142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13337" uniqueCount="8182">
   <si>
     <t>link</t>
   </si>
@@ -24444,6 +24444,126 @@
   </si>
   <si>
     <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/usmas-pag/bgfeo.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/tabores-pag/aalol.html</t>
+  </si>
+  <si>
+    <t>3 950 € (1.37 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/dobele-and-reg/auru-pag/cggjdx.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jekabpils-and-reg/mezares-pag/llgip.html</t>
+  </si>
+  <si>
+    <t>50 500 € (0.56 €/m²)</t>
+  </si>
+  <si>
+    <t>56760030102</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/vecpils-pag/imcko.html</t>
+  </si>
+  <si>
+    <t>72 000 € (0.72 €/m²)</t>
+  </si>
+  <si>
+    <t>64940020046</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/madona-and-reg/jumurdas-pag/gonnl.html</t>
+  </si>
+  <si>
+    <t>100 000 € (0.42 €/m²)</t>
+  </si>
+  <si>
+    <t>70600080001</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/birzgales-pag/hnhjl.html</t>
+  </si>
+  <si>
+    <t>26 800 € (0.70 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ogre/boxxp.html</t>
+  </si>
+  <si>
+    <t>35 000 € (29.17 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/taurupes-pag/gxdbe.html</t>
+  </si>
+  <si>
+    <t>30 000 € (1.25 €/m²)</t>
+  </si>
+  <si>
+    <t>74920080060</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ikskile/hnexb.html</t>
+  </si>
+  <si>
+    <t>33 500 € (13.96 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/rezekne/bxejig.html</t>
+  </si>
+  <si>
+    <t>15 000 € (4.55 €/m²)</t>
+  </si>
+  <si>
+    <t>21000080411</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/veremu-pag/amllb.html</t>
+  </si>
+  <si>
+    <t>17 000 € (1.70 €/m²)</t>
+  </si>
+  <si>
+    <t>78960040117</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/silmalas-pag/fjghb.html</t>
+  </si>
+  <si>
+    <t>9 000 € (0.39 €/m²)</t>
+  </si>
+  <si>
+    <t>78880080031</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/engures-pag/amghn.html</t>
+  </si>
+  <si>
+    <t>36 000 € (12.54 €/m²)</t>
+  </si>
+  <si>
+    <t>2871 m²</t>
+  </si>
+  <si>
+    <t>90500051582</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/engures-pag/cgckx.html</t>
+  </si>
+  <si>
+    <t>90500050693</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/rencenu-pag/hongl.html</t>
+  </si>
+  <si>
+    <t>6 900 € (2.11 €/m²)</t>
+  </si>
+  <si>
+    <t>3266 m²</t>
+  </si>
+  <si>
+    <t>96780060150</t>
   </si>
 </sst>
 </file>
@@ -24879,7 +24999,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -24918,602 +25038,302 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>8066</v>
+        <v>8142</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>8067</v>
+        <v>8143</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>8</v>
+        <v>1218</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>7501</v>
+        <v>4499</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>8068</v>
+        <v>1371</v>
       </c>
       <c r="F2" s="3">
-        <v>45943.79791666666</v>
+        <v>45945.44097222222</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>8069</v>
+        <v>8144</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>8070</v>
+        <v>3063</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>419</v>
+        <v>1569</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>8071</v>
+        <v>171</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>8072</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3">
-        <v>45943.986805555556</v>
+        <v>45945.56736111111</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>8073</v>
+        <v>8145</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>8074</v>
+        <v>8146</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>419</v>
+        <v>1733</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>8075</v>
+        <v>1430</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>8076</v>
+        <v>8147</v>
       </c>
       <c r="F4" s="3">
-        <v>45943.89513888889</v>
+        <v>45945.54791666666</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>8077</v>
+        <v>8148</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>905</v>
+        <v>8149</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>772</v>
+        <v>2846</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>906</v>
+        <v>325</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>907</v>
+        <v>8150</v>
       </c>
       <c r="F5" s="3">
-        <v>45944.55208333333</v>
+        <v>45945.4875</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>8078</v>
+        <v>8151</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>8079</v>
+        <v>8152</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>772</v>
+        <v>3868</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>10</v>
+        <v>8153</v>
       </c>
       <c r="F6" s="3">
-        <v>45943.85972222222</v>
+        <v>45945.50208333333</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>8080</v>
+        <v>8154</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>8081</v>
+        <v>8155</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>1218</v>
+        <v>4034</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>8082</v>
+        <v>4302</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>8083</v>
+        <v>4303</v>
       </c>
       <c r="F7" s="3">
-        <v>45943.8375</v>
+        <v>45945.45763888889</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>8084</v>
+        <v>8156</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>306</v>
+        <v>8157</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1569</v>
+        <v>4034</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>201</v>
+        <v>436</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>8085</v>
+        <v>10</v>
       </c>
       <c r="F8" s="3">
-        <v>45944.32916666666</v>
+        <v>45945.4375</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>8086</v>
+        <v>8158</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>8087</v>
+        <v>8159</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>1569</v>
+        <v>4034</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>3414</v>
+        <v>2244</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>8088</v>
+        <v>8160</v>
       </c>
       <c r="F9" s="3">
-        <v>45943.65694444445</v>
+        <v>45944.853472222225</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>8089</v>
+        <v>8161</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>331</v>
+        <v>8162</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>1733</v>
+        <v>4034</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>561</v>
+        <v>2912</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>8090</v>
+        <v>10</v>
       </c>
       <c r="F10" s="3">
-        <v>45944.57708333334</v>
+        <v>45944.714583333334</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>8091</v>
+        <v>8163</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>8092</v>
+        <v>8164</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>1929</v>
+        <v>4770</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>561</v>
+        <v>4433</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>8093</v>
+        <v>8165</v>
       </c>
       <c r="F11" s="3">
-        <v>45944.58472222222</v>
+        <v>45945.57430555555</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>8094</v>
+        <v>8166</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>8095</v>
+        <v>8167</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>1929</v>
+        <v>4770</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>8096</v>
+        <v>32</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>10</v>
+        <v>8168</v>
       </c>
       <c r="F12" s="3">
-        <v>45944.45833333333</v>
+        <v>45945.56875</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>8097</v>
+        <v>8169</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>8098</v>
+        <v>8170</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>1929</v>
+        <v>4770</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>8099</v>
+        <v>1913</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>10</v>
+        <v>8171</v>
       </c>
       <c r="F13" s="3">
-        <v>45944.444444444445</v>
+        <v>45944.683333333334</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>8100</v>
+        <v>8172</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>8101</v>
+        <v>8173</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>2488</v>
+        <v>5674</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>8102</v>
+        <v>8174</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>8103</v>
+        <v>8175</v>
       </c>
       <c r="F14" s="3">
-        <v>45944.45</v>
+        <v>45945.38125</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>8104</v>
+        <v>8176</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>3082</v>
+        <v>5831</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>2846</v>
+        <v>5674</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>3083</v>
+        <v>2912</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>10</v>
+        <v>8177</v>
       </c>
       <c r="F15" s="3">
-        <v>45943.743055555555</v>
+        <v>45945.38055555556</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>8105</v>
+        <v>8178</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>8106</v>
+        <v>8179</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>3398</v>
+        <v>6207</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>8107</v>
+        <v>8180</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>8108</v>
+        <v>8181</v>
       </c>
       <c r="F16" s="3">
-        <v>45944.584027777775</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>8109</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>4429</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>8110</v>
-      </c>
-      <c r="F17" s="3">
-        <v>45944.53472222222</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>8111</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>2710</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>474</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>8112</v>
-      </c>
-      <c r="F18" s="3">
-        <v>45944.52986111111</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>8113</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>8114</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>8115</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>8116</v>
-      </c>
-      <c r="F19" s="3">
-        <v>45944.45277777778</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>8117</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>8118</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>2166</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>8119</v>
-      </c>
-      <c r="F20" s="3">
-        <v>45944.43541666667</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>8120</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>4774</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>4034</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="3">
-        <v>45943.853472222225</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>8121</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>8122</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>4770</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>8123</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="3">
-        <v>45943.77638888889</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>8124</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>8125</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>5266</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>8126</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="3">
-        <v>45944.61111111111</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>8127</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>2804</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>5266</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>8128</v>
-      </c>
-      <c r="F24" s="3">
-        <v>45944.58541666667</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>8129</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>8130</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>5266</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>8131</v>
-      </c>
-      <c r="F25" s="3">
-        <v>45944.46805555555</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>8132</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>5359</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>5266</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>5360</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>5361</v>
-      </c>
-      <c r="F26" s="3">
-        <v>45943.85486111111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>8133</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>5886</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>5674</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>2446</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>5887</v>
-      </c>
-      <c r="F27" s="3">
-        <v>45944.41111111111</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>8134</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>5627</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>5674</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>1632</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" s="3">
-        <v>45943.804861111115</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
-        <v>8135</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>2615</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>6207</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>325</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>8136</v>
-      </c>
-      <c r="F29" s="3">
-        <v>45943.853472222225</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>8137</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>8138</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>6207</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>8139</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>8140</v>
-      </c>
-      <c r="F30" s="3">
-        <v>45943.683333333334</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>8141</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>5870</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>383</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="3">
-        <v>45943.85972222222</v>
+        <v>45945.18194444444</v>
       </c>
     </row>
   </sheetData>
@@ -25533,21 +25353,6 @@
     <hyperlink ref="A14" r:id="rId13"/>
     <hyperlink ref="A15" r:id="rId14"/>
     <hyperlink ref="A16" r:id="rId15"/>
-    <hyperlink ref="A17" r:id="rId16"/>
-    <hyperlink ref="A18" r:id="rId17"/>
-    <hyperlink ref="A19" r:id="rId18"/>
-    <hyperlink ref="A20" r:id="rId19"/>
-    <hyperlink ref="A21" r:id="rId20"/>
-    <hyperlink ref="A22" r:id="rId21"/>
-    <hyperlink ref="A23" r:id="rId22"/>
-    <hyperlink ref="A24" r:id="rId23"/>
-    <hyperlink ref="A25" r:id="rId24"/>
-    <hyperlink ref="A26" r:id="rId25"/>
-    <hyperlink ref="A27" r:id="rId26"/>
-    <hyperlink ref="A28" r:id="rId27"/>
-    <hyperlink ref="A29" r:id="rId28"/>
-    <hyperlink ref="A30" r:id="rId29"/>
-    <hyperlink ref="A31" r:id="rId30"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -25556,7 +25361,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2621"/>
+  <dimension ref="A1:F2651"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -77992,6 +77797,606 @@
       </c>
       <c r="F2621" s="3">
         <v>45941.54166666667</v>
+      </c>
+    </row>
+    <row r="2622" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2622" s="4" t="s">
+        <v>8066</v>
+      </c>
+      <c r="B2622" s="3" t="s">
+        <v>8067</v>
+      </c>
+      <c r="C2622" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2622" s="3" t="s">
+        <v>7501</v>
+      </c>
+      <c r="E2622" s="3" t="s">
+        <v>8068</v>
+      </c>
+      <c r="F2622" s="3">
+        <v>45943.79791666666</v>
+      </c>
+    </row>
+    <row r="2623" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2623" s="4" t="s">
+        <v>8069</v>
+      </c>
+      <c r="B2623" s="3" t="s">
+        <v>8070</v>
+      </c>
+      <c r="C2623" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2623" s="3" t="s">
+        <v>8071</v>
+      </c>
+      <c r="E2623" s="3" t="s">
+        <v>8072</v>
+      </c>
+      <c r="F2623" s="3">
+        <v>45943.986805555556</v>
+      </c>
+    </row>
+    <row r="2624" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2624" s="4" t="s">
+        <v>8073</v>
+      </c>
+      <c r="B2624" s="3" t="s">
+        <v>8074</v>
+      </c>
+      <c r="C2624" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2624" s="3" t="s">
+        <v>8075</v>
+      </c>
+      <c r="E2624" s="3" t="s">
+        <v>8076</v>
+      </c>
+      <c r="F2624" s="3">
+        <v>45943.89513888889</v>
+      </c>
+    </row>
+    <row r="2625" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2625" s="4" t="s">
+        <v>8077</v>
+      </c>
+      <c r="B2625" s="3" t="s">
+        <v>905</v>
+      </c>
+      <c r="C2625" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2625" s="3" t="s">
+        <v>906</v>
+      </c>
+      <c r="E2625" s="3" t="s">
+        <v>907</v>
+      </c>
+      <c r="F2625" s="3">
+        <v>45944.55208333333</v>
+      </c>
+    </row>
+    <row r="2626" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2626" s="4" t="s">
+        <v>8078</v>
+      </c>
+      <c r="B2626" s="3" t="s">
+        <v>8079</v>
+      </c>
+      <c r="C2626" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2626" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2626" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2626" s="3">
+        <v>45943.85972222222</v>
+      </c>
+    </row>
+    <row r="2627" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2627" s="4" t="s">
+        <v>8080</v>
+      </c>
+      <c r="B2627" s="3" t="s">
+        <v>8081</v>
+      </c>
+      <c r="C2627" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2627" s="3" t="s">
+        <v>8082</v>
+      </c>
+      <c r="E2627" s="3" t="s">
+        <v>8083</v>
+      </c>
+      <c r="F2627" s="3">
+        <v>45943.8375</v>
+      </c>
+    </row>
+    <row r="2628" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2628" s="4" t="s">
+        <v>8084</v>
+      </c>
+      <c r="B2628" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C2628" s="3" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D2628" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2628" s="3" t="s">
+        <v>8085</v>
+      </c>
+      <c r="F2628" s="3">
+        <v>45944.32916666666</v>
+      </c>
+    </row>
+    <row r="2629" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2629" s="4" t="s">
+        <v>8086</v>
+      </c>
+      <c r="B2629" s="3" t="s">
+        <v>8087</v>
+      </c>
+      <c r="C2629" s="3" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D2629" s="3" t="s">
+        <v>3414</v>
+      </c>
+      <c r="E2629" s="3" t="s">
+        <v>8088</v>
+      </c>
+      <c r="F2629" s="3">
+        <v>45943.65694444445</v>
+      </c>
+    </row>
+    <row r="2630" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2630" s="4" t="s">
+        <v>8089</v>
+      </c>
+      <c r="B2630" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C2630" s="3" t="s">
+        <v>1733</v>
+      </c>
+      <c r="D2630" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="E2630" s="3" t="s">
+        <v>8090</v>
+      </c>
+      <c r="F2630" s="3">
+        <v>45944.57708333334</v>
+      </c>
+    </row>
+    <row r="2631" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2631" s="4" t="s">
+        <v>8091</v>
+      </c>
+      <c r="B2631" s="3" t="s">
+        <v>8092</v>
+      </c>
+      <c r="C2631" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2631" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="E2631" s="3" t="s">
+        <v>8093</v>
+      </c>
+      <c r="F2631" s="3">
+        <v>45944.58472222222</v>
+      </c>
+    </row>
+    <row r="2632" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2632" s="4" t="s">
+        <v>8094</v>
+      </c>
+      <c r="B2632" s="3" t="s">
+        <v>8095</v>
+      </c>
+      <c r="C2632" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2632" s="3" t="s">
+        <v>8096</v>
+      </c>
+      <c r="E2632" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2632" s="3">
+        <v>45944.45833333333</v>
+      </c>
+    </row>
+    <row r="2633" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2633" s="4" t="s">
+        <v>8097</v>
+      </c>
+      <c r="B2633" s="3" t="s">
+        <v>8098</v>
+      </c>
+      <c r="C2633" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2633" s="3" t="s">
+        <v>8099</v>
+      </c>
+      <c r="E2633" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2633" s="3">
+        <v>45944.444444444445</v>
+      </c>
+    </row>
+    <row r="2634" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2634" s="4" t="s">
+        <v>8100</v>
+      </c>
+      <c r="B2634" s="3" t="s">
+        <v>8101</v>
+      </c>
+      <c r="C2634" s="3" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D2634" s="3" t="s">
+        <v>8102</v>
+      </c>
+      <c r="E2634" s="3" t="s">
+        <v>8103</v>
+      </c>
+      <c r="F2634" s="3">
+        <v>45944.45</v>
+      </c>
+    </row>
+    <row r="2635" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2635" s="4" t="s">
+        <v>8104</v>
+      </c>
+      <c r="B2635" s="3" t="s">
+        <v>3082</v>
+      </c>
+      <c r="C2635" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2635" s="3" t="s">
+        <v>3083</v>
+      </c>
+      <c r="E2635" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2635" s="3">
+        <v>45943.743055555555</v>
+      </c>
+    </row>
+    <row r="2636" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2636" s="4" t="s">
+        <v>8105</v>
+      </c>
+      <c r="B2636" s="3" t="s">
+        <v>8106</v>
+      </c>
+      <c r="C2636" s="3" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D2636" s="3" t="s">
+        <v>8107</v>
+      </c>
+      <c r="E2636" s="3" t="s">
+        <v>8108</v>
+      </c>
+      <c r="F2636" s="3">
+        <v>45944.584027777775</v>
+      </c>
+    </row>
+    <row r="2637" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2637" s="4" t="s">
+        <v>8109</v>
+      </c>
+      <c r="B2637" s="3" t="s">
+        <v>4429</v>
+      </c>
+      <c r="C2637" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2637" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2637" s="3" t="s">
+        <v>8110</v>
+      </c>
+      <c r="F2637" s="3">
+        <v>45944.53472222222</v>
+      </c>
+    </row>
+    <row r="2638" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2638" s="4" t="s">
+        <v>8111</v>
+      </c>
+      <c r="B2638" s="3" t="s">
+        <v>2710</v>
+      </c>
+      <c r="C2638" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2638" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="E2638" s="3" t="s">
+        <v>8112</v>
+      </c>
+      <c r="F2638" s="3">
+        <v>45944.52986111111</v>
+      </c>
+    </row>
+    <row r="2639" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2639" s="4" t="s">
+        <v>8113</v>
+      </c>
+      <c r="B2639" s="3" t="s">
+        <v>8114</v>
+      </c>
+      <c r="C2639" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2639" s="3" t="s">
+        <v>8115</v>
+      </c>
+      <c r="E2639" s="3" t="s">
+        <v>8116</v>
+      </c>
+      <c r="F2639" s="3">
+        <v>45944.45277777778</v>
+      </c>
+    </row>
+    <row r="2640" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2640" s="4" t="s">
+        <v>8117</v>
+      </c>
+      <c r="B2640" s="3" t="s">
+        <v>8118</v>
+      </c>
+      <c r="C2640" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2640" s="3" t="s">
+        <v>2166</v>
+      </c>
+      <c r="E2640" s="3" t="s">
+        <v>8119</v>
+      </c>
+      <c r="F2640" s="3">
+        <v>45944.43541666667</v>
+      </c>
+    </row>
+    <row r="2641" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2641" s="4" t="s">
+        <v>8120</v>
+      </c>
+      <c r="B2641" s="3" t="s">
+        <v>4774</v>
+      </c>
+      <c r="C2641" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2641" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2641" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2641" s="3">
+        <v>45943.853472222225</v>
+      </c>
+    </row>
+    <row r="2642" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2642" s="4" t="s">
+        <v>8121</v>
+      </c>
+      <c r="B2642" s="3" t="s">
+        <v>8122</v>
+      </c>
+      <c r="C2642" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2642" s="3" t="s">
+        <v>8123</v>
+      </c>
+      <c r="E2642" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2642" s="3">
+        <v>45943.77638888889</v>
+      </c>
+    </row>
+    <row r="2643" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2643" s="4" t="s">
+        <v>8124</v>
+      </c>
+      <c r="B2643" s="3" t="s">
+        <v>8125</v>
+      </c>
+      <c r="C2643" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2643" s="3" t="s">
+        <v>8126</v>
+      </c>
+      <c r="E2643" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2643" s="3">
+        <v>45944.61111111111</v>
+      </c>
+    </row>
+    <row r="2644" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2644" s="4" t="s">
+        <v>8127</v>
+      </c>
+      <c r="B2644" s="3" t="s">
+        <v>2804</v>
+      </c>
+      <c r="C2644" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2644" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2644" s="3" t="s">
+        <v>8128</v>
+      </c>
+      <c r="F2644" s="3">
+        <v>45944.58541666667</v>
+      </c>
+    </row>
+    <row r="2645" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2645" s="4" t="s">
+        <v>8129</v>
+      </c>
+      <c r="B2645" s="3" t="s">
+        <v>8130</v>
+      </c>
+      <c r="C2645" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2645" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2645" s="3" t="s">
+        <v>8131</v>
+      </c>
+      <c r="F2645" s="3">
+        <v>45944.46805555555</v>
+      </c>
+    </row>
+    <row r="2646" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2646" s="4" t="s">
+        <v>8132</v>
+      </c>
+      <c r="B2646" s="3" t="s">
+        <v>5359</v>
+      </c>
+      <c r="C2646" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2646" s="3" t="s">
+        <v>5360</v>
+      </c>
+      <c r="E2646" s="3" t="s">
+        <v>5361</v>
+      </c>
+      <c r="F2646" s="3">
+        <v>45943.85486111111</v>
+      </c>
+    </row>
+    <row r="2647" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2647" s="4" t="s">
+        <v>8133</v>
+      </c>
+      <c r="B2647" s="3" t="s">
+        <v>5886</v>
+      </c>
+      <c r="C2647" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2647" s="3" t="s">
+        <v>2446</v>
+      </c>
+      <c r="E2647" s="3" t="s">
+        <v>5887</v>
+      </c>
+      <c r="F2647" s="3">
+        <v>45944.41111111111</v>
+      </c>
+    </row>
+    <row r="2648" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2648" s="4" t="s">
+        <v>8134</v>
+      </c>
+      <c r="B2648" s="3" t="s">
+        <v>5627</v>
+      </c>
+      <c r="C2648" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2648" s="3" t="s">
+        <v>1632</v>
+      </c>
+      <c r="E2648" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2648" s="3">
+        <v>45943.804861111115</v>
+      </c>
+    </row>
+    <row r="2649" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2649" s="4" t="s">
+        <v>8135</v>
+      </c>
+      <c r="B2649" s="3" t="s">
+        <v>2615</v>
+      </c>
+      <c r="C2649" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2649" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2649" s="3" t="s">
+        <v>8136</v>
+      </c>
+      <c r="F2649" s="3">
+        <v>45943.853472222225</v>
+      </c>
+    </row>
+    <row r="2650" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2650" s="4" t="s">
+        <v>8137</v>
+      </c>
+      <c r="B2650" s="3" t="s">
+        <v>8138</v>
+      </c>
+      <c r="C2650" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2650" s="3" t="s">
+        <v>8139</v>
+      </c>
+      <c r="E2650" s="3" t="s">
+        <v>8140</v>
+      </c>
+      <c r="F2650" s="3">
+        <v>45943.683333333334</v>
+      </c>
+    </row>
+    <row r="2651" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2651" s="4" t="s">
+        <v>8141</v>
+      </c>
+      <c r="B2651" s="3" t="s">
+        <v>5870</v>
+      </c>
+      <c r="C2651" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2651" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E2651" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2651" s="3">
+        <v>45943.85972222222</v>
       </c>
     </row>
   </sheetData>
@@ -80616,6 +81021,36 @@
     <hyperlink ref="A2619" r:id="rId2618"/>
     <hyperlink ref="A2620" r:id="rId2619"/>
     <hyperlink ref="A2621" r:id="rId2620"/>
+    <hyperlink ref="A2622" r:id="rId2621"/>
+    <hyperlink ref="A2623" r:id="rId2622"/>
+    <hyperlink ref="A2624" r:id="rId2623"/>
+    <hyperlink ref="A2625" r:id="rId2624"/>
+    <hyperlink ref="A2626" r:id="rId2625"/>
+    <hyperlink ref="A2627" r:id="rId2626"/>
+    <hyperlink ref="A2628" r:id="rId2627"/>
+    <hyperlink ref="A2629" r:id="rId2628"/>
+    <hyperlink ref="A2630" r:id="rId2629"/>
+    <hyperlink ref="A2631" r:id="rId2630"/>
+    <hyperlink ref="A2632" r:id="rId2631"/>
+    <hyperlink ref="A2633" r:id="rId2632"/>
+    <hyperlink ref="A2634" r:id="rId2633"/>
+    <hyperlink ref="A2635" r:id="rId2634"/>
+    <hyperlink ref="A2636" r:id="rId2635"/>
+    <hyperlink ref="A2637" r:id="rId2636"/>
+    <hyperlink ref="A2638" r:id="rId2637"/>
+    <hyperlink ref="A2639" r:id="rId2638"/>
+    <hyperlink ref="A2640" r:id="rId2639"/>
+    <hyperlink ref="A2641" r:id="rId2640"/>
+    <hyperlink ref="A2642" r:id="rId2641"/>
+    <hyperlink ref="A2643" r:id="rId2642"/>
+    <hyperlink ref="A2644" r:id="rId2643"/>
+    <hyperlink ref="A2645" r:id="rId2644"/>
+    <hyperlink ref="A2646" r:id="rId2645"/>
+    <hyperlink ref="A2647" r:id="rId2646"/>
+    <hyperlink ref="A2648" r:id="rId2647"/>
+    <hyperlink ref="A2649" r:id="rId2648"/>
+    <hyperlink ref="A2650" r:id="rId2649"/>
+    <hyperlink ref="A2651" r:id="rId2650"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Update lands data - 2025-10-16 12:21
</commit_message>
<xml_diff>
--- a/lands-scraped.xlsx
+++ b/lands-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13337" uniqueCount="8182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13412" uniqueCount="8227">
   <si>
     <t>link</t>
   </si>
@@ -24564,6 +24564,141 @@
   </si>
   <si>
     <t>96780060150</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/aizkraukle-and-reg/kokneses-pag/hndpl.html</t>
+  </si>
+  <si>
+    <t>26 000 € (1.50 €/m²)</t>
+  </si>
+  <si>
+    <t>1.73 ha.</t>
+  </si>
+  <si>
+    <t>32600120088</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/vecumnieku-pag/bdnlb.html</t>
+  </si>
+  <si>
+    <t>82 500 € (0.75 €/m²)</t>
+  </si>
+  <si>
+    <t>32620060046</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/nitaures-pag/inkic.html</t>
+  </si>
+  <si>
+    <t>42680060126</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/kalkunes-pag/akxpb.html</t>
+  </si>
+  <si>
+    <t>9 800 € (0.55 €/m²)</t>
+  </si>
+  <si>
+    <t>17900 m²</t>
+  </si>
+  <si>
+    <t>4600042151</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/naujenes-pag/kdcxk.html</t>
+  </si>
+  <si>
+    <t>91 500 € (0.74 €/m²)</t>
+  </si>
+  <si>
+    <t>12.35 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/laucesas-pag/jngmc.html</t>
+  </si>
+  <si>
+    <t>12 000 € (0.40 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/pavilosta/eejlm.html</t>
+  </si>
+  <si>
+    <t>175 000 € (174.30 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/jumpravas-pag/hbnmx.html</t>
+  </si>
+  <si>
+    <t>20 000 € (2.63 €/m²)</t>
+  </si>
+  <si>
+    <t>74480020326</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/keguma-l-t/blxmje.html</t>
+  </si>
+  <si>
+    <t>35 000 € (1.52 €/m²)</t>
+  </si>
+  <si>
+    <t>74290050003</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/preili-and-reg/preili/bfiei.html</t>
+  </si>
+  <si>
+    <t>13 800 € (21.50 €/m²)</t>
+  </si>
+  <si>
+    <t>642 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/nautrenu-pag/icgxe.html</t>
+  </si>
+  <si>
+    <t>520 200 € (0.45 €/m²)</t>
+  </si>
+  <si>
+    <t>115.60 ha.</t>
+  </si>
+  <si>
+    <t>68760010050</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/gibulu-pag/akljb.html</t>
+  </si>
+  <si>
+    <t>70 000 € (2.33 €/m²)</t>
+  </si>
+  <si>
+    <t>88540160060</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/jaunpils-pag/apopp.html</t>
+  </si>
+  <si>
+    <t>140 000 € (0.93 €/m²)</t>
+  </si>
+  <si>
+    <t>90560030123</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/valmiera/hkhpm.html</t>
+  </si>
+  <si>
+    <t>42 000 € (30.59 €/m²)</t>
+  </si>
+  <si>
+    <t>1373 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/ventspils/bjhge.html</t>
+  </si>
+  <si>
+    <t>35 000 € (14.49 €/m²)</t>
+  </si>
+  <si>
+    <t>2415 m²</t>
   </si>
 </sst>
 </file>
@@ -25038,302 +25173,302 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>8142</v>
+        <v>8182</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>8143</v>
+        <v>8183</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>1218</v>
+        <v>8</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>4499</v>
+        <v>8184</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>1371</v>
+        <v>8185</v>
       </c>
       <c r="F2" s="3">
-        <v>45945.44097222222</v>
+        <v>45945.87777777778</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>8144</v>
+        <v>8186</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>3063</v>
+        <v>8187</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1569</v>
+        <v>419</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>171</v>
+        <v>683</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>10</v>
+        <v>8188</v>
       </c>
       <c r="F3" s="3">
-        <v>45945.56736111111</v>
+        <v>45946.44861111111</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>8145</v>
+        <v>8189</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>8146</v>
+        <v>729</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>1733</v>
+        <v>772</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>1430</v>
+        <v>32</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>8147</v>
+        <v>8190</v>
       </c>
       <c r="F4" s="3">
-        <v>45945.54791666666</v>
+        <v>45945.87430555555</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>8148</v>
+        <v>8191</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>8149</v>
+        <v>8192</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>2846</v>
+        <v>1218</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>325</v>
+        <v>8193</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>8150</v>
+        <v>8194</v>
       </c>
       <c r="F5" s="3">
-        <v>45945.4875</v>
+        <v>45946.45625</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>8151</v>
+        <v>8195</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>8152</v>
+        <v>8196</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>3868</v>
+        <v>1218</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>189</v>
+        <v>8197</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>8153</v>
+        <v>10</v>
       </c>
       <c r="F6" s="3">
-        <v>45945.50208333333</v>
+        <v>45945.975</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>8154</v>
+        <v>8198</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>8155</v>
+        <v>8199</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>4034</v>
+        <v>1218</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>4302</v>
+        <v>201</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>4303</v>
+        <v>10</v>
       </c>
       <c r="F7" s="3">
-        <v>45945.45763888889</v>
+        <v>45945.79236111111</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>8156</v>
+        <v>8200</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>8157</v>
+        <v>8201</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>4034</v>
+        <v>2846</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>436</v>
+        <v>2417</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="3">
-        <v>45945.4375</v>
+        <v>45945.768055555556</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>8158</v>
+        <v>8202</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>8159</v>
+        <v>8203</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>4034</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>2244</v>
+        <v>2998</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>8160</v>
+        <v>8204</v>
       </c>
       <c r="F9" s="3">
-        <v>45944.853472222225</v>
+        <v>45946.554861111115</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>8161</v>
+        <v>8205</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>8162</v>
+        <v>8206</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>4034</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>2912</v>
+        <v>4698</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>10</v>
+        <v>8207</v>
       </c>
       <c r="F10" s="3">
-        <v>45944.714583333334</v>
+        <v>45946.44930555555</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>8163</v>
+        <v>8208</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>8164</v>
+        <v>8209</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>4770</v>
+        <v>4671</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>4433</v>
+        <v>8210</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>8165</v>
+        <v>10</v>
       </c>
       <c r="F11" s="3">
-        <v>45945.57430555555</v>
+        <v>45946.3375</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>8166</v>
+        <v>8211</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>8167</v>
+        <v>8212</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>4770</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>32</v>
+        <v>8213</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>8168</v>
+        <v>8214</v>
       </c>
       <c r="F12" s="3">
-        <v>45945.56875</v>
+        <v>45945.70486111111</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>8169</v>
+        <v>8215</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>8170</v>
+        <v>8216</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>4770</v>
+        <v>5266</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>1913</v>
+        <v>201</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>8171</v>
+        <v>8217</v>
       </c>
       <c r="F13" s="3">
-        <v>45944.683333333334</v>
+        <v>45946.60833333334</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>8172</v>
+        <v>8218</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>8173</v>
+        <v>8219</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>5674</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>8174</v>
+        <v>2191</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>8175</v>
+        <v>8220</v>
       </c>
       <c r="F14" s="3">
-        <v>45945.38125</v>
+        <v>45945.839583333334</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>8176</v>
+        <v>8221</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>5831</v>
+        <v>8222</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>5674</v>
+        <v>6207</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>2912</v>
+        <v>8223</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>8177</v>
+        <v>10</v>
       </c>
       <c r="F15" s="3">
-        <v>45945.38055555556</v>
+        <v>45945.64444444445</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>8178</v>
+        <v>8224</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>8179</v>
+        <v>8225</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>6207</v>
+        <v>6439</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>8180</v>
+        <v>8226</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>8181</v>
+        <v>10</v>
       </c>
       <c r="F16" s="3">
-        <v>45945.18194444444</v>
+        <v>45946.56805555556</v>
       </c>
     </row>
   </sheetData>
@@ -25361,7 +25496,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2651"/>
+  <dimension ref="A1:F2666"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -78397,6 +78532,306 @@
       </c>
       <c r="F2651" s="3">
         <v>45943.85972222222</v>
+      </c>
+    </row>
+    <row r="2652" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2652" s="4" t="s">
+        <v>8142</v>
+      </c>
+      <c r="B2652" s="3" t="s">
+        <v>8143</v>
+      </c>
+      <c r="C2652" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2652" s="3" t="s">
+        <v>4499</v>
+      </c>
+      <c r="E2652" s="3" t="s">
+        <v>1371</v>
+      </c>
+      <c r="F2652" s="3">
+        <v>45945.44097222222</v>
+      </c>
+    </row>
+    <row r="2653" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2653" s="4" t="s">
+        <v>8144</v>
+      </c>
+      <c r="B2653" s="3" t="s">
+        <v>3063</v>
+      </c>
+      <c r="C2653" s="3" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D2653" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2653" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2653" s="3">
+        <v>45945.56736111111</v>
+      </c>
+    </row>
+    <row r="2654" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2654" s="4" t="s">
+        <v>8145</v>
+      </c>
+      <c r="B2654" s="3" t="s">
+        <v>8146</v>
+      </c>
+      <c r="C2654" s="3" t="s">
+        <v>1733</v>
+      </c>
+      <c r="D2654" s="3" t="s">
+        <v>1430</v>
+      </c>
+      <c r="E2654" s="3" t="s">
+        <v>8147</v>
+      </c>
+      <c r="F2654" s="3">
+        <v>45945.54791666666</v>
+      </c>
+    </row>
+    <row r="2655" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2655" s="4" t="s">
+        <v>8148</v>
+      </c>
+      <c r="B2655" s="3" t="s">
+        <v>8149</v>
+      </c>
+      <c r="C2655" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2655" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2655" s="3" t="s">
+        <v>8150</v>
+      </c>
+      <c r="F2655" s="3">
+        <v>45945.4875</v>
+      </c>
+    </row>
+    <row r="2656" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2656" s="4" t="s">
+        <v>8151</v>
+      </c>
+      <c r="B2656" s="3" t="s">
+        <v>8152</v>
+      </c>
+      <c r="C2656" s="3" t="s">
+        <v>3868</v>
+      </c>
+      <c r="D2656" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2656" s="3" t="s">
+        <v>8153</v>
+      </c>
+      <c r="F2656" s="3">
+        <v>45945.50208333333</v>
+      </c>
+    </row>
+    <row r="2657" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2657" s="4" t="s">
+        <v>8154</v>
+      </c>
+      <c r="B2657" s="3" t="s">
+        <v>8155</v>
+      </c>
+      <c r="C2657" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2657" s="3" t="s">
+        <v>4302</v>
+      </c>
+      <c r="E2657" s="3" t="s">
+        <v>4303</v>
+      </c>
+      <c r="F2657" s="3">
+        <v>45945.45763888889</v>
+      </c>
+    </row>
+    <row r="2658" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2658" s="4" t="s">
+        <v>8156</v>
+      </c>
+      <c r="B2658" s="3" t="s">
+        <v>8157</v>
+      </c>
+      <c r="C2658" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2658" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="E2658" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2658" s="3">
+        <v>45945.4375</v>
+      </c>
+    </row>
+    <row r="2659" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2659" s="4" t="s">
+        <v>8158</v>
+      </c>
+      <c r="B2659" s="3" t="s">
+        <v>8159</v>
+      </c>
+      <c r="C2659" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2659" s="3" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E2659" s="3" t="s">
+        <v>8160</v>
+      </c>
+      <c r="F2659" s="3">
+        <v>45944.853472222225</v>
+      </c>
+    </row>
+    <row r="2660" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2660" s="4" t="s">
+        <v>8161</v>
+      </c>
+      <c r="B2660" s="3" t="s">
+        <v>8162</v>
+      </c>
+      <c r="C2660" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2660" s="3" t="s">
+        <v>2912</v>
+      </c>
+      <c r="E2660" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2660" s="3">
+        <v>45944.714583333334</v>
+      </c>
+    </row>
+    <row r="2661" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2661" s="4" t="s">
+        <v>8163</v>
+      </c>
+      <c r="B2661" s="3" t="s">
+        <v>8164</v>
+      </c>
+      <c r="C2661" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2661" s="3" t="s">
+        <v>4433</v>
+      </c>
+      <c r="E2661" s="3" t="s">
+        <v>8165</v>
+      </c>
+      <c r="F2661" s="3">
+        <v>45945.57430555555</v>
+      </c>
+    </row>
+    <row r="2662" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2662" s="4" t="s">
+        <v>8166</v>
+      </c>
+      <c r="B2662" s="3" t="s">
+        <v>8167</v>
+      </c>
+      <c r="C2662" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2662" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2662" s="3" t="s">
+        <v>8168</v>
+      </c>
+      <c r="F2662" s="3">
+        <v>45945.56875</v>
+      </c>
+    </row>
+    <row r="2663" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2663" s="4" t="s">
+        <v>8169</v>
+      </c>
+      <c r="B2663" s="3" t="s">
+        <v>8170</v>
+      </c>
+      <c r="C2663" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2663" s="3" t="s">
+        <v>1913</v>
+      </c>
+      <c r="E2663" s="3" t="s">
+        <v>8171</v>
+      </c>
+      <c r="F2663" s="3">
+        <v>45944.683333333334</v>
+      </c>
+    </row>
+    <row r="2664" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2664" s="4" t="s">
+        <v>8172</v>
+      </c>
+      <c r="B2664" s="3" t="s">
+        <v>8173</v>
+      </c>
+      <c r="C2664" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2664" s="3" t="s">
+        <v>8174</v>
+      </c>
+      <c r="E2664" s="3" t="s">
+        <v>8175</v>
+      </c>
+      <c r="F2664" s="3">
+        <v>45945.38125</v>
+      </c>
+    </row>
+    <row r="2665" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2665" s="4" t="s">
+        <v>8176</v>
+      </c>
+      <c r="B2665" s="3" t="s">
+        <v>5831</v>
+      </c>
+      <c r="C2665" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2665" s="3" t="s">
+        <v>2912</v>
+      </c>
+      <c r="E2665" s="3" t="s">
+        <v>8177</v>
+      </c>
+      <c r="F2665" s="3">
+        <v>45945.38055555556</v>
+      </c>
+    </row>
+    <row r="2666" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2666" s="4" t="s">
+        <v>8178</v>
+      </c>
+      <c r="B2666" s="3" t="s">
+        <v>8179</v>
+      </c>
+      <c r="C2666" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2666" s="3" t="s">
+        <v>8180</v>
+      </c>
+      <c r="E2666" s="3" t="s">
+        <v>8181</v>
+      </c>
+      <c r="F2666" s="3">
+        <v>45945.18194444444</v>
       </c>
     </row>
   </sheetData>
@@ -81051,6 +81486,21 @@
     <hyperlink ref="A2649" r:id="rId2648"/>
     <hyperlink ref="A2650" r:id="rId2649"/>
     <hyperlink ref="A2651" r:id="rId2650"/>
+    <hyperlink ref="A2652" r:id="rId2651"/>
+    <hyperlink ref="A2653" r:id="rId2652"/>
+    <hyperlink ref="A2654" r:id="rId2653"/>
+    <hyperlink ref="A2655" r:id="rId2654"/>
+    <hyperlink ref="A2656" r:id="rId2655"/>
+    <hyperlink ref="A2657" r:id="rId2656"/>
+    <hyperlink ref="A2658" r:id="rId2657"/>
+    <hyperlink ref="A2659" r:id="rId2658"/>
+    <hyperlink ref="A2660" r:id="rId2659"/>
+    <hyperlink ref="A2661" r:id="rId2660"/>
+    <hyperlink ref="A2662" r:id="rId2661"/>
+    <hyperlink ref="A2663" r:id="rId2662"/>
+    <hyperlink ref="A2664" r:id="rId2663"/>
+    <hyperlink ref="A2665" r:id="rId2664"/>
+    <hyperlink ref="A2666" r:id="rId2665"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Update lands data - 2025-10-17 12:20
</commit_message>
<xml_diff>
--- a/lands-scraped.xlsx
+++ b/lands-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13412" uniqueCount="8227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13507" uniqueCount="8283">
   <si>
     <t>link</t>
   </si>
@@ -24699,6 +24699,174 @@
   </si>
   <si>
     <t>2415 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/bauska/bldfn.html</t>
+  </si>
+  <si>
+    <t>9 000 € (12.68 €/m²)</t>
+  </si>
+  <si>
+    <t>710 m²</t>
+  </si>
+  <si>
+    <t>40500010114</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/marsnenu-pag/jxcmd.html</t>
+  </si>
+  <si>
+    <t>6 000 € (0.57 €/m²)</t>
+  </si>
+  <si>
+    <t>42640030222</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/amatas-pag/ogbid.html</t>
+  </si>
+  <si>
+    <t>180 000 € (1.06 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/dobele-and-reg/dobeles-pag/hojkc.html</t>
+  </si>
+  <si>
+    <t>16 900 € (14.02 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/gulbene-and-reg/galgauskas-pag/kepbd.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jelgava/bddpgj.html</t>
+  </si>
+  <si>
+    <t>89 000 € (24.75 €/m²)</t>
+  </si>
+  <si>
+    <t>3596 m²</t>
+  </si>
+  <si>
+    <t>09000070224</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jelgava/dijlf.html</t>
+  </si>
+  <si>
+    <t>40 120 € (40 €/m²)</t>
+  </si>
+  <si>
+    <t>1003 m²</t>
+  </si>
+  <si>
+    <t>09000210930</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jelgava/bdcif.html</t>
+  </si>
+  <si>
+    <t>32 000 € (30.19 €/m²)</t>
+  </si>
+  <si>
+    <t>1060 m²</t>
+  </si>
+  <si>
+    <t>09000100152</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/cenu-pag/ancip.html</t>
+  </si>
+  <si>
+    <t>20 000 € (1.87 €/m²)</t>
+  </si>
+  <si>
+    <t>10700 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jelgava/bdomoc.html</t>
+  </si>
+  <si>
+    <t>28 500 € (18.58 €/m²)</t>
+  </si>
+  <si>
+    <t>1534 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kraslava-and-reg/dagdas-pag/beddh.html</t>
+  </si>
+  <si>
+    <t>60540040296</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/limbadzi-and-reg/salacgriva/bdioj.html</t>
+  </si>
+  <si>
+    <t>390 990 € (30 €/m²)</t>
+  </si>
+  <si>
+    <t>13033 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/madona-and-reg/vestienas-pag/decik.html</t>
+  </si>
+  <si>
+    <t>98 761 € (3.29 €/m²)</t>
+  </si>
+  <si>
+    <t>70960040091</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ikskile/afmgf.html</t>
+  </si>
+  <si>
+    <t>47 000 € (10.56 €/m²)</t>
+  </si>
+  <si>
+    <t>4450 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/kegums/cpfig.html</t>
+  </si>
+  <si>
+    <t>40 000 € (4 €/m²)</t>
+  </si>
+  <si>
+    <t>74090030087</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/kocenu-pag/cinix.html</t>
+  </si>
+  <si>
+    <t>9 500 € (4.10 €/m²)</t>
+  </si>
+  <si>
+    <t>2315 m²</t>
+  </si>
+  <si>
+    <t>96640140072</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/valmiera/bdlhnp.html</t>
+  </si>
+  <si>
+    <t>35 000 € (20.72 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/varves-pag/gjkic.html</t>
+  </si>
+  <si>
+    <t>16 500 € (6.60 €/m²)</t>
+  </si>
+  <si>
+    <t>98840010213</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/other/bjmkl.html</t>
+  </si>
+  <si>
+    <t>654 321 € (93.47 €/m²)</t>
+  </si>
+  <si>
+    <t>7352036Uk9375S0001Dj</t>
   </si>
 </sst>
 </file>
@@ -25134,7 +25302,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -25173,302 +25341,382 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>8182</v>
+        <v>8227</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>8183</v>
+        <v>8228</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>8</v>
+        <v>419</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>8184</v>
+        <v>8229</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>8185</v>
+        <v>8230</v>
       </c>
       <c r="F2" s="3">
-        <v>45945.87777777778</v>
+        <v>45946.691666666666</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>8186</v>
+        <v>8231</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>8187</v>
+        <v>8232</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>419</v>
+        <v>772</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>683</v>
+        <v>2454</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>8188</v>
+        <v>8233</v>
       </c>
       <c r="F3" s="3">
-        <v>45946.44861111111</v>
+        <v>45947.61319444445</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>8189</v>
+        <v>8234</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>729</v>
+        <v>8235</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>772</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>8190</v>
+        <v>10</v>
       </c>
       <c r="F4" s="3">
-        <v>45945.87430555555</v>
+        <v>45947.37986111111</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>8191</v>
+        <v>8236</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>8192</v>
+        <v>8237</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>1218</v>
+        <v>1569</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>8193</v>
+        <v>2135</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>8194</v>
+        <v>10</v>
       </c>
       <c r="F5" s="3">
-        <v>45946.45625</v>
+        <v>45946.648611111115</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>8195</v>
+        <v>8238</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>8196</v>
+        <v>1708</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1218</v>
+        <v>1671</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>8197</v>
+        <v>1709</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="3">
-        <v>45945.975</v>
+        <v>45947.507638888885</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>8198</v>
+        <v>8239</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>8199</v>
+        <v>8240</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>1218</v>
+        <v>1929</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>201</v>
+        <v>8241</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>10</v>
+        <v>8242</v>
       </c>
       <c r="F7" s="3">
-        <v>45945.79236111111</v>
+        <v>45947.63680555555</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>8200</v>
+        <v>8243</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>8201</v>
+        <v>8244</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>2846</v>
+        <v>1929</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>2417</v>
+        <v>8245</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>10</v>
+        <v>8246</v>
       </c>
       <c r="F8" s="3">
-        <v>45945.768055555556</v>
+        <v>45947.63333333333</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>8202</v>
+        <v>8247</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>8203</v>
+        <v>8248</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>4034</v>
+        <v>1929</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>2998</v>
+        <v>8249</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>8204</v>
+        <v>8250</v>
       </c>
       <c r="F9" s="3">
-        <v>45946.554861111115</v>
+        <v>45947.63333333333</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>8205</v>
+        <v>8251</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>8206</v>
+        <v>8252</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>4034</v>
+        <v>1929</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>4698</v>
+        <v>8253</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>8207</v>
+        <v>10</v>
       </c>
       <c r="F10" s="3">
-        <v>45946.44930555555</v>
+        <v>45947.586111111115</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>8208</v>
+        <v>8254</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>8209</v>
+        <v>8255</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>4671</v>
+        <v>1929</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>8210</v>
+        <v>8256</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F11" s="3">
-        <v>45946.3375</v>
+        <v>45947.41458333333</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>8211</v>
+        <v>8257</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>8212</v>
+        <v>2609</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>4770</v>
+        <v>2488</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>8213</v>
+        <v>407</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>8214</v>
+        <v>8258</v>
       </c>
       <c r="F12" s="3">
-        <v>45945.70486111111</v>
+        <v>45946.75555555556</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>8215</v>
+        <v>8259</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>8216</v>
+        <v>8260</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>5266</v>
+        <v>3398</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>201</v>
+        <v>8261</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>8217</v>
+        <v>10</v>
       </c>
       <c r="F13" s="3">
-        <v>45946.60833333334</v>
+        <v>45947.44236111111</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>8218</v>
+        <v>8262</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>8219</v>
+        <v>8263</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>5674</v>
+        <v>3868</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>2191</v>
+        <v>201</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>8220</v>
+        <v>8264</v>
       </c>
       <c r="F14" s="3">
-        <v>45945.839583333334</v>
+        <v>45946.975</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>8221</v>
+        <v>8265</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>8222</v>
+        <v>8266</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>6207</v>
+        <v>4034</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>8223</v>
+        <v>8267</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F15" s="3">
-        <v>45945.64444444445</v>
+        <v>45947.57916666666</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>8224</v>
+        <v>8268</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>8225</v>
+        <v>8269</v>
       </c>
       <c r="C16" s="9" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>8270</v>
+      </c>
+      <c r="F16" s="3">
+        <v>45946.85902777778</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>8271</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>8272</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>8273</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>8274</v>
+      </c>
+      <c r="F17" s="3">
+        <v>45947.600694444445</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>8275</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>8276</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>4220</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="3">
+        <v>45947.495833333334</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>8277</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>8278</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>6439</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>8226</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="3">
-        <v>45946.56805555556</v>
+      <c r="D19" s="9" t="s">
+        <v>1632</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>8279</v>
+      </c>
+      <c r="F19" s="3">
+        <v>45946.77569444444</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>8280</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>8281</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>8282</v>
+      </c>
+      <c r="F20" s="3">
+        <v>45946.96736111111</v>
       </c>
     </row>
   </sheetData>
@@ -25488,6 +25736,10 @@
     <hyperlink ref="A14" r:id="rId13"/>
     <hyperlink ref="A15" r:id="rId14"/>
     <hyperlink ref="A16" r:id="rId15"/>
+    <hyperlink ref="A17" r:id="rId16"/>
+    <hyperlink ref="A18" r:id="rId17"/>
+    <hyperlink ref="A19" r:id="rId18"/>
+    <hyperlink ref="A20" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -25496,7 +25748,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2666"/>
+  <dimension ref="A1:F2681"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -78832,6 +79084,306 @@
       </c>
       <c r="F2666" s="3">
         <v>45945.18194444444</v>
+      </c>
+    </row>
+    <row r="2667" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2667" s="4" t="s">
+        <v>8182</v>
+      </c>
+      <c r="B2667" s="3" t="s">
+        <v>8183</v>
+      </c>
+      <c r="C2667" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2667" s="3" t="s">
+        <v>8184</v>
+      </c>
+      <c r="E2667" s="3" t="s">
+        <v>8185</v>
+      </c>
+      <c r="F2667" s="3">
+        <v>45945.87777777778</v>
+      </c>
+    </row>
+    <row r="2668" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2668" s="4" t="s">
+        <v>8186</v>
+      </c>
+      <c r="B2668" s="3" t="s">
+        <v>8187</v>
+      </c>
+      <c r="C2668" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2668" s="3" t="s">
+        <v>683</v>
+      </c>
+      <c r="E2668" s="3" t="s">
+        <v>8188</v>
+      </c>
+      <c r="F2668" s="3">
+        <v>45946.44861111111</v>
+      </c>
+    </row>
+    <row r="2669" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2669" s="4" t="s">
+        <v>8189</v>
+      </c>
+      <c r="B2669" s="3" t="s">
+        <v>729</v>
+      </c>
+      <c r="C2669" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2669" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2669" s="3" t="s">
+        <v>8190</v>
+      </c>
+      <c r="F2669" s="3">
+        <v>45945.87430555555</v>
+      </c>
+    </row>
+    <row r="2670" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2670" s="4" t="s">
+        <v>8191</v>
+      </c>
+      <c r="B2670" s="3" t="s">
+        <v>8192</v>
+      </c>
+      <c r="C2670" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2670" s="3" t="s">
+        <v>8193</v>
+      </c>
+      <c r="E2670" s="3" t="s">
+        <v>8194</v>
+      </c>
+      <c r="F2670" s="3">
+        <v>45946.45625</v>
+      </c>
+    </row>
+    <row r="2671" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2671" s="4" t="s">
+        <v>8195</v>
+      </c>
+      <c r="B2671" s="3" t="s">
+        <v>8196</v>
+      </c>
+      <c r="C2671" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2671" s="3" t="s">
+        <v>8197</v>
+      </c>
+      <c r="E2671" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2671" s="3">
+        <v>45945.975</v>
+      </c>
+    </row>
+    <row r="2672" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2672" s="4" t="s">
+        <v>8198</v>
+      </c>
+      <c r="B2672" s="3" t="s">
+        <v>8199</v>
+      </c>
+      <c r="C2672" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D2672" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2672" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2672" s="3">
+        <v>45945.79236111111</v>
+      </c>
+    </row>
+    <row r="2673" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2673" s="4" t="s">
+        <v>8200</v>
+      </c>
+      <c r="B2673" s="3" t="s">
+        <v>8201</v>
+      </c>
+      <c r="C2673" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2673" s="3" t="s">
+        <v>2417</v>
+      </c>
+      <c r="E2673" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2673" s="3">
+        <v>45945.768055555556</v>
+      </c>
+    </row>
+    <row r="2674" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2674" s="4" t="s">
+        <v>8202</v>
+      </c>
+      <c r="B2674" s="3" t="s">
+        <v>8203</v>
+      </c>
+      <c r="C2674" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2674" s="3" t="s">
+        <v>2998</v>
+      </c>
+      <c r="E2674" s="3" t="s">
+        <v>8204</v>
+      </c>
+      <c r="F2674" s="3">
+        <v>45946.554861111115</v>
+      </c>
+    </row>
+    <row r="2675" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2675" s="4" t="s">
+        <v>8205</v>
+      </c>
+      <c r="B2675" s="3" t="s">
+        <v>8206</v>
+      </c>
+      <c r="C2675" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2675" s="3" t="s">
+        <v>4698</v>
+      </c>
+      <c r="E2675" s="3" t="s">
+        <v>8207</v>
+      </c>
+      <c r="F2675" s="3">
+        <v>45946.44930555555</v>
+      </c>
+    </row>
+    <row r="2676" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2676" s="4" t="s">
+        <v>8208</v>
+      </c>
+      <c r="B2676" s="3" t="s">
+        <v>8209</v>
+      </c>
+      <c r="C2676" s="3" t="s">
+        <v>4671</v>
+      </c>
+      <c r="D2676" s="3" t="s">
+        <v>8210</v>
+      </c>
+      <c r="E2676" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2676" s="3">
+        <v>45946.3375</v>
+      </c>
+    </row>
+    <row r="2677" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2677" s="4" t="s">
+        <v>8211</v>
+      </c>
+      <c r="B2677" s="3" t="s">
+        <v>8212</v>
+      </c>
+      <c r="C2677" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2677" s="3" t="s">
+        <v>8213</v>
+      </c>
+      <c r="E2677" s="3" t="s">
+        <v>8214</v>
+      </c>
+      <c r="F2677" s="3">
+        <v>45945.70486111111</v>
+      </c>
+    </row>
+    <row r="2678" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2678" s="4" t="s">
+        <v>8215</v>
+      </c>
+      <c r="B2678" s="3" t="s">
+        <v>8216</v>
+      </c>
+      <c r="C2678" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2678" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2678" s="3" t="s">
+        <v>8217</v>
+      </c>
+      <c r="F2678" s="3">
+        <v>45946.60833333334</v>
+      </c>
+    </row>
+    <row r="2679" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2679" s="4" t="s">
+        <v>8218</v>
+      </c>
+      <c r="B2679" s="3" t="s">
+        <v>8219</v>
+      </c>
+      <c r="C2679" s="3" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2679" s="3" t="s">
+        <v>2191</v>
+      </c>
+      <c r="E2679" s="3" t="s">
+        <v>8220</v>
+      </c>
+      <c r="F2679" s="3">
+        <v>45945.839583333334</v>
+      </c>
+    </row>
+    <row r="2680" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2680" s="4" t="s">
+        <v>8221</v>
+      </c>
+      <c r="B2680" s="3" t="s">
+        <v>8222</v>
+      </c>
+      <c r="C2680" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2680" s="3" t="s">
+        <v>8223</v>
+      </c>
+      <c r="E2680" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2680" s="3">
+        <v>45945.64444444445</v>
+      </c>
+    </row>
+    <row r="2681" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2681" s="4" t="s">
+        <v>8224</v>
+      </c>
+      <c r="B2681" s="3" t="s">
+        <v>8225</v>
+      </c>
+      <c r="C2681" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2681" s="3" t="s">
+        <v>8226</v>
+      </c>
+      <c r="E2681" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2681" s="3">
+        <v>45946.56805555556</v>
       </c>
     </row>
   </sheetData>
@@ -81501,6 +82053,21 @@
     <hyperlink ref="A2664" r:id="rId2663"/>
     <hyperlink ref="A2665" r:id="rId2664"/>
     <hyperlink ref="A2666" r:id="rId2665"/>
+    <hyperlink ref="A2667" r:id="rId2666"/>
+    <hyperlink ref="A2668" r:id="rId2667"/>
+    <hyperlink ref="A2669" r:id="rId2668"/>
+    <hyperlink ref="A2670" r:id="rId2669"/>
+    <hyperlink ref="A2671" r:id="rId2670"/>
+    <hyperlink ref="A2672" r:id="rId2671"/>
+    <hyperlink ref="A2673" r:id="rId2672"/>
+    <hyperlink ref="A2674" r:id="rId2673"/>
+    <hyperlink ref="A2675" r:id="rId2674"/>
+    <hyperlink ref="A2676" r:id="rId2675"/>
+    <hyperlink ref="A2677" r:id="rId2676"/>
+    <hyperlink ref="A2678" r:id="rId2677"/>
+    <hyperlink ref="A2679" r:id="rId2678"/>
+    <hyperlink ref="A2680" r:id="rId2679"/>
+    <hyperlink ref="A2681" r:id="rId2680"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Update lands data - 2025-10-20 12:22
</commit_message>
<xml_diff>
--- a/lands-scraped.xlsx
+++ b/lands-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13507" uniqueCount="8283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13702" uniqueCount="8388">
   <si>
     <t>link</t>
   </si>
@@ -24867,6 +24867,321 @@
   </si>
   <si>
     <t>7352036Uk9375S0001Dj</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/aizkraukle-and-reg/serenes-pag/afmik.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/aizkraukle-and-reg/seces-pag/fkxjx.html</t>
+  </si>
+  <si>
+    <t>32780050049</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/aizkraukle-and-reg/seces-pag/chokn.html</t>
+  </si>
+  <si>
+    <t>270 000 € (0.96 €/m²)</t>
+  </si>
+  <si>
+    <t>32780050048</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/aizkraukle-and-reg/zalves-pag/jkhfx.html</t>
+  </si>
+  <si>
+    <t>25 000 € (0.25 €/m²)</t>
+  </si>
+  <si>
+    <t>32960120103</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/iecavas-nov/bdkxgh.html</t>
+  </si>
+  <si>
+    <t>40640020145</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/drabesu-pag/bboolc.html</t>
+  </si>
+  <si>
+    <t>62 000 € (3.10 €/m²)</t>
+  </si>
+  <si>
+    <t>42460010227</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/cesis/aoeki.html</t>
+  </si>
+  <si>
+    <t>100 000 € (10.08 €/m²)</t>
+  </si>
+  <si>
+    <t>9918 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/priekulu-pag/gkpnp.html</t>
+  </si>
+  <si>
+    <t>23 000 € (0.89 €/m²)</t>
+  </si>
+  <si>
+    <t>25900 m²</t>
+  </si>
+  <si>
+    <t>42720090053</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/drabesu-pag/dkehh.html</t>
+  </si>
+  <si>
+    <t>57 000 € (2.85 €/m²)</t>
+  </si>
+  <si>
+    <t>42460020503</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jekabpils-and-reg/salas-pag/aimcc.html</t>
+  </si>
+  <si>
+    <t>52 000 € (0.40 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/valgundes-nov/cgdok.html</t>
+  </si>
+  <si>
+    <t>150 000 € (0.71 €/m²)</t>
+  </si>
+  <si>
+    <t>54860070028</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/jelgava/fxlhj.html</t>
+  </si>
+  <si>
+    <t>140 800 € (21.83 €/m²)</t>
+  </si>
+  <si>
+    <t>6450 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/cenu-pag/ihjbo.html</t>
+  </si>
+  <si>
+    <t>30 000 € (13.26 €/m²)</t>
+  </si>
+  <si>
+    <t>2262 m²</t>
+  </si>
+  <si>
+    <t>54440020424</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/livberzes-pag/benpjb.html</t>
+  </si>
+  <si>
+    <t>85 000 € (1.21 €/m²)</t>
+  </si>
+  <si>
+    <t>54620070003</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/svetes-pag/dboel.html</t>
+  </si>
+  <si>
+    <t>12 695 € (0.91 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/svetes-pag/accmf.html</t>
+  </si>
+  <si>
+    <t>177 777 € (3.11 €/m²)</t>
+  </si>
+  <si>
+    <t>57200 m²</t>
+  </si>
+  <si>
+    <t>54820030015</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kraslava-and-reg/skeltovas-pag/cbfki.html</t>
+  </si>
+  <si>
+    <t>60940050113</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/priekule/bfngox.html</t>
+  </si>
+  <si>
+    <t>15 000 € (0.84 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/liepaja/dbmje.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/liepaja/edjph.html</t>
+  </si>
+  <si>
+    <t>14 000 € (20 €/m²)</t>
+  </si>
+  <si>
+    <t>4064760021878</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/limbadzi-and-reg/liepupes-pag/dflnd.html</t>
+  </si>
+  <si>
+    <t>8 500 € (1.06 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ludza-and-reg/mezvidu-pag/cjkin.html</t>
+  </si>
+  <si>
+    <t>47 700 € (0.48 €/m²)</t>
+  </si>
+  <si>
+    <t>68700030088</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/madona-and-reg/sausnejas-pag/cfompg.html</t>
+  </si>
+  <si>
+    <t>584 200 € (0.46 €/m²)</t>
+  </si>
+  <si>
+    <t>127 ha.</t>
+  </si>
+  <si>
+    <t>70920010012</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/lielvarde/hecln.html</t>
+  </si>
+  <si>
+    <t>7 500 € (1 €/m²)</t>
+  </si>
+  <si>
+    <t>0.75 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/rembates-pag/bfknen.html</t>
+  </si>
+  <si>
+    <t>15 000 € (8.33 €/m²)</t>
+  </si>
+  <si>
+    <t>74840040281</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ogresgala-pag/djjpk.html</t>
+  </si>
+  <si>
+    <t>23 500 € (12.03 €/m²)</t>
+  </si>
+  <si>
+    <t>74800041362</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ogre-and-reg/ogre/anegk.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/cornajas-pag/bkdpi.html</t>
+  </si>
+  <si>
+    <t>22 000 € (0.37 €/m²)</t>
+  </si>
+  <si>
+    <t>78460050014</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/rezekne/enpdl.html</t>
+  </si>
+  <si>
+    <t>150 000 € (8.33 €/m²)</t>
+  </si>
+  <si>
+    <t>21000020036</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/kolkas-pag/edbmh.html</t>
+  </si>
+  <si>
+    <t>60 000 € (13.95 €/m²)</t>
+  </si>
+  <si>
+    <t>88620070141</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valka-and-reg/valka/glmfj.html</t>
+  </si>
+  <si>
+    <t>24 000 € (1.12 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valka-and-reg/strenci/kfien.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/valmiera/ahmeo.html</t>
+  </si>
+  <si>
+    <t>1 125 000 € (16 €/m²)</t>
+  </si>
+  <si>
+    <t>70313 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/valmiera/ajflk.html</t>
+  </si>
+  <si>
+    <t>42 000 € (25.41 €/m²)</t>
+  </si>
+  <si>
+    <t>1653 m²</t>
+  </si>
+  <si>
+    <t>96010041129</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/kocenu-pag/ddonl.html</t>
+  </si>
+  <si>
+    <t>200 000 € (6.67 €/m²)</t>
+  </si>
+  <si>
+    <t>96640120146</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/vilpulkas-pag/gcmpe.html</t>
+  </si>
+  <si>
+    <t>220 000 € (0.55 €/m²)</t>
+  </si>
+  <si>
+    <t>39.70 ha.</t>
+  </si>
+  <si>
+    <t>96940040037</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/piltenes-l-t/hmppb.html</t>
+  </si>
+  <si>
+    <t>9833-003-0041</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/ventspils/cgiki.html</t>
+  </si>
+  <si>
+    <t>20 000 € (9.88 €/m²)</t>
+  </si>
+  <si>
+    <t>27000260743</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/ventspils-and-reg/varves-pag/bgehfl.html</t>
+  </si>
+  <si>
+    <t>9 000 € (3 €/m²)</t>
   </si>
 </sst>
 </file>
@@ -25302,7 +25617,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -25341,382 +25656,782 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>8227</v>
+        <v>8283</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>8228</v>
+        <v>7317</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>419</v>
+        <v>8</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>8229</v>
+        <v>71</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>8230</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3">
-        <v>45946.691666666666</v>
+        <v>45949.85208333333</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>8231</v>
+        <v>8284</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>8232</v>
+        <v>7913</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>772</v>
+        <v>8</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>2454</v>
+        <v>325</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>8233</v>
+        <v>8285</v>
       </c>
       <c r="F3" s="3">
-        <v>45947.61319444445</v>
+        <v>45948.00138888889</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>8234</v>
+        <v>8286</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>8235</v>
+        <v>8287</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>772</v>
+        <v>8</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>100</v>
+        <v>1063</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>10</v>
+        <v>8288</v>
       </c>
       <c r="F4" s="3">
-        <v>45947.37986111111</v>
+        <v>45948.00138888889</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>8236</v>
+        <v>8289</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>8237</v>
+        <v>8290</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>1569</v>
+        <v>8</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>2135</v>
+        <v>325</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>10</v>
+        <v>8291</v>
       </c>
       <c r="F5" s="3">
-        <v>45946.648611111115</v>
+        <v>45947.66736111111</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>8238</v>
+        <v>8292</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>1708</v>
+        <v>5315</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1671</v>
+        <v>419</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>1709</v>
+        <v>201</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>10</v>
+        <v>8293</v>
       </c>
       <c r="F6" s="3">
-        <v>45947.507638888885</v>
+        <v>45950.367361111115</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>8239</v>
+        <v>8294</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>8240</v>
+        <v>8295</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>1929</v>
+        <v>772</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>8241</v>
+        <v>171</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>8242</v>
+        <v>8296</v>
       </c>
       <c r="F7" s="3">
-        <v>45947.63680555555</v>
+        <v>45950.3875</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>8243</v>
+        <v>8297</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>8244</v>
+        <v>8298</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1929</v>
+        <v>772</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>8245</v>
+        <v>8299</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>8246</v>
+        <v>6782</v>
       </c>
       <c r="F8" s="3">
-        <v>45947.63333333333</v>
+        <v>45949.76944444445</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>8247</v>
+        <v>8300</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>8248</v>
+        <v>8301</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>1929</v>
+        <v>772</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>8249</v>
+        <v>8302</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>8250</v>
+        <v>8303</v>
       </c>
       <c r="F9" s="3">
-        <v>45947.63333333333</v>
+        <v>45949.56458333333</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>8251</v>
+        <v>8304</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>8252</v>
+        <v>8305</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>1929</v>
+        <v>772</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>8253</v>
+        <v>171</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>10</v>
+        <v>8306</v>
       </c>
       <c r="F10" s="3">
-        <v>45947.586111111115</v>
+        <v>45947.87361111111</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>8254</v>
+        <v>8307</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>8255</v>
+        <v>8308</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>1929</v>
+        <v>1733</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>8256</v>
+        <v>474</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F11" s="3">
-        <v>45947.41458333333</v>
+        <v>45950.50625</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>8257</v>
+        <v>8309</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>2609</v>
+        <v>8310</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>2488</v>
+        <v>1929</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>407</v>
+        <v>1709</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>8258</v>
+        <v>8311</v>
       </c>
       <c r="F12" s="3">
-        <v>45946.75555555556</v>
+        <v>45950.63055555556</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>8259</v>
+        <v>8312</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>8260</v>
+        <v>8313</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>3398</v>
+        <v>1929</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>8261</v>
+        <v>8314</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="3">
-        <v>45947.44236111111</v>
+        <v>45949.93819444445</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>8262</v>
+        <v>8315</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>8263</v>
+        <v>8316</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>3868</v>
+        <v>1929</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>201</v>
+        <v>8317</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>8264</v>
+        <v>8318</v>
       </c>
       <c r="F14" s="3">
-        <v>45946.975</v>
+        <v>45949.86875</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>8265</v>
+        <v>8319</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>8266</v>
+        <v>8320</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>4034</v>
+        <v>1929</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>8267</v>
+        <v>407</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>10</v>
+        <v>8321</v>
       </c>
       <c r="F15" s="3">
-        <v>45947.57916666666</v>
+        <v>45949.680555555555</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>8268</v>
+        <v>8322</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>8269</v>
+        <v>8323</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>4034</v>
+        <v>1929</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>32</v>
+        <v>5650</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>8270</v>
+        <v>10</v>
       </c>
       <c r="F16" s="3">
-        <v>45946.85902777778</v>
+        <v>45948.64791666667</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>8271</v>
+        <v>8324</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>8272</v>
+        <v>8325</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>6207</v>
+        <v>1929</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>8273</v>
+        <v>8326</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>8274</v>
+        <v>8327</v>
       </c>
       <c r="F17" s="3">
-        <v>45947.600694444445</v>
+        <v>45948.64166666666</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>8275</v>
+        <v>8328</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>8276</v>
+        <v>6317</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>6207</v>
+        <v>2488</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>4220</v>
+        <v>383</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>10</v>
+        <v>8329</v>
       </c>
       <c r="F18" s="3">
-        <v>45947.495833333334</v>
+        <v>45947.941666666666</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>8277</v>
+        <v>8330</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>8278</v>
+        <v>8331</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>6439</v>
+        <v>2846</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>1632</v>
+        <v>1203</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>8279</v>
+        <v>10</v>
       </c>
       <c r="F19" s="3">
-        <v>45946.77569444444</v>
+        <v>45950.58472222222</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>8280</v>
+        <v>8332</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>8281</v>
+        <v>2973</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>1194</v>
+        <v>2846</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>9</v>
+        <v>2974</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>8282</v>
+        <v>10</v>
       </c>
       <c r="F20" s="3">
-        <v>45946.96736111111</v>
+        <v>45950.37361111111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>8333</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>8334</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>3349</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>8335</v>
+      </c>
+      <c r="F21" s="3">
+        <v>45949.944444444445</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>8336</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>8337</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>2030</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="3">
+        <v>45948.54305555555</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>8338</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>8339</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>8340</v>
+      </c>
+      <c r="F23" s="3">
+        <v>45949.930555555555</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>8341</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>8342</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>3868</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>8343</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>8344</v>
+      </c>
+      <c r="F24" s="3">
+        <v>45950.54375</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>8345</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>8346</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>8347</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="3">
+        <v>45950.575</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>8348</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>8349</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>1618</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>8350</v>
+      </c>
+      <c r="F26" s="3">
+        <v>45947.89722222222</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>8351</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>8352</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>4399</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>8353</v>
+      </c>
+      <c r="F27" s="3">
+        <v>45947.78055555555</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>8354</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="3">
+        <v>45947.7375</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>8355</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>8356</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>8357</v>
+      </c>
+      <c r="F29" s="3">
+        <v>45949.705555555556</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>8358</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>8359</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>4254</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>8360</v>
+      </c>
+      <c r="F30" s="3">
+        <v>45949.429861111115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>8361</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>8362</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>2082</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>8363</v>
+      </c>
+      <c r="F31" s="3">
+        <v>45950.615277777775</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>8364</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>8365</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>6133</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>6196</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>6197</v>
+      </c>
+      <c r="F32" s="3">
+        <v>45950.48888888889</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>8366</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>6911</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>6133</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>6912</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="3">
+        <v>45950.4125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>8367</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>8368</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>8369</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="3">
+        <v>45949.81319444445</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>8370</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>8371</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>8372</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>8373</v>
+      </c>
+      <c r="F35" s="3">
+        <v>45949.81319444445</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>8374</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>8375</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>8376</v>
+      </c>
+      <c r="F36" s="3">
+        <v>45949.8125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>8377</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>8378</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>8379</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>8380</v>
+      </c>
+      <c r="F37" s="3">
+        <v>45947.691666666666</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>8381</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>6371</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>1416</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>8382</v>
+      </c>
+      <c r="F38" s="3">
+        <v>45950.50069444445</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>8383</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>8384</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>5377</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>8385</v>
+      </c>
+      <c r="F39" s="3">
+        <v>45949.48263888889</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>8386</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>8387</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="3">
+        <v>45948.44027777778</v>
       </c>
     </row>
   </sheetData>
@@ -25740,6 +26455,26 @@
     <hyperlink ref="A18" r:id="rId17"/>
     <hyperlink ref="A19" r:id="rId18"/>
     <hyperlink ref="A20" r:id="rId19"/>
+    <hyperlink ref="A21" r:id="rId20"/>
+    <hyperlink ref="A22" r:id="rId21"/>
+    <hyperlink ref="A23" r:id="rId22"/>
+    <hyperlink ref="A24" r:id="rId23"/>
+    <hyperlink ref="A25" r:id="rId24"/>
+    <hyperlink ref="A26" r:id="rId25"/>
+    <hyperlink ref="A27" r:id="rId26"/>
+    <hyperlink ref="A28" r:id="rId27"/>
+    <hyperlink ref="A29" r:id="rId28"/>
+    <hyperlink ref="A30" r:id="rId29"/>
+    <hyperlink ref="A31" r:id="rId30"/>
+    <hyperlink ref="A32" r:id="rId31"/>
+    <hyperlink ref="A33" r:id="rId32"/>
+    <hyperlink ref="A34" r:id="rId33"/>
+    <hyperlink ref="A35" r:id="rId34"/>
+    <hyperlink ref="A36" r:id="rId35"/>
+    <hyperlink ref="A37" r:id="rId36"/>
+    <hyperlink ref="A38" r:id="rId37"/>
+    <hyperlink ref="A39" r:id="rId38"/>
+    <hyperlink ref="A40" r:id="rId39"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -25748,7 +26483,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2681"/>
+  <dimension ref="A1:F2700"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -79384,6 +80119,386 @@
       </c>
       <c r="F2681" s="3">
         <v>45946.56805555556</v>
+      </c>
+    </row>
+    <row r="2682" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2682" s="4" t="s">
+        <v>8227</v>
+      </c>
+      <c r="B2682" s="3" t="s">
+        <v>8228</v>
+      </c>
+      <c r="C2682" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2682" s="3" t="s">
+        <v>8229</v>
+      </c>
+      <c r="E2682" s="3" t="s">
+        <v>8230</v>
+      </c>
+      <c r="F2682" s="3">
+        <v>45946.691666666666</v>
+      </c>
+    </row>
+    <row r="2683" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2683" s="4" t="s">
+        <v>8231</v>
+      </c>
+      <c r="B2683" s="3" t="s">
+        <v>8232</v>
+      </c>
+      <c r="C2683" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2683" s="3" t="s">
+        <v>2454</v>
+      </c>
+      <c r="E2683" s="3" t="s">
+        <v>8233</v>
+      </c>
+      <c r="F2683" s="3">
+        <v>45947.61319444445</v>
+      </c>
+    </row>
+    <row r="2684" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2684" s="4" t="s">
+        <v>8234</v>
+      </c>
+      <c r="B2684" s="3" t="s">
+        <v>8235</v>
+      </c>
+      <c r="C2684" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2684" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2684" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2684" s="3">
+        <v>45947.37986111111</v>
+      </c>
+    </row>
+    <row r="2685" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2685" s="4" t="s">
+        <v>8236</v>
+      </c>
+      <c r="B2685" s="3" t="s">
+        <v>8237</v>
+      </c>
+      <c r="C2685" s="3" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D2685" s="3" t="s">
+        <v>2135</v>
+      </c>
+      <c r="E2685" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2685" s="3">
+        <v>45946.648611111115</v>
+      </c>
+    </row>
+    <row r="2686" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2686" s="4" t="s">
+        <v>8238</v>
+      </c>
+      <c r="B2686" s="3" t="s">
+        <v>1708</v>
+      </c>
+      <c r="C2686" s="3" t="s">
+        <v>1671</v>
+      </c>
+      <c r="D2686" s="3" t="s">
+        <v>1709</v>
+      </c>
+      <c r="E2686" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2686" s="3">
+        <v>45947.507638888885</v>
+      </c>
+    </row>
+    <row r="2687" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2687" s="4" t="s">
+        <v>8239</v>
+      </c>
+      <c r="B2687" s="3" t="s">
+        <v>8240</v>
+      </c>
+      <c r="C2687" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2687" s="3" t="s">
+        <v>8241</v>
+      </c>
+      <c r="E2687" s="3" t="s">
+        <v>8242</v>
+      </c>
+      <c r="F2687" s="3">
+        <v>45947.63680555555</v>
+      </c>
+    </row>
+    <row r="2688" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2688" s="4" t="s">
+        <v>8243</v>
+      </c>
+      <c r="B2688" s="3" t="s">
+        <v>8244</v>
+      </c>
+      <c r="C2688" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2688" s="3" t="s">
+        <v>8245</v>
+      </c>
+      <c r="E2688" s="3" t="s">
+        <v>8246</v>
+      </c>
+      <c r="F2688" s="3">
+        <v>45947.63333333333</v>
+      </c>
+    </row>
+    <row r="2689" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2689" s="4" t="s">
+        <v>8247</v>
+      </c>
+      <c r="B2689" s="3" t="s">
+        <v>8248</v>
+      </c>
+      <c r="C2689" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2689" s="3" t="s">
+        <v>8249</v>
+      </c>
+      <c r="E2689" s="3" t="s">
+        <v>8250</v>
+      </c>
+      <c r="F2689" s="3">
+        <v>45947.63333333333</v>
+      </c>
+    </row>
+    <row r="2690" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2690" s="4" t="s">
+        <v>8251</v>
+      </c>
+      <c r="B2690" s="3" t="s">
+        <v>8252</v>
+      </c>
+      <c r="C2690" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2690" s="3" t="s">
+        <v>8253</v>
+      </c>
+      <c r="E2690" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2690" s="3">
+        <v>45947.586111111115</v>
+      </c>
+    </row>
+    <row r="2691" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2691" s="4" t="s">
+        <v>8254</v>
+      </c>
+      <c r="B2691" s="3" t="s">
+        <v>8255</v>
+      </c>
+      <c r="C2691" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2691" s="3" t="s">
+        <v>8256</v>
+      </c>
+      <c r="E2691" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2691" s="3">
+        <v>45947.41458333333</v>
+      </c>
+    </row>
+    <row r="2692" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2692" s="4" t="s">
+        <v>8257</v>
+      </c>
+      <c r="B2692" s="3" t="s">
+        <v>2609</v>
+      </c>
+      <c r="C2692" s="3" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D2692" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="E2692" s="3" t="s">
+        <v>8258</v>
+      </c>
+      <c r="F2692" s="3">
+        <v>45946.75555555556</v>
+      </c>
+    </row>
+    <row r="2693" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2693" s="4" t="s">
+        <v>8259</v>
+      </c>
+      <c r="B2693" s="3" t="s">
+        <v>8260</v>
+      </c>
+      <c r="C2693" s="3" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D2693" s="3" t="s">
+        <v>8261</v>
+      </c>
+      <c r="E2693" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2693" s="3">
+        <v>45947.44236111111</v>
+      </c>
+    </row>
+    <row r="2694" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2694" s="4" t="s">
+        <v>8262</v>
+      </c>
+      <c r="B2694" s="3" t="s">
+        <v>8263</v>
+      </c>
+      <c r="C2694" s="3" t="s">
+        <v>3868</v>
+      </c>
+      <c r="D2694" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2694" s="3" t="s">
+        <v>8264</v>
+      </c>
+      <c r="F2694" s="3">
+        <v>45946.975</v>
+      </c>
+    </row>
+    <row r="2695" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2695" s="4" t="s">
+        <v>8265</v>
+      </c>
+      <c r="B2695" s="3" t="s">
+        <v>8266</v>
+      </c>
+      <c r="C2695" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2695" s="3" t="s">
+        <v>8267</v>
+      </c>
+      <c r="E2695" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2695" s="3">
+        <v>45947.57916666666</v>
+      </c>
+    </row>
+    <row r="2696" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2696" s="4" t="s">
+        <v>8268</v>
+      </c>
+      <c r="B2696" s="3" t="s">
+        <v>8269</v>
+      </c>
+      <c r="C2696" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2696" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2696" s="3" t="s">
+        <v>8270</v>
+      </c>
+      <c r="F2696" s="3">
+        <v>45946.85902777778</v>
+      </c>
+    </row>
+    <row r="2697" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2697" s="4" t="s">
+        <v>8271</v>
+      </c>
+      <c r="B2697" s="3" t="s">
+        <v>8272</v>
+      </c>
+      <c r="C2697" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2697" s="3" t="s">
+        <v>8273</v>
+      </c>
+      <c r="E2697" s="3" t="s">
+        <v>8274</v>
+      </c>
+      <c r="F2697" s="3">
+        <v>45947.600694444445</v>
+      </c>
+    </row>
+    <row r="2698" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2698" s="4" t="s">
+        <v>8275</v>
+      </c>
+      <c r="B2698" s="3" t="s">
+        <v>8276</v>
+      </c>
+      <c r="C2698" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2698" s="3" t="s">
+        <v>4220</v>
+      </c>
+      <c r="E2698" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2698" s="3">
+        <v>45947.495833333334</v>
+      </c>
+    </row>
+    <row r="2699" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2699" s="4" t="s">
+        <v>8277</v>
+      </c>
+      <c r="B2699" s="3" t="s">
+        <v>8278</v>
+      </c>
+      <c r="C2699" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2699" s="3" t="s">
+        <v>1632</v>
+      </c>
+      <c r="E2699" s="3" t="s">
+        <v>8279</v>
+      </c>
+      <c r="F2699" s="3">
+        <v>45946.77569444444</v>
+      </c>
+    </row>
+    <row r="2700" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2700" s="4" t="s">
+        <v>8280</v>
+      </c>
+      <c r="B2700" s="3" t="s">
+        <v>8281</v>
+      </c>
+      <c r="C2700" s="3" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D2700" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2700" s="3" t="s">
+        <v>8282</v>
+      </c>
+      <c r="F2700" s="3">
+        <v>45946.96736111111</v>
       </c>
     </row>
   </sheetData>
@@ -82068,6 +83183,25 @@
     <hyperlink ref="A2679" r:id="rId2678"/>
     <hyperlink ref="A2680" r:id="rId2679"/>
     <hyperlink ref="A2681" r:id="rId2680"/>
+    <hyperlink ref="A2682" r:id="rId2681"/>
+    <hyperlink ref="A2683" r:id="rId2682"/>
+    <hyperlink ref="A2684" r:id="rId2683"/>
+    <hyperlink ref="A2685" r:id="rId2684"/>
+    <hyperlink ref="A2686" r:id="rId2685"/>
+    <hyperlink ref="A2687" r:id="rId2686"/>
+    <hyperlink ref="A2688" r:id="rId2687"/>
+    <hyperlink ref="A2689" r:id="rId2688"/>
+    <hyperlink ref="A2690" r:id="rId2689"/>
+    <hyperlink ref="A2691" r:id="rId2690"/>
+    <hyperlink ref="A2692" r:id="rId2691"/>
+    <hyperlink ref="A2693" r:id="rId2692"/>
+    <hyperlink ref="A2694" r:id="rId2693"/>
+    <hyperlink ref="A2695" r:id="rId2694"/>
+    <hyperlink ref="A2696" r:id="rId2695"/>
+    <hyperlink ref="A2697" r:id="rId2696"/>
+    <hyperlink ref="A2698" r:id="rId2697"/>
+    <hyperlink ref="A2699" r:id="rId2698"/>
+    <hyperlink ref="A2700" r:id="rId2699"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Update lands data - 2025-10-21 12:22
</commit_message>
<xml_diff>
--- a/lands-scraped.xlsx
+++ b/lands-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13702" uniqueCount="8388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13877" uniqueCount="8490">
   <si>
     <t>link</t>
   </si>
@@ -25182,6 +25182,312 @@
   </si>
   <si>
     <t>9 000 € (3 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/balvi-and-reg/krisjanu-pag/bxjnjo.html</t>
+  </si>
+  <si>
+    <t>3 000 € (0.44 €/m²)</t>
+  </si>
+  <si>
+    <t>0.68 ha.</t>
+  </si>
+  <si>
+    <t>38560040093</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/bauska-and-reg/bauska/ggccj.html</t>
+  </si>
+  <si>
+    <t>635 000 € (18.17 €/m²)</t>
+  </si>
+  <si>
+    <t>34953 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/cesis-and-reg/inesu-pag/ahiml.html</t>
+  </si>
+  <si>
+    <t>59 000 € (0.74 €/m²)</t>
+  </si>
+  <si>
+    <t>42540020314</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/naujenes-pag/hhjgf.html</t>
+  </si>
+  <si>
+    <t>750 000 € (2.03 €/m²)</t>
+  </si>
+  <si>
+    <t>4474 002 0403</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/daugavpils/eljjp.html</t>
+  </si>
+  <si>
+    <t>599 000 € (14.98 €/m²)</t>
+  </si>
+  <si>
+    <t>0500 011 0503</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/medumu-pag/lxgbn.html</t>
+  </si>
+  <si>
+    <t>6 500 € (0.32 €/m²)</t>
+  </si>
+  <si>
+    <t>2.03 ha.</t>
+  </si>
+  <si>
+    <t>44720020036</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/daugavpils-and-reg/liksnas-pag/diiei.html</t>
+  </si>
+  <si>
+    <t>3.91 ha.</t>
+  </si>
+  <si>
+    <t>44680050439</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/dobele-and-reg/bukaisu-pag/npxxm.html</t>
+  </si>
+  <si>
+    <t>46560010010</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/gulbene-and-reg/stradu-pag/ngnlm.html</t>
+  </si>
+  <si>
+    <t>8 000 € (0.34 €/m²)</t>
+  </si>
+  <si>
+    <t>2.37 ha.</t>
+  </si>
+  <si>
+    <t>50900060106</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jekabpils-and-reg/kuku-pag/cikfo.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/jelgava-and-reg/valgundes-nov/ceejf.html</t>
+  </si>
+  <si>
+    <t>54860130855</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kraslava-and-reg/skaistas-pag/ikefl.html</t>
+  </si>
+  <si>
+    <t>40 000 € (0.47 €/m²)</t>
+  </si>
+  <si>
+    <t>60880030029</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kraslava-and-reg/kastulinas-pag/cmpxj.html</t>
+  </si>
+  <si>
+    <t>23 000 € (0.43 €/m²)</t>
+  </si>
+  <si>
+    <t>60720080102</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kuldiga-and-reg/kuldiga/ahhkd.html</t>
+  </si>
+  <si>
+    <t>22 000 € (18.33 €/m²)</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/kuldiga-and-reg/kuldiga/eedkb.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/liepaja-and-reg/medzes-pag/cgglin.html</t>
+  </si>
+  <si>
+    <t>20 000 € (0.61 €/m²)</t>
+  </si>
+  <si>
+    <t>3.29 ha.</t>
+  </si>
+  <si>
+    <t>64760030022</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/limbadzi-and-reg/ainazi/gjbhi.html</t>
+  </si>
+  <si>
+    <t>30 765 € (21 €/m²)</t>
+  </si>
+  <si>
+    <t>1465 m²</t>
+  </si>
+  <si>
+    <t>66050060048</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/madona-and-reg/metrienas-pag/cggmce.html</t>
+  </si>
+  <si>
+    <t>25 000 € (0.51 €/m²)</t>
+  </si>
+  <si>
+    <t>4.90 ha.</t>
+  </si>
+  <si>
+    <t>70760080050</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/madona-and-reg/laudonas-pag/ljpof.html</t>
+  </si>
+  <si>
+    <t>29 000 € (0.36 €/m²)</t>
+  </si>
+  <si>
+    <t>70700020055</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/preili-and-reg/rozupes-pag/ilhic.html</t>
+  </si>
+  <si>
+    <t>76660080228</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/preili-and-reg/varkavas-pag/hnnxx.html</t>
+  </si>
+  <si>
+    <t>76940030221</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/silmalas-pag/bdxddo.html</t>
+  </si>
+  <si>
+    <t>15 000 € (0.41 €/m²)</t>
+  </si>
+  <si>
+    <t>3.70 ha.</t>
+  </si>
+  <si>
+    <t>78880030133</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/griskanu-pag/bdkjci.html</t>
+  </si>
+  <si>
+    <t>32 500 € (2.50 €/m²)</t>
+  </si>
+  <si>
+    <t>78560040413</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/silmalas-pag/aifmf.html</t>
+  </si>
+  <si>
+    <t>26 400 € (0.38 €/m²)</t>
+  </si>
+  <si>
+    <t>78880030036</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/sakstagala-pag/bllenj.html</t>
+  </si>
+  <si>
+    <t>62 240 € (0.39 €/m²)</t>
+  </si>
+  <si>
+    <t>78860060178</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/sokolku-pag/bhkjmk.html</t>
+  </si>
+  <si>
+    <t>41 400 € (0.40 €/m²)</t>
+  </si>
+  <si>
+    <t>10.35 ha.</t>
+  </si>
+  <si>
+    <t>78900050227</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/sokolku-pag/omxfg.html</t>
+  </si>
+  <si>
+    <t>27 600 € (0.40 €/m²)</t>
+  </si>
+  <si>
+    <t>78900050247</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/rezekne-and-reg/sokolku-pag/afcin.html</t>
+  </si>
+  <si>
+    <t>60 800 € (0.41 €/m²)</t>
+  </si>
+  <si>
+    <t>7890 005 0090</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/talsi-and-reg/laucienes-pag/bpxdc.html</t>
+  </si>
+  <si>
+    <t>49 000 € (0.38 €/m²)</t>
+  </si>
+  <si>
+    <t>88700100099</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/kandava/bdolc.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/zentenes-pag/imxig.html</t>
+  </si>
+  <si>
+    <t>14 000 € (0.51 €/m²)</t>
+  </si>
+  <si>
+    <t>2.74 ha.</t>
+  </si>
+  <si>
+    <t>90960030057</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/zentenes-pag/ieinp.html</t>
+  </si>
+  <si>
+    <t>10 000 € (0.42 €/m²)</t>
+  </si>
+  <si>
+    <t>2.36 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/kandavas-pag/afmme.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/tukums-and-reg/smardes-pag/dnmig.html</t>
+  </si>
+  <si>
+    <t>100 000 € (28.62 €/m²)</t>
+  </si>
+  <si>
+    <t>3494 m²</t>
+  </si>
+  <si>
+    <t>90820100481</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/plots-and-lands/valmiera-and-reg/valmiera/bdoedp.html</t>
+  </si>
+  <si>
+    <t>90 000 € (49.40 €/m²)</t>
+  </si>
+  <si>
+    <t>1822 m²</t>
   </si>
 </sst>
 </file>
@@ -25617,7 +25923,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -25656,782 +25962,702 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>8283</v>
+        <v>8388</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>7317</v>
+        <v>8389</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>8</v>
+        <v>324</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>71</v>
+        <v>8390</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>10</v>
+        <v>8391</v>
       </c>
       <c r="F2" s="3">
-        <v>45949.85208333333</v>
+        <v>45950.773611111115</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>8284</v>
+        <v>8392</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>7913</v>
+        <v>8393</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>8</v>
+        <v>419</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>325</v>
+        <v>8394</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>8285</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3">
-        <v>45948.00138888889</v>
+        <v>45950.64027777778</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>8286</v>
+        <v>8395</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>8287</v>
+        <v>8396</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>8</v>
+        <v>772</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>1063</v>
+        <v>1416</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>8288</v>
+        <v>8397</v>
       </c>
       <c r="F4" s="3">
-        <v>45948.00138888889</v>
+        <v>45950.75277777778</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>8289</v>
+        <v>8398</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>8290</v>
+        <v>8399</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>8</v>
+        <v>1218</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>325</v>
+        <v>508</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>8291</v>
+        <v>8400</v>
       </c>
       <c r="F5" s="3">
-        <v>45947.66736111111</v>
+        <v>45951.51597222222</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>8292</v>
+        <v>8401</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>5315</v>
+        <v>8402</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>419</v>
+        <v>1218</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>201</v>
+        <v>353</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>8293</v>
+        <v>8403</v>
       </c>
       <c r="F6" s="3">
-        <v>45950.367361111115</v>
+        <v>45951.51458333334</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>8294</v>
+        <v>8404</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>8295</v>
+        <v>8405</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>772</v>
+        <v>1218</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>171</v>
+        <v>8406</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>8296</v>
+        <v>8407</v>
       </c>
       <c r="F7" s="3">
-        <v>45950.3875</v>
+        <v>45951.39513888889</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>8297</v>
+        <v>8408</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>8298</v>
+        <v>3867</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>772</v>
+        <v>1218</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>8299</v>
+        <v>8409</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>6782</v>
+        <v>8410</v>
       </c>
       <c r="F8" s="3">
-        <v>45949.76944444445</v>
+        <v>45950.64513888889</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>8300</v>
+        <v>8411</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>8301</v>
+        <v>200</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>772</v>
+        <v>1569</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>8302</v>
+        <v>201</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>8303</v>
+        <v>8412</v>
       </c>
       <c r="F9" s="3">
-        <v>45949.56458333333</v>
+        <v>45951.475</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>8304</v>
+        <v>8413</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>8305</v>
+        <v>8414</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>772</v>
+        <v>1671</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>171</v>
+        <v>8415</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>8306</v>
+        <v>8416</v>
       </c>
       <c r="F10" s="3">
-        <v>45947.87361111111</v>
+        <v>45951.506944444445</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>8307</v>
+        <v>8417</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>8308</v>
+        <v>1834</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>1733</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>474</v>
+        <v>108</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>10</v>
+        <v>1835</v>
       </c>
       <c r="F11" s="3">
-        <v>45950.50625</v>
+        <v>45951.59027777778</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>8309</v>
+        <v>8418</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>8310</v>
+        <v>2194</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>1929</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>1709</v>
+        <v>171</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>8311</v>
+        <v>8419</v>
       </c>
       <c r="F12" s="3">
-        <v>45950.63055555556</v>
+        <v>45951.41527777778</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>8312</v>
+        <v>8420</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>8313</v>
+        <v>8421</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>1929</v>
+        <v>2488</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>8314</v>
+        <v>1621</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>10</v>
+        <v>8422</v>
       </c>
       <c r="F13" s="3">
-        <v>45949.93819444445</v>
+        <v>45951.44236111111</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>8315</v>
+        <v>8423</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>8316</v>
+        <v>8424</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>1929</v>
+        <v>2488</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>8317</v>
+        <v>858</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>8318</v>
+        <v>8425</v>
       </c>
       <c r="F14" s="3">
-        <v>45949.86875</v>
+        <v>45950.75347222222</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>8319</v>
+        <v>8426</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>8320</v>
+        <v>8427</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>1929</v>
+        <v>2671</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>407</v>
+        <v>436</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>8321</v>
+        <v>10</v>
       </c>
       <c r="F15" s="3">
-        <v>45949.680555555555</v>
+        <v>45950.82986111111</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>8322</v>
+        <v>8428</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>8323</v>
+        <v>2688</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>1929</v>
+        <v>2671</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>5650</v>
+        <v>596</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F16" s="3">
-        <v>45948.64791666667</v>
+        <v>45950.77083333333</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>8324</v>
+        <v>8429</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>8325</v>
+        <v>8430</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>1929</v>
+        <v>2846</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>8326</v>
+        <v>8431</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>8327</v>
+        <v>8432</v>
       </c>
       <c r="F17" s="3">
-        <v>45948.64166666666</v>
+        <v>45950.69930555555</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>8328</v>
+        <v>8433</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>6317</v>
+        <v>8434</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>2488</v>
+        <v>3398</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>383</v>
+        <v>8435</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>8329</v>
+        <v>8436</v>
       </c>
       <c r="F18" s="3">
-        <v>45947.941666666666</v>
+        <v>45951.49722222222</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>8330</v>
+        <v>8437</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>8331</v>
+        <v>8438</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>2846</v>
+        <v>3868</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>1203</v>
+        <v>8439</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>10</v>
+        <v>8440</v>
       </c>
       <c r="F19" s="3">
-        <v>45950.58472222222</v>
+        <v>45951.49652777778</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>8332</v>
+        <v>8441</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>2973</v>
+        <v>8442</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>2846</v>
+        <v>3868</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>2974</v>
+        <v>1416</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>10</v>
+        <v>8443</v>
       </c>
       <c r="F20" s="3">
-        <v>45950.37361111111</v>
+        <v>45951.39375</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>8333</v>
+        <v>8444</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>8334</v>
+        <v>4309</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>2846</v>
+        <v>4671</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>3349</v>
+        <v>171</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>8335</v>
+        <v>8445</v>
       </c>
       <c r="F21" s="3">
-        <v>45949.944444444445</v>
+        <v>45951.52638888889</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>8336</v>
+        <v>8446</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>8337</v>
+        <v>8414</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>3398</v>
+        <v>4671</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>2030</v>
+        <v>8415</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>10</v>
+        <v>8447</v>
       </c>
       <c r="F22" s="3">
-        <v>45948.54305555555</v>
+        <v>45951.38333333333</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>8338</v>
+        <v>8448</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>8339</v>
+        <v>8449</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>3762</v>
+        <v>4770</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>325</v>
+        <v>8450</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>8340</v>
+        <v>8451</v>
       </c>
       <c r="F23" s="3">
-        <v>45949.930555555555</v>
+        <v>45951.586111111115</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>8341</v>
+        <v>8452</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>8342</v>
+        <v>8453</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>3868</v>
+        <v>4770</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>8343</v>
+        <v>1391</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>8344</v>
+        <v>8454</v>
       </c>
       <c r="F24" s="3">
-        <v>45950.54375</v>
+        <v>45951.48541666666</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>8345</v>
+        <v>8455</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>8346</v>
+        <v>8456</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>4034</v>
+        <v>4770</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>8347</v>
+        <v>407</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>10</v>
+        <v>8457</v>
       </c>
       <c r="F25" s="3">
-        <v>45950.575</v>
+        <v>45950.85972222222</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>8348</v>
+        <v>8458</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>8349</v>
+        <v>8459</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>4034</v>
+        <v>4770</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>1618</v>
+        <v>575</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>8350</v>
+        <v>8460</v>
       </c>
       <c r="F26" s="3">
-        <v>45947.89722222222</v>
+        <v>45950.853472222225</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>8351</v>
+        <v>8461</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>8352</v>
+        <v>8462</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>4034</v>
+        <v>4770</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>4399</v>
+        <v>8463</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>8353</v>
+        <v>8464</v>
       </c>
       <c r="F27" s="3">
-        <v>45947.78055555555</v>
+        <v>45950.84722222222</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>8354</v>
+        <v>8465</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>316</v>
+        <v>8466</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>4034</v>
+        <v>4770</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>317</v>
+        <v>2667</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>10</v>
+        <v>8467</v>
       </c>
       <c r="F28" s="3">
-        <v>45947.7375</v>
+        <v>45950.77777777778</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>8355</v>
+        <v>8468</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>8356</v>
+        <v>8469</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>4770</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>383</v>
+        <v>2191</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>8357</v>
+        <v>8470</v>
       </c>
       <c r="F29" s="3">
-        <v>45949.705555555556</v>
+        <v>45950.77083333333</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>8358</v>
+        <v>8471</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>8359</v>
+        <v>8472</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>4770</v>
+        <v>5266</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>4254</v>
+        <v>474</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>8360</v>
+        <v>8473</v>
       </c>
       <c r="F30" s="3">
-        <v>45949.429861111115</v>
+        <v>45951.39236111111</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>8361</v>
+        <v>8474</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>8362</v>
+        <v>6015</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>5266</v>
+        <v>5674</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>2082</v>
+        <v>6016</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>8363</v>
+        <v>10</v>
       </c>
       <c r="F31" s="3">
-        <v>45950.615277777775</v>
+        <v>45951.52847222222</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>8364</v>
+        <v>8475</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>8365</v>
+        <v>8476</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>6133</v>
+        <v>5674</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>6196</v>
+        <v>8477</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>6197</v>
+        <v>8478</v>
       </c>
       <c r="F32" s="3">
-        <v>45950.48888888889</v>
+        <v>45951.525</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>8366</v>
+        <v>8479</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>6911</v>
+        <v>8480</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>6133</v>
+        <v>5674</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>6912</v>
+        <v>8481</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>10</v>
+        <v>8478</v>
       </c>
       <c r="F33" s="3">
-        <v>45950.4125</v>
+        <v>45951.523611111115</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>8367</v>
+        <v>8482</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>8368</v>
+        <v>6013</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>6207</v>
+        <v>5674</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>8369</v>
+        <v>5295</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F34" s="3">
-        <v>45949.81319444445</v>
+        <v>45951.51527777778</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>8370</v>
+        <v>8483</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>8371</v>
+        <v>8484</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>6207</v>
+        <v>5674</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>8372</v>
+        <v>8485</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>8373</v>
+        <v>8486</v>
       </c>
       <c r="F35" s="3">
-        <v>45949.81319444445</v>
+        <v>45950.79791666666</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>8374</v>
+        <v>8487</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>8375</v>
+        <v>8488</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>6207</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>201</v>
+        <v>8489</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>8376</v>
+        <v>10</v>
       </c>
       <c r="F36" s="3">
-        <v>45949.8125</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
-        <v>8377</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>8378</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>6207</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>8379</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>8380</v>
-      </c>
-      <c r="F37" s="3">
-        <v>45947.691666666666</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>8381</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>6371</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>1416</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>8382</v>
-      </c>
-      <c r="F38" s="3">
-        <v>45950.50069444445</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>8383</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>8384</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>5377</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>8385</v>
-      </c>
-      <c r="F39" s="3">
-        <v>45949.48263888889</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>8386</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>8387</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>6439</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F40" s="3">
-        <v>45948.44027777778</v>
+        <v>45951.34583333333</v>
       </c>
     </row>
   </sheetData>
@@ -26471,10 +26697,6 @@
     <hyperlink ref="A34" r:id="rId33"/>
     <hyperlink ref="A35" r:id="rId34"/>
     <hyperlink ref="A36" r:id="rId35"/>
-    <hyperlink ref="A37" r:id="rId36"/>
-    <hyperlink ref="A38" r:id="rId37"/>
-    <hyperlink ref="A39" r:id="rId38"/>
-    <hyperlink ref="A40" r:id="rId39"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -26483,7 +26705,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2700"/>
+  <dimension ref="A1:F2739"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -80499,6 +80721,786 @@
       </c>
       <c r="F2700" s="3">
         <v>45946.96736111111</v>
+      </c>
+    </row>
+    <row r="2701" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2701" s="4" t="s">
+        <v>8283</v>
+      </c>
+      <c r="B2701" s="3" t="s">
+        <v>7317</v>
+      </c>
+      <c r="C2701" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2701" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2701" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2701" s="3">
+        <v>45949.85208333333</v>
+      </c>
+    </row>
+    <row r="2702" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2702" s="4" t="s">
+        <v>8284</v>
+      </c>
+      <c r="B2702" s="3" t="s">
+        <v>7913</v>
+      </c>
+      <c r="C2702" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2702" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2702" s="3" t="s">
+        <v>8285</v>
+      </c>
+      <c r="F2702" s="3">
+        <v>45948.00138888889</v>
+      </c>
+    </row>
+    <row r="2703" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2703" s="4" t="s">
+        <v>8286</v>
+      </c>
+      <c r="B2703" s="3" t="s">
+        <v>8287</v>
+      </c>
+      <c r="C2703" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2703" s="3" t="s">
+        <v>1063</v>
+      </c>
+      <c r="E2703" s="3" t="s">
+        <v>8288</v>
+      </c>
+      <c r="F2703" s="3">
+        <v>45948.00138888889</v>
+      </c>
+    </row>
+    <row r="2704" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2704" s="4" t="s">
+        <v>8289</v>
+      </c>
+      <c r="B2704" s="3" t="s">
+        <v>8290</v>
+      </c>
+      <c r="C2704" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2704" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2704" s="3" t="s">
+        <v>8291</v>
+      </c>
+      <c r="F2704" s="3">
+        <v>45947.66736111111</v>
+      </c>
+    </row>
+    <row r="2705" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2705" s="4" t="s">
+        <v>8292</v>
+      </c>
+      <c r="B2705" s="3" t="s">
+        <v>5315</v>
+      </c>
+      <c r="C2705" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2705" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2705" s="3" t="s">
+        <v>8293</v>
+      </c>
+      <c r="F2705" s="3">
+        <v>45950.367361111115</v>
+      </c>
+    </row>
+    <row r="2706" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2706" s="4" t="s">
+        <v>8294</v>
+      </c>
+      <c r="B2706" s="3" t="s">
+        <v>8295</v>
+      </c>
+      <c r="C2706" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2706" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2706" s="3" t="s">
+        <v>8296</v>
+      </c>
+      <c r="F2706" s="3">
+        <v>45950.3875</v>
+      </c>
+    </row>
+    <row r="2707" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2707" s="4" t="s">
+        <v>8297</v>
+      </c>
+      <c r="B2707" s="3" t="s">
+        <v>8298</v>
+      </c>
+      <c r="C2707" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2707" s="3" t="s">
+        <v>8299</v>
+      </c>
+      <c r="E2707" s="3" t="s">
+        <v>6782</v>
+      </c>
+      <c r="F2707" s="3">
+        <v>45949.76944444445</v>
+      </c>
+    </row>
+    <row r="2708" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2708" s="4" t="s">
+        <v>8300</v>
+      </c>
+      <c r="B2708" s="3" t="s">
+        <v>8301</v>
+      </c>
+      <c r="C2708" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2708" s="3" t="s">
+        <v>8302</v>
+      </c>
+      <c r="E2708" s="3" t="s">
+        <v>8303</v>
+      </c>
+      <c r="F2708" s="3">
+        <v>45949.56458333333</v>
+      </c>
+    </row>
+    <row r="2709" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2709" s="4" t="s">
+        <v>8304</v>
+      </c>
+      <c r="B2709" s="3" t="s">
+        <v>8305</v>
+      </c>
+      <c r="C2709" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D2709" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2709" s="3" t="s">
+        <v>8306</v>
+      </c>
+      <c r="F2709" s="3">
+        <v>45947.87361111111</v>
+      </c>
+    </row>
+    <row r="2710" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2710" s="4" t="s">
+        <v>8307</v>
+      </c>
+      <c r="B2710" s="3" t="s">
+        <v>8308</v>
+      </c>
+      <c r="C2710" s="3" t="s">
+        <v>1733</v>
+      </c>
+      <c r="D2710" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="E2710" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2710" s="3">
+        <v>45950.50625</v>
+      </c>
+    </row>
+    <row r="2711" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2711" s="4" t="s">
+        <v>8309</v>
+      </c>
+      <c r="B2711" s="3" t="s">
+        <v>8310</v>
+      </c>
+      <c r="C2711" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2711" s="3" t="s">
+        <v>1709</v>
+      </c>
+      <c r="E2711" s="3" t="s">
+        <v>8311</v>
+      </c>
+      <c r="F2711" s="3">
+        <v>45950.63055555556</v>
+      </c>
+    </row>
+    <row r="2712" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2712" s="4" t="s">
+        <v>8312</v>
+      </c>
+      <c r="B2712" s="3" t="s">
+        <v>8313</v>
+      </c>
+      <c r="C2712" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2712" s="3" t="s">
+        <v>8314</v>
+      </c>
+      <c r="E2712" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2712" s="3">
+        <v>45949.93819444445</v>
+      </c>
+    </row>
+    <row r="2713" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2713" s="4" t="s">
+        <v>8315</v>
+      </c>
+      <c r="B2713" s="3" t="s">
+        <v>8316</v>
+      </c>
+      <c r="C2713" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2713" s="3" t="s">
+        <v>8317</v>
+      </c>
+      <c r="E2713" s="3" t="s">
+        <v>8318</v>
+      </c>
+      <c r="F2713" s="3">
+        <v>45949.86875</v>
+      </c>
+    </row>
+    <row r="2714" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2714" s="4" t="s">
+        <v>8319</v>
+      </c>
+      <c r="B2714" s="3" t="s">
+        <v>8320</v>
+      </c>
+      <c r="C2714" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2714" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="E2714" s="3" t="s">
+        <v>8321</v>
+      </c>
+      <c r="F2714" s="3">
+        <v>45949.680555555555</v>
+      </c>
+    </row>
+    <row r="2715" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2715" s="4" t="s">
+        <v>8322</v>
+      </c>
+      <c r="B2715" s="3" t="s">
+        <v>8323</v>
+      </c>
+      <c r="C2715" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2715" s="3" t="s">
+        <v>5650</v>
+      </c>
+      <c r="E2715" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2715" s="3">
+        <v>45948.64791666667</v>
+      </c>
+    </row>
+    <row r="2716" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2716" s="4" t="s">
+        <v>8324</v>
+      </c>
+      <c r="B2716" s="3" t="s">
+        <v>8325</v>
+      </c>
+      <c r="C2716" s="3" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D2716" s="3" t="s">
+        <v>8326</v>
+      </c>
+      <c r="E2716" s="3" t="s">
+        <v>8327</v>
+      </c>
+      <c r="F2716" s="3">
+        <v>45948.64166666666</v>
+      </c>
+    </row>
+    <row r="2717" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2717" s="4" t="s">
+        <v>8328</v>
+      </c>
+      <c r="B2717" s="3" t="s">
+        <v>6317</v>
+      </c>
+      <c r="C2717" s="3" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D2717" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E2717" s="3" t="s">
+        <v>8329</v>
+      </c>
+      <c r="F2717" s="3">
+        <v>45947.941666666666</v>
+      </c>
+    </row>
+    <row r="2718" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2718" s="4" t="s">
+        <v>8330</v>
+      </c>
+      <c r="B2718" s="3" t="s">
+        <v>8331</v>
+      </c>
+      <c r="C2718" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2718" s="3" t="s">
+        <v>1203</v>
+      </c>
+      <c r="E2718" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2718" s="3">
+        <v>45950.58472222222</v>
+      </c>
+    </row>
+    <row r="2719" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2719" s="4" t="s">
+        <v>8332</v>
+      </c>
+      <c r="B2719" s="3" t="s">
+        <v>2973</v>
+      </c>
+      <c r="C2719" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2719" s="3" t="s">
+        <v>2974</v>
+      </c>
+      <c r="E2719" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2719" s="3">
+        <v>45950.37361111111</v>
+      </c>
+    </row>
+    <row r="2720" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2720" s="4" t="s">
+        <v>8333</v>
+      </c>
+      <c r="B2720" s="3" t="s">
+        <v>8334</v>
+      </c>
+      <c r="C2720" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D2720" s="3" t="s">
+        <v>3349</v>
+      </c>
+      <c r="E2720" s="3" t="s">
+        <v>8335</v>
+      </c>
+      <c r="F2720" s="3">
+        <v>45949.944444444445</v>
+      </c>
+    </row>
+    <row r="2721" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2721" s="4" t="s">
+        <v>8336</v>
+      </c>
+      <c r="B2721" s="3" t="s">
+        <v>8337</v>
+      </c>
+      <c r="C2721" s="3" t="s">
+        <v>3398</v>
+      </c>
+      <c r="D2721" s="3" t="s">
+        <v>2030</v>
+      </c>
+      <c r="E2721" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2721" s="3">
+        <v>45948.54305555555</v>
+      </c>
+    </row>
+    <row r="2722" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2722" s="4" t="s">
+        <v>8338</v>
+      </c>
+      <c r="B2722" s="3" t="s">
+        <v>8339</v>
+      </c>
+      <c r="C2722" s="3" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D2722" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2722" s="3" t="s">
+        <v>8340</v>
+      </c>
+      <c r="F2722" s="3">
+        <v>45949.930555555555</v>
+      </c>
+    </row>
+    <row r="2723" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2723" s="4" t="s">
+        <v>8341</v>
+      </c>
+      <c r="B2723" s="3" t="s">
+        <v>8342</v>
+      </c>
+      <c r="C2723" s="3" t="s">
+        <v>3868</v>
+      </c>
+      <c r="D2723" s="3" t="s">
+        <v>8343</v>
+      </c>
+      <c r="E2723" s="3" t="s">
+        <v>8344</v>
+      </c>
+      <c r="F2723" s="3">
+        <v>45950.54375</v>
+      </c>
+    </row>
+    <row r="2724" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2724" s="4" t="s">
+        <v>8345</v>
+      </c>
+      <c r="B2724" s="3" t="s">
+        <v>8346</v>
+      </c>
+      <c r="C2724" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2724" s="3" t="s">
+        <v>8347</v>
+      </c>
+      <c r="E2724" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2724" s="3">
+        <v>45950.575</v>
+      </c>
+    </row>
+    <row r="2725" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2725" s="4" t="s">
+        <v>8348</v>
+      </c>
+      <c r="B2725" s="3" t="s">
+        <v>8349</v>
+      </c>
+      <c r="C2725" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2725" s="3" t="s">
+        <v>1618</v>
+      </c>
+      <c r="E2725" s="3" t="s">
+        <v>8350</v>
+      </c>
+      <c r="F2725" s="3">
+        <v>45947.89722222222</v>
+      </c>
+    </row>
+    <row r="2726" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2726" s="4" t="s">
+        <v>8351</v>
+      </c>
+      <c r="B2726" s="3" t="s">
+        <v>8352</v>
+      </c>
+      <c r="C2726" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2726" s="3" t="s">
+        <v>4399</v>
+      </c>
+      <c r="E2726" s="3" t="s">
+        <v>8353</v>
+      </c>
+      <c r="F2726" s="3">
+        <v>45947.78055555555</v>
+      </c>
+    </row>
+    <row r="2727" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2727" s="4" t="s">
+        <v>8354</v>
+      </c>
+      <c r="B2727" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="C2727" s="3" t="s">
+        <v>4034</v>
+      </c>
+      <c r="D2727" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E2727" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2727" s="3">
+        <v>45947.7375</v>
+      </c>
+    </row>
+    <row r="2728" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2728" s="4" t="s">
+        <v>8355</v>
+      </c>
+      <c r="B2728" s="3" t="s">
+        <v>8356</v>
+      </c>
+      <c r="C2728" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2728" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E2728" s="3" t="s">
+        <v>8357</v>
+      </c>
+      <c r="F2728" s="3">
+        <v>45949.705555555556</v>
+      </c>
+    </row>
+    <row r="2729" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2729" s="4" t="s">
+        <v>8358</v>
+      </c>
+      <c r="B2729" s="3" t="s">
+        <v>8359</v>
+      </c>
+      <c r="C2729" s="3" t="s">
+        <v>4770</v>
+      </c>
+      <c r="D2729" s="3" t="s">
+        <v>4254</v>
+      </c>
+      <c r="E2729" s="3" t="s">
+        <v>8360</v>
+      </c>
+      <c r="F2729" s="3">
+        <v>45949.429861111115</v>
+      </c>
+    </row>
+    <row r="2730" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2730" s="4" t="s">
+        <v>8361</v>
+      </c>
+      <c r="B2730" s="3" t="s">
+        <v>8362</v>
+      </c>
+      <c r="C2730" s="3" t="s">
+        <v>5266</v>
+      </c>
+      <c r="D2730" s="3" t="s">
+        <v>2082</v>
+      </c>
+      <c r="E2730" s="3" t="s">
+        <v>8363</v>
+      </c>
+      <c r="F2730" s="3">
+        <v>45950.615277777775</v>
+      </c>
+    </row>
+    <row r="2731" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2731" s="4" t="s">
+        <v>8364</v>
+      </c>
+      <c r="B2731" s="3" t="s">
+        <v>8365</v>
+      </c>
+      <c r="C2731" s="3" t="s">
+        <v>6133</v>
+      </c>
+      <c r="D2731" s="3" t="s">
+        <v>6196</v>
+      </c>
+      <c r="E2731" s="3" t="s">
+        <v>6197</v>
+      </c>
+      <c r="F2731" s="3">
+        <v>45950.48888888889</v>
+      </c>
+    </row>
+    <row r="2732" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2732" s="4" t="s">
+        <v>8366</v>
+      </c>
+      <c r="B2732" s="3" t="s">
+        <v>6911</v>
+      </c>
+      <c r="C2732" s="3" t="s">
+        <v>6133</v>
+      </c>
+      <c r="D2732" s="3" t="s">
+        <v>6912</v>
+      </c>
+      <c r="E2732" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2732" s="3">
+        <v>45950.4125</v>
+      </c>
+    </row>
+    <row r="2733" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2733" s="4" t="s">
+        <v>8367</v>
+      </c>
+      <c r="B2733" s="3" t="s">
+        <v>8368</v>
+      </c>
+      <c r="C2733" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2733" s="3" t="s">
+        <v>8369</v>
+      </c>
+      <c r="E2733" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2733" s="3">
+        <v>45949.81319444445</v>
+      </c>
+    </row>
+    <row r="2734" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2734" s="4" t="s">
+        <v>8370</v>
+      </c>
+      <c r="B2734" s="3" t="s">
+        <v>8371</v>
+      </c>
+      <c r="C2734" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2734" s="3" t="s">
+        <v>8372</v>
+      </c>
+      <c r="E2734" s="3" t="s">
+        <v>8373</v>
+      </c>
+      <c r="F2734" s="3">
+        <v>45949.81319444445</v>
+      </c>
+    </row>
+    <row r="2735" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2735" s="4" t="s">
+        <v>8374</v>
+      </c>
+      <c r="B2735" s="3" t="s">
+        <v>8375</v>
+      </c>
+      <c r="C2735" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2735" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2735" s="3" t="s">
+        <v>8376</v>
+      </c>
+      <c r="F2735" s="3">
+        <v>45949.8125</v>
+      </c>
+    </row>
+    <row r="2736" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2736" s="4" t="s">
+        <v>8377</v>
+      </c>
+      <c r="B2736" s="3" t="s">
+        <v>8378</v>
+      </c>
+      <c r="C2736" s="3" t="s">
+        <v>6207</v>
+      </c>
+      <c r="D2736" s="3" t="s">
+        <v>8379</v>
+      </c>
+      <c r="E2736" s="3" t="s">
+        <v>8380</v>
+      </c>
+      <c r="F2736" s="3">
+        <v>45947.691666666666</v>
+      </c>
+    </row>
+    <row r="2737" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2737" s="4" t="s">
+        <v>8381</v>
+      </c>
+      <c r="B2737" s="3" t="s">
+        <v>6371</v>
+      </c>
+      <c r="C2737" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2737" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="E2737" s="3" t="s">
+        <v>8382</v>
+      </c>
+      <c r="F2737" s="3">
+        <v>45950.50069444445</v>
+      </c>
+    </row>
+    <row r="2738" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2738" s="4" t="s">
+        <v>8383</v>
+      </c>
+      <c r="B2738" s="3" t="s">
+        <v>8384</v>
+      </c>
+      <c r="C2738" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2738" s="3" t="s">
+        <v>5377</v>
+      </c>
+      <c r="E2738" s="3" t="s">
+        <v>8385</v>
+      </c>
+      <c r="F2738" s="3">
+        <v>45949.48263888889</v>
+      </c>
+    </row>
+    <row r="2739" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2739" s="4" t="s">
+        <v>8386</v>
+      </c>
+      <c r="B2739" s="3" t="s">
+        <v>8387</v>
+      </c>
+      <c r="C2739" s="3" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D2739" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E2739" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2739" s="3">
+        <v>45948.44027777778</v>
       </c>
     </row>
   </sheetData>
@@ -83202,6 +84204,45 @@
     <hyperlink ref="A2698" r:id="rId2697"/>
     <hyperlink ref="A2699" r:id="rId2698"/>
     <hyperlink ref="A2700" r:id="rId2699"/>
+    <hyperlink ref="A2701" r:id="rId2700"/>
+    <hyperlink ref="A2702" r:id="rId2701"/>
+    <hyperlink ref="A2703" r:id="rId2702"/>
+    <hyperlink ref="A2704" r:id="rId2703"/>
+    <hyperlink ref="A2705" r:id="rId2704"/>
+    <hyperlink ref="A2706" r:id="rId2705"/>
+    <hyperlink ref="A2707" r:id="rId2706"/>
+    <hyperlink ref="A2708" r:id="rId2707"/>
+    <hyperlink ref="A2709" r:id="rId2708"/>
+    <hyperlink ref="A2710" r:id="rId2709"/>
+    <hyperlink ref="A2711" r:id="rId2710"/>
+    <hyperlink ref="A2712" r:id="rId2711"/>
+    <hyperlink ref="A2713" r:id="rId2712"/>
+    <hyperlink ref="A2714" r:id="rId2713"/>
+    <hyperlink ref="A2715" r:id="rId2714"/>
+    <hyperlink ref="A2716" r:id="rId2715"/>
+    <hyperlink ref="A2717" r:id="rId2716"/>
+    <hyperlink ref="A2718" r:id="rId2717"/>
+    <hyperlink ref="A2719" r:id="rId2718"/>
+    <hyperlink ref="A2720" r:id="rId2719"/>
+    <hyperlink ref="A2721" r:id="rId2720"/>
+    <hyperlink ref="A2722" r:id="rId2721"/>
+    <hyperlink ref="A2723" r:id="rId2722"/>
+    <hyperlink ref="A2724" r:id="rId2723"/>
+    <hyperlink ref="A2725" r:id="rId2724"/>
+    <hyperlink ref="A2726" r:id="rId2725"/>
+    <hyperlink ref="A2727" r:id="rId2726"/>
+    <hyperlink ref="A2728" r:id="rId2727"/>
+    <hyperlink ref="A2729" r:id="rId2728"/>
+    <hyperlink ref="A2730" r:id="rId2729"/>
+    <hyperlink ref="A2731" r:id="rId2730"/>
+    <hyperlink ref="A2732" r:id="rId2731"/>
+    <hyperlink ref="A2733" r:id="rId2732"/>
+    <hyperlink ref="A2734" r:id="rId2733"/>
+    <hyperlink ref="A2735" r:id="rId2734"/>
+    <hyperlink ref="A2736" r:id="rId2735"/>
+    <hyperlink ref="A2737" r:id="rId2736"/>
+    <hyperlink ref="A2738" r:id="rId2737"/>
+    <hyperlink ref="A2739" r:id="rId2738"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>